<commit_message>
Reduced SVG to figure out flex problem
I reduced the SVG for bar graph to a simple square to understand how flex is stretching the dimensions.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6165E4B5-9643-6C46-90A9-81C768D9093C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E680E62-B785-884F-92D0-9274C6D8F278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="126">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -444,6 +444,9 @@
   </si>
   <si>
     <t>laterAmount</t>
+  </si>
+  <si>
+    <t>drag</t>
   </si>
 </sst>
 </file>
@@ -2929,11 +2932,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -3089,10 +3092,10 @@
         <v>10</v>
       </c>
       <c r="N3">
-        <v>480</v>
+        <v>100</v>
       </c>
       <c r="O3">
-        <v>480</v>
+        <v>100</v>
       </c>
       <c r="P3">
         <v>0.5</v>
@@ -3107,11 +3110,9 @@
         <v>6</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3" si="0">R3+P3</f>
         <v>6.5</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3" si="1">S3+Q3</f>
         <v>6.5</v>
       </c>
       <c r="V3" t="s">
@@ -3126,13 +3127,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="E4" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F4">
         <v>500</v>
@@ -3144,13 +3145,37 @@
         <v>1000</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>1500</v>
+      </c>
+      <c r="M4">
+        <v>10</v>
+      </c>
+      <c r="N4">
+        <v>100</v>
+      </c>
+      <c r="O4">
+        <v>100</v>
+      </c>
+      <c r="P4">
+        <v>0.5</v>
+      </c>
+      <c r="Q4">
+        <v>0.5</v>
+      </c>
+      <c r="R4">
+        <v>6</v>
+      </c>
+      <c r="S4">
+        <v>6</v>
       </c>
       <c r="T4">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="U4">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="V4" t="s">
         <v>121</v>
@@ -3158,7 +3183,7 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3193,7 +3218,7 @@
     </row>
     <row r="6" spans="1:22">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3220,16 +3245,16 @@
         <v>10</v>
       </c>
       <c r="L6">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="M6">
         <v>10</v>
       </c>
       <c r="N6">
-        <v>480</v>
+        <v>100</v>
       </c>
       <c r="O6">
-        <v>480</v>
+        <v>100</v>
       </c>
       <c r="P6">
         <v>0.5</v>
@@ -3244,55 +3269,13 @@
         <v>6</v>
       </c>
       <c r="T6">
-        <f t="shared" ref="T6:U6" si="2">R6+P6</f>
         <v>6.5</v>
       </c>
       <c r="U6">
-        <f t="shared" si="2"/>
         <v>6.5</v>
       </c>
       <c r="V6" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F7">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E8" t="s">
-        <v>124</v>
-      </c>
-      <c r="F8">
-        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Icon chart is working!
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48F8932-6DB6-1D41-AC52-602BFBACFA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300A5F4E-15D2-D941-BB0B-480B6555CC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="540" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="145">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -498,6 +498,12 @@
   </si>
   <si>
     <t>Calendar year view with bar and no interaction.</t>
+  </si>
+  <si>
+    <t>calendarIcon</t>
+  </si>
+  <si>
+    <t>Calendar year view with icon and no interaction.</t>
   </si>
 </sst>
 </file>
@@ -2985,11 +2991,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V28"/>
+  <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomLeft" activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -4397,6 +4403,147 @@
       </c>
       <c r="V28" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22">
+      <c r="A29">
+        <v>16</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>143</v>
+      </c>
+      <c r="D29" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" t="s">
+        <v>118</v>
+      </c>
+      <c r="F29">
+        <v>300</v>
+      </c>
+      <c r="H29" s="36">
+        <v>44593</v>
+      </c>
+      <c r="I29">
+        <v>700</v>
+      </c>
+      <c r="K29" s="36">
+        <v>44703</v>
+      </c>
+      <c r="L29">
+        <v>1100</v>
+      </c>
+      <c r="N29">
+        <v>100</v>
+      </c>
+      <c r="O29">
+        <v>100</v>
+      </c>
+      <c r="T29">
+        <v>10</v>
+      </c>
+      <c r="U29">
+        <v>8</v>
+      </c>
+      <c r="V29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22">
+      <c r="A30">
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D30" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30">
+        <v>500</v>
+      </c>
+      <c r="H30" s="36">
+        <v>44621</v>
+      </c>
+      <c r="I30">
+        <v>800</v>
+      </c>
+      <c r="K30" s="36">
+        <v>44724</v>
+      </c>
+      <c r="L30">
+        <v>1100</v>
+      </c>
+      <c r="N30">
+        <v>100</v>
+      </c>
+      <c r="O30">
+        <v>100</v>
+      </c>
+      <c r="T30">
+        <v>10</v>
+      </c>
+      <c r="U30">
+        <v>8</v>
+      </c>
+      <c r="V30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22">
+      <c r="A31">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>143</v>
+      </c>
+      <c r="D31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E31" t="s">
+        <v>118</v>
+      </c>
+      <c r="F31">
+        <v>300</v>
+      </c>
+      <c r="H31" s="36">
+        <v>44652</v>
+      </c>
+      <c r="I31">
+        <v>1000</v>
+      </c>
+      <c r="K31" s="36">
+        <v>44757</v>
+      </c>
+      <c r="L31">
+        <v>1100</v>
+      </c>
+      <c r="N31">
+        <v>100</v>
+      </c>
+      <c r="O31">
+        <v>100</v>
+      </c>
+      <c r="T31">
+        <v>10</v>
+      </c>
+      <c r="U31">
+        <v>8</v>
+      </c>
+      <c r="V31" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added month calendar icon test treatment.
Changed pound sign to dollar sign.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300A5F4E-15D2-D941-BB0B-480B6555CC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE96DAE8-440A-5041-8676-1CD305CE576B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="540" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="146">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -504,6 +504,9 @@
   </si>
   <si>
     <t>Calendar year view with icon and no interaction.</t>
+  </si>
+  <si>
+    <t>Calendar month view with icon and no interaction.</t>
   </si>
 </sst>
 </file>
@@ -2991,11 +2994,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V30" sqref="V30"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -4544,6 +4547,147 @@
       </c>
       <c r="V31" t="s">
         <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22">
+      <c r="A32">
+        <v>17</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>143</v>
+      </c>
+      <c r="D32" t="s">
+        <v>118</v>
+      </c>
+      <c r="E32" t="s">
+        <v>118</v>
+      </c>
+      <c r="F32">
+        <v>300</v>
+      </c>
+      <c r="H32" s="36">
+        <v>44593</v>
+      </c>
+      <c r="I32">
+        <v>700</v>
+      </c>
+      <c r="K32" s="36">
+        <v>44614</v>
+      </c>
+      <c r="L32">
+        <v>1100</v>
+      </c>
+      <c r="N32">
+        <v>100</v>
+      </c>
+      <c r="O32">
+        <v>100</v>
+      </c>
+      <c r="T32">
+        <v>8</v>
+      </c>
+      <c r="U32">
+        <v>8</v>
+      </c>
+      <c r="V32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22">
+      <c r="A33">
+        <v>17</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" t="s">
+        <v>118</v>
+      </c>
+      <c r="F33">
+        <v>500</v>
+      </c>
+      <c r="H33" s="36">
+        <v>44621</v>
+      </c>
+      <c r="I33">
+        <v>800</v>
+      </c>
+      <c r="K33" s="36">
+        <v>44632</v>
+      </c>
+      <c r="L33">
+        <v>1100</v>
+      </c>
+      <c r="N33">
+        <v>100</v>
+      </c>
+      <c r="O33">
+        <v>100</v>
+      </c>
+      <c r="T33">
+        <v>8</v>
+      </c>
+      <c r="U33">
+        <v>8</v>
+      </c>
+      <c r="V33" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22">
+      <c r="A34">
+        <v>17</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>143</v>
+      </c>
+      <c r="D34" t="s">
+        <v>118</v>
+      </c>
+      <c r="E34" t="s">
+        <v>118</v>
+      </c>
+      <c r="F34">
+        <v>300</v>
+      </c>
+      <c r="H34" s="36">
+        <v>44652</v>
+      </c>
+      <c r="I34">
+        <v>1000</v>
+      </c>
+      <c r="K34" s="36">
+        <v>44666</v>
+      </c>
+      <c r="L34">
+        <v>1100</v>
+      </c>
+      <c r="N34">
+        <v>100</v>
+      </c>
+      <c r="O34">
+        <v>100</v>
+      </c>
+      <c r="T34">
+        <v>8</v>
+      </c>
+      <c r="U34">
+        <v>8</v>
+      </c>
+      <c r="V34" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added icon chart calendar titration treatment.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE96DAE8-440A-5041-8676-1CD305CE576B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581F1F04-9486-DF41-8023-BCB09ADA0E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="540" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="147">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -507,6 +507,9 @@
   </si>
   <si>
     <t>Calendar month view with icon and no interaction.</t>
+  </si>
+  <si>
+    <t>Calendar month view with icon and titration interaction.</t>
   </si>
 </sst>
 </file>
@@ -2994,11 +2997,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V34"/>
+  <dimension ref="A1:V37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -4688,6 +4691,147 @@
       </c>
       <c r="V34" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22">
+      <c r="A35">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>143</v>
+      </c>
+      <c r="D35" t="s">
+        <v>117</v>
+      </c>
+      <c r="E35" t="s">
+        <v>124</v>
+      </c>
+      <c r="F35">
+        <v>300</v>
+      </c>
+      <c r="H35" s="36">
+        <v>44593</v>
+      </c>
+      <c r="I35">
+        <v>700</v>
+      </c>
+      <c r="K35" s="36">
+        <v>44614</v>
+      </c>
+      <c r="L35">
+        <v>1100</v>
+      </c>
+      <c r="N35">
+        <v>100</v>
+      </c>
+      <c r="O35">
+        <v>100</v>
+      </c>
+      <c r="T35">
+        <v>8</v>
+      </c>
+      <c r="U35">
+        <v>8</v>
+      </c>
+      <c r="V35" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22">
+      <c r="A36">
+        <v>18</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>143</v>
+      </c>
+      <c r="D36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E36" t="s">
+        <v>124</v>
+      </c>
+      <c r="F36">
+        <v>500</v>
+      </c>
+      <c r="H36" s="36">
+        <v>44621</v>
+      </c>
+      <c r="I36">
+        <v>800</v>
+      </c>
+      <c r="K36" s="36">
+        <v>44632</v>
+      </c>
+      <c r="L36">
+        <v>1100</v>
+      </c>
+      <c r="N36">
+        <v>100</v>
+      </c>
+      <c r="O36">
+        <v>100</v>
+      </c>
+      <c r="T36">
+        <v>8</v>
+      </c>
+      <c r="U36">
+        <v>8</v>
+      </c>
+      <c r="V36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22">
+      <c r="A37">
+        <v>18</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>143</v>
+      </c>
+      <c r="D37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E37" t="s">
+        <v>124</v>
+      </c>
+      <c r="F37">
+        <v>300</v>
+      </c>
+      <c r="H37" s="36">
+        <v>44652</v>
+      </c>
+      <c r="I37">
+        <v>1000</v>
+      </c>
+      <c r="K37" s="36">
+        <v>44666</v>
+      </c>
+      <c r="L37">
+        <v>1100</v>
+      </c>
+      <c r="N37">
+        <v>100</v>
+      </c>
+      <c r="O37">
+        <v>100</v>
+      </c>
+      <c r="T37">
+        <v>8</v>
+      </c>
+      <c r="U37">
+        <v>8</v>
+      </c>
+      <c r="V37" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added invalid survey link component.
Created a component for invalid survey link and used it for invalid URLs as well as invalid URL parameters.  Updated treatments with what was the latest in the excel file.  Added amount and months labels to axis on bar chart.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542C3430-4182-B545-87CF-CC97373839AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA5AAD1-30D2-FF44-ADD4-C2C23FC7C8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="2" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="1800" yWindow="500" windowWidth="35840" windowHeight="21060" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Web Parameters" sheetId="8" r:id="rId1"/>
@@ -869,23 +869,57 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -915,6 +949,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -929,58 +972,15 @@
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1297,9 +1297,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
   <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomLeft" activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1553,16 +1553,16 @@
         <v>100</v>
       </c>
       <c r="P5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T5">
         <v>8.5</v>
@@ -1615,16 +1615,16 @@
         <v>100</v>
       </c>
       <c r="P6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T6">
         <v>8.5</v>
@@ -1677,16 +1677,16 @@
         <v>100</v>
       </c>
       <c r="P7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R7">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S7">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="T7">
         <v>4.5</v>
@@ -3441,198 +3441,198 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="13" max="14" width="10.83203125" style="57"/>
+    <col min="13" max="14" width="10.83203125" style="37"/>
     <col min="15" max="15" width="10.83203125" style="11"/>
-    <col min="16" max="17" width="10.83203125" style="57"/>
+    <col min="16" max="17" width="10.83203125" style="37"/>
     <col min="18" max="18" width="10.83203125" style="11"/>
-    <col min="19" max="20" width="10.83203125" style="57"/>
+    <col min="19" max="20" width="10.83203125" style="37"/>
     <col min="21" max="21" width="10.83203125" style="11"/>
-    <col min="22" max="23" width="10.83203125" style="57"/>
+    <col min="22" max="23" width="10.83203125" style="37"/>
     <col min="24" max="24" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="76" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="73" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="77"/>
-      <c r="E1" s="76" t="s">
+      <c r="D1" s="74"/>
+      <c r="E1" s="73" t="s">
         <v>159</v>
       </c>
-      <c r="F1" s="77"/>
-      <c r="G1" s="76" t="s">
+      <c r="F1" s="74"/>
+      <c r="G1" s="73" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="77"/>
-      <c r="I1" s="76" t="s">
+      <c r="H1" s="74"/>
+      <c r="I1" s="73" t="s">
         <v>161</v>
       </c>
-      <c r="J1" s="77"/>
-      <c r="K1" s="60" t="s">
+      <c r="J1" s="74"/>
+      <c r="K1" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="M1" s="84" t="s">
+      <c r="M1" s="70" t="s">
         <v>162</v>
       </c>
-      <c r="N1" s="62"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="84" t="s">
+      <c r="N1" s="71"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="70" t="s">
         <v>163</v>
       </c>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="92"/>
-      <c r="S1" s="84" t="s">
+      <c r="Q1" s="71"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="70" t="s">
         <v>164</v>
       </c>
-      <c r="T1" s="62"/>
-      <c r="U1" s="92"/>
-      <c r="V1" s="61" t="s">
+      <c r="T1" s="71"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="72" t="s">
         <v>165</v>
       </c>
-      <c r="W1" s="62"/>
+      <c r="W1" s="71"/>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="74"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="68" t="s">
+      <c r="A2" s="52"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="H2" s="78" t="s">
+      <c r="H2" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="I2" s="68" t="s">
+      <c r="I2" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="J2" s="78" t="s">
+      <c r="J2" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="80" t="s">
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="N2" s="81" t="s">
+      <c r="N2" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="O2" s="93"/>
-      <c r="P2" s="83" t="s">
+      <c r="O2" s="68"/>
+      <c r="P2" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="Q2" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="R2" s="93"/>
-      <c r="S2" s="83" t="s">
+      <c r="R2" s="68"/>
+      <c r="S2" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="T2" s="72" t="s">
+      <c r="T2" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="U2" s="93"/>
-      <c r="V2" s="71" t="s">
+      <c r="U2" s="68"/>
+      <c r="V2" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="W2" s="72" t="s">
+      <c r="W2" s="50" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="75">
-        <v>1</v>
-      </c>
-      <c r="B3" s="64" t="s">
+      <c r="A3" s="53">
+        <v>1</v>
+      </c>
+      <c r="B3" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="63">
+      <c r="C3" s="41">
         <v>370</v>
       </c>
-      <c r="D3" s="79">
+      <c r="D3" s="55">
         <v>450</v>
       </c>
-      <c r="E3" s="63">
+      <c r="E3" s="41">
         <v>520</v>
       </c>
-      <c r="F3" s="79">
+      <c r="F3" s="55">
         <v>740</v>
       </c>
-      <c r="G3" s="63">
+      <c r="G3" s="41">
         <v>770</v>
       </c>
-      <c r="H3" s="79">
+      <c r="H3" s="55">
         <v>1480</v>
       </c>
-      <c r="I3" s="63">
+      <c r="I3" s="41">
         <v>900</v>
       </c>
-      <c r="J3" s="79">
+      <c r="J3" s="55">
         <v>1200</v>
       </c>
-      <c r="K3" s="64">
+      <c r="K3" s="42">
         <v>1.6</v>
       </c>
-      <c r="L3" s="64">
+      <c r="L3" s="42">
         <v>1.5</v>
       </c>
-      <c r="M3" s="82">
+      <c r="M3" s="58">
         <f>C3/$K$3*$L$3</f>
         <v>346.875</v>
       </c>
-      <c r="N3" s="66">
+      <c r="N3" s="44">
         <f>D3/$K$3*$L$3</f>
         <v>421.875</v>
       </c>
-      <c r="O3" s="94">
+      <c r="O3" s="69">
         <f>(N3-M3)/N3</f>
         <v>0.17777777777777778</v>
       </c>
-      <c r="P3" s="82">
+      <c r="P3" s="58">
         <f>E3/$K$3*$L$3</f>
         <v>487.5</v>
       </c>
-      <c r="Q3" s="66">
+      <c r="Q3" s="44">
         <f>F3/$K$3*$L$3</f>
         <v>693.75</v>
       </c>
-      <c r="R3" s="94">
+      <c r="R3" s="69">
         <f>(Q3-P3)/Q3</f>
         <v>0.29729729729729731</v>
       </c>
-      <c r="S3" s="82">
+      <c r="S3" s="58">
         <f>G3/$K$3*$L$3</f>
         <v>721.875</v>
       </c>
-      <c r="T3" s="66">
+      <c r="T3" s="44">
         <f>H3/$K$3*$L$3</f>
         <v>1387.5</v>
       </c>
-      <c r="U3" s="94">
+      <c r="U3" s="69">
         <f>(T3-S3)/T3</f>
         <v>0.47972972972972971</v>
       </c>
-      <c r="V3" s="65">
+      <c r="V3" s="43">
         <f>I3/$K$3*$L$3</f>
         <v>843.75</v>
       </c>
-      <c r="W3" s="66">
+      <c r="W3" s="44">
         <f>J3/$K$3*$L$3</f>
         <v>1125</v>
       </c>
@@ -3642,212 +3642,212 @@
       </c>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" s="75"/>
-      <c r="B4" s="64" t="s">
+      <c r="A4" s="53"/>
+      <c r="B4" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="C4" s="90">
+      <c r="C4" s="65">
         <v>37890</v>
       </c>
-      <c r="D4" s="91">
+      <c r="D4" s="66">
         <v>38163</v>
       </c>
-      <c r="E4" s="90">
+      <c r="E4" s="65">
         <v>37797</v>
       </c>
-      <c r="F4" s="91">
+      <c r="F4" s="66">
         <v>38317</v>
       </c>
-      <c r="G4" s="90">
+      <c r="G4" s="65">
         <v>37953</v>
       </c>
-      <c r="H4" s="91">
+      <c r="H4" s="66">
         <v>38863</v>
       </c>
-      <c r="I4" s="90">
+      <c r="I4" s="65">
         <v>37862</v>
       </c>
-      <c r="J4" s="91">
+      <c r="J4" s="66">
         <v>38254</v>
       </c>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="94"/>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="66"/>
-      <c r="R4" s="94"/>
-      <c r="S4" s="82"/>
-      <c r="T4" s="66"/>
-      <c r="U4" s="94"/>
-      <c r="V4" s="65"/>
-      <c r="W4" s="66"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="69"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="69"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="44"/>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="75"/>
-      <c r="B5" s="64" t="s">
+      <c r="A5" s="53"/>
+      <c r="B5" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="63">
+      <c r="C5" s="41">
         <v>4</v>
       </c>
-      <c r="D5" s="79">
+      <c r="D5" s="55">
         <v>13</v>
       </c>
-      <c r="E5" s="63">
+      <c r="E5" s="41">
         <v>2</v>
       </c>
-      <c r="F5" s="79">
+      <c r="F5" s="55">
         <v>18</v>
       </c>
-      <c r="G5" s="63">
+      <c r="G5" s="41">
         <v>6</v>
       </c>
-      <c r="H5" s="79">
+      <c r="H5" s="55">
         <v>36</v>
       </c>
-      <c r="I5" s="63">
-        <v>3</v>
-      </c>
-      <c r="J5" s="79">
+      <c r="I5" s="41">
+        <v>3</v>
+      </c>
+      <c r="J5" s="55">
         <v>16</v>
       </c>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="82"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="94"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="94"/>
-      <c r="S5" s="82"/>
-      <c r="T5" s="66"/>
-      <c r="U5" s="94"/>
-      <c r="V5" s="65"/>
-      <c r="W5" s="66"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="58"/>
+      <c r="T5" s="44"/>
+      <c r="U5" s="69"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="44"/>
     </row>
     <row r="6" spans="1:24">
-      <c r="A6" s="75"/>
-      <c r="B6" s="64" t="s">
+      <c r="A6" s="53"/>
+      <c r="B6" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="63">
+      <c r="C6" s="41">
         <v>17</v>
       </c>
-      <c r="D6" s="79">
+      <c r="D6" s="55">
         <v>56</v>
       </c>
-      <c r="E6" s="63">
+      <c r="E6" s="41">
         <v>9</v>
       </c>
-      <c r="F6" s="79">
+      <c r="F6" s="55">
         <v>78</v>
       </c>
-      <c r="G6" s="63">
+      <c r="G6" s="41">
         <v>156</v>
       </c>
-      <c r="H6" s="79">
+      <c r="H6" s="55">
         <v>156</v>
       </c>
-      <c r="I6" s="63">
+      <c r="I6" s="41">
         <v>13</v>
       </c>
-      <c r="J6" s="79">
+      <c r="J6" s="55">
         <v>65</v>
       </c>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="82"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="94"/>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="66"/>
-      <c r="R6" s="94"/>
-      <c r="S6" s="82"/>
-      <c r="T6" s="66"/>
-      <c r="U6" s="94"/>
-      <c r="V6" s="65"/>
-      <c r="W6" s="66"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="69"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="69"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="69"/>
+      <c r="V6" s="43"/>
+      <c r="W6" s="44"/>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" s="73">
+      <c r="A7" s="51">
         <v>2</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="C7" s="58">
+      <c r="C7" s="38">
         <v>370</v>
       </c>
-      <c r="D7" s="85">
+      <c r="D7" s="60">
         <v>450</v>
       </c>
-      <c r="E7" s="58">
+      <c r="E7" s="38">
         <v>520</v>
       </c>
-      <c r="F7" s="85">
+      <c r="F7" s="60">
         <v>740</v>
       </c>
-      <c r="G7" s="58">
+      <c r="G7" s="38">
         <v>770</v>
       </c>
-      <c r="H7" s="85">
+      <c r="H7" s="60">
         <v>1480</v>
       </c>
-      <c r="I7" s="58">
+      <c r="I7" s="38">
         <v>900</v>
       </c>
-      <c r="J7" s="85">
+      <c r="J7" s="60">
         <v>1200</v>
       </c>
-      <c r="K7" s="59">
+      <c r="K7" s="39">
         <v>1.6</v>
       </c>
-      <c r="L7" s="59">
+      <c r="L7" s="39">
         <v>1.5</v>
       </c>
-      <c r="M7" s="86">
+      <c r="M7" s="61">
         <f>C7/$K$7*$L$7</f>
         <v>346.875</v>
       </c>
-      <c r="N7" s="87">
+      <c r="N7" s="62">
         <f>D7/$K$7*$L$7</f>
         <v>421.875</v>
       </c>
-      <c r="O7" s="94">
+      <c r="O7" s="69">
         <f>(N7-M7)/N7</f>
         <v>0.17777777777777778</v>
       </c>
-      <c r="P7" s="86">
+      <c r="P7" s="61">
         <f>E7/$K$7*$L$7</f>
         <v>487.5</v>
       </c>
-      <c r="Q7" s="87">
+      <c r="Q7" s="62">
         <f>F7/$K$7*$L$7</f>
         <v>693.75</v>
       </c>
-      <c r="R7" s="94">
+      <c r="R7" s="69">
         <f>(Q7-P7)/Q7</f>
         <v>0.29729729729729731</v>
       </c>
-      <c r="S7" s="86">
+      <c r="S7" s="61">
         <f>G7/$K$7*$L$7</f>
         <v>721.875</v>
       </c>
-      <c r="T7" s="87">
+      <c r="T7" s="62">
         <f>H7/$K$7*$L$7</f>
         <v>1387.5</v>
       </c>
-      <c r="U7" s="94">
+      <c r="U7" s="69">
         <f>(T7-S7)/T7</f>
         <v>0.47972972972972971</v>
       </c>
-      <c r="V7" s="88">
+      <c r="V7" s="63">
         <f>I7/$K$7*$L$7</f>
         <v>843.75</v>
       </c>
-      <c r="W7" s="87">
+      <c r="W7" s="62">
         <f>J7/$K$7*$L$7</f>
         <v>1125</v>
       </c>
@@ -3857,196 +3857,196 @@
       </c>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="75"/>
-      <c r="B8" s="64" t="s">
+      <c r="A8" s="53"/>
+      <c r="B8" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="C8" s="90">
+      <c r="C8" s="65">
         <v>37925</v>
       </c>
-      <c r="D8" s="91">
+      <c r="D8" s="66">
         <v>38175</v>
       </c>
-      <c r="E8" s="90">
+      <c r="E8" s="65">
         <v>37862</v>
       </c>
-      <c r="F8" s="91">
+      <c r="F8" s="66">
         <v>38352</v>
       </c>
-      <c r="G8" s="90">
+      <c r="G8" s="65">
         <v>37981</v>
       </c>
-      <c r="H8" s="91">
+      <c r="H8" s="66">
         <v>38898</v>
       </c>
-      <c r="I8" s="90">
+      <c r="I8" s="65">
         <v>37890</v>
       </c>
-      <c r="J8" s="91">
+      <c r="J8" s="66">
         <v>38289</v>
       </c>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="82"/>
-      <c r="N8" s="66"/>
-      <c r="O8" s="94"/>
-      <c r="P8" s="82"/>
-      <c r="Q8" s="66"/>
-      <c r="R8" s="94"/>
-      <c r="S8" s="82"/>
-      <c r="T8" s="66"/>
-      <c r="U8" s="94"/>
-      <c r="V8" s="65"/>
-      <c r="W8" s="66"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="69"/>
+      <c r="P8" s="58"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="69"/>
+      <c r="S8" s="58"/>
+      <c r="T8" s="44"/>
+      <c r="U8" s="69"/>
+      <c r="V8" s="43"/>
+      <c r="W8" s="44"/>
     </row>
     <row r="9" spans="1:24">
-      <c r="A9" s="75"/>
-      <c r="B9" s="64" t="s">
+      <c r="A9" s="53"/>
+      <c r="B9" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="C9" s="63">
+      <c r="C9" s="41">
         <v>4</v>
       </c>
-      <c r="D9" s="79">
+      <c r="D9" s="55">
         <v>13</v>
       </c>
-      <c r="E9" s="63">
+      <c r="E9" s="41">
         <v>2</v>
       </c>
-      <c r="F9" s="79">
+      <c r="F9" s="55">
         <v>18</v>
       </c>
-      <c r="G9" s="63">
+      <c r="G9" s="41">
         <v>6</v>
       </c>
-      <c r="H9" s="79">
+      <c r="H9" s="55">
         <v>36</v>
       </c>
-      <c r="I9" s="63">
-        <v>3</v>
-      </c>
-      <c r="J9" s="79">
+      <c r="I9" s="41">
+        <v>3</v>
+      </c>
+      <c r="J9" s="55">
         <v>16</v>
       </c>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="82"/>
-      <c r="N9" s="66"/>
-      <c r="O9" s="94"/>
-      <c r="P9" s="82"/>
-      <c r="Q9" s="66"/>
-      <c r="R9" s="94"/>
-      <c r="S9" s="82"/>
-      <c r="T9" s="66"/>
-      <c r="U9" s="94"/>
-      <c r="V9" s="65"/>
-      <c r="W9" s="66"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="44"/>
+      <c r="R9" s="69"/>
+      <c r="S9" s="58"/>
+      <c r="T9" s="44"/>
+      <c r="U9" s="69"/>
+      <c r="V9" s="43"/>
+      <c r="W9" s="44"/>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="75"/>
-      <c r="B10" s="64" t="s">
+      <c r="A10" s="53"/>
+      <c r="B10" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="C10" s="63"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="79"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="82"/>
-      <c r="N10" s="66"/>
-      <c r="O10" s="94"/>
-      <c r="P10" s="82"/>
-      <c r="Q10" s="66"/>
-      <c r="R10" s="94"/>
-      <c r="S10" s="82"/>
-      <c r="T10" s="66"/>
-      <c r="U10" s="94"/>
-      <c r="V10" s="65"/>
-      <c r="W10" s="66"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="58"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="58"/>
+      <c r="T10" s="44"/>
+      <c r="U10" s="69"/>
+      <c r="V10" s="43"/>
+      <c r="W10" s="44"/>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="73">
-        <v>3</v>
-      </c>
-      <c r="B11" s="89" t="s">
+      <c r="A11" s="51">
+        <v>3</v>
+      </c>
+      <c r="B11" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="C11" s="58">
+      <c r="C11" s="38">
         <v>37</v>
       </c>
-      <c r="D11" s="85">
+      <c r="D11" s="60">
         <v>46</v>
       </c>
-      <c r="E11" s="58">
+      <c r="E11" s="38">
         <v>52</v>
       </c>
-      <c r="F11" s="85">
+      <c r="F11" s="60">
         <v>82</v>
       </c>
-      <c r="G11" s="58">
+      <c r="G11" s="38">
         <v>77</v>
       </c>
-      <c r="H11" s="85">
+      <c r="H11" s="60">
         <v>128</v>
       </c>
-      <c r="I11" s="58">
+      <c r="I11" s="38">
         <v>90</v>
       </c>
-      <c r="J11" s="85">
+      <c r="J11" s="60">
         <v>138</v>
       </c>
-      <c r="K11" s="59">
+      <c r="K11" s="39">
         <v>1.75</v>
       </c>
-      <c r="L11" s="59">
+      <c r="L11" s="39">
         <v>1.5</v>
       </c>
-      <c r="M11" s="86">
+      <c r="M11" s="61">
         <f>C11/$K$11*$L$11</f>
         <v>31.714285714285715</v>
       </c>
-      <c r="N11" s="87">
+      <c r="N11" s="62">
         <f>D11/$K$11*$L$11</f>
         <v>39.428571428571431</v>
       </c>
-      <c r="O11" s="94">
+      <c r="O11" s="69">
         <f>(N11-M11)/N11</f>
         <v>0.19565217391304349</v>
       </c>
-      <c r="P11" s="86">
+      <c r="P11" s="61">
         <f>E11/$K$11*$L$11</f>
         <v>44.571428571428569</v>
       </c>
-      <c r="Q11" s="87">
+      <c r="Q11" s="62">
         <f>F11/$K$11*$L$11</f>
         <v>70.285714285714278</v>
       </c>
-      <c r="R11" s="94">
+      <c r="R11" s="69">
         <f>(Q11-P11)/Q11</f>
         <v>0.3658536585365853</v>
       </c>
-      <c r="S11" s="86">
+      <c r="S11" s="61">
         <f>G11/$K$11*$L$11</f>
         <v>66</v>
       </c>
-      <c r="T11" s="87">
+      <c r="T11" s="62">
         <f>H11/$K$11*$L$11</f>
         <v>109.71428571428571</v>
       </c>
-      <c r="U11" s="94">
+      <c r="U11" s="69">
         <f>(T11-S11)/T11</f>
         <v>0.39843749999999994</v>
       </c>
-      <c r="V11" s="88">
+      <c r="V11" s="63">
         <f>I11/$K$11*$L$11</f>
         <v>77.142857142857139</v>
       </c>
-      <c r="W11" s="87">
+      <c r="W11" s="62">
         <f>J11/$K$11*$L$11</f>
         <v>118.28571428571429</v>
       </c>
@@ -4056,196 +4056,196 @@
       </c>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" s="75"/>
-      <c r="B12" s="67" t="s">
+      <c r="A12" s="53"/>
+      <c r="B12" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="C12" s="90">
+      <c r="C12" s="65">
         <v>38436</v>
       </c>
-      <c r="D12" s="91">
+      <c r="D12" s="66">
         <v>38716</v>
       </c>
-      <c r="E12" s="90">
+      <c r="E12" s="65">
         <v>38380</v>
       </c>
-      <c r="F12" s="91">
+      <c r="F12" s="66">
         <v>38863</v>
       </c>
-      <c r="G12" s="90">
+      <c r="G12" s="65">
         <v>38499</v>
       </c>
-      <c r="H12" s="91">
+      <c r="H12" s="66">
         <v>39017</v>
       </c>
-      <c r="I12" s="90">
+      <c r="I12" s="65">
         <v>38408</v>
       </c>
-      <c r="J12" s="91">
+      <c r="J12" s="66">
         <v>38800</v>
       </c>
-      <c r="K12" s="64"/>
-      <c r="L12" s="64"/>
-      <c r="M12" s="82"/>
-      <c r="N12" s="66"/>
-      <c r="O12" s="94"/>
-      <c r="P12" s="82"/>
-      <c r="Q12" s="66"/>
-      <c r="R12" s="94"/>
-      <c r="S12" s="82"/>
-      <c r="T12" s="66"/>
-      <c r="U12" s="94"/>
-      <c r="V12" s="65"/>
-      <c r="W12" s="66"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="69"/>
+      <c r="P12" s="58"/>
+      <c r="Q12" s="44"/>
+      <c r="R12" s="69"/>
+      <c r="S12" s="58"/>
+      <c r="T12" s="44"/>
+      <c r="U12" s="69"/>
+      <c r="V12" s="43"/>
+      <c r="W12" s="44"/>
     </row>
     <row r="13" spans="1:24">
-      <c r="A13" s="75"/>
-      <c r="B13" s="67" t="s">
+      <c r="A13" s="53"/>
+      <c r="B13" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="C13" s="63">
+      <c r="C13" s="41">
         <v>4</v>
       </c>
-      <c r="D13" s="79">
+      <c r="D13" s="55">
         <v>13</v>
       </c>
-      <c r="E13" s="63">
+      <c r="E13" s="41">
         <v>2</v>
       </c>
-      <c r="F13" s="79">
+      <c r="F13" s="55">
         <v>18</v>
       </c>
-      <c r="G13" s="63">
+      <c r="G13" s="41">
         <v>6</v>
       </c>
-      <c r="H13" s="79">
+      <c r="H13" s="55">
         <v>23</v>
       </c>
-      <c r="I13" s="63">
-        <v>3</v>
-      </c>
-      <c r="J13" s="79">
+      <c r="I13" s="41">
+        <v>3</v>
+      </c>
+      <c r="J13" s="55">
         <v>16</v>
       </c>
-      <c r="K13" s="64"/>
-      <c r="L13" s="64"/>
-      <c r="M13" s="82"/>
-      <c r="N13" s="66"/>
-      <c r="O13" s="94"/>
-      <c r="P13" s="82"/>
-      <c r="Q13" s="66"/>
-      <c r="R13" s="94"/>
-      <c r="S13" s="82"/>
-      <c r="T13" s="66"/>
-      <c r="U13" s="94"/>
-      <c r="V13" s="65"/>
-      <c r="W13" s="66"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="58"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="69"/>
+      <c r="S13" s="58"/>
+      <c r="T13" s="44"/>
+      <c r="U13" s="69"/>
+      <c r="V13" s="43"/>
+      <c r="W13" s="44"/>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="75"/>
-      <c r="B14" s="67" t="s">
+      <c r="A14" s="53"/>
+      <c r="B14" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="C14" s="63"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="79"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="64"/>
-      <c r="M14" s="82"/>
-      <c r="N14" s="66"/>
-      <c r="O14" s="94"/>
-      <c r="P14" s="82"/>
-      <c r="Q14" s="66"/>
-      <c r="R14" s="94"/>
-      <c r="S14" s="82"/>
-      <c r="T14" s="66"/>
-      <c r="U14" s="94"/>
-      <c r="V14" s="65"/>
-      <c r="W14" s="66"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="69"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="44"/>
+      <c r="R14" s="69"/>
+      <c r="S14" s="58"/>
+      <c r="T14" s="44"/>
+      <c r="U14" s="69"/>
+      <c r="V14" s="43"/>
+      <c r="W14" s="44"/>
     </row>
     <row r="15" spans="1:24">
-      <c r="A15" s="73">
+      <c r="A15" s="51">
         <v>4</v>
       </c>
-      <c r="B15" s="89" t="s">
+      <c r="B15" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="C15" s="58">
+      <c r="C15" s="38">
         <v>900</v>
       </c>
-      <c r="D15" s="85">
+      <c r="D15" s="60">
         <v>1200</v>
       </c>
-      <c r="E15" s="58">
+      <c r="E15" s="38">
         <v>750</v>
       </c>
-      <c r="F15" s="85">
+      <c r="F15" s="60">
         <v>2000</v>
       </c>
-      <c r="G15" s="58">
+      <c r="G15" s="38">
         <v>520</v>
       </c>
-      <c r="H15" s="85">
+      <c r="H15" s="60">
         <v>780</v>
       </c>
-      <c r="I15" s="58">
+      <c r="I15" s="38">
         <v>465</v>
       </c>
-      <c r="J15" s="85">
+      <c r="J15" s="60">
         <v>870</v>
       </c>
-      <c r="K15" s="59">
+      <c r="K15" s="39">
         <v>1.7</v>
       </c>
-      <c r="L15" s="59">
+      <c r="L15" s="39">
         <v>1.5</v>
       </c>
-      <c r="M15" s="86">
+      <c r="M15" s="61">
         <f>C15/$K$15*$L$15</f>
         <v>794.11764705882342</v>
       </c>
-      <c r="N15" s="87">
+      <c r="N15" s="62">
         <f>D15/$K$15*$L$15</f>
         <v>1058.8235294117646</v>
       </c>
-      <c r="O15" s="94">
+      <c r="O15" s="69">
         <f>(N15-M15)/N15</f>
         <v>0.25000000000000006</v>
       </c>
-      <c r="P15" s="86">
+      <c r="P15" s="61">
         <f>E15/$K$15*$L$15</f>
         <v>661.76470588235293</v>
       </c>
-      <c r="Q15" s="87">
+      <c r="Q15" s="62">
         <f>F15/$K$15*$L$15</f>
         <v>1764.7058823529412</v>
       </c>
-      <c r="R15" s="94">
+      <c r="R15" s="69">
         <f>(Q15-P15)/Q15</f>
         <v>0.625</v>
       </c>
-      <c r="S15" s="86">
+      <c r="S15" s="61">
         <f>G15/$K$15*$L$15</f>
         <v>458.8235294117647</v>
       </c>
-      <c r="T15" s="87">
+      <c r="T15" s="62">
         <f>H15/$K$15*$L$15</f>
         <v>688.23529411764707</v>
       </c>
-      <c r="U15" s="94">
+      <c r="U15" s="69">
         <f>(T15-S15)/T15</f>
         <v>0.33333333333333337</v>
       </c>
-      <c r="V15" s="88">
+      <c r="V15" s="63">
         <f>I15/$K$15*$L$15</f>
         <v>410.2941176470589</v>
       </c>
-      <c r="W15" s="87">
+      <c r="W15" s="62">
         <f>J15/$K$15*$L$15</f>
         <v>767.64705882352939</v>
       </c>
@@ -4255,117 +4255,117 @@
       </c>
     </row>
     <row r="16" spans="1:24">
-      <c r="A16" s="75"/>
-      <c r="B16" s="67" t="s">
+      <c r="A16" s="53"/>
+      <c r="B16" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="C16" s="90">
+      <c r="C16" s="65">
         <v>38044</v>
       </c>
-      <c r="D16" s="91">
+      <c r="D16" s="66">
         <v>38527</v>
       </c>
-      <c r="E16" s="90">
+      <c r="E16" s="65">
         <v>38107</v>
       </c>
-      <c r="F16" s="91">
+      <c r="F16" s="66">
         <v>39752</v>
       </c>
-      <c r="G16" s="90">
+      <c r="G16" s="65">
         <v>37981</v>
       </c>
-      <c r="H16" s="91">
+      <c r="H16" s="66">
         <v>38653</v>
       </c>
-      <c r="I16" s="90">
+      <c r="I16" s="65">
         <v>38072</v>
       </c>
-      <c r="J16" s="91">
+      <c r="J16" s="66">
         <v>39136</v>
       </c>
-      <c r="K16" s="64"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="82"/>
-      <c r="N16" s="66"/>
-      <c r="O16" s="94"/>
-      <c r="P16" s="82"/>
-      <c r="Q16" s="66"/>
-      <c r="R16" s="94"/>
-      <c r="S16" s="82"/>
-      <c r="T16" s="66"/>
-      <c r="U16" s="94"/>
-      <c r="V16" s="65"/>
-      <c r="W16" s="66"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="69"/>
+      <c r="P16" s="58"/>
+      <c r="Q16" s="44"/>
+      <c r="R16" s="69"/>
+      <c r="S16" s="58"/>
+      <c r="T16" s="44"/>
+      <c r="U16" s="69"/>
+      <c r="V16" s="43"/>
+      <c r="W16" s="44"/>
     </row>
     <row r="17" spans="1:23">
-      <c r="A17" s="75"/>
-      <c r="B17" s="67" t="s">
+      <c r="A17" s="53"/>
+      <c r="B17" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="C17" s="63">
+      <c r="C17" s="41">
         <v>4</v>
       </c>
-      <c r="D17" s="79">
+      <c r="D17" s="55">
         <v>20</v>
       </c>
-      <c r="E17" s="63">
+      <c r="E17" s="41">
         <v>6</v>
       </c>
-      <c r="F17" s="79">
+      <c r="F17" s="55">
         <v>60</v>
       </c>
-      <c r="G17" s="63">
+      <c r="G17" s="41">
         <v>2</v>
       </c>
-      <c r="H17" s="79">
+      <c r="H17" s="55">
         <v>24</v>
       </c>
-      <c r="I17" s="63">
+      <c r="I17" s="41">
         <v>5</v>
       </c>
-      <c r="J17" s="79">
+      <c r="J17" s="55">
         <v>40</v>
       </c>
-      <c r="K17" s="64"/>
-      <c r="L17" s="64"/>
-      <c r="M17" s="82"/>
-      <c r="N17" s="66"/>
-      <c r="O17" s="94"/>
-      <c r="P17" s="82"/>
-      <c r="Q17" s="66"/>
-      <c r="R17" s="94"/>
-      <c r="S17" s="82"/>
-      <c r="T17" s="66"/>
-      <c r="U17" s="94"/>
-      <c r="V17" s="65"/>
-      <c r="W17" s="66"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="69"/>
+      <c r="P17" s="58"/>
+      <c r="Q17" s="44"/>
+      <c r="R17" s="69"/>
+      <c r="S17" s="58"/>
+      <c r="T17" s="44"/>
+      <c r="U17" s="69"/>
+      <c r="V17" s="43"/>
+      <c r="W17" s="44"/>
     </row>
     <row r="18" spans="1:23">
-      <c r="A18" s="74"/>
-      <c r="B18" s="69" t="s">
+      <c r="A18" s="52"/>
+      <c r="B18" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="C18" s="68"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="78"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="70"/>
-      <c r="M18" s="83"/>
-      <c r="N18" s="72"/>
-      <c r="O18" s="93"/>
-      <c r="P18" s="83"/>
-      <c r="Q18" s="72"/>
-      <c r="R18" s="93"/>
-      <c r="S18" s="83"/>
-      <c r="T18" s="72"/>
-      <c r="U18" s="93"/>
-      <c r="V18" s="71"/>
-      <c r="W18" s="72"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="68"/>
+      <c r="P18" s="59"/>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="68"/>
+      <c r="S18" s="59"/>
+      <c r="T18" s="50"/>
+      <c r="U18" s="68"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="50"/>
     </row>
     <row r="23" spans="1:23">
       <c r="B23" t="s">
@@ -4396,7 +4396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172F3C91-0245-C642-8607-0C1863490763}">
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -4423,105 +4423,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="43" t="s">
+      <c r="A2" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="40" t="s">
+      <c r="C2" s="76"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="75" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="76"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="55" t="s">
+      <c r="I2" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55" t="s">
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="40" t="s">
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="X2" s="37" t="s">
+      <c r="W2" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="37" t="s">
+      <c r="Y2" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="37" t="s">
+      <c r="Z2" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="37" t="s">
+      <c r="AA2" s="92" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="50"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="56" t="s">
+      <c r="A3" s="82"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54" t="s">
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54" t="s">
+      <c r="M3" s="89"/>
+      <c r="N3" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54" t="s">
+      <c r="O3" s="89"/>
+      <c r="P3" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="52" t="s">
+      <c r="Q3" s="89"/>
+      <c r="R3" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="52" t="s">
+      <c r="S3" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="52" t="s">
+      <c r="T3" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="52" t="s">
+      <c r="U3" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="41"/>
-      <c r="W3" s="41"/>
-      <c r="X3" s="38"/>
-      <c r="Y3" s="38"/>
-      <c r="Z3" s="38"/>
-      <c r="AA3" s="38"/>
+      <c r="V3" s="85"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="93"/>
+      <c r="Y3" s="93"/>
+      <c r="Z3" s="93"/>
+      <c r="AA3" s="93"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="51"/>
+      <c r="A4" s="83"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -4540,7 +4540,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="42"/>
+      <c r="H4" s="86"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -4568,16 +4568,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="53"/>
-      <c r="S4" s="53"/>
-      <c r="T4" s="53"/>
-      <c r="U4" s="53"/>
-      <c r="V4" s="42"/>
-      <c r="W4" s="42"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="38"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="88"/>
+      <c r="V4" s="86"/>
+      <c r="W4" s="86"/>
+      <c r="X4" s="94"/>
+      <c r="Y4" s="94"/>
+      <c r="Z4" s="94"/>
+      <c r="AA4" s="93"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -5078,6 +5078,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -5093,11 +5098,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
merge latest of main into release
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542C3430-4182-B545-87CF-CC97373839AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA5AAD1-30D2-FF44-ADD4-C2C23FC7C8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="2" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="1800" yWindow="500" windowWidth="35840" windowHeight="21060" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Web Parameters" sheetId="8" r:id="rId1"/>
@@ -869,23 +869,57 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -915,6 +949,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -929,58 +972,15 @@
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1297,9 +1297,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
   <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomLeft" activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1553,16 +1553,16 @@
         <v>100</v>
       </c>
       <c r="P5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T5">
         <v>8.5</v>
@@ -1615,16 +1615,16 @@
         <v>100</v>
       </c>
       <c r="P6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T6">
         <v>8.5</v>
@@ -1677,16 +1677,16 @@
         <v>100</v>
       </c>
       <c r="P7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R7">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S7">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="T7">
         <v>4.5</v>
@@ -3441,198 +3441,198 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="13" max="14" width="10.83203125" style="57"/>
+    <col min="13" max="14" width="10.83203125" style="37"/>
     <col min="15" max="15" width="10.83203125" style="11"/>
-    <col min="16" max="17" width="10.83203125" style="57"/>
+    <col min="16" max="17" width="10.83203125" style="37"/>
     <col min="18" max="18" width="10.83203125" style="11"/>
-    <col min="19" max="20" width="10.83203125" style="57"/>
+    <col min="19" max="20" width="10.83203125" style="37"/>
     <col min="21" max="21" width="10.83203125" style="11"/>
-    <col min="22" max="23" width="10.83203125" style="57"/>
+    <col min="22" max="23" width="10.83203125" style="37"/>
     <col min="24" max="24" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="76" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="73" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="77"/>
-      <c r="E1" s="76" t="s">
+      <c r="D1" s="74"/>
+      <c r="E1" s="73" t="s">
         <v>159</v>
       </c>
-      <c r="F1" s="77"/>
-      <c r="G1" s="76" t="s">
+      <c r="F1" s="74"/>
+      <c r="G1" s="73" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="77"/>
-      <c r="I1" s="76" t="s">
+      <c r="H1" s="74"/>
+      <c r="I1" s="73" t="s">
         <v>161</v>
       </c>
-      <c r="J1" s="77"/>
-      <c r="K1" s="60" t="s">
+      <c r="J1" s="74"/>
+      <c r="K1" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="M1" s="84" t="s">
+      <c r="M1" s="70" t="s">
         <v>162</v>
       </c>
-      <c r="N1" s="62"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="84" t="s">
+      <c r="N1" s="71"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="70" t="s">
         <v>163</v>
       </c>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="92"/>
-      <c r="S1" s="84" t="s">
+      <c r="Q1" s="71"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="70" t="s">
         <v>164</v>
       </c>
-      <c r="T1" s="62"/>
-      <c r="U1" s="92"/>
-      <c r="V1" s="61" t="s">
+      <c r="T1" s="71"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="72" t="s">
         <v>165</v>
       </c>
-      <c r="W1" s="62"/>
+      <c r="W1" s="71"/>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="74"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="68" t="s">
+      <c r="A2" s="52"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="H2" s="78" t="s">
+      <c r="H2" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="I2" s="68" t="s">
+      <c r="I2" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="J2" s="78" t="s">
+      <c r="J2" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="80" t="s">
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="N2" s="81" t="s">
+      <c r="N2" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="O2" s="93"/>
-      <c r="P2" s="83" t="s">
+      <c r="O2" s="68"/>
+      <c r="P2" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="Q2" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="R2" s="93"/>
-      <c r="S2" s="83" t="s">
+      <c r="R2" s="68"/>
+      <c r="S2" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="T2" s="72" t="s">
+      <c r="T2" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="U2" s="93"/>
-      <c r="V2" s="71" t="s">
+      <c r="U2" s="68"/>
+      <c r="V2" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="W2" s="72" t="s">
+      <c r="W2" s="50" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="75">
-        <v>1</v>
-      </c>
-      <c r="B3" s="64" t="s">
+      <c r="A3" s="53">
+        <v>1</v>
+      </c>
+      <c r="B3" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="63">
+      <c r="C3" s="41">
         <v>370</v>
       </c>
-      <c r="D3" s="79">
+      <c r="D3" s="55">
         <v>450</v>
       </c>
-      <c r="E3" s="63">
+      <c r="E3" s="41">
         <v>520</v>
       </c>
-      <c r="F3" s="79">
+      <c r="F3" s="55">
         <v>740</v>
       </c>
-      <c r="G3" s="63">
+      <c r="G3" s="41">
         <v>770</v>
       </c>
-      <c r="H3" s="79">
+      <c r="H3" s="55">
         <v>1480</v>
       </c>
-      <c r="I3" s="63">
+      <c r="I3" s="41">
         <v>900</v>
       </c>
-      <c r="J3" s="79">
+      <c r="J3" s="55">
         <v>1200</v>
       </c>
-      <c r="K3" s="64">
+      <c r="K3" s="42">
         <v>1.6</v>
       </c>
-      <c r="L3" s="64">
+      <c r="L3" s="42">
         <v>1.5</v>
       </c>
-      <c r="M3" s="82">
+      <c r="M3" s="58">
         <f>C3/$K$3*$L$3</f>
         <v>346.875</v>
       </c>
-      <c r="N3" s="66">
+      <c r="N3" s="44">
         <f>D3/$K$3*$L$3</f>
         <v>421.875</v>
       </c>
-      <c r="O3" s="94">
+      <c r="O3" s="69">
         <f>(N3-M3)/N3</f>
         <v>0.17777777777777778</v>
       </c>
-      <c r="P3" s="82">
+      <c r="P3" s="58">
         <f>E3/$K$3*$L$3</f>
         <v>487.5</v>
       </c>
-      <c r="Q3" s="66">
+      <c r="Q3" s="44">
         <f>F3/$K$3*$L$3</f>
         <v>693.75</v>
       </c>
-      <c r="R3" s="94">
+      <c r="R3" s="69">
         <f>(Q3-P3)/Q3</f>
         <v>0.29729729729729731</v>
       </c>
-      <c r="S3" s="82">
+      <c r="S3" s="58">
         <f>G3/$K$3*$L$3</f>
         <v>721.875</v>
       </c>
-      <c r="T3" s="66">
+      <c r="T3" s="44">
         <f>H3/$K$3*$L$3</f>
         <v>1387.5</v>
       </c>
-      <c r="U3" s="94">
+      <c r="U3" s="69">
         <f>(T3-S3)/T3</f>
         <v>0.47972972972972971</v>
       </c>
-      <c r="V3" s="65">
+      <c r="V3" s="43">
         <f>I3/$K$3*$L$3</f>
         <v>843.75</v>
       </c>
-      <c r="W3" s="66">
+      <c r="W3" s="44">
         <f>J3/$K$3*$L$3</f>
         <v>1125</v>
       </c>
@@ -3642,212 +3642,212 @@
       </c>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" s="75"/>
-      <c r="B4" s="64" t="s">
+      <c r="A4" s="53"/>
+      <c r="B4" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="C4" s="90">
+      <c r="C4" s="65">
         <v>37890</v>
       </c>
-      <c r="D4" s="91">
+      <c r="D4" s="66">
         <v>38163</v>
       </c>
-      <c r="E4" s="90">
+      <c r="E4" s="65">
         <v>37797</v>
       </c>
-      <c r="F4" s="91">
+      <c r="F4" s="66">
         <v>38317</v>
       </c>
-      <c r="G4" s="90">
+      <c r="G4" s="65">
         <v>37953</v>
       </c>
-      <c r="H4" s="91">
+      <c r="H4" s="66">
         <v>38863</v>
       </c>
-      <c r="I4" s="90">
+      <c r="I4" s="65">
         <v>37862</v>
       </c>
-      <c r="J4" s="91">
+      <c r="J4" s="66">
         <v>38254</v>
       </c>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="94"/>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="66"/>
-      <c r="R4" s="94"/>
-      <c r="S4" s="82"/>
-      <c r="T4" s="66"/>
-      <c r="U4" s="94"/>
-      <c r="V4" s="65"/>
-      <c r="W4" s="66"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="69"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="69"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="44"/>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="75"/>
-      <c r="B5" s="64" t="s">
+      <c r="A5" s="53"/>
+      <c r="B5" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="63">
+      <c r="C5" s="41">
         <v>4</v>
       </c>
-      <c r="D5" s="79">
+      <c r="D5" s="55">
         <v>13</v>
       </c>
-      <c r="E5" s="63">
+      <c r="E5" s="41">
         <v>2</v>
       </c>
-      <c r="F5" s="79">
+      <c r="F5" s="55">
         <v>18</v>
       </c>
-      <c r="G5" s="63">
+      <c r="G5" s="41">
         <v>6</v>
       </c>
-      <c r="H5" s="79">
+      <c r="H5" s="55">
         <v>36</v>
       </c>
-      <c r="I5" s="63">
-        <v>3</v>
-      </c>
-      <c r="J5" s="79">
+      <c r="I5" s="41">
+        <v>3</v>
+      </c>
+      <c r="J5" s="55">
         <v>16</v>
       </c>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="82"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="94"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="94"/>
-      <c r="S5" s="82"/>
-      <c r="T5" s="66"/>
-      <c r="U5" s="94"/>
-      <c r="V5" s="65"/>
-      <c r="W5" s="66"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="58"/>
+      <c r="T5" s="44"/>
+      <c r="U5" s="69"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="44"/>
     </row>
     <row r="6" spans="1:24">
-      <c r="A6" s="75"/>
-      <c r="B6" s="64" t="s">
+      <c r="A6" s="53"/>
+      <c r="B6" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="63">
+      <c r="C6" s="41">
         <v>17</v>
       </c>
-      <c r="D6" s="79">
+      <c r="D6" s="55">
         <v>56</v>
       </c>
-      <c r="E6" s="63">
+      <c r="E6" s="41">
         <v>9</v>
       </c>
-      <c r="F6" s="79">
+      <c r="F6" s="55">
         <v>78</v>
       </c>
-      <c r="G6" s="63">
+      <c r="G6" s="41">
         <v>156</v>
       </c>
-      <c r="H6" s="79">
+      <c r="H6" s="55">
         <v>156</v>
       </c>
-      <c r="I6" s="63">
+      <c r="I6" s="41">
         <v>13</v>
       </c>
-      <c r="J6" s="79">
+      <c r="J6" s="55">
         <v>65</v>
       </c>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="82"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="94"/>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="66"/>
-      <c r="R6" s="94"/>
-      <c r="S6" s="82"/>
-      <c r="T6" s="66"/>
-      <c r="U6" s="94"/>
-      <c r="V6" s="65"/>
-      <c r="W6" s="66"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="69"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="69"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="69"/>
+      <c r="V6" s="43"/>
+      <c r="W6" s="44"/>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" s="73">
+      <c r="A7" s="51">
         <v>2</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="C7" s="58">
+      <c r="C7" s="38">
         <v>370</v>
       </c>
-      <c r="D7" s="85">
+      <c r="D7" s="60">
         <v>450</v>
       </c>
-      <c r="E7" s="58">
+      <c r="E7" s="38">
         <v>520</v>
       </c>
-      <c r="F7" s="85">
+      <c r="F7" s="60">
         <v>740</v>
       </c>
-      <c r="G7" s="58">
+      <c r="G7" s="38">
         <v>770</v>
       </c>
-      <c r="H7" s="85">
+      <c r="H7" s="60">
         <v>1480</v>
       </c>
-      <c r="I7" s="58">
+      <c r="I7" s="38">
         <v>900</v>
       </c>
-      <c r="J7" s="85">
+      <c r="J7" s="60">
         <v>1200</v>
       </c>
-      <c r="K7" s="59">
+      <c r="K7" s="39">
         <v>1.6</v>
       </c>
-      <c r="L7" s="59">
+      <c r="L7" s="39">
         <v>1.5</v>
       </c>
-      <c r="M7" s="86">
+      <c r="M7" s="61">
         <f>C7/$K$7*$L$7</f>
         <v>346.875</v>
       </c>
-      <c r="N7" s="87">
+      <c r="N7" s="62">
         <f>D7/$K$7*$L$7</f>
         <v>421.875</v>
       </c>
-      <c r="O7" s="94">
+      <c r="O7" s="69">
         <f>(N7-M7)/N7</f>
         <v>0.17777777777777778</v>
       </c>
-      <c r="P7" s="86">
+      <c r="P7" s="61">
         <f>E7/$K$7*$L$7</f>
         <v>487.5</v>
       </c>
-      <c r="Q7" s="87">
+      <c r="Q7" s="62">
         <f>F7/$K$7*$L$7</f>
         <v>693.75</v>
       </c>
-      <c r="R7" s="94">
+      <c r="R7" s="69">
         <f>(Q7-P7)/Q7</f>
         <v>0.29729729729729731</v>
       </c>
-      <c r="S7" s="86">
+      <c r="S7" s="61">
         <f>G7/$K$7*$L$7</f>
         <v>721.875</v>
       </c>
-      <c r="T7" s="87">
+      <c r="T7" s="62">
         <f>H7/$K$7*$L$7</f>
         <v>1387.5</v>
       </c>
-      <c r="U7" s="94">
+      <c r="U7" s="69">
         <f>(T7-S7)/T7</f>
         <v>0.47972972972972971</v>
       </c>
-      <c r="V7" s="88">
+      <c r="V7" s="63">
         <f>I7/$K$7*$L$7</f>
         <v>843.75</v>
       </c>
-      <c r="W7" s="87">
+      <c r="W7" s="62">
         <f>J7/$K$7*$L$7</f>
         <v>1125</v>
       </c>
@@ -3857,196 +3857,196 @@
       </c>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="75"/>
-      <c r="B8" s="64" t="s">
+      <c r="A8" s="53"/>
+      <c r="B8" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="C8" s="90">
+      <c r="C8" s="65">
         <v>37925</v>
       </c>
-      <c r="D8" s="91">
+      <c r="D8" s="66">
         <v>38175</v>
       </c>
-      <c r="E8" s="90">
+      <c r="E8" s="65">
         <v>37862</v>
       </c>
-      <c r="F8" s="91">
+      <c r="F8" s="66">
         <v>38352</v>
       </c>
-      <c r="G8" s="90">
+      <c r="G8" s="65">
         <v>37981</v>
       </c>
-      <c r="H8" s="91">
+      <c r="H8" s="66">
         <v>38898</v>
       </c>
-      <c r="I8" s="90">
+      <c r="I8" s="65">
         <v>37890</v>
       </c>
-      <c r="J8" s="91">
+      <c r="J8" s="66">
         <v>38289</v>
       </c>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="82"/>
-      <c r="N8" s="66"/>
-      <c r="O8" s="94"/>
-      <c r="P8" s="82"/>
-      <c r="Q8" s="66"/>
-      <c r="R8" s="94"/>
-      <c r="S8" s="82"/>
-      <c r="T8" s="66"/>
-      <c r="U8" s="94"/>
-      <c r="V8" s="65"/>
-      <c r="W8" s="66"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="69"/>
+      <c r="P8" s="58"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="69"/>
+      <c r="S8" s="58"/>
+      <c r="T8" s="44"/>
+      <c r="U8" s="69"/>
+      <c r="V8" s="43"/>
+      <c r="W8" s="44"/>
     </row>
     <row r="9" spans="1:24">
-      <c r="A9" s="75"/>
-      <c r="B9" s="64" t="s">
+      <c r="A9" s="53"/>
+      <c r="B9" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="C9" s="63">
+      <c r="C9" s="41">
         <v>4</v>
       </c>
-      <c r="D9" s="79">
+      <c r="D9" s="55">
         <v>13</v>
       </c>
-      <c r="E9" s="63">
+      <c r="E9" s="41">
         <v>2</v>
       </c>
-      <c r="F9" s="79">
+      <c r="F9" s="55">
         <v>18</v>
       </c>
-      <c r="G9" s="63">
+      <c r="G9" s="41">
         <v>6</v>
       </c>
-      <c r="H9" s="79">
+      <c r="H9" s="55">
         <v>36</v>
       </c>
-      <c r="I9" s="63">
-        <v>3</v>
-      </c>
-      <c r="J9" s="79">
+      <c r="I9" s="41">
+        <v>3</v>
+      </c>
+      <c r="J9" s="55">
         <v>16</v>
       </c>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="82"/>
-      <c r="N9" s="66"/>
-      <c r="O9" s="94"/>
-      <c r="P9" s="82"/>
-      <c r="Q9" s="66"/>
-      <c r="R9" s="94"/>
-      <c r="S9" s="82"/>
-      <c r="T9" s="66"/>
-      <c r="U9" s="94"/>
-      <c r="V9" s="65"/>
-      <c r="W9" s="66"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="44"/>
+      <c r="R9" s="69"/>
+      <c r="S9" s="58"/>
+      <c r="T9" s="44"/>
+      <c r="U9" s="69"/>
+      <c r="V9" s="43"/>
+      <c r="W9" s="44"/>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="75"/>
-      <c r="B10" s="64" t="s">
+      <c r="A10" s="53"/>
+      <c r="B10" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="C10" s="63"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="79"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="82"/>
-      <c r="N10" s="66"/>
-      <c r="O10" s="94"/>
-      <c r="P10" s="82"/>
-      <c r="Q10" s="66"/>
-      <c r="R10" s="94"/>
-      <c r="S10" s="82"/>
-      <c r="T10" s="66"/>
-      <c r="U10" s="94"/>
-      <c r="V10" s="65"/>
-      <c r="W10" s="66"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="58"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="58"/>
+      <c r="T10" s="44"/>
+      <c r="U10" s="69"/>
+      <c r="V10" s="43"/>
+      <c r="W10" s="44"/>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="73">
-        <v>3</v>
-      </c>
-      <c r="B11" s="89" t="s">
+      <c r="A11" s="51">
+        <v>3</v>
+      </c>
+      <c r="B11" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="C11" s="58">
+      <c r="C11" s="38">
         <v>37</v>
       </c>
-      <c r="D11" s="85">
+      <c r="D11" s="60">
         <v>46</v>
       </c>
-      <c r="E11" s="58">
+      <c r="E11" s="38">
         <v>52</v>
       </c>
-      <c r="F11" s="85">
+      <c r="F11" s="60">
         <v>82</v>
       </c>
-      <c r="G11" s="58">
+      <c r="G11" s="38">
         <v>77</v>
       </c>
-      <c r="H11" s="85">
+      <c r="H11" s="60">
         <v>128</v>
       </c>
-      <c r="I11" s="58">
+      <c r="I11" s="38">
         <v>90</v>
       </c>
-      <c r="J11" s="85">
+      <c r="J11" s="60">
         <v>138</v>
       </c>
-      <c r="K11" s="59">
+      <c r="K11" s="39">
         <v>1.75</v>
       </c>
-      <c r="L11" s="59">
+      <c r="L11" s="39">
         <v>1.5</v>
       </c>
-      <c r="M11" s="86">
+      <c r="M11" s="61">
         <f>C11/$K$11*$L$11</f>
         <v>31.714285714285715</v>
       </c>
-      <c r="N11" s="87">
+      <c r="N11" s="62">
         <f>D11/$K$11*$L$11</f>
         <v>39.428571428571431</v>
       </c>
-      <c r="O11" s="94">
+      <c r="O11" s="69">
         <f>(N11-M11)/N11</f>
         <v>0.19565217391304349</v>
       </c>
-      <c r="P11" s="86">
+      <c r="P11" s="61">
         <f>E11/$K$11*$L$11</f>
         <v>44.571428571428569</v>
       </c>
-      <c r="Q11" s="87">
+      <c r="Q11" s="62">
         <f>F11/$K$11*$L$11</f>
         <v>70.285714285714278</v>
       </c>
-      <c r="R11" s="94">
+      <c r="R11" s="69">
         <f>(Q11-P11)/Q11</f>
         <v>0.3658536585365853</v>
       </c>
-      <c r="S11" s="86">
+      <c r="S11" s="61">
         <f>G11/$K$11*$L$11</f>
         <v>66</v>
       </c>
-      <c r="T11" s="87">
+      <c r="T11" s="62">
         <f>H11/$K$11*$L$11</f>
         <v>109.71428571428571</v>
       </c>
-      <c r="U11" s="94">
+      <c r="U11" s="69">
         <f>(T11-S11)/T11</f>
         <v>0.39843749999999994</v>
       </c>
-      <c r="V11" s="88">
+      <c r="V11" s="63">
         <f>I11/$K$11*$L$11</f>
         <v>77.142857142857139</v>
       </c>
-      <c r="W11" s="87">
+      <c r="W11" s="62">
         <f>J11/$K$11*$L$11</f>
         <v>118.28571428571429</v>
       </c>
@@ -4056,196 +4056,196 @@
       </c>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" s="75"/>
-      <c r="B12" s="67" t="s">
+      <c r="A12" s="53"/>
+      <c r="B12" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="C12" s="90">
+      <c r="C12" s="65">
         <v>38436</v>
       </c>
-      <c r="D12" s="91">
+      <c r="D12" s="66">
         <v>38716</v>
       </c>
-      <c r="E12" s="90">
+      <c r="E12" s="65">
         <v>38380</v>
       </c>
-      <c r="F12" s="91">
+      <c r="F12" s="66">
         <v>38863</v>
       </c>
-      <c r="G12" s="90">
+      <c r="G12" s="65">
         <v>38499</v>
       </c>
-      <c r="H12" s="91">
+      <c r="H12" s="66">
         <v>39017</v>
       </c>
-      <c r="I12" s="90">
+      <c r="I12" s="65">
         <v>38408</v>
       </c>
-      <c r="J12" s="91">
+      <c r="J12" s="66">
         <v>38800</v>
       </c>
-      <c r="K12" s="64"/>
-      <c r="L12" s="64"/>
-      <c r="M12" s="82"/>
-      <c r="N12" s="66"/>
-      <c r="O12" s="94"/>
-      <c r="P12" s="82"/>
-      <c r="Q12" s="66"/>
-      <c r="R12" s="94"/>
-      <c r="S12" s="82"/>
-      <c r="T12" s="66"/>
-      <c r="U12" s="94"/>
-      <c r="V12" s="65"/>
-      <c r="W12" s="66"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="69"/>
+      <c r="P12" s="58"/>
+      <c r="Q12" s="44"/>
+      <c r="R12" s="69"/>
+      <c r="S12" s="58"/>
+      <c r="T12" s="44"/>
+      <c r="U12" s="69"/>
+      <c r="V12" s="43"/>
+      <c r="W12" s="44"/>
     </row>
     <row r="13" spans="1:24">
-      <c r="A13" s="75"/>
-      <c r="B13" s="67" t="s">
+      <c r="A13" s="53"/>
+      <c r="B13" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="C13" s="63">
+      <c r="C13" s="41">
         <v>4</v>
       </c>
-      <c r="D13" s="79">
+      <c r="D13" s="55">
         <v>13</v>
       </c>
-      <c r="E13" s="63">
+      <c r="E13" s="41">
         <v>2</v>
       </c>
-      <c r="F13" s="79">
+      <c r="F13" s="55">
         <v>18</v>
       </c>
-      <c r="G13" s="63">
+      <c r="G13" s="41">
         <v>6</v>
       </c>
-      <c r="H13" s="79">
+      <c r="H13" s="55">
         <v>23</v>
       </c>
-      <c r="I13" s="63">
-        <v>3</v>
-      </c>
-      <c r="J13" s="79">
+      <c r="I13" s="41">
+        <v>3</v>
+      </c>
+      <c r="J13" s="55">
         <v>16</v>
       </c>
-      <c r="K13" s="64"/>
-      <c r="L13" s="64"/>
-      <c r="M13" s="82"/>
-      <c r="N13" s="66"/>
-      <c r="O13" s="94"/>
-      <c r="P13" s="82"/>
-      <c r="Q13" s="66"/>
-      <c r="R13" s="94"/>
-      <c r="S13" s="82"/>
-      <c r="T13" s="66"/>
-      <c r="U13" s="94"/>
-      <c r="V13" s="65"/>
-      <c r="W13" s="66"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="58"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="69"/>
+      <c r="S13" s="58"/>
+      <c r="T13" s="44"/>
+      <c r="U13" s="69"/>
+      <c r="V13" s="43"/>
+      <c r="W13" s="44"/>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="75"/>
-      <c r="B14" s="67" t="s">
+      <c r="A14" s="53"/>
+      <c r="B14" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="C14" s="63"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="79"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="64"/>
-      <c r="M14" s="82"/>
-      <c r="N14" s="66"/>
-      <c r="O14" s="94"/>
-      <c r="P14" s="82"/>
-      <c r="Q14" s="66"/>
-      <c r="R14" s="94"/>
-      <c r="S14" s="82"/>
-      <c r="T14" s="66"/>
-      <c r="U14" s="94"/>
-      <c r="V14" s="65"/>
-      <c r="W14" s="66"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="69"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="44"/>
+      <c r="R14" s="69"/>
+      <c r="S14" s="58"/>
+      <c r="T14" s="44"/>
+      <c r="U14" s="69"/>
+      <c r="V14" s="43"/>
+      <c r="W14" s="44"/>
     </row>
     <row r="15" spans="1:24">
-      <c r="A15" s="73">
+      <c r="A15" s="51">
         <v>4</v>
       </c>
-      <c r="B15" s="89" t="s">
+      <c r="B15" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="C15" s="58">
+      <c r="C15" s="38">
         <v>900</v>
       </c>
-      <c r="D15" s="85">
+      <c r="D15" s="60">
         <v>1200</v>
       </c>
-      <c r="E15" s="58">
+      <c r="E15" s="38">
         <v>750</v>
       </c>
-      <c r="F15" s="85">
+      <c r="F15" s="60">
         <v>2000</v>
       </c>
-      <c r="G15" s="58">
+      <c r="G15" s="38">
         <v>520</v>
       </c>
-      <c r="H15" s="85">
+      <c r="H15" s="60">
         <v>780</v>
       </c>
-      <c r="I15" s="58">
+      <c r="I15" s="38">
         <v>465</v>
       </c>
-      <c r="J15" s="85">
+      <c r="J15" s="60">
         <v>870</v>
       </c>
-      <c r="K15" s="59">
+      <c r="K15" s="39">
         <v>1.7</v>
       </c>
-      <c r="L15" s="59">
+      <c r="L15" s="39">
         <v>1.5</v>
       </c>
-      <c r="M15" s="86">
+      <c r="M15" s="61">
         <f>C15/$K$15*$L$15</f>
         <v>794.11764705882342</v>
       </c>
-      <c r="N15" s="87">
+      <c r="N15" s="62">
         <f>D15/$K$15*$L$15</f>
         <v>1058.8235294117646</v>
       </c>
-      <c r="O15" s="94">
+      <c r="O15" s="69">
         <f>(N15-M15)/N15</f>
         <v>0.25000000000000006</v>
       </c>
-      <c r="P15" s="86">
+      <c r="P15" s="61">
         <f>E15/$K$15*$L$15</f>
         <v>661.76470588235293</v>
       </c>
-      <c r="Q15" s="87">
+      <c r="Q15" s="62">
         <f>F15/$K$15*$L$15</f>
         <v>1764.7058823529412</v>
       </c>
-      <c r="R15" s="94">
+      <c r="R15" s="69">
         <f>(Q15-P15)/Q15</f>
         <v>0.625</v>
       </c>
-      <c r="S15" s="86">
+      <c r="S15" s="61">
         <f>G15/$K$15*$L$15</f>
         <v>458.8235294117647</v>
       </c>
-      <c r="T15" s="87">
+      <c r="T15" s="62">
         <f>H15/$K$15*$L$15</f>
         <v>688.23529411764707</v>
       </c>
-      <c r="U15" s="94">
+      <c r="U15" s="69">
         <f>(T15-S15)/T15</f>
         <v>0.33333333333333337</v>
       </c>
-      <c r="V15" s="88">
+      <c r="V15" s="63">
         <f>I15/$K$15*$L$15</f>
         <v>410.2941176470589</v>
       </c>
-      <c r="W15" s="87">
+      <c r="W15" s="62">
         <f>J15/$K$15*$L$15</f>
         <v>767.64705882352939</v>
       </c>
@@ -4255,117 +4255,117 @@
       </c>
     </row>
     <row r="16" spans="1:24">
-      <c r="A16" s="75"/>
-      <c r="B16" s="67" t="s">
+      <c r="A16" s="53"/>
+      <c r="B16" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="C16" s="90">
+      <c r="C16" s="65">
         <v>38044</v>
       </c>
-      <c r="D16" s="91">
+      <c r="D16" s="66">
         <v>38527</v>
       </c>
-      <c r="E16" s="90">
+      <c r="E16" s="65">
         <v>38107</v>
       </c>
-      <c r="F16" s="91">
+      <c r="F16" s="66">
         <v>39752</v>
       </c>
-      <c r="G16" s="90">
+      <c r="G16" s="65">
         <v>37981</v>
       </c>
-      <c r="H16" s="91">
+      <c r="H16" s="66">
         <v>38653</v>
       </c>
-      <c r="I16" s="90">
+      <c r="I16" s="65">
         <v>38072</v>
       </c>
-      <c r="J16" s="91">
+      <c r="J16" s="66">
         <v>39136</v>
       </c>
-      <c r="K16" s="64"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="82"/>
-      <c r="N16" s="66"/>
-      <c r="O16" s="94"/>
-      <c r="P16" s="82"/>
-      <c r="Q16" s="66"/>
-      <c r="R16" s="94"/>
-      <c r="S16" s="82"/>
-      <c r="T16" s="66"/>
-      <c r="U16" s="94"/>
-      <c r="V16" s="65"/>
-      <c r="W16" s="66"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="69"/>
+      <c r="P16" s="58"/>
+      <c r="Q16" s="44"/>
+      <c r="R16" s="69"/>
+      <c r="S16" s="58"/>
+      <c r="T16" s="44"/>
+      <c r="U16" s="69"/>
+      <c r="V16" s="43"/>
+      <c r="W16" s="44"/>
     </row>
     <row r="17" spans="1:23">
-      <c r="A17" s="75"/>
-      <c r="B17" s="67" t="s">
+      <c r="A17" s="53"/>
+      <c r="B17" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="C17" s="63">
+      <c r="C17" s="41">
         <v>4</v>
       </c>
-      <c r="D17" s="79">
+      <c r="D17" s="55">
         <v>20</v>
       </c>
-      <c r="E17" s="63">
+      <c r="E17" s="41">
         <v>6</v>
       </c>
-      <c r="F17" s="79">
+      <c r="F17" s="55">
         <v>60</v>
       </c>
-      <c r="G17" s="63">
+      <c r="G17" s="41">
         <v>2</v>
       </c>
-      <c r="H17" s="79">
+      <c r="H17" s="55">
         <v>24</v>
       </c>
-      <c r="I17" s="63">
+      <c r="I17" s="41">
         <v>5</v>
       </c>
-      <c r="J17" s="79">
+      <c r="J17" s="55">
         <v>40</v>
       </c>
-      <c r="K17" s="64"/>
-      <c r="L17" s="64"/>
-      <c r="M17" s="82"/>
-      <c r="N17" s="66"/>
-      <c r="O17" s="94"/>
-      <c r="P17" s="82"/>
-      <c r="Q17" s="66"/>
-      <c r="R17" s="94"/>
-      <c r="S17" s="82"/>
-      <c r="T17" s="66"/>
-      <c r="U17" s="94"/>
-      <c r="V17" s="65"/>
-      <c r="W17" s="66"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="69"/>
+      <c r="P17" s="58"/>
+      <c r="Q17" s="44"/>
+      <c r="R17" s="69"/>
+      <c r="S17" s="58"/>
+      <c r="T17" s="44"/>
+      <c r="U17" s="69"/>
+      <c r="V17" s="43"/>
+      <c r="W17" s="44"/>
     </row>
     <row r="18" spans="1:23">
-      <c r="A18" s="74"/>
-      <c r="B18" s="69" t="s">
+      <c r="A18" s="52"/>
+      <c r="B18" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="C18" s="68"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="78"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="70"/>
-      <c r="M18" s="83"/>
-      <c r="N18" s="72"/>
-      <c r="O18" s="93"/>
-      <c r="P18" s="83"/>
-      <c r="Q18" s="72"/>
-      <c r="R18" s="93"/>
-      <c r="S18" s="83"/>
-      <c r="T18" s="72"/>
-      <c r="U18" s="93"/>
-      <c r="V18" s="71"/>
-      <c r="W18" s="72"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="68"/>
+      <c r="P18" s="59"/>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="68"/>
+      <c r="S18" s="59"/>
+      <c r="T18" s="50"/>
+      <c r="U18" s="68"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="50"/>
     </row>
     <row r="23" spans="1:23">
       <c r="B23" t="s">
@@ -4396,7 +4396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172F3C91-0245-C642-8607-0C1863490763}">
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -4423,105 +4423,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="43" t="s">
+      <c r="A2" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="40" t="s">
+      <c r="C2" s="76"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="75" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="76"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="55" t="s">
+      <c r="I2" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55" t="s">
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="40" t="s">
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="X2" s="37" t="s">
+      <c r="W2" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="37" t="s">
+      <c r="Y2" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="37" t="s">
+      <c r="Z2" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="37" t="s">
+      <c r="AA2" s="92" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="50"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="56" t="s">
+      <c r="A3" s="82"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54" t="s">
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54" t="s">
+      <c r="M3" s="89"/>
+      <c r="N3" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54" t="s">
+      <c r="O3" s="89"/>
+      <c r="P3" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="52" t="s">
+      <c r="Q3" s="89"/>
+      <c r="R3" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="52" t="s">
+      <c r="S3" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="52" t="s">
+      <c r="T3" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="52" t="s">
+      <c r="U3" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="41"/>
-      <c r="W3" s="41"/>
-      <c r="X3" s="38"/>
-      <c r="Y3" s="38"/>
-      <c r="Z3" s="38"/>
-      <c r="AA3" s="38"/>
+      <c r="V3" s="85"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="93"/>
+      <c r="Y3" s="93"/>
+      <c r="Z3" s="93"/>
+      <c r="AA3" s="93"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="51"/>
+      <c r="A4" s="83"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -4540,7 +4540,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="42"/>
+      <c r="H4" s="86"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -4568,16 +4568,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="53"/>
-      <c r="S4" s="53"/>
-      <c r="T4" s="53"/>
-      <c r="U4" s="53"/>
-      <c r="V4" s="42"/>
-      <c r="W4" s="42"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="38"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="88"/>
+      <c r="V4" s="86"/>
+      <c r="W4" s="86"/>
+      <c r="X4" s="94"/>
+      <c r="Y4" s="94"/>
+      <c r="Z4" s="94"/>
+      <c r="AA4" s="93"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -5078,6 +5078,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -5093,11 +5098,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Changed barchart to render in px or in
Also added a new dev test link.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA5AAD1-30D2-FF44-ADD4-C2C23FC7C8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ADC001-E336-AA42-84F2-2147118A2E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="500" windowWidth="35840" windowHeight="21060" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Web Parameters" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="168">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -450,9 +450,6 @@
     <t>drag</t>
   </si>
   <si>
-    <t>Barchart MEL question with no interaction.</t>
-  </si>
-  <si>
     <t>calendarWord</t>
   </si>
   <si>
@@ -486,9 +483,6 @@
     <t>Calendar month view with barchart and no interaction.</t>
   </si>
   <si>
-    <t>Barchart with no interaction.</t>
-  </si>
-  <si>
     <t>Worded with no interaction and Read 2001 example values.</t>
   </si>
   <si>
@@ -568,6 +562,18 @@
   </si>
   <si>
     <t>Question 4 (USD)</t>
+  </si>
+  <si>
+    <t>Barchart MEL question with no interaction inches.</t>
+  </si>
+  <si>
+    <t>Barchart with no interaction inches.</t>
+  </si>
+  <si>
+    <t>Barchart MEL question with no interaction pixels.</t>
+  </si>
+  <si>
+    <t>Barchart with no interaction pixels.</t>
   </si>
 </sst>
 </file>
@@ -1295,11 +1301,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V47"/>
+  <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S7" sqref="S7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1427,7 +1433,7 @@
         <v>4</v>
       </c>
       <c r="V2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -1468,7 +1474,7 @@
         <v>8</v>
       </c>
       <c r="V3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -1509,7 +1515,7 @@
         <v>8</v>
       </c>
       <c r="V4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -1546,12 +1552,6 @@
       <c r="M5">
         <v>10</v>
       </c>
-      <c r="N5">
-        <v>100</v>
-      </c>
-      <c r="O5">
-        <v>100</v>
-      </c>
       <c r="P5">
         <v>1</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>8.5</v>
       </c>
       <c r="V5" t="s">
-        <v>126</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -1608,12 +1608,6 @@
       <c r="M6">
         <v>15</v>
       </c>
-      <c r="N6">
-        <v>100</v>
-      </c>
-      <c r="O6">
-        <v>100</v>
-      </c>
       <c r="P6">
         <v>1</v>
       </c>
@@ -1633,7 +1627,7 @@
         <v>8.5</v>
       </c>
       <c r="V6" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -1670,12 +1664,6 @@
       <c r="M7">
         <v>15</v>
       </c>
-      <c r="N7">
-        <v>100</v>
-      </c>
-      <c r="O7">
-        <v>100</v>
-      </c>
       <c r="P7">
         <v>1</v>
       </c>
@@ -1695,7 +1683,7 @@
         <v>4.5</v>
       </c>
       <c r="V7" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -1706,7 +1694,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
         <v>118</v>
@@ -1717,32 +1705,29 @@
       <c r="F8">
         <v>300</v>
       </c>
-      <c r="H8" s="36">
-        <v>44593</v>
+      <c r="G8">
+        <v>2</v>
       </c>
       <c r="I8">
         <v>700</v>
       </c>
-      <c r="K8" s="36">
-        <v>44614</v>
+      <c r="J8">
+        <v>5</v>
       </c>
       <c r="L8">
         <v>1100</v>
       </c>
+      <c r="M8">
+        <v>10</v>
+      </c>
       <c r="N8">
-        <v>100</v>
+        <v>800</v>
       </c>
       <c r="O8">
-        <v>100</v>
-      </c>
-      <c r="T8">
-        <v>8</v>
-      </c>
-      <c r="U8">
-        <v>8</v>
+        <v>200</v>
       </c>
       <c r="V8" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -1753,7 +1738,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="D9" t="s">
         <v>118</v>
@@ -1764,32 +1749,29 @@
       <c r="F9">
         <v>500</v>
       </c>
-      <c r="H9" s="36">
-        <v>44621</v>
+      <c r="G9">
+        <v>2</v>
       </c>
       <c r="I9">
         <v>800</v>
       </c>
-      <c r="K9" s="36">
-        <v>44632</v>
+      <c r="J9">
+        <v>7</v>
       </c>
       <c r="L9">
         <v>1100</v>
       </c>
+      <c r="M9">
+        <v>15</v>
+      </c>
       <c r="N9">
-        <v>100</v>
+        <v>800</v>
       </c>
       <c r="O9">
-        <v>100</v>
-      </c>
-      <c r="T9">
-        <v>8</v>
-      </c>
-      <c r="U9">
-        <v>8</v>
+        <v>200</v>
       </c>
       <c r="V9" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:22">
@@ -1800,7 +1782,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="D10" t="s">
         <v>118</v>
@@ -1811,32 +1793,29 @@
       <c r="F10">
         <v>300</v>
       </c>
-      <c r="H10" s="36">
-        <v>44652</v>
+      <c r="G10">
+        <v>2</v>
       </c>
       <c r="I10">
         <v>1000</v>
       </c>
-      <c r="K10" s="36">
-        <v>44666</v>
+      <c r="J10">
+        <v>7</v>
       </c>
       <c r="L10">
         <v>1100</v>
       </c>
+      <c r="M10">
+        <v>15</v>
+      </c>
       <c r="N10">
-        <v>100</v>
+        <v>800</v>
       </c>
       <c r="O10">
-        <v>100</v>
-      </c>
-      <c r="T10">
-        <v>8</v>
-      </c>
-      <c r="U10">
-        <v>8</v>
+        <v>200</v>
       </c>
       <c r="V10" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -1988,31 +1967,28 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D14" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E14" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F14">
-        <v>500</v>
-      </c>
-      <c r="G14">
-        <v>2</v>
+        <v>300</v>
+      </c>
+      <c r="H14" s="36">
+        <v>44593</v>
       </c>
       <c r="I14">
-        <v>1000</v>
-      </c>
-      <c r="J14">
-        <v>10</v>
+        <v>700</v>
+      </c>
+      <c r="K14" s="36">
+        <v>44614</v>
       </c>
       <c r="L14">
-        <v>1500</v>
-      </c>
-      <c r="M14">
-        <v>10</v>
+        <v>1100</v>
       </c>
       <c r="N14">
         <v>100</v>
@@ -2020,23 +1996,11 @@
       <c r="O14">
         <v>100</v>
       </c>
-      <c r="P14">
-        <v>0.5</v>
-      </c>
-      <c r="Q14">
-        <v>0.5</v>
-      </c>
-      <c r="R14">
+      <c r="T14">
         <v>8</v>
       </c>
-      <c r="S14">
+      <c r="U14">
         <v>8</v>
-      </c>
-      <c r="T14">
-        <v>8.5</v>
-      </c>
-      <c r="U14">
-        <v>8.5</v>
       </c>
       <c r="V14" t="s">
         <v>135</v>
@@ -2044,31 +2008,31 @@
     </row>
     <row r="15" spans="1:22">
       <c r="A15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="D15" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E15" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F15">
         <v>500</v>
       </c>
       <c r="H15" s="36">
-        <v>44593</v>
+        <v>44621</v>
       </c>
       <c r="I15">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="K15" s="36">
-        <v>44614</v>
+        <v>44632</v>
       </c>
       <c r="L15">
         <v>1100</v>
@@ -2086,39 +2050,45 @@
         <v>8</v>
       </c>
       <c r="V15" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:22">
       <c r="A16">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="D16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E16" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F16">
-        <v>500</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
+        <v>300</v>
+      </c>
+      <c r="H16" s="36">
+        <v>44652</v>
       </c>
       <c r="I16">
         <v>1000</v>
       </c>
-      <c r="J16">
-        <v>3</v>
-      </c>
-      <c r="M16">
-        <v>10</v>
+      <c r="K16" s="36">
+        <v>44666</v>
+      </c>
+      <c r="L16">
+        <v>1100</v>
+      </c>
+      <c r="N16">
+        <v>100</v>
+      </c>
+      <c r="O16">
+        <v>100</v>
       </c>
       <c r="T16">
         <v>8</v>
@@ -2127,12 +2097,12 @@
         <v>8</v>
       </c>
       <c r="V16" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:22">
       <c r="A17">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2141,7 +2111,7 @@
         <v>104</v>
       </c>
       <c r="D17" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E17" t="s">
         <v>124</v>
@@ -2189,21 +2159,21 @@
         <v>8.5</v>
       </c>
       <c r="V17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:22">
       <c r="A18">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="D18" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E18" t="s">
         <v>124</v>
@@ -2236,18 +2206,18 @@
         <v>8</v>
       </c>
       <c r="V18" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:22">
       <c r="A19">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D19" t="s">
         <v>117</v>
@@ -2258,23 +2228,17 @@
       <c r="F19">
         <v>500</v>
       </c>
-      <c r="H19" s="36">
-        <v>44593</v>
+      <c r="G19">
+        <v>2</v>
       </c>
       <c r="I19">
         <v>1000</v>
       </c>
-      <c r="K19" s="36">
-        <v>44614</v>
-      </c>
-      <c r="L19">
-        <v>1100</v>
-      </c>
-      <c r="N19">
-        <v>100</v>
-      </c>
-      <c r="O19">
-        <v>100</v>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="M19">
+        <v>10</v>
       </c>
       <c r="T19">
         <v>8</v>
@@ -2283,21 +2247,21 @@
         <v>8</v>
       </c>
       <c r="V19" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:22">
       <c r="A20">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="D20" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E20" t="s">
         <v>124</v>
@@ -2305,17 +2269,20 @@
       <c r="F20">
         <v>500</v>
       </c>
-      <c r="H20" s="36">
-        <v>44593</v>
+      <c r="G20">
+        <v>2</v>
       </c>
       <c r="I20">
         <v>1000</v>
       </c>
-      <c r="K20" s="36">
-        <v>44614</v>
+      <c r="J20">
+        <v>10</v>
       </c>
       <c r="L20">
-        <v>1100</v>
+        <v>1500</v>
+      </c>
+      <c r="M20">
+        <v>10</v>
       </c>
       <c r="N20">
         <v>100</v>
@@ -2323,19 +2290,31 @@
       <c r="O20">
         <v>100</v>
       </c>
+      <c r="P20">
+        <v>0.5</v>
+      </c>
+      <c r="Q20">
+        <v>0.5</v>
+      </c>
+      <c r="R20">
+        <v>8</v>
+      </c>
+      <c r="S20">
+        <v>8</v>
+      </c>
       <c r="T20">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="U20">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="V20" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:22">
       <c r="A21">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2359,7 +2338,7 @@
         <v>1000</v>
       </c>
       <c r="K21" s="36">
-        <v>44835</v>
+        <v>44614</v>
       </c>
       <c r="L21">
         <v>1100</v>
@@ -2371,27 +2350,27 @@
         <v>100</v>
       </c>
       <c r="T21">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U21">
         <v>8</v>
       </c>
       <c r="V21" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:22">
       <c r="A22">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D22" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E22" t="s">
         <v>124</v>
@@ -2406,7 +2385,7 @@
         <v>1000</v>
       </c>
       <c r="K22" s="36">
-        <v>44835</v>
+        <v>44614</v>
       </c>
       <c r="L22">
         <v>1100</v>
@@ -2418,18 +2397,18 @@
         <v>100</v>
       </c>
       <c r="T22">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U22">
         <v>8</v>
       </c>
       <c r="V22" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:22">
       <c r="A23">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2438,22 +2417,22 @@
         <v>127</v>
       </c>
       <c r="D23" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="E23" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F23">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="H23" s="36">
         <v>44593</v>
       </c>
       <c r="I23">
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="K23" s="36">
-        <v>44703</v>
+        <v>44614</v>
       </c>
       <c r="L23">
         <v>1100</v>
@@ -2465,42 +2444,42 @@
         <v>100</v>
       </c>
       <c r="T23">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U23">
         <v>8</v>
       </c>
       <c r="V23" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:22">
       <c r="A24">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E24" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F24">
         <v>500</v>
       </c>
       <c r="H24" s="36">
-        <v>44621</v>
+        <v>44593</v>
       </c>
       <c r="I24">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="K24" s="36">
-        <v>44724</v>
+        <v>44835</v>
       </c>
       <c r="L24">
         <v>1100</v>
@@ -2518,7 +2497,7 @@
         <v>8</v>
       </c>
       <c r="V24" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:22">
@@ -2526,28 +2505,28 @@
         <v>14</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
         <v>127</v>
       </c>
       <c r="D25" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="E25" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F25">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="H25" s="36">
-        <v>44652</v>
+        <v>44593</v>
       </c>
       <c r="I25">
         <v>1000</v>
       </c>
       <c r="K25" s="36">
-        <v>44757</v>
+        <v>44835</v>
       </c>
       <c r="L25">
         <v>1100</v>
@@ -2565,7 +2544,7 @@
         <v>8</v>
       </c>
       <c r="V25" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:22">
@@ -2576,7 +2555,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D26" t="s">
         <v>118</v>
@@ -2612,7 +2591,7 @@
         <v>8</v>
       </c>
       <c r="V26" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:22">
@@ -2623,7 +2602,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D27" t="s">
         <v>118</v>
@@ -2659,7 +2638,7 @@
         <v>8</v>
       </c>
       <c r="V27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:22">
@@ -2670,7 +2649,7 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D28" t="s">
         <v>118</v>
@@ -2706,7 +2685,7 @@
         <v>8</v>
       </c>
       <c r="V28" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:22">
@@ -2717,7 +2696,7 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D29" t="s">
         <v>118</v>
@@ -2753,7 +2732,7 @@
         <v>8</v>
       </c>
       <c r="V29" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:22">
@@ -2764,7 +2743,7 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D30" t="s">
         <v>118</v>
@@ -2800,7 +2779,7 @@
         <v>8</v>
       </c>
       <c r="V30" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:22">
@@ -2811,7 +2790,7 @@
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D31" t="s">
         <v>118</v>
@@ -2847,7 +2826,7 @@
         <v>8</v>
       </c>
       <c r="V31" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:22">
@@ -2858,7 +2837,7 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D32" t="s">
         <v>118</v>
@@ -2876,7 +2855,7 @@
         <v>700</v>
       </c>
       <c r="K32" s="36">
-        <v>44614</v>
+        <v>44703</v>
       </c>
       <c r="L32">
         <v>1100</v>
@@ -2888,13 +2867,13 @@
         <v>100</v>
       </c>
       <c r="T32">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="U32">
         <v>8</v>
       </c>
       <c r="V32" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:22">
@@ -2905,7 +2884,7 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D33" t="s">
         <v>118</v>
@@ -2923,7 +2902,7 @@
         <v>800</v>
       </c>
       <c r="K33" s="36">
-        <v>44632</v>
+        <v>44724</v>
       </c>
       <c r="L33">
         <v>1100</v>
@@ -2935,13 +2914,13 @@
         <v>100</v>
       </c>
       <c r="T33">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="U33">
         <v>8</v>
       </c>
       <c r="V33" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:22">
@@ -2952,7 +2931,7 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D34" t="s">
         <v>118</v>
@@ -2970,7 +2949,7 @@
         <v>1000</v>
       </c>
       <c r="K34" s="36">
-        <v>44666</v>
+        <v>44757</v>
       </c>
       <c r="L34">
         <v>1100</v>
@@ -2982,13 +2961,13 @@
         <v>100</v>
       </c>
       <c r="T34">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="U34">
         <v>8</v>
       </c>
       <c r="V34" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:22">
@@ -2999,13 +2978,13 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D35" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E35" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F35">
         <v>300</v>
@@ -3035,7 +3014,7 @@
         <v>8</v>
       </c>
       <c r="V35" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:22">
@@ -3046,13 +3025,13 @@
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D36" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E36" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F36">
         <v>500</v>
@@ -3082,7 +3061,7 @@
         <v>8</v>
       </c>
       <c r="V36" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:22">
@@ -3093,13 +3072,13 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D37" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E37" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F37">
         <v>300</v>
@@ -3129,80 +3108,92 @@
         <v>8</v>
       </c>
       <c r="V37" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:22">
       <c r="A38">
+        <v>19</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>141</v>
+      </c>
+      <c r="D38" t="s">
+        <v>117</v>
+      </c>
+      <c r="E38" t="s">
+        <v>124</v>
+      </c>
+      <c r="F38">
+        <v>300</v>
+      </c>
+      <c r="H38" s="36">
+        <v>44593</v>
+      </c>
+      <c r="I38">
+        <v>700</v>
+      </c>
+      <c r="K38" s="36">
+        <v>44614</v>
+      </c>
+      <c r="L38">
+        <v>1100</v>
+      </c>
+      <c r="N38">
         <v>100</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>120</v>
-      </c>
-      <c r="D38" t="s">
-        <v>118</v>
-      </c>
-      <c r="E38" t="s">
-        <v>118</v>
-      </c>
-      <c r="F38">
-        <v>350</v>
-      </c>
-      <c r="G38">
-        <v>4</v>
-      </c>
-      <c r="I38">
-        <v>420</v>
-      </c>
-      <c r="J38">
-        <v>12</v>
-      </c>
-      <c r="M38">
-        <v>12</v>
+      <c r="O38">
+        <v>100</v>
       </c>
       <c r="T38">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="U38">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="V38" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:22">
       <c r="A39">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="B39">
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="D39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E39" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F39">
-        <v>490</v>
-      </c>
-      <c r="G39">
-        <v>2</v>
+        <v>500</v>
+      </c>
+      <c r="H39" s="36">
+        <v>44621</v>
       </c>
       <c r="I39">
-        <v>700</v>
-      </c>
-      <c r="J39">
-        <v>12</v>
-      </c>
-      <c r="M39">
-        <v>12</v>
+        <v>800</v>
+      </c>
+      <c r="K39" s="36">
+        <v>44632</v>
+      </c>
+      <c r="L39">
+        <v>1100</v>
+      </c>
+      <c r="N39">
+        <v>100</v>
+      </c>
+      <c r="O39">
+        <v>100</v>
       </c>
       <c r="T39">
         <v>8</v>
@@ -3211,39 +3202,45 @@
         <v>8</v>
       </c>
       <c r="V39" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:22">
       <c r="A40">
+        <v>19</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>141</v>
+      </c>
+      <c r="D40" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" t="s">
+        <v>124</v>
+      </c>
+      <c r="F40">
+        <v>300</v>
+      </c>
+      <c r="H40" s="36">
+        <v>44652</v>
+      </c>
+      <c r="I40">
+        <v>1000</v>
+      </c>
+      <c r="K40" s="36">
+        <v>44666</v>
+      </c>
+      <c r="L40">
+        <v>1100</v>
+      </c>
+      <c r="N40">
         <v>100</v>
       </c>
-      <c r="B40">
-        <v>3</v>
-      </c>
-      <c r="C40" t="s">
-        <v>120</v>
-      </c>
-      <c r="D40" t="s">
-        <v>118</v>
-      </c>
-      <c r="E40" t="s">
-        <v>118</v>
-      </c>
-      <c r="F40">
-        <v>720</v>
-      </c>
-      <c r="G40">
-        <v>6</v>
-      </c>
-      <c r="I40">
-        <v>1380</v>
-      </c>
-      <c r="J40">
-        <v>12</v>
-      </c>
-      <c r="M40">
-        <v>12</v>
+      <c r="O40">
+        <v>100</v>
       </c>
       <c r="T40">
         <v>8</v>
@@ -3252,7 +3249,7 @@
         <v>8</v>
       </c>
       <c r="V40" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:22">
@@ -3260,7 +3257,7 @@
         <v>100</v>
       </c>
       <c r="B41">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
         <v>120</v>
@@ -3272,19 +3269,28 @@
         <v>118</v>
       </c>
       <c r="F41">
-        <v>840</v>
+        <v>350</v>
       </c>
       <c r="G41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I41">
-        <v>1130</v>
+        <v>420</v>
       </c>
       <c r="J41">
         <v>12</v>
       </c>
       <c r="M41">
         <v>12</v>
+      </c>
+      <c r="T41">
+        <v>4</v>
+      </c>
+      <c r="U41">
+        <v>4</v>
+      </c>
+      <c r="V41" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:22">
@@ -3292,7 +3298,7 @@
         <v>100</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
         <v>120</v>
@@ -3304,19 +3310,28 @@
         <v>118</v>
       </c>
       <c r="F42">
-        <v>32</v>
+        <v>490</v>
       </c>
       <c r="G42">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I42">
-        <v>39</v>
+        <v>700</v>
       </c>
       <c r="J42">
         <v>12</v>
       </c>
       <c r="M42">
         <v>12</v>
+      </c>
+      <c r="T42">
+        <v>8</v>
+      </c>
+      <c r="U42">
+        <v>8</v>
+      </c>
+      <c r="V42" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:22">
@@ -3324,7 +3339,7 @@
         <v>100</v>
       </c>
       <c r="B43">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C43" t="s">
         <v>120</v>
@@ -3336,19 +3351,28 @@
         <v>118</v>
       </c>
       <c r="F43">
-        <v>794</v>
+        <v>720</v>
       </c>
       <c r="G43">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I43">
-        <v>1069</v>
+        <v>1380</v>
       </c>
       <c r="J43">
         <v>12</v>
       </c>
       <c r="M43">
         <v>12</v>
+      </c>
+      <c r="T43">
+        <v>8</v>
+      </c>
+      <c r="U43">
+        <v>8</v>
+      </c>
+      <c r="V43" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:22">
@@ -3356,7 +3380,7 @@
         <v>100</v>
       </c>
       <c r="B44">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C44" t="s">
         <v>120</v>
@@ -3367,8 +3391,20 @@
       <c r="E44" t="s">
         <v>118</v>
       </c>
+      <c r="F44">
+        <v>840</v>
+      </c>
+      <c r="G44">
+        <v>3</v>
+      </c>
       <c r="I44">
-        <v>6000</v>
+        <v>1130</v>
+      </c>
+      <c r="J44">
+        <v>12</v>
+      </c>
+      <c r="M44">
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:22">
@@ -3376,7 +3412,7 @@
         <v>100</v>
       </c>
       <c r="B45">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
         <v>120</v>
@@ -3387,8 +3423,20 @@
       <c r="E45" t="s">
         <v>118</v>
       </c>
+      <c r="F45">
+        <v>32</v>
+      </c>
+      <c r="G45">
+        <v>4</v>
+      </c>
       <c r="I45">
-        <v>6000</v>
+        <v>39</v>
+      </c>
+      <c r="J45">
+        <v>12</v>
+      </c>
+      <c r="M45">
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:22">
@@ -3396,7 +3444,7 @@
         <v>100</v>
       </c>
       <c r="B46">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C46" t="s">
         <v>120</v>
@@ -3406,6 +3454,21 @@
       </c>
       <c r="E46" t="s">
         <v>118</v>
+      </c>
+      <c r="F46">
+        <v>794</v>
+      </c>
+      <c r="G46">
+        <v>4</v>
+      </c>
+      <c r="I46">
+        <v>1069</v>
+      </c>
+      <c r="J46">
+        <v>12</v>
+      </c>
+      <c r="M46">
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:22">
@@ -3413,7 +3476,7 @@
         <v>100</v>
       </c>
       <c r="B47">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C47" t="s">
         <v>120</v>
@@ -3422,6 +3485,63 @@
         <v>118</v>
       </c>
       <c r="E47" t="s">
+        <v>118</v>
+      </c>
+      <c r="I47">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22">
+      <c r="A48">
+        <v>100</v>
+      </c>
+      <c r="B48">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>120</v>
+      </c>
+      <c r="D48" t="s">
+        <v>118</v>
+      </c>
+      <c r="E48" t="s">
+        <v>118</v>
+      </c>
+      <c r="I48">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>100</v>
+      </c>
+      <c r="B49">
+        <v>9</v>
+      </c>
+      <c r="C49" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" t="s">
+        <v>118</v>
+      </c>
+      <c r="E49" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>100</v>
+      </c>
+      <c r="B50">
+        <v>10</v>
+      </c>
+      <c r="C50" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" t="s">
+        <v>118</v>
+      </c>
+      <c r="E50" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3453,48 +3573,48 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" s="51" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="73" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D1" s="74"/>
       <c r="E1" s="73" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F1" s="74"/>
       <c r="G1" s="73" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H1" s="74"/>
       <c r="I1" s="73" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J1" s="74"/>
       <c r="K1" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="L1" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="L1" s="40" t="s">
-        <v>156</v>
-      </c>
       <c r="M1" s="70" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="N1" s="71"/>
       <c r="O1" s="67"/>
       <c r="P1" s="70" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Q1" s="71"/>
       <c r="R1" s="67"/>
       <c r="S1" s="70" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="T1" s="71"/>
       <c r="U1" s="67"/>
       <c r="V1" s="72" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="W1" s="71"/>
     </row>
@@ -3502,57 +3622,57 @@
       <c r="A2" s="52"/>
       <c r="B2" s="48"/>
       <c r="C2" s="46" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D2" s="54" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E2" s="46" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F2" s="54" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G2" s="46" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H2" s="54" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I2" s="46" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J2" s="54" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K2" s="48"/>
       <c r="L2" s="48"/>
       <c r="M2" s="56" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="N2" s="57" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="O2" s="68"/>
       <c r="P2" s="59" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="Q2" s="50" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="R2" s="68"/>
       <c r="S2" s="59" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="T2" s="50" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="U2" s="68"/>
       <c r="V2" s="49" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="W2" s="50" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:24">
@@ -3560,7 +3680,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C3" s="41">
         <v>370</v>
@@ -3644,7 +3764,7 @@
     <row r="4" spans="1:24">
       <c r="A4" s="53"/>
       <c r="B4" s="42" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C4" s="65">
         <v>37890</v>
@@ -3687,7 +3807,7 @@
     <row r="5" spans="1:24">
       <c r="A5" s="53"/>
       <c r="B5" s="42" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C5" s="41">
         <v>4</v>
@@ -3730,7 +3850,7 @@
     <row r="6" spans="1:24">
       <c r="A6" s="53"/>
       <c r="B6" s="42" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C6" s="41">
         <v>17</v>
@@ -3775,7 +3895,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C7" s="38">
         <v>370</v>
@@ -3859,7 +3979,7 @@
     <row r="8" spans="1:24">
       <c r="A8" s="53"/>
       <c r="B8" s="42" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C8" s="65">
         <v>37925</v>
@@ -3902,7 +4022,7 @@
     <row r="9" spans="1:24">
       <c r="A9" s="53"/>
       <c r="B9" s="42" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C9" s="41">
         <v>4</v>
@@ -3945,7 +4065,7 @@
     <row r="10" spans="1:24">
       <c r="A10" s="53"/>
       <c r="B10" s="42" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C10" s="41"/>
       <c r="D10" s="55"/>
@@ -3974,7 +4094,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="64" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C11" s="38">
         <v>37</v>
@@ -4058,7 +4178,7 @@
     <row r="12" spans="1:24">
       <c r="A12" s="53"/>
       <c r="B12" s="45" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C12" s="65">
         <v>38436</v>
@@ -4101,7 +4221,7 @@
     <row r="13" spans="1:24">
       <c r="A13" s="53"/>
       <c r="B13" s="45" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C13" s="41">
         <v>4</v>
@@ -4144,7 +4264,7 @@
     <row r="14" spans="1:24">
       <c r="A14" s="53"/>
       <c r="B14" s="45" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C14" s="41"/>
       <c r="D14" s="55"/>
@@ -4173,7 +4293,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="64" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C15" s="38">
         <v>900</v>
@@ -4257,7 +4377,7 @@
     <row r="16" spans="1:24">
       <c r="A16" s="53"/>
       <c r="B16" s="45" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C16" s="65">
         <v>38044</v>
@@ -4300,7 +4420,7 @@
     <row r="17" spans="1:23">
       <c r="A17" s="53"/>
       <c r="B17" s="45" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C17" s="41">
         <v>4</v>
@@ -4343,7 +4463,7 @@
     <row r="18" spans="1:23">
       <c r="A18" s="52"/>
       <c r="B18" s="47" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C18" s="46"/>
       <c r="D18" s="54"/>
@@ -4369,12 +4489,12 @@
     </row>
     <row r="23" spans="1:23">
       <c r="B23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:23">
       <c r="B24" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed y axis centering.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ADC001-E336-AA42-84F2-2147118A2E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52022229-C69B-5245-A0E6-9875F7660DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -927,6 +927,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -955,15 +973,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -977,15 +986,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1304,8 +1304,8 @@
   <dimension ref="A1:V50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -4543,105 +4543,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="75" t="s">
+      <c r="A2" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="75" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="76"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="84" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="82"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="90" t="s">
+      <c r="I2" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="90" t="s">
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="90"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="84" t="s">
+      <c r="S2" s="93"/>
+      <c r="T2" s="93"/>
+      <c r="U2" s="93"/>
+      <c r="V2" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="84" t="s">
+      <c r="W2" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="92" t="s">
+      <c r="X2" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="92" t="s">
+      <c r="Y2" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="92" t="s">
+      <c r="Z2" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="92" t="s">
+      <c r="AA2" s="75" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="82"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="91" t="s">
+      <c r="A3" s="88"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89" t="s">
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89" t="s">
+      <c r="M3" s="92"/>
+      <c r="N3" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89" t="s">
+      <c r="O3" s="92"/>
+      <c r="P3" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="87" t="s">
+      <c r="Q3" s="92"/>
+      <c r="R3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="87" t="s">
+      <c r="S3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="87" t="s">
+      <c r="T3" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="87" t="s">
+      <c r="U3" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="85"/>
-      <c r="W3" s="85"/>
-      <c r="X3" s="93"/>
-      <c r="Y3" s="93"/>
-      <c r="Z3" s="93"/>
-      <c r="AA3" s="93"/>
+      <c r="V3" s="79"/>
+      <c r="W3" s="79"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="76"/>
+      <c r="Z3" s="76"/>
+      <c r="AA3" s="76"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="83"/>
+      <c r="A4" s="89"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -4660,7 +4660,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="86"/>
+      <c r="H4" s="80"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -4688,16 +4688,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="86"/>
-      <c r="X4" s="94"/>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="94"/>
-      <c r="AA4" s="93"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="80"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="77"/>
+      <c r="Z4" s="77"/>
+      <c r="AA4" s="76"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -5198,11 +5198,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -5218,6 +5213,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Set LL time to 24 months to fix horizontal scale.
Set the largest LL time to 24 months.  Fixed the font size of labels.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C79D2C5-3B5D-7947-81FF-A0668807CF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11EC721-A181-5241-937E-CAFF68FB8DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -957,9 +957,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -978,23 +975,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1024,6 +1006,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1037,6 +1028,15 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1356,7 +1356,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1566,14 +1566,14 @@
         <v>1390</v>
       </c>
       <c r="J4" s="70">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="K4" s="71"/>
       <c r="L4">
         <v>1390</v>
       </c>
       <c r="M4">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="N4">
         <v>400</v>
@@ -1751,14 +1751,14 @@
         <v>1390</v>
       </c>
       <c r="J8" s="70">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="K8" s="71"/>
       <c r="L8">
         <v>1390</v>
       </c>
       <c r="M8">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="N8">
         <v>800</v>
@@ -5798,7 +5798,7 @@
       <c r="F2" s="71"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.85954777800089432</v>
+        <v>0.75964145260143401</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -5818,7 +5818,7 @@
       <c r="F3" s="71"/>
       <c r="G3">
         <f t="shared" ref="G3:G5" ca="1" si="0">RAND()</f>
-        <v>0.83479094015949928</v>
+        <v>0.92197293349524667</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5839,7 +5839,7 @@
       <c r="F4" s="71"/>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62721566724432698</v>
+        <v>0.64711392912696031</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5859,7 +5859,7 @@
       <c r="F5" s="71"/>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12934531904512536</v>
+        <v>5.1889264169065363E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5936,7 +5936,7 @@
   <dimension ref="A1:X40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N29" sqref="N29:N32"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5953,48 +5953,48 @@
         <v>145</v>
       </c>
       <c r="B1" s="39"/>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="73" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="75"/>
-      <c r="E1" s="74" t="s">
+      <c r="D1" s="74"/>
+      <c r="E1" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="F1" s="75"/>
-      <c r="G1" s="74" t="s">
+      <c r="F1" s="74"/>
+      <c r="G1" s="73" t="s">
         <v>158</v>
       </c>
-      <c r="H1" s="75"/>
-      <c r="I1" s="74" t="s">
+      <c r="H1" s="74"/>
+      <c r="I1" s="73" t="s">
         <v>159</v>
       </c>
-      <c r="J1" s="75"/>
+      <c r="J1" s="74"/>
       <c r="K1" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L1" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M1" s="76" t="s">
+      <c r="M1" s="75" t="s">
         <v>160</v>
       </c>
-      <c r="N1" s="77"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="76" t="s">
+      <c r="N1" s="76"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="76" t="s">
+      <c r="Q1" s="76"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="79" t="s">
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="78" t="s">
         <v>163</v>
       </c>
-      <c r="W1" s="79"/>
-      <c r="X1" s="79"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="52"/>
@@ -6887,16 +6887,16 @@
       </c>
     </row>
     <row r="27" spans="1:23">
-      <c r="C27" s="73" t="s">
+      <c r="C27" s="79" t="s">
         <v>169</v>
       </c>
-      <c r="D27" s="73"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73" t="s">
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79" t="s">
         <v>171</v>
       </c>
-      <c r="G27" s="73"/>
-      <c r="H27" s="73"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="79"/>
       <c r="I27" s="69" t="s">
         <v>170</v>
       </c>
@@ -7412,16 +7412,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="V1:X1"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7458,105 +7458,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="86" t="s">
+      <c r="A2" s="86" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="86" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="87"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="83" t="s">
+      <c r="C2" s="81"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="80" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="81"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="98" t="s">
+      <c r="I2" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
-      <c r="Q2" s="98"/>
-      <c r="R2" s="98" t="s">
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="95"/>
+      <c r="Q2" s="95"/>
+      <c r="R2" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="98"/>
-      <c r="T2" s="98"/>
-      <c r="U2" s="98"/>
-      <c r="V2" s="83" t="s">
+      <c r="S2" s="95"/>
+      <c r="T2" s="95"/>
+      <c r="U2" s="95"/>
+      <c r="V2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="83" t="s">
+      <c r="W2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="80" t="s">
+      <c r="X2" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="80" t="s">
+      <c r="Y2" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="80" t="s">
+      <c r="Z2" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="80" t="s">
+      <c r="AA2" s="97" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="93"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="99" t="s">
+      <c r="A3" s="87"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97" t="s">
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
+      <c r="L3" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97" t="s">
+      <c r="M3" s="94"/>
+      <c r="N3" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97" t="s">
+      <c r="O3" s="94"/>
+      <c r="P3" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="95" t="s">
+      <c r="Q3" s="94"/>
+      <c r="R3" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="95" t="s">
+      <c r="S3" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="95" t="s">
+      <c r="T3" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="95" t="s">
+      <c r="U3" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="84"/>
-      <c r="W3" s="84"/>
-      <c r="X3" s="81"/>
-      <c r="Y3" s="81"/>
-      <c r="Z3" s="81"/>
-      <c r="AA3" s="81"/>
+      <c r="V3" s="90"/>
+      <c r="W3" s="90"/>
+      <c r="X3" s="98"/>
+      <c r="Y3" s="98"/>
+      <c r="Z3" s="98"/>
+      <c r="AA3" s="98"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="94"/>
+      <c r="A4" s="88"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -7575,7 +7575,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="85"/>
+      <c r="H4" s="91"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -7603,16 +7603,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="96"/>
-      <c r="S4" s="96"/>
-      <c r="T4" s="96"/>
-      <c r="U4" s="96"/>
-      <c r="V4" s="85"/>
-      <c r="W4" s="85"/>
-      <c r="X4" s="82"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="82"/>
-      <c r="AA4" s="81"/>
+      <c r="R4" s="93"/>
+      <c r="S4" s="93"/>
+      <c r="T4" s="93"/>
+      <c r="U4" s="93"/>
+      <c r="V4" s="91"/>
+      <c r="W4" s="91"/>
+      <c r="X4" s="99"/>
+      <c r="Y4" s="99"/>
+      <c r="Z4" s="99"/>
+      <c r="AA4" s="98"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -8113,6 +8113,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -8128,11 +8133,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update staging branch to latest of main
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64EA149-FD03-754E-A7A2-9B3AF49BA6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2D468D-FED0-DC44-B123-DA6319684D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="1" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Web Parameters Prod" sheetId="10" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="191">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -986,9 +986,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1007,23 +1004,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1053,6 +1035,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1066,6 +1057,15 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1383,9 +1383,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6462F7B1-F956-1241-A84D-BB94A5075354}">
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M38" sqref="M38"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1873,7 +1873,7 @@
         <v>110</v>
       </c>
       <c r="J12" s="70">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K12" s="71"/>
       <c r="L12">
@@ -1916,9 +1916,6 @@
       <c r="L13">
         <v>120</v>
       </c>
-      <c r="M13">
-        <v>17</v>
-      </c>
       <c r="N13">
         <v>600</v>
       </c>
@@ -2417,14 +2414,14 @@
         <v>110</v>
       </c>
       <c r="J24" s="70">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K24" s="71"/>
       <c r="L24">
         <v>110</v>
       </c>
       <c r="M24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N24">
         <v>600</v>
@@ -2516,7 +2513,7 @@
         <v>430</v>
       </c>
       <c r="M26">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N26">
         <v>1200</v>
@@ -2562,7 +2559,7 @@
         <v>700</v>
       </c>
       <c r="M27">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N27">
         <v>1200</v>
@@ -2609,7 +2606,7 @@
         <v>1390</v>
       </c>
       <c r="M28">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N28">
         <v>1200</v>
@@ -2655,7 +2652,7 @@
         <v>1120</v>
       </c>
       <c r="M29">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N29">
         <v>1200</v>
@@ -2701,7 +2698,7 @@
         <v>14000</v>
       </c>
       <c r="M30">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="N30">
         <v>1200</v>
@@ -2747,7 +2744,7 @@
         <v>23000</v>
       </c>
       <c r="M31">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N31">
         <v>1200</v>
@@ -2793,7 +2790,7 @@
         <v>46000</v>
       </c>
       <c r="M32">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N32">
         <v>1200</v>
@@ -2839,7 +2836,7 @@
         <v>37000</v>
       </c>
       <c r="M33">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N33">
         <v>1200</v>
@@ -2885,7 +2882,7 @@
         <v>40</v>
       </c>
       <c r="M34">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N34">
         <v>1200</v>
@@ -2931,7 +2928,7 @@
         <v>70</v>
       </c>
       <c r="M35">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N35">
         <v>1200</v>
@@ -2970,14 +2967,14 @@
         <v>110</v>
       </c>
       <c r="J36" s="70">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K36" s="71"/>
       <c r="L36">
         <v>110</v>
       </c>
       <c r="M36">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="N36">
         <v>1200</v>
@@ -3023,7 +3020,7 @@
         <v>120</v>
       </c>
       <c r="M37">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N37">
         <v>1200</v>
@@ -4718,11 +4715,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V50"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -5141,7 +5138,7 @@
         <v>800</v>
       </c>
       <c r="O8">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="V8" t="s">
         <v>166</v>
@@ -5164,31 +5161,31 @@
         <v>118</v>
       </c>
       <c r="F9">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="G9">
         <v>2</v>
       </c>
       <c r="I9">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="J9">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L9">
         <v>1100</v>
       </c>
       <c r="M9">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="N9">
         <v>800</v>
       </c>
       <c r="O9">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="V9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:22">
@@ -5208,13 +5205,13 @@
         <v>118</v>
       </c>
       <c r="F10">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="G10">
         <v>2</v>
       </c>
       <c r="I10">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="J10">
         <v>7</v>
@@ -5229,7 +5226,7 @@
         <v>800</v>
       </c>
       <c r="O10">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="V10" t="s">
         <v>167</v>
@@ -5237,13 +5234,13 @@
     </row>
     <row r="11" spans="1:22">
       <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
         <v>4</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
       <c r="C11" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="D11" t="s">
         <v>118</v>
@@ -5252,81 +5249,75 @@
         <v>118</v>
       </c>
       <c r="F11">
-        <v>300</v>
-      </c>
-      <c r="H11" s="36">
-        <v>44593</v>
+        <v>500</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
       </c>
       <c r="I11">
-        <v>700</v>
-      </c>
-      <c r="K11" s="36">
-        <v>44614</v>
+        <v>800</v>
+      </c>
+      <c r="J11">
+        <v>7</v>
       </c>
       <c r="L11">
         <v>1100</v>
       </c>
+      <c r="M11">
+        <v>8</v>
+      </c>
       <c r="N11">
-        <v>100</v>
+        <v>800</v>
       </c>
       <c r="O11">
-        <v>100</v>
-      </c>
-      <c r="T11">
-        <v>8</v>
-      </c>
-      <c r="U11">
-        <v>8</v>
+        <v>300</v>
       </c>
       <c r="V11" t="s">
-        <v>136</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:22">
       <c r="A12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12">
+        <v>300</v>
+      </c>
+      <c r="G12">
         <v>2</v>
       </c>
-      <c r="C12" t="s">
-        <v>127</v>
-      </c>
-      <c r="D12" t="s">
-        <v>118</v>
-      </c>
-      <c r="E12" t="s">
-        <v>118</v>
-      </c>
-      <c r="F12">
-        <v>500</v>
-      </c>
-      <c r="H12" s="36">
-        <v>44621</v>
-      </c>
       <c r="I12">
-        <v>800</v>
-      </c>
-      <c r="K12" s="36">
-        <v>44632</v>
+        <v>1000</v>
+      </c>
+      <c r="J12">
+        <v>7</v>
       </c>
       <c r="L12">
         <v>1100</v>
       </c>
+      <c r="M12">
+        <v>15</v>
+      </c>
       <c r="N12">
-        <v>100</v>
+        <v>800</v>
       </c>
       <c r="O12">
-        <v>100</v>
-      </c>
-      <c r="T12">
-        <v>8</v>
-      </c>
-      <c r="U12">
-        <v>8</v>
+        <v>300</v>
       </c>
       <c r="V12" t="s">
-        <v>136</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:22">
@@ -5334,7 +5325,7 @@
         <v>4</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
         <v>127</v>
@@ -5349,13 +5340,13 @@
         <v>300</v>
       </c>
       <c r="H13" s="36">
-        <v>44652</v>
+        <v>44593</v>
       </c>
       <c r="I13">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="K13" s="36">
-        <v>44666</v>
+        <v>44614</v>
       </c>
       <c r="L13">
         <v>1100</v>
@@ -5378,13 +5369,13 @@
     </row>
     <row r="14" spans="1:22">
       <c r="A14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D14" t="s">
         <v>118</v>
@@ -5393,16 +5384,16 @@
         <v>118</v>
       </c>
       <c r="F14">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="H14" s="36">
-        <v>44593</v>
+        <v>44621</v>
       </c>
       <c r="I14">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="K14" s="36">
-        <v>44614</v>
+        <v>44632</v>
       </c>
       <c r="L14">
         <v>1100</v>
@@ -5420,18 +5411,18 @@
         <v>8</v>
       </c>
       <c r="V14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:22">
       <c r="A15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D15" t="s">
         <v>118</v>
@@ -5440,16 +5431,16 @@
         <v>118</v>
       </c>
       <c r="F15">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="H15" s="36">
-        <v>44621</v>
+        <v>44652</v>
       </c>
       <c r="I15">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="K15" s="36">
-        <v>44632</v>
+        <v>44666</v>
       </c>
       <c r="L15">
         <v>1100</v>
@@ -5467,7 +5458,7 @@
         <v>8</v>
       </c>
       <c r="V15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -5475,7 +5466,7 @@
         <v>5</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
         <v>126</v>
@@ -5490,13 +5481,13 @@
         <v>300</v>
       </c>
       <c r="H16" s="36">
-        <v>44652</v>
+        <v>44593</v>
       </c>
       <c r="I16">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="K16" s="36">
-        <v>44666</v>
+        <v>44614</v>
       </c>
       <c r="L16">
         <v>1100</v>
@@ -5519,37 +5510,34 @@
     </row>
     <row r="17" spans="1:22">
       <c r="A17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D17" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E17" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F17">
         <v>500</v>
       </c>
-      <c r="G17">
-        <v>2</v>
+      <c r="H17" s="36">
+        <v>44621</v>
       </c>
       <c r="I17">
-        <v>1000</v>
-      </c>
-      <c r="J17">
-        <v>10</v>
+        <v>800</v>
+      </c>
+      <c r="K17" s="36">
+        <v>44632</v>
       </c>
       <c r="L17">
-        <v>1500</v>
-      </c>
-      <c r="M17">
-        <v>10</v>
+        <v>1100</v>
       </c>
       <c r="N17">
         <v>100</v>
@@ -5557,55 +5545,43 @@
       <c r="O17">
         <v>100</v>
       </c>
-      <c r="P17">
-        <v>0.5</v>
-      </c>
-      <c r="Q17">
-        <v>0.5</v>
-      </c>
-      <c r="R17">
+      <c r="T17">
         <v>8</v>
       </c>
-      <c r="S17">
+      <c r="U17">
         <v>8</v>
       </c>
-      <c r="T17">
-        <v>8.5</v>
-      </c>
-      <c r="U17">
-        <v>8.5</v>
-      </c>
       <c r="V17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:22">
       <c r="A18">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="D18" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E18" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F18">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="H18" s="36">
-        <v>44593</v>
+        <v>44652</v>
       </c>
       <c r="I18">
         <v>1000</v>
       </c>
       <c r="K18" s="36">
-        <v>44614</v>
+        <v>44666</v>
       </c>
       <c r="L18">
         <v>1100</v>
@@ -5623,21 +5599,21 @@
         <v>8</v>
       </c>
       <c r="V18" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:22">
       <c r="A19">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E19" t="s">
         <v>124</v>
@@ -5652,33 +5628,54 @@
         <v>1000</v>
       </c>
       <c r="J19">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="L19">
+        <v>1500</v>
       </c>
       <c r="M19">
         <v>10</v>
       </c>
+      <c r="N19">
+        <v>100</v>
+      </c>
+      <c r="O19">
+        <v>100</v>
+      </c>
+      <c r="P19">
+        <v>0.5</v>
+      </c>
+      <c r="Q19">
+        <v>0.5</v>
+      </c>
+      <c r="R19">
+        <v>8</v>
+      </c>
+      <c r="S19">
+        <v>8</v>
+      </c>
       <c r="T19">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="U19">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="V19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:22">
       <c r="A20">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D20" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E20" t="s">
         <v>124</v>
@@ -5686,20 +5683,17 @@
       <c r="F20">
         <v>500</v>
       </c>
-      <c r="G20">
-        <v>2</v>
+      <c r="H20" s="36">
+        <v>44593</v>
       </c>
       <c r="I20">
         <v>1000</v>
       </c>
-      <c r="J20">
-        <v>10</v>
+      <c r="K20" s="36">
+        <v>44614</v>
       </c>
       <c r="L20">
-        <v>1500</v>
-      </c>
-      <c r="M20">
-        <v>10</v>
+        <v>1100</v>
       </c>
       <c r="N20">
         <v>100</v>
@@ -5707,37 +5701,25 @@
       <c r="O20">
         <v>100</v>
       </c>
-      <c r="P20">
-        <v>0.5</v>
-      </c>
-      <c r="Q20">
-        <v>0.5</v>
-      </c>
-      <c r="R20">
+      <c r="T20">
         <v>8</v>
       </c>
-      <c r="S20">
+      <c r="U20">
         <v>8</v>
       </c>
-      <c r="T20">
-        <v>8.5</v>
-      </c>
-      <c r="U20">
-        <v>8.5</v>
-      </c>
       <c r="V20" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:22">
       <c r="A21">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D21" t="s">
         <v>117</v>
@@ -5748,23 +5730,17 @@
       <c r="F21">
         <v>500</v>
       </c>
-      <c r="H21" s="36">
-        <v>44593</v>
+      <c r="G21">
+        <v>2</v>
       </c>
       <c r="I21">
         <v>1000</v>
       </c>
-      <c r="K21" s="36">
-        <v>44614</v>
-      </c>
-      <c r="L21">
-        <v>1100</v>
-      </c>
-      <c r="N21">
-        <v>100</v>
-      </c>
-      <c r="O21">
-        <v>100</v>
+      <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="M21">
+        <v>10</v>
       </c>
       <c r="T21">
         <v>8</v>
@@ -5773,18 +5749,18 @@
         <v>8</v>
       </c>
       <c r="V21" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:22">
       <c r="A22">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="D22" t="s">
         <v>117</v>
@@ -5795,17 +5771,20 @@
       <c r="F22">
         <v>500</v>
       </c>
-      <c r="H22" s="36">
-        <v>44593</v>
+      <c r="G22">
+        <v>2</v>
       </c>
       <c r="I22">
         <v>1000</v>
       </c>
-      <c r="K22" s="36">
-        <v>44614</v>
+      <c r="J22">
+        <v>10</v>
       </c>
       <c r="L22">
-        <v>1100</v>
+        <v>1500</v>
+      </c>
+      <c r="M22">
+        <v>10</v>
       </c>
       <c r="N22">
         <v>100</v>
@@ -5813,19 +5792,31 @@
       <c r="O22">
         <v>100</v>
       </c>
+      <c r="P22">
+        <v>0.5</v>
+      </c>
+      <c r="Q22">
+        <v>0.5</v>
+      </c>
+      <c r="R22">
+        <v>8</v>
+      </c>
+      <c r="S22">
+        <v>8</v>
+      </c>
       <c r="T22">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="U22">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="V22" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:22">
       <c r="A23">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -5834,7 +5825,7 @@
         <v>127</v>
       </c>
       <c r="D23" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E23" t="s">
         <v>124</v>
@@ -5867,12 +5858,12 @@
         <v>8</v>
       </c>
       <c r="V23" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:22">
       <c r="A24">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -5896,7 +5887,7 @@
         <v>1000</v>
       </c>
       <c r="K24" s="36">
-        <v>44835</v>
+        <v>44614</v>
       </c>
       <c r="L24">
         <v>1100</v>
@@ -5908,18 +5899,18 @@
         <v>100</v>
       </c>
       <c r="T24">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U24">
         <v>8</v>
       </c>
       <c r="V24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:22">
       <c r="A25">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -5943,7 +5934,7 @@
         <v>1000</v>
       </c>
       <c r="K25" s="36">
-        <v>44835</v>
+        <v>44614</v>
       </c>
       <c r="L25">
         <v>1100</v>
@@ -5955,18 +5946,18 @@
         <v>100</v>
       </c>
       <c r="T25">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U25">
         <v>8</v>
       </c>
       <c r="V25" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:22">
       <c r="A26">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -5975,22 +5966,22 @@
         <v>126</v>
       </c>
       <c r="D26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E26" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F26">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="H26" s="36">
         <v>44593</v>
       </c>
       <c r="I26">
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="K26" s="36">
-        <v>44703</v>
+        <v>44835</v>
       </c>
       <c r="L26">
         <v>1100</v>
@@ -6008,36 +5999,36 @@
         <v>8</v>
       </c>
       <c r="V26" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:22">
       <c r="A27">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D27" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="E27" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F27">
         <v>500</v>
       </c>
       <c r="H27" s="36">
-        <v>44621</v>
+        <v>44593</v>
       </c>
       <c r="I27">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="K27" s="36">
-        <v>44724</v>
+        <v>44835</v>
       </c>
       <c r="L27">
         <v>1100</v>
@@ -6055,7 +6046,7 @@
         <v>8</v>
       </c>
       <c r="V27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:22">
@@ -6063,7 +6054,7 @@
         <v>15</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C28" t="s">
         <v>126</v>
@@ -6078,13 +6069,13 @@
         <v>300</v>
       </c>
       <c r="H28" s="36">
-        <v>44652</v>
+        <v>44593</v>
       </c>
       <c r="I28">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="K28" s="36">
-        <v>44757</v>
+        <v>44703</v>
       </c>
       <c r="L28">
         <v>1100</v>
@@ -6107,13 +6098,13 @@
     </row>
     <row r="29" spans="1:22">
       <c r="A29">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D29" t="s">
         <v>118</v>
@@ -6122,16 +6113,16 @@
         <v>118</v>
       </c>
       <c r="F29">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="H29" s="36">
-        <v>44593</v>
+        <v>44621</v>
       </c>
       <c r="I29">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="K29" s="36">
-        <v>44703</v>
+        <v>44724</v>
       </c>
       <c r="L29">
         <v>1100</v>
@@ -6149,18 +6140,18 @@
         <v>8</v>
       </c>
       <c r="V29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:22">
       <c r="A30">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D30" t="s">
         <v>118</v>
@@ -6169,16 +6160,16 @@
         <v>118</v>
       </c>
       <c r="F30">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="H30" s="36">
-        <v>44621</v>
+        <v>44652</v>
       </c>
       <c r="I30">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="K30" s="36">
-        <v>44724</v>
+        <v>44757</v>
       </c>
       <c r="L30">
         <v>1100</v>
@@ -6196,7 +6187,7 @@
         <v>8</v>
       </c>
       <c r="V30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:22">
@@ -6204,7 +6195,7 @@
         <v>16</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
         <v>127</v>
@@ -6219,13 +6210,13 @@
         <v>300</v>
       </c>
       <c r="H31" s="36">
-        <v>44652</v>
+        <v>44593</v>
       </c>
       <c r="I31">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="K31" s="36">
-        <v>44757</v>
+        <v>44703</v>
       </c>
       <c r="L31">
         <v>1100</v>
@@ -6248,13 +6239,13 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="D32" t="s">
         <v>118</v>
@@ -6263,16 +6254,16 @@
         <v>118</v>
       </c>
       <c r="F32">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="H32" s="36">
-        <v>44593</v>
+        <v>44621</v>
       </c>
       <c r="I32">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="K32" s="36">
-        <v>44703</v>
+        <v>44724</v>
       </c>
       <c r="L32">
         <v>1100</v>
@@ -6290,18 +6281,18 @@
         <v>8</v>
       </c>
       <c r="V32" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:22">
       <c r="A33">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="D33" t="s">
         <v>118</v>
@@ -6310,16 +6301,16 @@
         <v>118</v>
       </c>
       <c r="F33">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="H33" s="36">
-        <v>44621</v>
+        <v>44652</v>
       </c>
       <c r="I33">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="K33" s="36">
-        <v>44724</v>
+        <v>44757</v>
       </c>
       <c r="L33">
         <v>1100</v>
@@ -6337,7 +6328,7 @@
         <v>8</v>
       </c>
       <c r="V33" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:22">
@@ -6345,7 +6336,7 @@
         <v>17</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
         <v>141</v>
@@ -6360,13 +6351,13 @@
         <v>300</v>
       </c>
       <c r="H34" s="36">
-        <v>44652</v>
+        <v>44593</v>
       </c>
       <c r="I34">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="K34" s="36">
-        <v>44757</v>
+        <v>44703</v>
       </c>
       <c r="L34">
         <v>1100</v>
@@ -6389,10 +6380,10 @@
     </row>
     <row r="35" spans="1:22">
       <c r="A35">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
         <v>141</v>
@@ -6404,16 +6395,16 @@
         <v>118</v>
       </c>
       <c r="F35">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="H35" s="36">
-        <v>44593</v>
+        <v>44621</v>
       </c>
       <c r="I35">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="K35" s="36">
-        <v>44614</v>
+        <v>44724</v>
       </c>
       <c r="L35">
         <v>1100</v>
@@ -6425,21 +6416,21 @@
         <v>100</v>
       </c>
       <c r="T35">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="U35">
         <v>8</v>
       </c>
       <c r="V35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:22">
       <c r="A36">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C36" t="s">
         <v>141</v>
@@ -6451,16 +6442,16 @@
         <v>118</v>
       </c>
       <c r="F36">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="H36" s="36">
-        <v>44621</v>
+        <v>44652</v>
       </c>
       <c r="I36">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="K36" s="36">
-        <v>44632</v>
+        <v>44757</v>
       </c>
       <c r="L36">
         <v>1100</v>
@@ -6472,13 +6463,13 @@
         <v>100</v>
       </c>
       <c r="T36">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="U36">
         <v>8</v>
       </c>
       <c r="V36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:22">
@@ -6486,7 +6477,7 @@
         <v>18</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
         <v>141</v>
@@ -6501,13 +6492,13 @@
         <v>300</v>
       </c>
       <c r="H37" s="36">
-        <v>44652</v>
+        <v>44593</v>
       </c>
       <c r="I37">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="K37" s="36">
-        <v>44666</v>
+        <v>44614</v>
       </c>
       <c r="L37">
         <v>1100</v>
@@ -6530,31 +6521,31 @@
     </row>
     <row r="38" spans="1:22">
       <c r="A38">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
         <v>141</v>
       </c>
       <c r="D38" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E38" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F38">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="H38" s="36">
-        <v>44593</v>
+        <v>44621</v>
       </c>
       <c r="I38">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="K38" s="36">
-        <v>44614</v>
+        <v>44632</v>
       </c>
       <c r="L38">
         <v>1100</v>
@@ -6572,36 +6563,36 @@
         <v>8</v>
       </c>
       <c r="V38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:22">
       <c r="A39">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C39" t="s">
         <v>141</v>
       </c>
       <c r="D39" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E39" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F39">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="H39" s="36">
-        <v>44621</v>
+        <v>44652</v>
       </c>
       <c r="I39">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="K39" s="36">
-        <v>44632</v>
+        <v>44666</v>
       </c>
       <c r="L39">
         <v>1100</v>
@@ -6619,7 +6610,7 @@
         <v>8</v>
       </c>
       <c r="V39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:22">
@@ -6627,7 +6618,7 @@
         <v>19</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
         <v>141</v>
@@ -6642,13 +6633,13 @@
         <v>300</v>
       </c>
       <c r="H40" s="36">
-        <v>44652</v>
+        <v>44593</v>
       </c>
       <c r="I40">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="K40" s="36">
-        <v>44666</v>
+        <v>44614</v>
       </c>
       <c r="L40">
         <v>1100</v>
@@ -6671,75 +6662,87 @@
     </row>
     <row r="41" spans="1:22">
       <c r="A41">
+        <v>19</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>141</v>
+      </c>
+      <c r="D41" t="s">
+        <v>117</v>
+      </c>
+      <c r="E41" t="s">
+        <v>124</v>
+      </c>
+      <c r="F41">
+        <v>500</v>
+      </c>
+      <c r="H41" s="36">
+        <v>44621</v>
+      </c>
+      <c r="I41">
+        <v>800</v>
+      </c>
+      <c r="K41" s="36">
+        <v>44632</v>
+      </c>
+      <c r="L41">
+        <v>1100</v>
+      </c>
+      <c r="N41">
         <v>100</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>120</v>
-      </c>
-      <c r="D41" t="s">
-        <v>118</v>
-      </c>
-      <c r="E41" t="s">
-        <v>118</v>
-      </c>
-      <c r="F41">
-        <v>350</v>
-      </c>
-      <c r="G41">
-        <v>4</v>
-      </c>
-      <c r="I41">
-        <v>420</v>
-      </c>
-      <c r="J41">
-        <v>12</v>
-      </c>
-      <c r="M41">
-        <v>12</v>
+      <c r="O41">
+        <v>100</v>
       </c>
       <c r="T41">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="U41">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="V41" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:22">
       <c r="A42">
+        <v>19</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>141</v>
+      </c>
+      <c r="D42" t="s">
+        <v>117</v>
+      </c>
+      <c r="E42" t="s">
+        <v>124</v>
+      </c>
+      <c r="F42">
+        <v>300</v>
+      </c>
+      <c r="H42" s="36">
+        <v>44652</v>
+      </c>
+      <c r="I42">
+        <v>1000</v>
+      </c>
+      <c r="K42" s="36">
+        <v>44666</v>
+      </c>
+      <c r="L42">
+        <v>1100</v>
+      </c>
+      <c r="N42">
         <v>100</v>
       </c>
-      <c r="B42">
-        <v>2</v>
-      </c>
-      <c r="C42" t="s">
-        <v>120</v>
-      </c>
-      <c r="D42" t="s">
-        <v>118</v>
-      </c>
-      <c r="E42" t="s">
-        <v>118</v>
-      </c>
-      <c r="F42">
-        <v>490</v>
-      </c>
-      <c r="G42">
-        <v>2</v>
-      </c>
-      <c r="I42">
-        <v>700</v>
-      </c>
-      <c r="J42">
-        <v>12</v>
-      </c>
-      <c r="M42">
-        <v>12</v>
+      <c r="O42">
+        <v>100</v>
       </c>
       <c r="T42">
         <v>8</v>
@@ -6748,218 +6751,7 @@
         <v>8</v>
       </c>
       <c r="V42" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22">
-      <c r="A43">
-        <v>100</v>
-      </c>
-      <c r="B43">
-        <v>3</v>
-      </c>
-      <c r="C43" t="s">
-        <v>120</v>
-      </c>
-      <c r="D43" t="s">
-        <v>118</v>
-      </c>
-      <c r="E43" t="s">
-        <v>118</v>
-      </c>
-      <c r="F43">
-        <v>720</v>
-      </c>
-      <c r="G43">
-        <v>6</v>
-      </c>
-      <c r="I43">
-        <v>1380</v>
-      </c>
-      <c r="J43">
-        <v>12</v>
-      </c>
-      <c r="M43">
-        <v>12</v>
-      </c>
-      <c r="T43">
-        <v>8</v>
-      </c>
-      <c r="U43">
-        <v>8</v>
-      </c>
-      <c r="V43" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22">
-      <c r="A44">
-        <v>100</v>
-      </c>
-      <c r="B44">
-        <v>4</v>
-      </c>
-      <c r="C44" t="s">
-        <v>120</v>
-      </c>
-      <c r="D44" t="s">
-        <v>118</v>
-      </c>
-      <c r="E44" t="s">
-        <v>118</v>
-      </c>
-      <c r="F44">
-        <v>840</v>
-      </c>
-      <c r="G44">
-        <v>3</v>
-      </c>
-      <c r="I44">
-        <v>1130</v>
-      </c>
-      <c r="J44">
-        <v>12</v>
-      </c>
-      <c r="M44">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22">
-      <c r="A45">
-        <v>100</v>
-      </c>
-      <c r="B45">
-        <v>5</v>
-      </c>
-      <c r="C45" t="s">
-        <v>120</v>
-      </c>
-      <c r="D45" t="s">
-        <v>118</v>
-      </c>
-      <c r="E45" t="s">
-        <v>118</v>
-      </c>
-      <c r="F45">
-        <v>32</v>
-      </c>
-      <c r="G45">
-        <v>4</v>
-      </c>
-      <c r="I45">
-        <v>39</v>
-      </c>
-      <c r="J45">
-        <v>12</v>
-      </c>
-      <c r="M45">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:22">
-      <c r="A46">
-        <v>100</v>
-      </c>
-      <c r="B46">
-        <v>6</v>
-      </c>
-      <c r="C46" t="s">
-        <v>120</v>
-      </c>
-      <c r="D46" t="s">
-        <v>118</v>
-      </c>
-      <c r="E46" t="s">
-        <v>118</v>
-      </c>
-      <c r="F46">
-        <v>794</v>
-      </c>
-      <c r="G46">
-        <v>4</v>
-      </c>
-      <c r="I46">
-        <v>1069</v>
-      </c>
-      <c r="J46">
-        <v>12</v>
-      </c>
-      <c r="M46">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22">
-      <c r="A47">
-        <v>100</v>
-      </c>
-      <c r="B47">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s">
-        <v>120</v>
-      </c>
-      <c r="D47" t="s">
-        <v>118</v>
-      </c>
-      <c r="E47" t="s">
-        <v>118</v>
-      </c>
-      <c r="I47">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:22">
-      <c r="A48">
-        <v>100</v>
-      </c>
-      <c r="B48">
-        <v>8</v>
-      </c>
-      <c r="C48" t="s">
-        <v>120</v>
-      </c>
-      <c r="D48" t="s">
-        <v>118</v>
-      </c>
-      <c r="E48" t="s">
-        <v>118</v>
-      </c>
-      <c r="I48">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49">
-        <v>100</v>
-      </c>
-      <c r="B49">
-        <v>9</v>
-      </c>
-      <c r="C49" t="s">
-        <v>120</v>
-      </c>
-      <c r="D49" t="s">
-        <v>118</v>
-      </c>
-      <c r="E49" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50">
-        <v>100</v>
-      </c>
-      <c r="B50">
-        <v>10</v>
-      </c>
-      <c r="C50" t="s">
-        <v>120</v>
-      </c>
-      <c r="D50" t="s">
-        <v>118</v>
-      </c>
-      <c r="E50" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -7017,7 +6809,7 @@
       <c r="F2" s="71"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.1475853002199059</v>
+        <v>0.37826136589236448</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -7037,7 +6829,7 @@
       <c r="F3" s="71"/>
       <c r="G3">
         <f t="shared" ref="G3:G5" ca="1" si="0">RAND()</f>
-        <v>0.83783752761327801</v>
+        <v>4.9985773454486737E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -7058,7 +6850,7 @@
       <c r="F4" s="71"/>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93614877039216271</v>
+        <v>0.30378838689256205</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7078,7 +6870,7 @@
       <c r="F5" s="71"/>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.39692756486924441</v>
+        <v>0.91517421219494421</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -7155,7 +6947,7 @@
   <dimension ref="A1:X40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7172,48 +6964,48 @@
         <v>145</v>
       </c>
       <c r="B1" s="39"/>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="75" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="77"/>
-      <c r="E1" s="76" t="s">
+      <c r="D1" s="76"/>
+      <c r="E1" s="75" t="s">
         <v>157</v>
       </c>
-      <c r="F1" s="77"/>
-      <c r="G1" s="76" t="s">
+      <c r="F1" s="76"/>
+      <c r="G1" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="H1" s="77"/>
-      <c r="I1" s="76" t="s">
+      <c r="H1" s="76"/>
+      <c r="I1" s="75" t="s">
         <v>159</v>
       </c>
-      <c r="J1" s="77"/>
+      <c r="J1" s="76"/>
       <c r="K1" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L1" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M1" s="78" t="s">
+      <c r="M1" s="77" t="s">
         <v>160</v>
       </c>
-      <c r="N1" s="79"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="78" t="s">
+      <c r="N1" s="78"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="77" t="s">
         <v>161</v>
       </c>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="78" t="s">
+      <c r="Q1" s="78"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="77" t="s">
         <v>162</v>
       </c>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="81" t="s">
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="80" t="s">
         <v>163</v>
       </c>
-      <c r="W1" s="81"/>
-      <c r="X1" s="81"/>
+      <c r="W1" s="80"/>
+      <c r="X1" s="80"/>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="52"/>
@@ -8106,16 +7898,16 @@
       </c>
     </row>
     <row r="27" spans="1:23">
-      <c r="C27" s="75" t="s">
+      <c r="C27" s="81" t="s">
         <v>169</v>
       </c>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75" t="s">
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="81" t="s">
         <v>171</v>
       </c>
-      <c r="G27" s="75"/>
-      <c r="H27" s="75"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="81"/>
       <c r="J27" s="69" t="s">
         <v>170</v>
       </c>
@@ -8736,16 +8528,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="V1:X1"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8782,105 +8574,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="94" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="88" t="s">
+      <c r="A2" s="88" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="88" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="89"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="85" t="s">
+      <c r="C2" s="83"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="82" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="83"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="100" t="s">
+      <c r="I2" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="M2" s="100"/>
-      <c r="N2" s="100"/>
-      <c r="O2" s="100"/>
-      <c r="P2" s="100"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="100" t="s">
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
+      <c r="Q2" s="97"/>
+      <c r="R2" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="100"/>
-      <c r="T2" s="100"/>
-      <c r="U2" s="100"/>
-      <c r="V2" s="85" t="s">
+      <c r="S2" s="97"/>
+      <c r="T2" s="97"/>
+      <c r="U2" s="97"/>
+      <c r="V2" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="85" t="s">
+      <c r="W2" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="82" t="s">
+      <c r="X2" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="82" t="s">
+      <c r="Y2" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="82" t="s">
+      <c r="Z2" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="82" t="s">
+      <c r="AA2" s="99" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="95"/>
-      <c r="B3" s="91"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="101" t="s">
+      <c r="A3" s="89"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99" t="s">
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99" t="s">
+      <c r="M3" s="96"/>
+      <c r="N3" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="99"/>
-      <c r="P3" s="99" t="s">
+      <c r="O3" s="96"/>
+      <c r="P3" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="99"/>
-      <c r="R3" s="97" t="s">
+      <c r="Q3" s="96"/>
+      <c r="R3" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="97" t="s">
+      <c r="S3" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="97" t="s">
+      <c r="T3" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="97" t="s">
+      <c r="U3" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="86"/>
-      <c r="W3" s="86"/>
-      <c r="X3" s="83"/>
-      <c r="Y3" s="83"/>
-      <c r="Z3" s="83"/>
-      <c r="AA3" s="83"/>
+      <c r="V3" s="92"/>
+      <c r="W3" s="92"/>
+      <c r="X3" s="100"/>
+      <c r="Y3" s="100"/>
+      <c r="Z3" s="100"/>
+      <c r="AA3" s="100"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="96"/>
+      <c r="A4" s="90"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -8899,7 +8691,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="87"/>
+      <c r="H4" s="93"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -8927,16 +8719,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="98"/>
-      <c r="S4" s="98"/>
-      <c r="T4" s="98"/>
-      <c r="U4" s="98"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="87"/>
-      <c r="X4" s="84"/>
-      <c r="Y4" s="84"/>
-      <c r="Z4" s="84"/>
-      <c r="AA4" s="83"/>
+      <c r="R4" s="95"/>
+      <c r="S4" s="95"/>
+      <c r="T4" s="95"/>
+      <c r="U4" s="95"/>
+      <c r="V4" s="93"/>
+      <c r="W4" s="93"/>
+      <c r="X4" s="101"/>
+      <c r="Y4" s="101"/>
+      <c r="Z4" s="101"/>
+      <c r="AA4" s="100"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -9437,6 +9229,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -9452,11 +9249,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update release to latest of main
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2D468D-FED0-DC44-B123-DA6319684D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AD9BE3-02EA-264E-BE15-661ED6263586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="1" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Web Parameters Prod" sheetId="10" r:id="rId1"/>
@@ -890,7 +890,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -953,10 +953,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -979,13 +977,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1001,11 +997,26 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1035,15 +1046,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1057,15 +1059,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1383,9 +1376,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6462F7B1-F956-1241-A84D-BB94A5075354}">
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1423,22 +1416,22 @@
       <c r="E1" t="s">
         <v>123</v>
       </c>
-      <c r="F1" s="70" t="s">
+      <c r="F1" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="70" t="s">
+      <c r="G1" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="71" t="s">
+      <c r="H1" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="70" t="s">
+      <c r="I1" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="70" t="s">
+      <c r="J1" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="71" t="s">
+      <c r="K1" s="66" t="s">
         <v>92</v>
       </c>
       <c r="L1" t="s">
@@ -1491,20 +1484,20 @@
       <c r="E2" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="72">
+      <c r="F2">
         <v>350</v>
       </c>
-      <c r="G2" s="70">
+      <c r="G2" s="43">
         <v>4</v>
       </c>
-      <c r="H2" s="71"/>
-      <c r="I2" s="72">
+      <c r="H2" s="66"/>
+      <c r="I2">
         <v>430</v>
       </c>
-      <c r="J2" s="70">
+      <c r="J2" s="43">
         <v>13</v>
       </c>
-      <c r="K2" s="71"/>
+      <c r="K2" s="66"/>
       <c r="L2">
         <v>430</v>
       </c>
@@ -1528,20 +1521,20 @@
       <c r="E3" t="s">
         <v>118</v>
       </c>
-      <c r="F3" s="72">
+      <c r="F3">
         <v>490</v>
       </c>
-      <c r="G3" s="70">
+      <c r="G3" s="43">
         <v>2</v>
       </c>
-      <c r="H3" s="71"/>
-      <c r="I3" s="72">
+      <c r="H3" s="66"/>
+      <c r="I3">
         <v>700</v>
       </c>
-      <c r="J3" s="70">
+      <c r="J3" s="43">
         <v>18</v>
       </c>
-      <c r="K3" s="71"/>
+      <c r="K3" s="66"/>
       <c r="L3">
         <v>700</v>
       </c>
@@ -1565,21 +1558,21 @@
       <c r="E4" t="s">
         <v>118</v>
       </c>
-      <c r="F4" s="72">
+      <c r="F4">
         <f>720</f>
         <v>720</v>
       </c>
-      <c r="G4" s="70">
+      <c r="G4" s="43">
         <v>6</v>
       </c>
-      <c r="H4" s="71"/>
-      <c r="I4" s="72">
+      <c r="H4" s="66"/>
+      <c r="I4">
         <v>1390</v>
       </c>
-      <c r="J4" s="70">
+      <c r="J4" s="43">
         <v>24</v>
       </c>
-      <c r="K4" s="71"/>
+      <c r="K4" s="66"/>
       <c r="L4">
         <v>1390</v>
       </c>
@@ -1603,20 +1596,20 @@
       <c r="E5" t="s">
         <v>118</v>
       </c>
-      <c r="F5" s="72">
+      <c r="F5">
         <v>840</v>
       </c>
-      <c r="G5" s="70">
-        <v>3</v>
-      </c>
-      <c r="H5" s="71"/>
-      <c r="I5" s="72">
+      <c r="G5" s="43">
+        <v>3</v>
+      </c>
+      <c r="H5" s="66"/>
+      <c r="I5">
         <v>1120</v>
       </c>
-      <c r="J5" s="70">
+      <c r="J5" s="43">
         <v>16</v>
       </c>
-      <c r="K5" s="71"/>
+      <c r="K5" s="66"/>
       <c r="L5">
         <v>1120</v>
       </c>
@@ -1640,20 +1633,20 @@
       <c r="E6" t="s">
         <v>118</v>
       </c>
-      <c r="F6" s="72">
+      <c r="F6">
         <v>11600</v>
       </c>
-      <c r="G6" s="70">
+      <c r="G6" s="43">
         <v>4</v>
       </c>
-      <c r="H6" s="71"/>
-      <c r="I6" s="72">
+      <c r="H6" s="66"/>
+      <c r="I6">
         <v>14000</v>
       </c>
-      <c r="J6" s="70">
+      <c r="J6" s="43">
         <v>13</v>
       </c>
-      <c r="K6" s="71"/>
+      <c r="K6" s="66"/>
       <c r="L6">
         <v>14000</v>
       </c>
@@ -1677,20 +1670,20 @@
       <c r="E7" t="s">
         <v>118</v>
       </c>
-      <c r="F7" s="72">
+      <c r="F7">
         <v>16300</v>
       </c>
-      <c r="G7" s="70">
+      <c r="G7" s="43">
         <v>2</v>
       </c>
-      <c r="H7" s="71"/>
-      <c r="I7" s="72">
+      <c r="H7" s="66"/>
+      <c r="I7">
         <v>23000</v>
       </c>
-      <c r="J7" s="70">
+      <c r="J7" s="43">
         <v>18</v>
       </c>
-      <c r="K7" s="71"/>
+      <c r="K7" s="66"/>
       <c r="L7">
         <v>23000</v>
       </c>
@@ -1714,20 +1707,20 @@
       <c r="E8" t="s">
         <v>118</v>
       </c>
-      <c r="F8" s="72">
+      <c r="F8">
         <v>24000</v>
       </c>
-      <c r="G8" s="70">
+      <c r="G8" s="43">
         <v>6</v>
       </c>
-      <c r="H8" s="71"/>
-      <c r="I8" s="72">
+      <c r="H8" s="66"/>
+      <c r="I8">
         <v>46000</v>
       </c>
-      <c r="J8" s="70">
+      <c r="J8" s="43">
         <v>24</v>
       </c>
-      <c r="K8" s="71"/>
+      <c r="K8" s="66"/>
       <c r="L8">
         <v>46000</v>
       </c>
@@ -1751,20 +1744,20 @@
       <c r="E9" t="s">
         <v>118</v>
       </c>
-      <c r="F9" s="72">
+      <c r="F9">
         <v>28000</v>
       </c>
-      <c r="G9" s="70">
-        <v>3</v>
-      </c>
-      <c r="H9" s="71"/>
-      <c r="I9" s="72">
+      <c r="G9" s="43">
+        <v>3</v>
+      </c>
+      <c r="H9" s="66"/>
+      <c r="I9">
         <v>37000</v>
       </c>
-      <c r="J9" s="70">
+      <c r="J9" s="43">
         <v>16</v>
       </c>
-      <c r="K9" s="71"/>
+      <c r="K9" s="66"/>
       <c r="L9">
         <v>37000</v>
       </c>
@@ -1788,20 +1781,20 @@
       <c r="E10" t="s">
         <v>118</v>
       </c>
-      <c r="F10" s="74">
+      <c r="F10" s="37">
         <v>31.714285714285715</v>
       </c>
-      <c r="G10" s="70">
+      <c r="G10" s="43">
         <v>4</v>
       </c>
-      <c r="H10" s="71"/>
+      <c r="H10" s="66"/>
       <c r="I10" s="37">
         <v>39</v>
       </c>
-      <c r="J10" s="70">
+      <c r="J10" s="43">
         <v>13</v>
       </c>
-      <c r="K10" s="71"/>
+      <c r="K10" s="66"/>
       <c r="L10">
         <v>40</v>
       </c>
@@ -1825,20 +1818,20 @@
       <c r="E11" t="s">
         <v>118</v>
       </c>
-      <c r="F11" s="74">
+      <c r="F11" s="37">
         <v>44.571428571428569</v>
       </c>
-      <c r="G11" s="70">
+      <c r="G11" s="43">
         <v>2</v>
       </c>
-      <c r="H11" s="71"/>
+      <c r="H11" s="66"/>
       <c r="I11" s="37">
         <v>70</v>
       </c>
-      <c r="J11" s="70">
+      <c r="J11" s="43">
         <v>18</v>
       </c>
-      <c r="K11" s="71"/>
+      <c r="K11" s="66"/>
       <c r="L11">
         <v>70</v>
       </c>
@@ -1862,20 +1855,20 @@
       <c r="E12" t="s">
         <v>118</v>
       </c>
-      <c r="F12" s="74">
+      <c r="F12" s="37">
         <v>66</v>
       </c>
-      <c r="G12" s="70">
+      <c r="G12" s="43">
         <v>6</v>
       </c>
-      <c r="H12" s="71"/>
+      <c r="H12" s="66"/>
       <c r="I12" s="37">
         <v>110</v>
       </c>
-      <c r="J12" s="70">
+      <c r="J12" s="43">
         <v>24</v>
       </c>
-      <c r="K12" s="71"/>
+      <c r="K12" s="66"/>
       <c r="L12">
         <v>110</v>
       </c>
@@ -1899,20 +1892,20 @@
       <c r="E13" t="s">
         <v>118</v>
       </c>
-      <c r="F13" s="74">
+      <c r="F13" s="37">
         <v>77.142857142857139</v>
       </c>
-      <c r="G13" s="70">
-        <v>3</v>
-      </c>
-      <c r="H13" s="71"/>
+      <c r="G13" s="43">
+        <v>3</v>
+      </c>
+      <c r="H13" s="66"/>
       <c r="I13" s="37">
         <v>118</v>
       </c>
-      <c r="J13" s="70">
+      <c r="J13" s="43">
         <v>16</v>
       </c>
-      <c r="K13" s="71"/>
+      <c r="K13" s="66"/>
       <c r="L13">
         <v>120</v>
       </c>
@@ -1942,20 +1935,20 @@
       <c r="E14" t="s">
         <v>118</v>
       </c>
-      <c r="F14" s="72">
+      <c r="F14">
         <v>350</v>
       </c>
-      <c r="G14" s="70">
+      <c r="G14" s="43">
         <v>4</v>
       </c>
-      <c r="H14" s="71"/>
-      <c r="I14" s="72">
+      <c r="H14" s="66"/>
+      <c r="I14">
         <v>430</v>
       </c>
-      <c r="J14" s="70">
+      <c r="J14" s="43">
         <v>13</v>
       </c>
-      <c r="K14" s="71"/>
+      <c r="K14" s="66"/>
       <c r="L14">
         <v>430</v>
       </c>
@@ -1988,20 +1981,20 @@
       <c r="E15" t="s">
         <v>118</v>
       </c>
-      <c r="F15" s="72">
+      <c r="F15">
         <v>490</v>
       </c>
-      <c r="G15" s="70">
+      <c r="G15" s="43">
         <v>2</v>
       </c>
-      <c r="H15" s="71"/>
-      <c r="I15" s="72">
+      <c r="H15" s="66"/>
+      <c r="I15">
         <v>700</v>
       </c>
-      <c r="J15" s="70">
+      <c r="J15" s="43">
         <v>18</v>
       </c>
-      <c r="K15" s="71"/>
+      <c r="K15" s="66"/>
       <c r="L15">
         <v>700</v>
       </c>
@@ -2034,21 +2027,21 @@
       <c r="E16" t="s">
         <v>118</v>
       </c>
-      <c r="F16" s="72">
+      <c r="F16">
         <f>720</f>
         <v>720</v>
       </c>
-      <c r="G16" s="70">
+      <c r="G16" s="43">
         <v>6</v>
       </c>
-      <c r="H16" s="71"/>
-      <c r="I16" s="72">
+      <c r="H16" s="66"/>
+      <c r="I16">
         <v>1390</v>
       </c>
-      <c r="J16" s="70">
+      <c r="J16" s="43">
         <v>24</v>
       </c>
-      <c r="K16" s="71"/>
+      <c r="K16" s="66"/>
       <c r="L16">
         <v>1390</v>
       </c>
@@ -2081,20 +2074,20 @@
       <c r="E17" t="s">
         <v>118</v>
       </c>
-      <c r="F17" s="72">
+      <c r="F17">
         <v>840</v>
       </c>
-      <c r="G17" s="70">
-        <v>3</v>
-      </c>
-      <c r="H17" s="71"/>
-      <c r="I17" s="72">
+      <c r="G17" s="43">
+        <v>3</v>
+      </c>
+      <c r="H17" s="66"/>
+      <c r="I17">
         <v>1120</v>
       </c>
-      <c r="J17" s="70">
+      <c r="J17" s="43">
         <v>16</v>
       </c>
-      <c r="K17" s="71"/>
+      <c r="K17" s="66"/>
       <c r="L17">
         <v>1120</v>
       </c>
@@ -2127,20 +2120,20 @@
       <c r="E18" t="s">
         <v>118</v>
       </c>
-      <c r="F18" s="72">
+      <c r="F18">
         <v>11600</v>
       </c>
-      <c r="G18" s="70">
+      <c r="G18" s="43">
         <v>4</v>
       </c>
-      <c r="H18" s="71"/>
-      <c r="I18" s="72">
+      <c r="H18" s="66"/>
+      <c r="I18">
         <v>14000</v>
       </c>
-      <c r="J18" s="70">
+      <c r="J18" s="43">
         <v>13</v>
       </c>
-      <c r="K18" s="71"/>
+      <c r="K18" s="66"/>
       <c r="L18">
         <v>14000</v>
       </c>
@@ -2173,20 +2166,20 @@
       <c r="E19" t="s">
         <v>118</v>
       </c>
-      <c r="F19" s="72">
+      <c r="F19">
         <v>16300</v>
       </c>
-      <c r="G19" s="70">
+      <c r="G19" s="43">
         <v>2</v>
       </c>
-      <c r="H19" s="71"/>
-      <c r="I19" s="72">
+      <c r="H19" s="66"/>
+      <c r="I19">
         <v>23000</v>
       </c>
-      <c r="J19" s="70">
+      <c r="J19" s="43">
         <v>18</v>
       </c>
-      <c r="K19" s="71"/>
+      <c r="K19" s="66"/>
       <c r="L19">
         <v>23000</v>
       </c>
@@ -2219,20 +2212,20 @@
       <c r="E20" t="s">
         <v>118</v>
       </c>
-      <c r="F20" s="72">
+      <c r="F20">
         <v>24000</v>
       </c>
-      <c r="G20" s="70">
+      <c r="G20" s="43">
         <v>6</v>
       </c>
-      <c r="H20" s="71"/>
-      <c r="I20" s="72">
+      <c r="H20" s="66"/>
+      <c r="I20">
         <v>46000</v>
       </c>
-      <c r="J20" s="70">
+      <c r="J20" s="43">
         <v>24</v>
       </c>
-      <c r="K20" s="71"/>
+      <c r="K20" s="66"/>
       <c r="L20">
         <v>46000</v>
       </c>
@@ -2265,20 +2258,20 @@
       <c r="E21" t="s">
         <v>118</v>
       </c>
-      <c r="F21" s="72">
+      <c r="F21">
         <v>28000</v>
       </c>
-      <c r="G21" s="70">
-        <v>3</v>
-      </c>
-      <c r="H21" s="71"/>
-      <c r="I21" s="72">
+      <c r="G21" s="43">
+        <v>3</v>
+      </c>
+      <c r="H21" s="66"/>
+      <c r="I21">
         <v>37000</v>
       </c>
-      <c r="J21" s="70">
+      <c r="J21" s="43">
         <v>16</v>
       </c>
-      <c r="K21" s="71"/>
+      <c r="K21" s="66"/>
       <c r="L21">
         <v>37000</v>
       </c>
@@ -2311,20 +2304,20 @@
       <c r="E22" t="s">
         <v>118</v>
       </c>
-      <c r="F22" s="74">
+      <c r="F22" s="37">
         <v>31.714285714285715</v>
       </c>
-      <c r="G22" s="70">
+      <c r="G22" s="43">
         <v>4</v>
       </c>
-      <c r="H22" s="71"/>
+      <c r="H22" s="66"/>
       <c r="I22" s="37">
         <v>39</v>
       </c>
-      <c r="J22" s="70">
+      <c r="J22" s="43">
         <v>13</v>
       </c>
-      <c r="K22" s="71"/>
+      <c r="K22" s="66"/>
       <c r="L22">
         <v>40</v>
       </c>
@@ -2357,20 +2350,20 @@
       <c r="E23" t="s">
         <v>118</v>
       </c>
-      <c r="F23" s="74">
+      <c r="F23" s="37">
         <v>44.571428571428569</v>
       </c>
-      <c r="G23" s="70">
+      <c r="G23" s="43">
         <v>2</v>
       </c>
-      <c r="H23" s="71"/>
+      <c r="H23" s="66"/>
       <c r="I23" s="37">
         <v>70</v>
       </c>
-      <c r="J23" s="70">
+      <c r="J23" s="43">
         <v>18</v>
       </c>
-      <c r="K23" s="71"/>
+      <c r="K23" s="66"/>
       <c r="L23">
         <v>70</v>
       </c>
@@ -2403,20 +2396,20 @@
       <c r="E24" t="s">
         <v>118</v>
       </c>
-      <c r="F24" s="74">
+      <c r="F24" s="37">
         <v>66</v>
       </c>
-      <c r="G24" s="70">
+      <c r="G24" s="43">
         <v>6</v>
       </c>
-      <c r="H24" s="71"/>
+      <c r="H24" s="66"/>
       <c r="I24" s="37">
         <v>110</v>
       </c>
-      <c r="J24" s="70">
+      <c r="J24" s="43">
         <v>24</v>
       </c>
-      <c r="K24" s="71"/>
+      <c r="K24" s="66"/>
       <c r="L24">
         <v>110</v>
       </c>
@@ -2449,20 +2442,20 @@
       <c r="E25" t="s">
         <v>118</v>
       </c>
-      <c r="F25" s="74">
+      <c r="F25" s="37">
         <v>77.142857142857139</v>
       </c>
-      <c r="G25" s="70">
-        <v>3</v>
-      </c>
-      <c r="H25" s="71"/>
+      <c r="G25" s="43">
+        <v>3</v>
+      </c>
+      <c r="H25" s="66"/>
       <c r="I25" s="37">
         <v>118</v>
       </c>
-      <c r="J25" s="70">
+      <c r="J25" s="43">
         <v>16</v>
       </c>
-      <c r="K25" s="71"/>
+      <c r="K25" s="66"/>
       <c r="L25">
         <v>120</v>
       </c>
@@ -2495,20 +2488,20 @@
       <c r="E26" t="s">
         <v>118</v>
       </c>
-      <c r="F26" s="72">
+      <c r="F26">
         <v>350</v>
       </c>
-      <c r="G26" s="70">
+      <c r="G26" s="43">
         <v>4</v>
       </c>
-      <c r="H26" s="71"/>
-      <c r="I26" s="72">
+      <c r="H26" s="66"/>
+      <c r="I26">
         <v>430</v>
       </c>
-      <c r="J26" s="70">
+      <c r="J26" s="43">
         <v>13</v>
       </c>
-      <c r="K26" s="71"/>
+      <c r="K26" s="66"/>
       <c r="L26">
         <v>430</v>
       </c>
@@ -2541,20 +2534,20 @@
       <c r="E27" t="s">
         <v>118</v>
       </c>
-      <c r="F27" s="72">
+      <c r="F27">
         <v>490</v>
       </c>
-      <c r="G27" s="70">
+      <c r="G27" s="43">
         <v>2</v>
       </c>
-      <c r="H27" s="71"/>
-      <c r="I27" s="72">
+      <c r="H27" s="66"/>
+      <c r="I27">
         <v>700</v>
       </c>
-      <c r="J27" s="70">
+      <c r="J27" s="43">
         <v>18</v>
       </c>
-      <c r="K27" s="71"/>
+      <c r="K27" s="66"/>
       <c r="L27">
         <v>700</v>
       </c>
@@ -2587,21 +2580,21 @@
       <c r="E28" t="s">
         <v>118</v>
       </c>
-      <c r="F28" s="72">
+      <c r="F28">
         <f>720</f>
         <v>720</v>
       </c>
-      <c r="G28" s="70">
+      <c r="G28" s="43">
         <v>6</v>
       </c>
-      <c r="H28" s="71"/>
-      <c r="I28" s="72">
+      <c r="H28" s="66"/>
+      <c r="I28">
         <v>1390</v>
       </c>
-      <c r="J28" s="70">
+      <c r="J28" s="43">
         <v>24</v>
       </c>
-      <c r="K28" s="71"/>
+      <c r="K28" s="66"/>
       <c r="L28">
         <v>1390</v>
       </c>
@@ -2634,20 +2627,20 @@
       <c r="E29" t="s">
         <v>118</v>
       </c>
-      <c r="F29" s="72">
+      <c r="F29">
         <v>840</v>
       </c>
-      <c r="G29" s="70">
-        <v>3</v>
-      </c>
-      <c r="H29" s="71"/>
-      <c r="I29" s="72">
+      <c r="G29" s="43">
+        <v>3</v>
+      </c>
+      <c r="H29" s="66"/>
+      <c r="I29">
         <v>1120</v>
       </c>
-      <c r="J29" s="70">
+      <c r="J29" s="43">
         <v>16</v>
       </c>
-      <c r="K29" s="71"/>
+      <c r="K29" s="66"/>
       <c r="L29">
         <v>1120</v>
       </c>
@@ -2680,20 +2673,20 @@
       <c r="E30" t="s">
         <v>118</v>
       </c>
-      <c r="F30" s="72">
+      <c r="F30">
         <v>11600</v>
       </c>
-      <c r="G30" s="70">
+      <c r="G30" s="43">
         <v>4</v>
       </c>
-      <c r="H30" s="71"/>
-      <c r="I30" s="72">
+      <c r="H30" s="66"/>
+      <c r="I30">
         <v>14000</v>
       </c>
-      <c r="J30" s="70">
+      <c r="J30" s="43">
         <v>13</v>
       </c>
-      <c r="K30" s="71"/>
+      <c r="K30" s="66"/>
       <c r="L30">
         <v>14000</v>
       </c>
@@ -2726,20 +2719,20 @@
       <c r="E31" t="s">
         <v>118</v>
       </c>
-      <c r="F31" s="72">
+      <c r="F31">
         <v>16300</v>
       </c>
-      <c r="G31" s="70">
+      <c r="G31" s="43">
         <v>2</v>
       </c>
-      <c r="H31" s="71"/>
-      <c r="I31" s="72">
+      <c r="H31" s="66"/>
+      <c r="I31">
         <v>23000</v>
       </c>
-      <c r="J31" s="70">
+      <c r="J31" s="43">
         <v>18</v>
       </c>
-      <c r="K31" s="71"/>
+      <c r="K31" s="66"/>
       <c r="L31">
         <v>23000</v>
       </c>
@@ -2772,20 +2765,20 @@
       <c r="E32" t="s">
         <v>118</v>
       </c>
-      <c r="F32" s="72">
+      <c r="F32">
         <v>24000</v>
       </c>
-      <c r="G32" s="70">
+      <c r="G32" s="43">
         <v>6</v>
       </c>
-      <c r="H32" s="71"/>
-      <c r="I32" s="72">
+      <c r="H32" s="66"/>
+      <c r="I32">
         <v>46000</v>
       </c>
-      <c r="J32" s="70">
+      <c r="J32" s="43">
         <v>24</v>
       </c>
-      <c r="K32" s="71"/>
+      <c r="K32" s="66"/>
       <c r="L32">
         <v>46000</v>
       </c>
@@ -2818,20 +2811,20 @@
       <c r="E33" t="s">
         <v>118</v>
       </c>
-      <c r="F33" s="72">
+      <c r="F33">
         <v>28000</v>
       </c>
-      <c r="G33" s="70">
-        <v>3</v>
-      </c>
-      <c r="H33" s="71"/>
-      <c r="I33" s="72">
+      <c r="G33" s="43">
+        <v>3</v>
+      </c>
+      <c r="H33" s="66"/>
+      <c r="I33">
         <v>37000</v>
       </c>
-      <c r="J33" s="70">
+      <c r="J33" s="43">
         <v>16</v>
       </c>
-      <c r="K33" s="71"/>
+      <c r="K33" s="66"/>
       <c r="L33">
         <v>37000</v>
       </c>
@@ -2864,20 +2857,20 @@
       <c r="E34" t="s">
         <v>118</v>
       </c>
-      <c r="F34" s="74">
+      <c r="F34" s="37">
         <v>31.714285714285715</v>
       </c>
-      <c r="G34" s="70">
+      <c r="G34" s="43">
         <v>4</v>
       </c>
-      <c r="H34" s="71"/>
+      <c r="H34" s="66"/>
       <c r="I34" s="37">
         <v>39</v>
       </c>
-      <c r="J34" s="70">
+      <c r="J34" s="43">
         <v>13</v>
       </c>
-      <c r="K34" s="71"/>
+      <c r="K34" s="66"/>
       <c r="L34">
         <v>40</v>
       </c>
@@ -2910,20 +2903,20 @@
       <c r="E35" t="s">
         <v>118</v>
       </c>
-      <c r="F35" s="74">
+      <c r="F35" s="37">
         <v>44.571428571428569</v>
       </c>
-      <c r="G35" s="70">
+      <c r="G35" s="43">
         <v>2</v>
       </c>
-      <c r="H35" s="71"/>
+      <c r="H35" s="66"/>
       <c r="I35" s="37">
         <v>70</v>
       </c>
-      <c r="J35" s="70">
+      <c r="J35" s="43">
         <v>18</v>
       </c>
-      <c r="K35" s="71"/>
+      <c r="K35" s="66"/>
       <c r="L35">
         <v>70</v>
       </c>
@@ -2956,20 +2949,20 @@
       <c r="E36" t="s">
         <v>118</v>
       </c>
-      <c r="F36" s="74">
+      <c r="F36" s="37">
         <v>66</v>
       </c>
-      <c r="G36" s="70">
+      <c r="G36" s="43">
         <v>6</v>
       </c>
-      <c r="H36" s="71"/>
+      <c r="H36" s="66"/>
       <c r="I36" s="37">
         <v>110</v>
       </c>
-      <c r="J36" s="70">
+      <c r="J36" s="43">
         <v>24</v>
       </c>
-      <c r="K36" s="71"/>
+      <c r="K36" s="66"/>
       <c r="L36">
         <v>110</v>
       </c>
@@ -3002,20 +2995,20 @@
       <c r="E37" t="s">
         <v>118</v>
       </c>
-      <c r="F37" s="74">
+      <c r="F37" s="37">
         <v>77.142857142857139</v>
       </c>
-      <c r="G37" s="70">
-        <v>3</v>
-      </c>
-      <c r="H37" s="71"/>
+      <c r="G37" s="43">
+        <v>3</v>
+      </c>
+      <c r="H37" s="66"/>
       <c r="I37" s="37">
         <v>118</v>
       </c>
-      <c r="J37" s="70">
+      <c r="J37" s="43">
         <v>16</v>
       </c>
-      <c r="K37" s="71"/>
+      <c r="K37" s="66"/>
       <c r="L37">
         <v>120</v>
       </c>
@@ -4717,7 +4710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N11" sqref="N11"/>
     </sheetView>
@@ -6770,172 +6763,172 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="70" t="s">
+      <c r="E1" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="70" t="s">
+      <c r="G1" s="43" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="72">
+      <c r="A2">
         <v>350</v>
       </c>
-      <c r="B2" s="70">
+      <c r="B2" s="43">
         <v>4</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="72">
+      <c r="C2" s="66"/>
+      <c r="D2">
         <v>430</v>
       </c>
-      <c r="E2" s="70">
+      <c r="E2" s="43">
         <v>13</v>
       </c>
-      <c r="F2" s="71"/>
+      <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.37826136589236448</v>
+        <v>0.9468781556884639</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="72">
+      <c r="A3">
         <v>490</v>
       </c>
-      <c r="B3" s="70">
+      <c r="B3" s="43">
         <v>2</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="72">
+      <c r="C3" s="66"/>
+      <c r="D3">
         <v>700</v>
       </c>
-      <c r="E3" s="70">
+      <c r="E3" s="43">
         <v>18</v>
       </c>
-      <c r="F3" s="71"/>
+      <c r="F3" s="66"/>
       <c r="G3">
         <f t="shared" ref="G3:G5" ca="1" si="0">RAND()</f>
-        <v>4.9985773454486737E-2</v>
+        <v>0.32689831263997271</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="72">
+      <c r="A4">
         <f>720</f>
         <v>720</v>
       </c>
-      <c r="B4" s="70">
+      <c r="B4" s="43">
         <v>6</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="72">
+      <c r="C4" s="66"/>
+      <c r="D4">
         <v>1390</v>
       </c>
-      <c r="E4" s="70">
+      <c r="E4" s="43">
         <v>36</v>
       </c>
-      <c r="F4" s="71"/>
+      <c r="F4" s="66"/>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30378838689256205</v>
+        <v>0.17605241837960361</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="72">
+      <c r="A5">
         <v>840</v>
       </c>
-      <c r="B5" s="70">
-        <v>3</v>
-      </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="72">
+      <c r="B5" s="43">
+        <v>3</v>
+      </c>
+      <c r="C5" s="66"/>
+      <c r="D5">
         <v>1120</v>
       </c>
-      <c r="E5" s="70">
+      <c r="E5" s="43">
         <v>16</v>
       </c>
-      <c r="F5" s="71"/>
+      <c r="F5" s="66"/>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91517421219494421</v>
+        <v>0.10710845512511591</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="8"/>
-      <c r="B6" s="70"/>
-      <c r="C6" s="71"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="71"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="66"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="8"/>
-      <c r="B7" s="70"/>
-      <c r="C7" s="71"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="66"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="71"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="66"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="8"/>
-      <c r="B8" s="70"/>
-      <c r="C8" s="71"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="66"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="71"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="66"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="8"/>
-      <c r="B9" s="70"/>
-      <c r="C9" s="71"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="66"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="70"/>
-      <c r="F9" s="71"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="66"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="8"/>
-      <c r="B10" s="70"/>
-      <c r="C10" s="71"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="71"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="66"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="8"/>
-      <c r="B11" s="70"/>
-      <c r="C11" s="71"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="71"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="66"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="8"/>
-      <c r="B12" s="70"/>
-      <c r="C12" s="71"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="66"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="71"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="66"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="8"/>
-      <c r="B13" s="70"/>
-      <c r="C13" s="71"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="71"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="66"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6960,188 +6953,188 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="49" t="s">
         <v>145</v>
       </c>
       <c r="B1" s="39"/>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="69" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="76"/>
-      <c r="E1" s="75" t="s">
+      <c r="D1" s="70"/>
+      <c r="E1" s="69" t="s">
         <v>157</v>
       </c>
-      <c r="F1" s="76"/>
-      <c r="G1" s="75" t="s">
+      <c r="F1" s="70"/>
+      <c r="G1" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="H1" s="76"/>
-      <c r="I1" s="75" t="s">
+      <c r="H1" s="70"/>
+      <c r="I1" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="J1" s="76"/>
+      <c r="J1" s="70"/>
       <c r="K1" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L1" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M1" s="77" t="s">
+      <c r="M1" s="71" t="s">
         <v>160</v>
       </c>
-      <c r="N1" s="78"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="77" t="s">
+      <c r="N1" s="72"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="71" t="s">
         <v>161</v>
       </c>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="77" t="s">
+      <c r="Q1" s="72"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="80" t="s">
+      <c r="T1" s="72"/>
+      <c r="U1" s="72"/>
+      <c r="V1" s="74" t="s">
         <v>163</v>
       </c>
-      <c r="W1" s="80"/>
-      <c r="X1" s="80"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="52"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="46" t="s">
+      <c r="A2" s="50"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="I2" s="46" t="s">
+      <c r="I2" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="56" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="54" t="s">
         <v>146</v>
       </c>
-      <c r="N2" s="57" t="s">
+      <c r="N2" s="55" t="s">
         <v>147</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="59" t="s">
+      <c r="O2" s="47"/>
+      <c r="P2" s="57" t="s">
         <v>146</v>
       </c>
-      <c r="Q2" s="50" t="s">
+      <c r="Q2" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="R2" s="49"/>
-      <c r="S2" s="59" t="s">
+      <c r="R2" s="47"/>
+      <c r="S2" s="57" t="s">
         <v>146</v>
       </c>
-      <c r="T2" s="50" t="s">
+      <c r="T2" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="U2" s="67"/>
-      <c r="V2" s="49" t="s">
+      <c r="U2" s="65"/>
+      <c r="V2" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="W2" s="50" t="s">
+      <c r="W2" s="48" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="53">
-        <v>1</v>
-      </c>
-      <c r="B3" s="42" t="s">
+      <c r="A3" s="51">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>148</v>
       </c>
       <c r="C3" s="41">
         <v>370</v>
       </c>
-      <c r="D3" s="55">
+      <c r="D3" s="53">
         <v>450</v>
       </c>
       <c r="E3" s="41">
         <v>520</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="53">
         <v>740</v>
       </c>
       <c r="G3" s="41">
         <v>770</v>
       </c>
-      <c r="H3" s="55">
+      <c r="H3" s="53">
         <v>1480</v>
       </c>
       <c r="I3" s="41">
         <v>900</v>
       </c>
-      <c r="J3" s="55">
+      <c r="J3" s="53">
         <v>1200</v>
       </c>
-      <c r="K3" s="42">
+      <c r="K3">
         <v>1.6</v>
       </c>
-      <c r="L3" s="42">
+      <c r="L3">
         <v>1.5</v>
       </c>
-      <c r="M3" s="58">
+      <c r="M3" s="56">
         <f>C3/$K$3*$L$3</f>
         <v>346.875</v>
       </c>
-      <c r="N3" s="44">
+      <c r="N3" s="42">
         <f>D3/$K$3*$L$3</f>
         <v>421.875</v>
       </c>
-      <c r="O3" s="43">
+      <c r="O3" s="37">
         <f>(N3-M3)</f>
         <v>75</v>
       </c>
-      <c r="P3" s="58">
+      <c r="P3" s="56">
         <f>E3/$K$3*$L$3</f>
         <v>487.5</v>
       </c>
-      <c r="Q3" s="44">
+      <c r="Q3" s="42">
         <f>F3/$K$3*$L$3</f>
         <v>693.75</v>
       </c>
-      <c r="R3" s="43">
+      <c r="R3" s="37">
         <f>(Q3-P3)</f>
         <v>206.25</v>
       </c>
-      <c r="S3" s="58">
+      <c r="S3" s="56">
         <f>G3/$K$3*$L$3</f>
         <v>721.875</v>
       </c>
-      <c r="T3" s="44">
+      <c r="T3" s="42">
         <f>H3/$K$3*$L$3</f>
         <v>1387.5</v>
       </c>
-      <c r="U3" s="68">
+      <c r="U3" s="11">
         <f>(T3-S3)/T3</f>
         <v>0.47972972972972971</v>
       </c>
-      <c r="V3" s="43">
+      <c r="V3" s="37">
         <f>I3/$K$3*$L$3</f>
         <v>843.75</v>
       </c>
-      <c r="W3" s="44">
+      <c r="W3" s="42">
         <f>J3/$K$3*$L$3</f>
         <v>1125</v>
       </c>
@@ -7151,136 +7144,118 @@
       </c>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" s="53"/>
-      <c r="B4" s="42" t="s">
+      <c r="A4" s="51"/>
+      <c r="B4" t="s">
         <v>149</v>
       </c>
-      <c r="C4" s="65">
+      <c r="C4" s="63">
         <v>37890</v>
       </c>
-      <c r="D4" s="66">
+      <c r="D4" s="64">
         <v>38163</v>
       </c>
-      <c r="E4" s="65">
+      <c r="E4" s="63">
         <v>37797</v>
       </c>
-      <c r="F4" s="66">
+      <c r="F4" s="64">
         <v>38317</v>
       </c>
-      <c r="G4" s="65">
+      <c r="G4" s="63">
         <v>37953</v>
       </c>
-      <c r="H4" s="66">
+      <c r="H4" s="64">
         <v>38863</v>
       </c>
-      <c r="I4" s="65">
+      <c r="I4" s="63">
         <v>37862</v>
       </c>
-      <c r="J4" s="66">
+      <c r="J4" s="64">
         <v>38254</v>
       </c>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="44"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="58"/>
-      <c r="T4" s="44"/>
-      <c r="U4" s="68"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="44"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="42"/>
+      <c r="P4" s="56"/>
+      <c r="Q4" s="42"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="42"/>
+      <c r="W4" s="42"/>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="53"/>
-      <c r="B5" s="42" t="s">
+      <c r="A5" s="51"/>
+      <c r="B5" t="s">
         <v>150</v>
       </c>
       <c r="C5" s="41">
         <v>4</v>
       </c>
-      <c r="D5" s="55">
+      <c r="D5" s="53">
         <v>13</v>
       </c>
       <c r="E5" s="41">
         <v>2</v>
       </c>
-      <c r="F5" s="55">
+      <c r="F5" s="53">
         <v>18</v>
       </c>
       <c r="G5" s="41">
         <v>6</v>
       </c>
-      <c r="H5" s="55">
+      <c r="H5" s="53">
         <v>36</v>
       </c>
       <c r="I5" s="41">
         <v>3</v>
       </c>
-      <c r="J5" s="55">
+      <c r="J5" s="53">
         <v>16</v>
       </c>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="58"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="58"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="68"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="44"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="42"/>
+      <c r="P5" s="56"/>
+      <c r="Q5" s="42"/>
+      <c r="S5" s="56"/>
+      <c r="T5" s="42"/>
+      <c r="W5" s="42"/>
     </row>
     <row r="6" spans="1:24">
-      <c r="A6" s="53"/>
-      <c r="B6" s="42" t="s">
+      <c r="A6" s="51"/>
+      <c r="B6" t="s">
         <v>151</v>
       </c>
       <c r="C6" s="41">
         <v>17</v>
       </c>
-      <c r="D6" s="55">
+      <c r="D6" s="53">
         <v>56</v>
       </c>
       <c r="E6" s="41">
         <v>9</v>
       </c>
-      <c r="F6" s="55">
+      <c r="F6" s="53">
         <v>78</v>
       </c>
       <c r="G6" s="41">
         <v>156</v>
       </c>
-      <c r="H6" s="55">
+      <c r="H6" s="53">
         <v>156</v>
       </c>
       <c r="I6" s="41">
         <v>13</v>
       </c>
-      <c r="J6" s="55">
+      <c r="J6" s="53">
         <v>65</v>
       </c>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="44"/>
-      <c r="R6" s="43"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="44"/>
-      <c r="U6" s="68"/>
-      <c r="V6" s="43"/>
-      <c r="W6" s="44"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="42"/>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="42"/>
+      <c r="S6" s="56"/>
+      <c r="T6" s="42"/>
+      <c r="W6" s="42"/>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" s="51">
+      <c r="A7" s="49">
         <v>2</v>
       </c>
       <c r="B7" s="39" t="s">
@@ -7289,25 +7264,25 @@
       <c r="C7" s="38">
         <v>370</v>
       </c>
-      <c r="D7" s="60">
+      <c r="D7" s="58">
         <v>450</v>
       </c>
       <c r="E7" s="38">
         <v>520</v>
       </c>
-      <c r="F7" s="60">
+      <c r="F7" s="58">
         <v>740</v>
       </c>
       <c r="G7" s="38">
         <v>770</v>
       </c>
-      <c r="H7" s="60">
+      <c r="H7" s="58">
         <v>1480</v>
       </c>
       <c r="I7" s="38">
         <v>900</v>
       </c>
-      <c r="J7" s="60">
+      <c r="J7" s="58">
         <v>1200</v>
       </c>
       <c r="K7" s="39">
@@ -7316,47 +7291,47 @@
       <c r="L7" s="39">
         <v>1.5</v>
       </c>
-      <c r="M7" s="61">
+      <c r="M7" s="59">
         <f>C7/$K$7*$L$7</f>
         <v>346.875</v>
       </c>
-      <c r="N7" s="62">
+      <c r="N7" s="60">
         <f>D7/$K$7*$L$7</f>
         <v>421.875</v>
       </c>
-      <c r="O7" s="43">
+      <c r="O7" s="37">
         <f>(N7-M7)</f>
         <v>75</v>
       </c>
-      <c r="P7" s="61">
+      <c r="P7" s="59">
         <f>E7/$K$7*$L$7</f>
         <v>487.5</v>
       </c>
-      <c r="Q7" s="62">
+      <c r="Q7" s="60">
         <f>F7/$K$7*$L$7</f>
         <v>693.75</v>
       </c>
-      <c r="R7" s="43">
+      <c r="R7" s="37">
         <f>(Q7-P7)</f>
         <v>206.25</v>
       </c>
-      <c r="S7" s="61">
+      <c r="S7" s="59">
         <f>G7/$K$7*$L$7</f>
         <v>721.875</v>
       </c>
-      <c r="T7" s="62">
+      <c r="T7" s="60">
         <f>H7/$K$7*$L$7</f>
         <v>1387.5</v>
       </c>
-      <c r="U7" s="68">
+      <c r="U7" s="11">
         <f>(T7-S7)/T7</f>
         <v>0.47972972972972971</v>
       </c>
-      <c r="V7" s="63">
+      <c r="V7" s="61">
         <f>I7/$K$7*$L$7</f>
         <v>843.75</v>
       </c>
-      <c r="W7" s="62">
+      <c r="W7" s="60">
         <f>J7/$K$7*$L$7</f>
         <v>1125</v>
       </c>
@@ -7366,147 +7341,129 @@
       </c>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="53"/>
-      <c r="B8" s="42" t="s">
+      <c r="A8" s="51"/>
+      <c r="B8" t="s">
         <v>149</v>
       </c>
-      <c r="C8" s="65">
+      <c r="C8" s="63">
         <v>37925</v>
       </c>
-      <c r="D8" s="66">
+      <c r="D8" s="64">
         <v>38175</v>
       </c>
-      <c r="E8" s="65">
+      <c r="E8" s="63">
         <v>37862</v>
       </c>
-      <c r="F8" s="66">
+      <c r="F8" s="64">
         <v>38352</v>
       </c>
-      <c r="G8" s="65">
+      <c r="G8" s="63">
         <v>37981</v>
       </c>
-      <c r="H8" s="66">
+      <c r="H8" s="64">
         <v>38898</v>
       </c>
-      <c r="I8" s="65">
+      <c r="I8" s="63">
         <v>37890</v>
       </c>
-      <c r="J8" s="66">
+      <c r="J8" s="64">
         <v>38289</v>
       </c>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="44"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="58"/>
-      <c r="Q8" s="44"/>
-      <c r="R8" s="43"/>
-      <c r="S8" s="58"/>
-      <c r="T8" s="44"/>
-      <c r="U8" s="68"/>
-      <c r="V8" s="43"/>
-      <c r="W8" s="44"/>
+      <c r="M8" s="56"/>
+      <c r="N8" s="42"/>
+      <c r="P8" s="56"/>
+      <c r="Q8" s="42"/>
+      <c r="S8" s="56"/>
+      <c r="T8" s="42"/>
+      <c r="W8" s="42"/>
     </row>
     <row r="9" spans="1:24">
-      <c r="A9" s="53"/>
-      <c r="B9" s="42" t="s">
+      <c r="A9" s="51"/>
+      <c r="B9" t="s">
         <v>150</v>
       </c>
       <c r="C9" s="41">
         <v>4</v>
       </c>
-      <c r="D9" s="55">
+      <c r="D9" s="53">
         <v>13</v>
       </c>
       <c r="E9" s="41">
         <v>2</v>
       </c>
-      <c r="F9" s="55">
+      <c r="F9" s="53">
         <v>18</v>
       </c>
       <c r="G9" s="41">
         <v>6</v>
       </c>
-      <c r="H9" s="55">
+      <c r="H9" s="53">
         <v>36</v>
       </c>
       <c r="I9" s="41">
         <v>3</v>
       </c>
-      <c r="J9" s="55">
+      <c r="J9" s="53">
         <v>16</v>
       </c>
-      <c r="K9" s="42"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="44"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="58"/>
-      <c r="Q9" s="44"/>
-      <c r="R9" s="43"/>
-      <c r="S9" s="58"/>
-      <c r="T9" s="44"/>
-      <c r="U9" s="68"/>
-      <c r="V9" s="43"/>
-      <c r="W9" s="44"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="42"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="42"/>
+      <c r="S9" s="56"/>
+      <c r="T9" s="42"/>
+      <c r="W9" s="42"/>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="53"/>
-      <c r="B10" s="42" t="s">
+      <c r="A10" s="51"/>
+      <c r="B10" t="s">
         <v>151</v>
       </c>
       <c r="C10" s="41"/>
-      <c r="D10" s="55"/>
+      <c r="D10" s="53"/>
       <c r="E10" s="41"/>
-      <c r="F10" s="55"/>
+      <c r="F10" s="53"/>
       <c r="G10" s="41"/>
-      <c r="H10" s="55"/>
+      <c r="H10" s="53"/>
       <c r="I10" s="41"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="44"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="58"/>
-      <c r="Q10" s="44"/>
-      <c r="R10" s="43"/>
-      <c r="S10" s="58"/>
-      <c r="T10" s="44"/>
-      <c r="U10" s="68"/>
-      <c r="V10" s="43"/>
-      <c r="W10" s="44"/>
+      <c r="J10" s="53"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="42"/>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="42"/>
+      <c r="S10" s="56"/>
+      <c r="T10" s="42"/>
+      <c r="W10" s="42"/>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="51">
-        <v>3</v>
-      </c>
-      <c r="B11" s="64" t="s">
+      <c r="A11" s="49">
+        <v>3</v>
+      </c>
+      <c r="B11" s="62" t="s">
         <v>148</v>
       </c>
       <c r="C11" s="38">
         <v>37</v>
       </c>
-      <c r="D11" s="60">
+      <c r="D11" s="58">
         <v>46</v>
       </c>
       <c r="E11" s="38">
         <v>52</v>
       </c>
-      <c r="F11" s="60">
+      <c r="F11" s="58">
         <v>82</v>
       </c>
       <c r="G11" s="38">
         <v>77</v>
       </c>
-      <c r="H11" s="60">
+      <c r="H11" s="58">
         <v>128</v>
       </c>
       <c r="I11" s="38">
         <v>90</v>
       </c>
-      <c r="J11" s="60">
+      <c r="J11" s="58">
         <v>138</v>
       </c>
       <c r="K11" s="39">
@@ -7515,47 +7472,47 @@
       <c r="L11" s="39">
         <v>1.5</v>
       </c>
-      <c r="M11" s="61">
+      <c r="M11" s="59">
         <f>C11/$K$11*$L$11</f>
         <v>31.714285714285715</v>
       </c>
-      <c r="N11" s="62">
+      <c r="N11" s="60">
         <f>D11/$K$11*$L$11</f>
         <v>39.428571428571431</v>
       </c>
-      <c r="O11" s="43">
+      <c r="O11" s="37">
         <f>(N11-M11)</f>
         <v>7.7142857142857153</v>
       </c>
-      <c r="P11" s="61">
+      <c r="P11" s="59">
         <f>E11/$K$11*$L$11</f>
         <v>44.571428571428569</v>
       </c>
-      <c r="Q11" s="62">
+      <c r="Q11" s="60">
         <f>F11/$K$11*$L$11</f>
         <v>70.285714285714278</v>
       </c>
-      <c r="R11" s="43">
+      <c r="R11" s="37">
         <f>(Q11-P11)</f>
         <v>25.714285714285708</v>
       </c>
-      <c r="S11" s="61">
+      <c r="S11" s="59">
         <f>G11/$K$11*$L$11</f>
         <v>66</v>
       </c>
-      <c r="T11" s="62">
+      <c r="T11" s="60">
         <f>H11/$K$11*$L$11</f>
         <v>109.71428571428571</v>
       </c>
-      <c r="U11" s="68">
+      <c r="U11" s="11">
         <f>(T11-S11)/T11</f>
         <v>0.39843749999999994</v>
       </c>
-      <c r="V11" s="63">
+      <c r="V11" s="61">
         <f>I11/$K$11*$L$11</f>
         <v>77.142857142857139</v>
       </c>
-      <c r="W11" s="62">
+      <c r="W11" s="60">
         <f>J11/$K$11*$L$11</f>
         <v>118.28571428571429</v>
       </c>
@@ -7565,147 +7522,129 @@
       </c>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" s="53"/>
-      <c r="B12" s="45" t="s">
+      <c r="A12" s="51"/>
+      <c r="B12" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="C12" s="65">
+      <c r="C12" s="63">
         <v>38436</v>
       </c>
-      <c r="D12" s="66">
+      <c r="D12" s="64">
         <v>38716</v>
       </c>
-      <c r="E12" s="65">
+      <c r="E12" s="63">
         <v>38380</v>
       </c>
-      <c r="F12" s="66">
+      <c r="F12" s="64">
         <v>38863</v>
       </c>
-      <c r="G12" s="65">
+      <c r="G12" s="63">
         <v>38499</v>
       </c>
-      <c r="H12" s="66">
+      <c r="H12" s="64">
         <v>39017</v>
       </c>
-      <c r="I12" s="65">
+      <c r="I12" s="63">
         <v>38408</v>
       </c>
-      <c r="J12" s="66">
+      <c r="J12" s="64">
         <v>38800</v>
       </c>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="44"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="44"/>
-      <c r="R12" s="43"/>
-      <c r="S12" s="58"/>
-      <c r="T12" s="44"/>
-      <c r="U12" s="68"/>
-      <c r="V12" s="43"/>
-      <c r="W12" s="44"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="42"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="42"/>
+      <c r="S12" s="56"/>
+      <c r="T12" s="42"/>
+      <c r="W12" s="42"/>
     </row>
     <row r="13" spans="1:24">
-      <c r="A13" s="53"/>
-      <c r="B13" s="45" t="s">
+      <c r="A13" s="51"/>
+      <c r="B13" s="43" t="s">
         <v>150</v>
       </c>
       <c r="C13" s="41">
         <v>4</v>
       </c>
-      <c r="D13" s="55">
+      <c r="D13" s="53">
         <v>13</v>
       </c>
       <c r="E13" s="41">
         <v>2</v>
       </c>
-      <c r="F13" s="55">
+      <c r="F13" s="53">
         <v>18</v>
       </c>
       <c r="G13" s="41">
         <v>6</v>
       </c>
-      <c r="H13" s="55">
+      <c r="H13" s="53">
         <v>23</v>
       </c>
       <c r="I13" s="41">
         <v>3</v>
       </c>
-      <c r="J13" s="55">
+      <c r="J13" s="53">
         <v>16</v>
       </c>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="44"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="58"/>
-      <c r="Q13" s="44"/>
-      <c r="R13" s="43"/>
-      <c r="S13" s="58"/>
-      <c r="T13" s="44"/>
-      <c r="U13" s="68"/>
-      <c r="V13" s="43"/>
-      <c r="W13" s="44"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="42"/>
+      <c r="P13" s="56"/>
+      <c r="Q13" s="42"/>
+      <c r="S13" s="56"/>
+      <c r="T13" s="42"/>
+      <c r="W13" s="42"/>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="53"/>
-      <c r="B14" s="45" t="s">
+      <c r="A14" s="51"/>
+      <c r="B14" s="43" t="s">
         <v>151</v>
       </c>
       <c r="C14" s="41"/>
-      <c r="D14" s="55"/>
+      <c r="D14" s="53"/>
       <c r="E14" s="41"/>
-      <c r="F14" s="55"/>
+      <c r="F14" s="53"/>
       <c r="G14" s="41"/>
-      <c r="H14" s="55"/>
+      <c r="H14" s="53"/>
       <c r="I14" s="41"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="44"/>
-      <c r="O14" s="43"/>
-      <c r="P14" s="58"/>
-      <c r="Q14" s="44"/>
-      <c r="R14" s="43"/>
-      <c r="S14" s="58"/>
-      <c r="T14" s="44"/>
-      <c r="U14" s="68"/>
-      <c r="V14" s="43"/>
-      <c r="W14" s="44"/>
+      <c r="J14" s="53"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="42"/>
+      <c r="P14" s="56"/>
+      <c r="Q14" s="42"/>
+      <c r="S14" s="56"/>
+      <c r="T14" s="42"/>
+      <c r="W14" s="42"/>
     </row>
     <row r="15" spans="1:24">
-      <c r="A15" s="51">
+      <c r="A15" s="49">
         <v>4</v>
       </c>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="62" t="s">
         <v>148</v>
       </c>
       <c r="C15" s="38">
         <v>900</v>
       </c>
-      <c r="D15" s="60">
+      <c r="D15" s="58">
         <v>1200</v>
       </c>
       <c r="E15" s="38">
         <v>750</v>
       </c>
-      <c r="F15" s="60">
+      <c r="F15" s="58">
         <v>2000</v>
       </c>
       <c r="G15" s="38">
         <v>520</v>
       </c>
-      <c r="H15" s="60">
+      <c r="H15" s="58">
         <v>780</v>
       </c>
       <c r="I15" s="38">
         <v>465</v>
       </c>
-      <c r="J15" s="60">
+      <c r="J15" s="58">
         <v>870</v>
       </c>
       <c r="K15" s="39">
@@ -7714,47 +7653,47 @@
       <c r="L15" s="39">
         <v>1.5</v>
       </c>
-      <c r="M15" s="61">
+      <c r="M15" s="59">
         <f>C15/$K$15*$L$15</f>
         <v>794.11764705882342</v>
       </c>
-      <c r="N15" s="62">
+      <c r="N15" s="60">
         <f>D15/$K$15*$L$15</f>
         <v>1058.8235294117646</v>
       </c>
-      <c r="O15" s="43">
+      <c r="O15" s="37">
         <f>(N15-M15)</f>
         <v>264.70588235294122</v>
       </c>
-      <c r="P15" s="61">
+      <c r="P15" s="59">
         <f>E15/$K$15*$L$15</f>
         <v>661.76470588235293</v>
       </c>
-      <c r="Q15" s="62">
+      <c r="Q15" s="60">
         <f>F15/$K$15*$L$15</f>
         <v>1764.7058823529412</v>
       </c>
-      <c r="R15" s="43">
+      <c r="R15" s="37">
         <f>(Q15-P15)</f>
         <v>1102.9411764705883</v>
       </c>
-      <c r="S15" s="61">
+      <c r="S15" s="59">
         <f>G15/$K$15*$L$15</f>
         <v>458.8235294117647</v>
       </c>
-      <c r="T15" s="62">
+      <c r="T15" s="60">
         <f>H15/$K$15*$L$15</f>
         <v>688.23529411764707</v>
       </c>
-      <c r="U15" s="68">
+      <c r="U15" s="11">
         <f>(T15-S15)/T15</f>
         <v>0.33333333333333337</v>
       </c>
-      <c r="V15" s="63">
+      <c r="V15" s="61">
         <f>I15/$K$15*$L$15</f>
         <v>410.2941176470589</v>
       </c>
-      <c r="W15" s="62">
+      <c r="W15" s="60">
         <f>J15/$K$15*$L$15</f>
         <v>767.64705882352939</v>
       </c>
@@ -7764,117 +7703,105 @@
       </c>
     </row>
     <row r="16" spans="1:24">
-      <c r="A16" s="53"/>
-      <c r="B16" s="45" t="s">
+      <c r="A16" s="51"/>
+      <c r="B16" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="C16" s="65">
+      <c r="C16" s="63">
         <v>38044</v>
       </c>
-      <c r="D16" s="66">
+      <c r="D16" s="64">
         <v>38527</v>
       </c>
-      <c r="E16" s="65">
+      <c r="E16" s="63">
         <v>38107</v>
       </c>
-      <c r="F16" s="66">
+      <c r="F16" s="64">
         <v>39752</v>
       </c>
-      <c r="G16" s="65">
+      <c r="G16" s="63">
         <v>37981</v>
       </c>
-      <c r="H16" s="66">
+      <c r="H16" s="64">
         <v>38653</v>
       </c>
-      <c r="I16" s="65">
+      <c r="I16" s="63">
         <v>38072</v>
       </c>
-      <c r="J16" s="66">
+      <c r="J16" s="64">
         <v>39136</v>
       </c>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="58"/>
-      <c r="N16" s="44"/>
-      <c r="O16" s="43"/>
-      <c r="P16" s="58"/>
-      <c r="Q16" s="44"/>
-      <c r="R16" s="43"/>
-      <c r="S16" s="58"/>
-      <c r="T16" s="44"/>
-      <c r="U16" s="68"/>
-      <c r="V16" s="43"/>
-      <c r="W16" s="44"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="42"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="42"/>
+      <c r="S16" s="56"/>
+      <c r="T16" s="42"/>
+      <c r="W16" s="42"/>
     </row>
     <row r="17" spans="1:23">
-      <c r="A17" s="53"/>
-      <c r="B17" s="45" t="s">
+      <c r="A17" s="51"/>
+      <c r="B17" s="43" t="s">
         <v>150</v>
       </c>
       <c r="C17" s="41">
         <v>4</v>
       </c>
-      <c r="D17" s="55">
+      <c r="D17" s="53">
         <v>20</v>
       </c>
       <c r="E17" s="41">
         <v>6</v>
       </c>
-      <c r="F17" s="55">
+      <c r="F17" s="53">
         <v>60</v>
       </c>
       <c r="G17" s="41">
         <v>2</v>
       </c>
-      <c r="H17" s="55">
+      <c r="H17" s="53">
         <v>24</v>
       </c>
       <c r="I17" s="41">
         <v>5</v>
       </c>
-      <c r="J17" s="55">
+      <c r="J17" s="53">
         <v>40</v>
       </c>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="44"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="58"/>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="43"/>
-      <c r="S17" s="58"/>
-      <c r="T17" s="44"/>
-      <c r="U17" s="68"/>
-      <c r="V17" s="43"/>
-      <c r="W17" s="44"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="42"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="42"/>
+      <c r="S17" s="56"/>
+      <c r="T17" s="42"/>
+      <c r="W17" s="42"/>
     </row>
     <row r="18" spans="1:23">
-      <c r="A18" s="52"/>
-      <c r="B18" s="47" t="s">
+      <c r="A18" s="50"/>
+      <c r="B18" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="50"/>
-      <c r="O18" s="49"/>
-      <c r="P18" s="59"/>
-      <c r="Q18" s="50"/>
-      <c r="R18" s="49"/>
-      <c r="S18" s="59"/>
-      <c r="T18" s="50"/>
-      <c r="U18" s="67"/>
-      <c r="V18" s="49"/>
-      <c r="W18" s="50"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="47"/>
+      <c r="P18" s="57"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="47"/>
+      <c r="S18" s="57"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="65"/>
+      <c r="V18" s="47"/>
+      <c r="W18" s="48"/>
     </row>
     <row r="23" spans="1:23">
       <c r="B23" t="s">
@@ -7898,20 +7825,19 @@
       </c>
     </row>
     <row r="27" spans="1:23">
-      <c r="C27" s="81" t="s">
+      <c r="C27" s="68" t="s">
         <v>169</v>
       </c>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81" t="s">
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="G27" s="81"/>
-      <c r="H27" s="81"/>
-      <c r="J27" s="69" t="s">
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="J27" t="s">
         <v>170</v>
       </c>
-      <c r="K27" s="69"/>
       <c r="M27"/>
     </row>
     <row r="28" spans="1:23">
@@ -7939,7 +7865,7 @@
       <c r="I28" t="s">
         <v>180</v>
       </c>
-      <c r="J28" s="72" t="s">
+      <c r="J28" t="s">
         <v>146</v>
       </c>
       <c r="K28" s="8" t="s">
@@ -8209,14 +8135,14 @@
         <v>5</v>
       </c>
       <c r="H33" s="37"/>
-      <c r="J33" s="72">
+      <c r="J33">
         <f>K29*R33</f>
         <v>11654.999999999998</v>
       </c>
       <c r="K33" s="8">
         <v>11600</v>
       </c>
-      <c r="L33" s="72">
+      <c r="L33">
         <f>M29*R33</f>
         <v>14318.999999999998</v>
       </c>
@@ -8245,7 +8171,7 @@
         <v>6</v>
       </c>
       <c r="H34" s="37"/>
-      <c r="J34" s="72">
+      <c r="J34">
         <f>K30*R34</f>
         <v>16316.999999999998</v>
       </c>
@@ -8281,7 +8207,7 @@
         <v>7</v>
       </c>
       <c r="H35" s="37"/>
-      <c r="J35" s="72">
+      <c r="J35">
         <f>K31*R35</f>
         <v>23975.999999999996</v>
       </c>
@@ -8317,7 +8243,7 @@
         <v>8</v>
       </c>
       <c r="H36" s="37"/>
-      <c r="J36" s="72">
+      <c r="J36">
         <f>K32*R36</f>
         <v>27971.999999999996</v>
       </c>
@@ -8365,7 +8291,7 @@
         <f>M11</f>
         <v>31.714285714285715</v>
       </c>
-      <c r="K37" s="73">
+      <c r="K37" s="67">
         <v>32</v>
       </c>
       <c r="L37" s="37">
@@ -8410,7 +8336,7 @@
         <f>P11</f>
         <v>44.571428571428569</v>
       </c>
-      <c r="K38" s="73">
+      <c r="K38" s="67">
         <v>45</v>
       </c>
       <c r="L38" s="37">
@@ -8454,7 +8380,7 @@
         <f>S11</f>
         <v>66</v>
       </c>
-      <c r="K39" s="73">
+      <c r="K39" s="67">
         <v>66</v>
       </c>
       <c r="L39" s="37">
@@ -8498,7 +8424,7 @@
         <f>V11</f>
         <v>77.142857142857139</v>
       </c>
-      <c r="K40" s="73">
+      <c r="K40" s="67">
         <v>77</v>
       </c>
       <c r="L40" s="37">
@@ -8528,16 +8454,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="V1:X1"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="F27:H27"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="V1:X1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8574,105 +8500,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="88" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="82" t="s">
+      <c r="A2" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="83"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="91" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="82"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="97" t="s">
+      <c r="I2" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
-      <c r="Q2" s="97"/>
-      <c r="R2" s="97" t="s">
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="97"/>
-      <c r="T2" s="97"/>
-      <c r="U2" s="97"/>
-      <c r="V2" s="91" t="s">
+      <c r="S2" s="93"/>
+      <c r="T2" s="93"/>
+      <c r="U2" s="93"/>
+      <c r="V2" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="91" t="s">
+      <c r="W2" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="99" t="s">
+      <c r="X2" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="99" t="s">
+      <c r="Y2" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="99" t="s">
+      <c r="Z2" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="99" t="s">
+      <c r="AA2" s="75" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="89"/>
-      <c r="B3" s="85"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="98" t="s">
+      <c r="A3" s="88"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96" t="s">
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96" t="s">
+      <c r="M3" s="92"/>
+      <c r="N3" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="96"/>
-      <c r="P3" s="96" t="s">
+      <c r="O3" s="92"/>
+      <c r="P3" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="96"/>
-      <c r="R3" s="94" t="s">
+      <c r="Q3" s="92"/>
+      <c r="R3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="94" t="s">
+      <c r="S3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="94" t="s">
+      <c r="T3" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="94" t="s">
+      <c r="U3" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="92"/>
-      <c r="W3" s="92"/>
-      <c r="X3" s="100"/>
-      <c r="Y3" s="100"/>
-      <c r="Z3" s="100"/>
-      <c r="AA3" s="100"/>
+      <c r="V3" s="79"/>
+      <c r="W3" s="79"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="76"/>
+      <c r="Z3" s="76"/>
+      <c r="AA3" s="76"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="90"/>
+      <c r="A4" s="89"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -8691,7 +8617,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="93"/>
+      <c r="H4" s="80"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -8719,16 +8645,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="95"/>
-      <c r="S4" s="95"/>
-      <c r="T4" s="95"/>
-      <c r="U4" s="95"/>
-      <c r="V4" s="93"/>
-      <c r="W4" s="93"/>
-      <c r="X4" s="101"/>
-      <c r="Y4" s="101"/>
-      <c r="Z4" s="101"/>
-      <c r="AA4" s="100"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="80"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="77"/>
+      <c r="Z4" s="77"/>
+      <c r="AA4" s="76"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -9229,11 +9155,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -9249,6 +9170,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Removed large amount questions.  Added production treatments to dev page.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D365563-D7E2-3242-933F-78A0B92D54F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3DB7C0-13C2-584B-879E-B0525298CA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="3" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="1" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Web Parameters Prod" sheetId="10" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="189">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -620,9 +620,6 @@
     <t>Worded MEL question experiment 1 date/delay paper.</t>
   </si>
   <si>
-    <t>Worded MEL question 33.3 DWR of experiment 1 to test magnitude effect.</t>
-  </si>
-  <si>
     <t>Worded MEL question experiment 3 of date/delay paper.</t>
   </si>
   <si>
@@ -632,16 +629,10 @@
     <t>Barchart MEL question experiment 1 date/delay paper half the screen.</t>
   </si>
   <si>
-    <t>Barchart MEL question 33.3 DWR of experiment 1 to test magnitude effect half the screen.</t>
-  </si>
-  <si>
     <t>Barchart MEL question experiment 3 of date/delay paper half the screen.</t>
   </si>
   <si>
     <t>Barchart MEL question experiment 1 date/delay paper full screen.</t>
-  </si>
-  <si>
-    <t>Barchart MEL question 33.3 DWR of experiment 1 to test magnitude effect full screen.</t>
   </si>
   <si>
     <t>Barchart MEL question experiment 3 of date/delay paper full screen.</t>
@@ -982,6 +973,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1000,8 +994,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1031,15 +1040,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1053,15 +1053,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1377,11 +1368,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6462F7B1-F956-1241-A84D-BB94A5075354}">
-  <dimension ref="A1:V37"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1636,22 +1627,22 @@
       <c r="E6" t="s">
         <v>118</v>
       </c>
-      <c r="F6">
-        <v>11600</v>
+      <c r="F6" s="37">
+        <v>31.714285714285715</v>
       </c>
       <c r="G6" s="43">
         <v>4</v>
       </c>
       <c r="H6" s="66"/>
-      <c r="I6">
-        <v>14000</v>
+      <c r="I6" s="37">
+        <v>39</v>
       </c>
       <c r="J6" s="43">
         <v>13</v>
       </c>
       <c r="K6" s="66"/>
       <c r="L6">
-        <v>14000</v>
+        <v>40</v>
       </c>
       <c r="V6" t="s">
         <v>182</v>
@@ -1673,22 +1664,22 @@
       <c r="E7" t="s">
         <v>118</v>
       </c>
-      <c r="F7">
-        <v>16300</v>
+      <c r="F7" s="37">
+        <v>44.571428571428569</v>
       </c>
       <c r="G7" s="43">
         <v>2</v>
       </c>
       <c r="H7" s="66"/>
-      <c r="I7">
-        <v>23000</v>
+      <c r="I7" s="37">
+        <v>70</v>
       </c>
       <c r="J7" s="43">
         <v>18</v>
       </c>
       <c r="K7" s="66"/>
       <c r="L7">
-        <v>23000</v>
+        <v>70</v>
       </c>
       <c r="V7" t="s">
         <v>182</v>
@@ -1710,22 +1701,22 @@
       <c r="E8" t="s">
         <v>118</v>
       </c>
-      <c r="F8">
-        <v>24000</v>
+      <c r="F8" s="37">
+        <v>66</v>
       </c>
       <c r="G8" s="43">
         <v>6</v>
       </c>
       <c r="H8" s="66"/>
-      <c r="I8">
-        <v>46000</v>
+      <c r="I8" s="37">
+        <v>110</v>
       </c>
       <c r="J8" s="43">
         <v>24</v>
       </c>
       <c r="K8" s="66"/>
       <c r="L8">
-        <v>46000</v>
+        <v>110</v>
       </c>
       <c r="V8" t="s">
         <v>182</v>
@@ -1747,22 +1738,28 @@
       <c r="E9" t="s">
         <v>118</v>
       </c>
-      <c r="F9">
-        <v>28000</v>
+      <c r="F9" s="37">
+        <v>77.142857142857139</v>
       </c>
       <c r="G9" s="43">
         <v>3</v>
       </c>
       <c r="H9" s="66"/>
-      <c r="I9">
-        <v>37000</v>
+      <c r="I9" s="37">
+        <v>118</v>
       </c>
       <c r="J9" s="43">
         <v>16</v>
       </c>
       <c r="K9" s="66"/>
       <c r="L9">
-        <v>37000</v>
+        <v>120</v>
+      </c>
+      <c r="N9">
+        <v>600</v>
+      </c>
+      <c r="O9">
+        <v>300</v>
       </c>
       <c r="V9" t="s">
         <v>182</v>
@@ -1770,13 +1767,13 @@
     </row>
     <row r="10" spans="1:22">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D10" t="s">
         <v>118</v>
@@ -1784,36 +1781,45 @@
       <c r="E10" t="s">
         <v>118</v>
       </c>
-      <c r="F10" s="37">
-        <v>31.714285714285715</v>
+      <c r="F10">
+        <v>350</v>
       </c>
       <c r="G10" s="43">
         <v>4</v>
       </c>
       <c r="H10" s="66"/>
-      <c r="I10" s="37">
-        <v>39</v>
+      <c r="I10">
+        <v>430</v>
       </c>
       <c r="J10" s="43">
         <v>13</v>
       </c>
       <c r="K10" s="66"/>
       <c r="L10">
-        <v>40</v>
+        <v>430</v>
+      </c>
+      <c r="M10">
+        <v>14</v>
+      </c>
+      <c r="N10">
+        <v>600</v>
+      </c>
+      <c r="O10">
+        <v>300</v>
       </c>
       <c r="V10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:22">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D11" t="s">
         <v>118</v>
@@ -1821,36 +1827,45 @@
       <c r="E11" t="s">
         <v>118</v>
       </c>
-      <c r="F11" s="37">
-        <v>44.571428571428569</v>
+      <c r="F11">
+        <v>490</v>
       </c>
       <c r="G11" s="43">
         <v>2</v>
       </c>
       <c r="H11" s="66"/>
-      <c r="I11" s="37">
-        <v>70</v>
+      <c r="I11">
+        <v>700</v>
       </c>
       <c r="J11" s="43">
         <v>18</v>
       </c>
       <c r="K11" s="66"/>
       <c r="L11">
-        <v>70</v>
+        <v>700</v>
+      </c>
+      <c r="M11">
+        <v>19</v>
+      </c>
+      <c r="N11">
+        <v>600</v>
+      </c>
+      <c r="O11">
+        <v>300</v>
       </c>
       <c r="V11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:22">
       <c r="A12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D12" t="s">
         <v>118</v>
@@ -1858,36 +1873,46 @@
       <c r="E12" t="s">
         <v>118</v>
       </c>
-      <c r="F12" s="37">
-        <v>66</v>
+      <c r="F12">
+        <f>720</f>
+        <v>720</v>
       </c>
       <c r="G12" s="43">
         <v>6</v>
       </c>
       <c r="H12" s="66"/>
-      <c r="I12" s="37">
-        <v>110</v>
+      <c r="I12">
+        <v>1390</v>
       </c>
       <c r="J12" s="43">
         <v>24</v>
       </c>
       <c r="K12" s="66"/>
       <c r="L12">
-        <v>110</v>
+        <v>1390</v>
+      </c>
+      <c r="M12">
+        <v>25</v>
+      </c>
+      <c r="N12">
+        <v>600</v>
+      </c>
+      <c r="O12">
+        <v>300</v>
       </c>
       <c r="V12" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:22">
       <c r="A13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D13" t="s">
         <v>118</v>
@@ -1895,22 +1920,25 @@
       <c r="E13" t="s">
         <v>118</v>
       </c>
-      <c r="F13" s="37">
-        <v>77.142857142857139</v>
+      <c r="F13">
+        <v>840</v>
       </c>
       <c r="G13" s="43">
         <v>3</v>
       </c>
       <c r="H13" s="66"/>
-      <c r="I13" s="37">
-        <v>118</v>
+      <c r="I13">
+        <v>1120</v>
       </c>
       <c r="J13" s="43">
         <v>16</v>
       </c>
       <c r="K13" s="66"/>
       <c r="L13">
-        <v>120</v>
+        <v>1120</v>
+      </c>
+      <c r="M13">
+        <v>17</v>
       </c>
       <c r="N13">
         <v>600</v>
@@ -1919,7 +1947,7 @@
         <v>300</v>
       </c>
       <c r="V13" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:22">
@@ -1927,7 +1955,7 @@
         <v>2</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
         <v>104</v>
@@ -1938,22 +1966,22 @@
       <c r="E14" t="s">
         <v>118</v>
       </c>
-      <c r="F14">
-        <v>350</v>
+      <c r="F14" s="37">
+        <v>31.714285714285715</v>
       </c>
       <c r="G14" s="43">
         <v>4</v>
       </c>
       <c r="H14" s="66"/>
-      <c r="I14">
-        <v>430</v>
+      <c r="I14" s="37">
+        <v>39</v>
       </c>
       <c r="J14" s="43">
         <v>13</v>
       </c>
       <c r="K14" s="66"/>
       <c r="L14">
-        <v>430</v>
+        <v>40</v>
       </c>
       <c r="M14">
         <v>14</v>
@@ -1973,7 +2001,7 @@
         <v>2</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
         <v>104</v>
@@ -1984,22 +2012,22 @@
       <c r="E15" t="s">
         <v>118</v>
       </c>
-      <c r="F15">
-        <v>490</v>
+      <c r="F15" s="37">
+        <v>44.571428571428569</v>
       </c>
       <c r="G15" s="43">
         <v>2</v>
       </c>
       <c r="H15" s="66"/>
-      <c r="I15">
-        <v>700</v>
+      <c r="I15" s="37">
+        <v>70</v>
       </c>
       <c r="J15" s="43">
         <v>18</v>
       </c>
       <c r="K15" s="66"/>
       <c r="L15">
-        <v>700</v>
+        <v>70</v>
       </c>
       <c r="M15">
         <v>19</v>
@@ -2019,7 +2047,7 @@
         <v>2</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
         <v>104</v>
@@ -2030,23 +2058,22 @@
       <c r="E16" t="s">
         <v>118</v>
       </c>
-      <c r="F16">
-        <f>720</f>
-        <v>720</v>
+      <c r="F16" s="37">
+        <v>66</v>
       </c>
       <c r="G16" s="43">
         <v>6</v>
       </c>
       <c r="H16" s="66"/>
-      <c r="I16">
-        <v>1390</v>
+      <c r="I16" s="37">
+        <v>110</v>
       </c>
       <c r="J16" s="43">
         <v>24</v>
       </c>
       <c r="K16" s="66"/>
       <c r="L16">
-        <v>1390</v>
+        <v>110</v>
       </c>
       <c r="M16">
         <v>25</v>
@@ -2058,7 +2085,7 @@
         <v>300</v>
       </c>
       <c r="V16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:22">
@@ -2066,7 +2093,7 @@
         <v>2</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
         <v>104</v>
@@ -2077,22 +2104,22 @@
       <c r="E17" t="s">
         <v>118</v>
       </c>
-      <c r="F17">
-        <v>840</v>
+      <c r="F17" s="37">
+        <v>77.142857142857139</v>
       </c>
       <c r="G17" s="43">
         <v>3</v>
       </c>
       <c r="H17" s="66"/>
-      <c r="I17">
-        <v>1120</v>
+      <c r="I17" s="37">
+        <v>118</v>
       </c>
       <c r="J17" s="43">
         <v>16</v>
       </c>
       <c r="K17" s="66"/>
       <c r="L17">
-        <v>1120</v>
+        <v>120</v>
       </c>
       <c r="M17">
         <v>17</v>
@@ -2109,10 +2136,10 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
         <v>104</v>
@@ -2124,27 +2151,27 @@
         <v>118</v>
       </c>
       <c r="F18">
-        <v>11600</v>
+        <v>350</v>
       </c>
       <c r="G18" s="43">
         <v>4</v>
       </c>
       <c r="H18" s="66"/>
       <c r="I18">
-        <v>14000</v>
+        <v>430</v>
       </c>
       <c r="J18" s="43">
         <v>13</v>
       </c>
       <c r="K18" s="66"/>
       <c r="L18">
-        <v>14000</v>
+        <v>430</v>
       </c>
       <c r="M18">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="N18">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="O18">
         <v>300</v>
@@ -2155,10 +2182,10 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
         <v>2</v>
-      </c>
-      <c r="B19">
-        <v>6</v>
       </c>
       <c r="C19" t="s">
         <v>104</v>
@@ -2170,27 +2197,27 @@
         <v>118</v>
       </c>
       <c r="F19">
-        <v>16300</v>
+        <v>490</v>
       </c>
       <c r="G19" s="43">
         <v>2</v>
       </c>
       <c r="H19" s="66"/>
       <c r="I19">
-        <v>23000</v>
+        <v>700</v>
       </c>
       <c r="J19" s="43">
         <v>18</v>
       </c>
       <c r="K19" s="66"/>
       <c r="L19">
-        <v>23000</v>
+        <v>700</v>
       </c>
       <c r="M19">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="N19">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="O19">
         <v>300</v>
@@ -2201,10 +2228,10 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B20">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
         <v>104</v>
@@ -2216,27 +2243,28 @@
         <v>118</v>
       </c>
       <c r="F20">
-        <v>24000</v>
+        <f>720</f>
+        <v>720</v>
       </c>
       <c r="G20" s="43">
         <v>6</v>
       </c>
       <c r="H20" s="66"/>
       <c r="I20">
-        <v>46000</v>
+        <v>1390</v>
       </c>
       <c r="J20" s="43">
         <v>24</v>
       </c>
       <c r="K20" s="66"/>
       <c r="L20">
-        <v>46000</v>
+        <v>1390</v>
       </c>
       <c r="M20">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="N20">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="O20">
         <v>300</v>
@@ -2247,10 +2275,10 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
         <v>104</v>
@@ -2262,27 +2290,27 @@
         <v>118</v>
       </c>
       <c r="F21">
-        <v>28000</v>
+        <v>840</v>
       </c>
       <c r="G21" s="43">
         <v>3</v>
       </c>
       <c r="H21" s="66"/>
       <c r="I21">
-        <v>37000</v>
+        <v>1120</v>
       </c>
       <c r="J21" s="43">
         <v>16</v>
       </c>
       <c r="K21" s="66"/>
       <c r="L21">
-        <v>37000</v>
+        <v>1120</v>
       </c>
       <c r="M21">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="N21">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="O21">
         <v>300</v>
@@ -2293,10 +2321,10 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
         <v>104</v>
@@ -2325,10 +2353,10 @@
         <v>40</v>
       </c>
       <c r="M22">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="N22">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="O22">
         <v>300</v>
@@ -2339,10 +2367,10 @@
     </row>
     <row r="23" spans="1:22">
       <c r="A23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B23">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
         <v>104</v>
@@ -2371,10 +2399,10 @@
         <v>70</v>
       </c>
       <c r="M23">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="N23">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="O23">
         <v>300</v>
@@ -2385,10 +2413,10 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B24">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
         <v>104</v>
@@ -2417,24 +2445,24 @@
         <v>110</v>
       </c>
       <c r="M24">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="N24">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="O24">
         <v>300</v>
       </c>
       <c r="V24" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:22">
       <c r="A25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B25">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
         <v>104</v>
@@ -2463,569 +2491,16 @@
         <v>120</v>
       </c>
       <c r="M25">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="N25">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="O25">
         <v>300</v>
       </c>
       <c r="V25" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22">
-      <c r="A26">
-        <v>3</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>104</v>
-      </c>
-      <c r="D26" t="s">
-        <v>118</v>
-      </c>
-      <c r="E26" t="s">
-        <v>118</v>
-      </c>
-      <c r="F26">
-        <v>350</v>
-      </c>
-      <c r="G26" s="43">
-        <v>4</v>
-      </c>
-      <c r="H26" s="66"/>
-      <c r="I26">
-        <v>430</v>
-      </c>
-      <c r="J26" s="43">
-        <v>13</v>
-      </c>
-      <c r="K26" s="66"/>
-      <c r="L26">
-        <v>430</v>
-      </c>
-      <c r="M26">
-        <v>27</v>
-      </c>
-      <c r="N26">
-        <v>1200</v>
-      </c>
-      <c r="O26">
-        <v>300</v>
-      </c>
-      <c r="V26" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22">
-      <c r="A27">
-        <v>3</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>104</v>
-      </c>
-      <c r="D27" t="s">
-        <v>118</v>
-      </c>
-      <c r="E27" t="s">
-        <v>118</v>
-      </c>
-      <c r="F27">
-        <v>490</v>
-      </c>
-      <c r="G27" s="43">
-        <v>2</v>
-      </c>
-      <c r="H27" s="66"/>
-      <c r="I27">
-        <v>700</v>
-      </c>
-      <c r="J27" s="43">
-        <v>18</v>
-      </c>
-      <c r="K27" s="66"/>
-      <c r="L27">
-        <v>700</v>
-      </c>
-      <c r="M27">
-        <v>37</v>
-      </c>
-      <c r="N27">
-        <v>1200</v>
-      </c>
-      <c r="O27">
-        <v>300</v>
-      </c>
-      <c r="V27" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22">
-      <c r="A28">
-        <v>3</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>104</v>
-      </c>
-      <c r="D28" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" t="s">
-        <v>118</v>
-      </c>
-      <c r="F28">
-        <f>720</f>
-        <v>720</v>
-      </c>
-      <c r="G28" s="43">
-        <v>6</v>
-      </c>
-      <c r="H28" s="66"/>
-      <c r="I28">
-        <v>1390</v>
-      </c>
-      <c r="J28" s="43">
-        <v>24</v>
-      </c>
-      <c r="K28" s="66"/>
-      <c r="L28">
-        <v>1390</v>
-      </c>
-      <c r="M28">
-        <v>49</v>
-      </c>
-      <c r="N28">
-        <v>1200</v>
-      </c>
-      <c r="O28">
-        <v>300</v>
-      </c>
-      <c r="V28" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22">
-      <c r="A29">
-        <v>3</v>
-      </c>
-      <c r="B29">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>104</v>
-      </c>
-      <c r="D29" t="s">
-        <v>118</v>
-      </c>
-      <c r="E29" t="s">
-        <v>118</v>
-      </c>
-      <c r="F29">
-        <v>840</v>
-      </c>
-      <c r="G29" s="43">
-        <v>3</v>
-      </c>
-      <c r="H29" s="66"/>
-      <c r="I29">
-        <v>1120</v>
-      </c>
-      <c r="J29" s="43">
-        <v>16</v>
-      </c>
-      <c r="K29" s="66"/>
-      <c r="L29">
-        <v>1120</v>
-      </c>
-      <c r="M29">
-        <v>33</v>
-      </c>
-      <c r="N29">
-        <v>1200</v>
-      </c>
-      <c r="O29">
-        <v>300</v>
-      </c>
-      <c r="V29" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22">
-      <c r="A30">
-        <v>3</v>
-      </c>
-      <c r="B30">
-        <v>5</v>
-      </c>
-      <c r="C30" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" t="s">
-        <v>118</v>
-      </c>
-      <c r="E30" t="s">
-        <v>118</v>
-      </c>
-      <c r="F30">
-        <v>11600</v>
-      </c>
-      <c r="G30" s="43">
-        <v>4</v>
-      </c>
-      <c r="H30" s="66"/>
-      <c r="I30">
-        <v>14000</v>
-      </c>
-      <c r="J30" s="43">
-        <v>13</v>
-      </c>
-      <c r="K30" s="66"/>
-      <c r="L30">
-        <v>14000</v>
-      </c>
-      <c r="M30">
-        <v>37</v>
-      </c>
-      <c r="N30">
-        <v>1200</v>
-      </c>
-      <c r="O30">
-        <v>300</v>
-      </c>
-      <c r="V30" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22">
-      <c r="A31">
-        <v>3</v>
-      </c>
-      <c r="B31">
-        <v>6</v>
-      </c>
-      <c r="C31" t="s">
-        <v>104</v>
-      </c>
-      <c r="D31" t="s">
-        <v>118</v>
-      </c>
-      <c r="E31" t="s">
-        <v>118</v>
-      </c>
-      <c r="F31">
-        <v>16300</v>
-      </c>
-      <c r="G31" s="43">
-        <v>2</v>
-      </c>
-      <c r="H31" s="66"/>
-      <c r="I31">
-        <v>23000</v>
-      </c>
-      <c r="J31" s="43">
-        <v>18</v>
-      </c>
-      <c r="K31" s="66"/>
-      <c r="L31">
-        <v>23000</v>
-      </c>
-      <c r="M31">
-        <v>37</v>
-      </c>
-      <c r="N31">
-        <v>1200</v>
-      </c>
-      <c r="O31">
-        <v>300</v>
-      </c>
-      <c r="V31" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22">
-      <c r="A32">
-        <v>3</v>
-      </c>
-      <c r="B32">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>104</v>
-      </c>
-      <c r="D32" t="s">
-        <v>118</v>
-      </c>
-      <c r="E32" t="s">
-        <v>118</v>
-      </c>
-      <c r="F32">
-        <v>24000</v>
-      </c>
-      <c r="G32" s="43">
-        <v>6</v>
-      </c>
-      <c r="H32" s="66"/>
-      <c r="I32">
-        <v>46000</v>
-      </c>
-      <c r="J32" s="43">
-        <v>24</v>
-      </c>
-      <c r="K32" s="66"/>
-      <c r="L32">
-        <v>46000</v>
-      </c>
-      <c r="M32">
-        <v>49</v>
-      </c>
-      <c r="N32">
-        <v>1200</v>
-      </c>
-      <c r="O32">
-        <v>300</v>
-      </c>
-      <c r="V32" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22">
-      <c r="A33">
-        <v>3</v>
-      </c>
-      <c r="B33">
-        <v>8</v>
-      </c>
-      <c r="C33" t="s">
-        <v>104</v>
-      </c>
-      <c r="D33" t="s">
-        <v>118</v>
-      </c>
-      <c r="E33" t="s">
-        <v>118</v>
-      </c>
-      <c r="F33">
-        <v>28000</v>
-      </c>
-      <c r="G33" s="43">
-        <v>3</v>
-      </c>
-      <c r="H33" s="66"/>
-      <c r="I33">
-        <v>37000</v>
-      </c>
-      <c r="J33" s="43">
-        <v>16</v>
-      </c>
-      <c r="K33" s="66"/>
-      <c r="L33">
-        <v>37000</v>
-      </c>
-      <c r="M33">
-        <v>33</v>
-      </c>
-      <c r="N33">
-        <v>1200</v>
-      </c>
-      <c r="O33">
-        <v>300</v>
-      </c>
-      <c r="V33" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22">
-      <c r="A34">
-        <v>3</v>
-      </c>
-      <c r="B34">
-        <v>9</v>
-      </c>
-      <c r="C34" t="s">
-        <v>104</v>
-      </c>
-      <c r="D34" t="s">
-        <v>118</v>
-      </c>
-      <c r="E34" t="s">
-        <v>118</v>
-      </c>
-      <c r="F34" s="37">
-        <v>31.714285714285715</v>
-      </c>
-      <c r="G34" s="43">
-        <v>4</v>
-      </c>
-      <c r="H34" s="66"/>
-      <c r="I34" s="37">
-        <v>39</v>
-      </c>
-      <c r="J34" s="43">
-        <v>13</v>
-      </c>
-      <c r="K34" s="66"/>
-      <c r="L34">
-        <v>40</v>
-      </c>
-      <c r="M34">
-        <v>27</v>
-      </c>
-      <c r="N34">
-        <v>1200</v>
-      </c>
-      <c r="O34">
-        <v>300</v>
-      </c>
-      <c r="V34" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22">
-      <c r="A35">
-        <v>3</v>
-      </c>
-      <c r="B35">
-        <v>10</v>
-      </c>
-      <c r="C35" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" t="s">
-        <v>118</v>
-      </c>
-      <c r="E35" t="s">
-        <v>118</v>
-      </c>
-      <c r="F35" s="37">
-        <v>44.571428571428569</v>
-      </c>
-      <c r="G35" s="43">
-        <v>2</v>
-      </c>
-      <c r="H35" s="66"/>
-      <c r="I35" s="37">
-        <v>70</v>
-      </c>
-      <c r="J35" s="43">
-        <v>18</v>
-      </c>
-      <c r="K35" s="66"/>
-      <c r="L35">
-        <v>70</v>
-      </c>
-      <c r="M35">
-        <v>37</v>
-      </c>
-      <c r="N35">
-        <v>1200</v>
-      </c>
-      <c r="O35">
-        <v>300</v>
-      </c>
-      <c r="V35" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22">
-      <c r="A36">
-        <v>3</v>
-      </c>
-      <c r="B36">
-        <v>11</v>
-      </c>
-      <c r="C36" t="s">
-        <v>104</v>
-      </c>
-      <c r="D36" t="s">
-        <v>118</v>
-      </c>
-      <c r="E36" t="s">
-        <v>118</v>
-      </c>
-      <c r="F36" s="37">
-        <v>66</v>
-      </c>
-      <c r="G36" s="43">
-        <v>6</v>
-      </c>
-      <c r="H36" s="66"/>
-      <c r="I36" s="37">
-        <v>110</v>
-      </c>
-      <c r="J36" s="43">
-        <v>24</v>
-      </c>
-      <c r="K36" s="66"/>
-      <c r="L36">
-        <v>110</v>
-      </c>
-      <c r="M36">
-        <v>49</v>
-      </c>
-      <c r="N36">
-        <v>1200</v>
-      </c>
-      <c r="O36">
-        <v>300</v>
-      </c>
-      <c r="V36" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22">
-      <c r="A37">
-        <v>3</v>
-      </c>
-      <c r="B37">
-        <v>12</v>
-      </c>
-      <c r="C37" t="s">
-        <v>104</v>
-      </c>
-      <c r="D37" t="s">
-        <v>118</v>
-      </c>
-      <c r="E37" t="s">
-        <v>118</v>
-      </c>
-      <c r="F37" s="37">
-        <v>77.142857142857139</v>
-      </c>
-      <c r="G37" s="43">
-        <v>3</v>
-      </c>
-      <c r="H37" s="66"/>
-      <c r="I37" s="37">
-        <v>118</v>
-      </c>
-      <c r="J37" s="43">
-        <v>16</v>
-      </c>
-      <c r="K37" s="66"/>
-      <c r="L37">
-        <v>120</v>
-      </c>
-      <c r="M37">
-        <v>33</v>
-      </c>
-      <c r="N37">
-        <v>1200</v>
-      </c>
-      <c r="O37">
-        <v>300</v>
-      </c>
-      <c r="V37" t="s">
-        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -4711,11 +4186,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:V66"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -6750,6 +6225,1047 @@
         <v>144</v>
       </c>
     </row>
+    <row r="43" spans="1:22">
+      <c r="A43">
+        <v>20</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43" t="s">
+        <v>118</v>
+      </c>
+      <c r="E43" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43">
+        <v>350</v>
+      </c>
+      <c r="G43" s="43">
+        <v>4</v>
+      </c>
+      <c r="H43" s="66"/>
+      <c r="I43">
+        <v>430</v>
+      </c>
+      <c r="J43" s="43">
+        <v>13</v>
+      </c>
+      <c r="K43" s="66"/>
+      <c r="L43">
+        <v>430</v>
+      </c>
+      <c r="V43" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22">
+      <c r="A44">
+        <v>20</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" t="s">
+        <v>118</v>
+      </c>
+      <c r="E44" t="s">
+        <v>118</v>
+      </c>
+      <c r="F44">
+        <v>490</v>
+      </c>
+      <c r="G44" s="43">
+        <v>2</v>
+      </c>
+      <c r="H44" s="66"/>
+      <c r="I44">
+        <v>700</v>
+      </c>
+      <c r="J44" s="43">
+        <v>18</v>
+      </c>
+      <c r="K44" s="66"/>
+      <c r="L44">
+        <v>700</v>
+      </c>
+      <c r="V44" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
+      <c r="A45">
+        <v>20</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>120</v>
+      </c>
+      <c r="D45" t="s">
+        <v>118</v>
+      </c>
+      <c r="E45" t="s">
+        <v>118</v>
+      </c>
+      <c r="F45">
+        <f>720</f>
+        <v>720</v>
+      </c>
+      <c r="G45" s="43">
+        <v>6</v>
+      </c>
+      <c r="H45" s="66"/>
+      <c r="I45">
+        <v>1390</v>
+      </c>
+      <c r="J45" s="43">
+        <v>24</v>
+      </c>
+      <c r="K45" s="66"/>
+      <c r="L45">
+        <v>1390</v>
+      </c>
+      <c r="V45" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22">
+      <c r="A46">
+        <v>20</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" t="s">
+        <v>118</v>
+      </c>
+      <c r="E46" t="s">
+        <v>118</v>
+      </c>
+      <c r="F46">
+        <v>840</v>
+      </c>
+      <c r="G46" s="43">
+        <v>3</v>
+      </c>
+      <c r="H46" s="66"/>
+      <c r="I46">
+        <v>1120</v>
+      </c>
+      <c r="J46" s="43">
+        <v>16</v>
+      </c>
+      <c r="K46" s="66"/>
+      <c r="L46">
+        <v>1120</v>
+      </c>
+      <c r="V46" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22">
+      <c r="A47">
+        <v>20</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" t="s">
+        <v>118</v>
+      </c>
+      <c r="E47" t="s">
+        <v>118</v>
+      </c>
+      <c r="F47" s="37">
+        <v>31.714285714285715</v>
+      </c>
+      <c r="G47" s="43">
+        <v>4</v>
+      </c>
+      <c r="H47" s="66"/>
+      <c r="I47" s="37">
+        <v>39</v>
+      </c>
+      <c r="J47" s="43">
+        <v>13</v>
+      </c>
+      <c r="K47" s="66"/>
+      <c r="L47">
+        <v>40</v>
+      </c>
+      <c r="V47" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22">
+      <c r="A48">
+        <v>20</v>
+      </c>
+      <c r="B48">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>120</v>
+      </c>
+      <c r="D48" t="s">
+        <v>118</v>
+      </c>
+      <c r="E48" t="s">
+        <v>118</v>
+      </c>
+      <c r="F48" s="37">
+        <v>44.571428571428569</v>
+      </c>
+      <c r="G48" s="43">
+        <v>2</v>
+      </c>
+      <c r="H48" s="66"/>
+      <c r="I48" s="37">
+        <v>70</v>
+      </c>
+      <c r="J48" s="43">
+        <v>18</v>
+      </c>
+      <c r="K48" s="66"/>
+      <c r="L48">
+        <v>70</v>
+      </c>
+      <c r="V48" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22">
+      <c r="A49">
+        <v>20</v>
+      </c>
+      <c r="B49">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" t="s">
+        <v>118</v>
+      </c>
+      <c r="E49" t="s">
+        <v>118</v>
+      </c>
+      <c r="F49" s="37">
+        <v>66</v>
+      </c>
+      <c r="G49" s="43">
+        <v>6</v>
+      </c>
+      <c r="H49" s="66"/>
+      <c r="I49" s="37">
+        <v>110</v>
+      </c>
+      <c r="J49" s="43">
+        <v>24</v>
+      </c>
+      <c r="K49" s="66"/>
+      <c r="L49">
+        <v>110</v>
+      </c>
+      <c r="V49" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22">
+      <c r="A50">
+        <v>20</v>
+      </c>
+      <c r="B50">
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" t="s">
+        <v>118</v>
+      </c>
+      <c r="E50" t="s">
+        <v>118</v>
+      </c>
+      <c r="F50" s="37">
+        <v>77.142857142857139</v>
+      </c>
+      <c r="G50" s="43">
+        <v>3</v>
+      </c>
+      <c r="H50" s="66"/>
+      <c r="I50" s="37">
+        <v>118</v>
+      </c>
+      <c r="J50" s="43">
+        <v>16</v>
+      </c>
+      <c r="K50" s="66"/>
+      <c r="L50">
+        <v>120</v>
+      </c>
+      <c r="N50">
+        <v>600</v>
+      </c>
+      <c r="O50">
+        <v>300</v>
+      </c>
+      <c r="V50" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22">
+      <c r="A51">
+        <v>21</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>104</v>
+      </c>
+      <c r="D51" t="s">
+        <v>118</v>
+      </c>
+      <c r="E51" t="s">
+        <v>118</v>
+      </c>
+      <c r="F51">
+        <v>350</v>
+      </c>
+      <c r="G51" s="43">
+        <v>4</v>
+      </c>
+      <c r="H51" s="66"/>
+      <c r="I51">
+        <v>430</v>
+      </c>
+      <c r="J51" s="43">
+        <v>13</v>
+      </c>
+      <c r="K51" s="66"/>
+      <c r="L51">
+        <v>430</v>
+      </c>
+      <c r="M51">
+        <v>14</v>
+      </c>
+      <c r="N51">
+        <v>600</v>
+      </c>
+      <c r="O51">
+        <v>300</v>
+      </c>
+      <c r="V51" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22">
+      <c r="A52">
+        <v>21</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>104</v>
+      </c>
+      <c r="D52" t="s">
+        <v>118</v>
+      </c>
+      <c r="E52" t="s">
+        <v>118</v>
+      </c>
+      <c r="F52">
+        <v>490</v>
+      </c>
+      <c r="G52" s="43">
+        <v>2</v>
+      </c>
+      <c r="H52" s="66"/>
+      <c r="I52">
+        <v>700</v>
+      </c>
+      <c r="J52" s="43">
+        <v>18</v>
+      </c>
+      <c r="K52" s="66"/>
+      <c r="L52">
+        <v>700</v>
+      </c>
+      <c r="M52">
+        <v>19</v>
+      </c>
+      <c r="N52">
+        <v>600</v>
+      </c>
+      <c r="O52">
+        <v>300</v>
+      </c>
+      <c r="V52" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22">
+      <c r="A53">
+        <v>21</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>104</v>
+      </c>
+      <c r="D53" t="s">
+        <v>118</v>
+      </c>
+      <c r="E53" t="s">
+        <v>118</v>
+      </c>
+      <c r="F53">
+        <f>720</f>
+        <v>720</v>
+      </c>
+      <c r="G53" s="43">
+        <v>6</v>
+      </c>
+      <c r="H53" s="66"/>
+      <c r="I53">
+        <v>1390</v>
+      </c>
+      <c r="J53" s="43">
+        <v>24</v>
+      </c>
+      <c r="K53" s="66"/>
+      <c r="L53">
+        <v>1390</v>
+      </c>
+      <c r="M53">
+        <v>25</v>
+      </c>
+      <c r="N53">
+        <v>600</v>
+      </c>
+      <c r="O53">
+        <v>300</v>
+      </c>
+      <c r="V53" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22">
+      <c r="A54">
+        <v>21</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" t="s">
+        <v>118</v>
+      </c>
+      <c r="E54" t="s">
+        <v>118</v>
+      </c>
+      <c r="F54">
+        <v>840</v>
+      </c>
+      <c r="G54" s="43">
+        <v>3</v>
+      </c>
+      <c r="H54" s="66"/>
+      <c r="I54">
+        <v>1120</v>
+      </c>
+      <c r="J54" s="43">
+        <v>16</v>
+      </c>
+      <c r="K54" s="66"/>
+      <c r="L54">
+        <v>1120</v>
+      </c>
+      <c r="M54">
+        <v>17</v>
+      </c>
+      <c r="N54">
+        <v>600</v>
+      </c>
+      <c r="O54">
+        <v>300</v>
+      </c>
+      <c r="V54" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22">
+      <c r="A55">
+        <v>21</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" t="s">
+        <v>118</v>
+      </c>
+      <c r="E55" t="s">
+        <v>118</v>
+      </c>
+      <c r="F55" s="37">
+        <v>31.714285714285715</v>
+      </c>
+      <c r="G55" s="43">
+        <v>4</v>
+      </c>
+      <c r="H55" s="66"/>
+      <c r="I55" s="37">
+        <v>39</v>
+      </c>
+      <c r="J55" s="43">
+        <v>13</v>
+      </c>
+      <c r="K55" s="66"/>
+      <c r="L55">
+        <v>40</v>
+      </c>
+      <c r="M55">
+        <v>14</v>
+      </c>
+      <c r="N55">
+        <v>600</v>
+      </c>
+      <c r="O55">
+        <v>300</v>
+      </c>
+      <c r="V55" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22">
+      <c r="A56">
+        <v>21</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+      <c r="C56" t="s">
+        <v>104</v>
+      </c>
+      <c r="D56" t="s">
+        <v>118</v>
+      </c>
+      <c r="E56" t="s">
+        <v>118</v>
+      </c>
+      <c r="F56" s="37">
+        <v>44.571428571428569</v>
+      </c>
+      <c r="G56" s="43">
+        <v>2</v>
+      </c>
+      <c r="H56" s="66"/>
+      <c r="I56" s="37">
+        <v>70</v>
+      </c>
+      <c r="J56" s="43">
+        <v>18</v>
+      </c>
+      <c r="K56" s="66"/>
+      <c r="L56">
+        <v>70</v>
+      </c>
+      <c r="M56">
+        <v>19</v>
+      </c>
+      <c r="N56">
+        <v>600</v>
+      </c>
+      <c r="O56">
+        <v>300</v>
+      </c>
+      <c r="V56" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22">
+      <c r="A57">
+        <v>21</v>
+      </c>
+      <c r="B57">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>104</v>
+      </c>
+      <c r="D57" t="s">
+        <v>118</v>
+      </c>
+      <c r="E57" t="s">
+        <v>118</v>
+      </c>
+      <c r="F57" s="37">
+        <v>66</v>
+      </c>
+      <c r="G57" s="43">
+        <v>6</v>
+      </c>
+      <c r="H57" s="66"/>
+      <c r="I57" s="37">
+        <v>110</v>
+      </c>
+      <c r="J57" s="43">
+        <v>24</v>
+      </c>
+      <c r="K57" s="66"/>
+      <c r="L57">
+        <v>110</v>
+      </c>
+      <c r="M57">
+        <v>25</v>
+      </c>
+      <c r="N57">
+        <v>600</v>
+      </c>
+      <c r="O57">
+        <v>300</v>
+      </c>
+      <c r="V57" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22">
+      <c r="A58">
+        <v>21</v>
+      </c>
+      <c r="B58">
+        <v>8</v>
+      </c>
+      <c r="C58" t="s">
+        <v>104</v>
+      </c>
+      <c r="D58" t="s">
+        <v>118</v>
+      </c>
+      <c r="E58" t="s">
+        <v>118</v>
+      </c>
+      <c r="F58" s="37">
+        <v>77.142857142857139</v>
+      </c>
+      <c r="G58" s="43">
+        <v>3</v>
+      </c>
+      <c r="H58" s="66"/>
+      <c r="I58" s="37">
+        <v>118</v>
+      </c>
+      <c r="J58" s="43">
+        <v>16</v>
+      </c>
+      <c r="K58" s="66"/>
+      <c r="L58">
+        <v>120</v>
+      </c>
+      <c r="M58">
+        <v>17</v>
+      </c>
+      <c r="N58">
+        <v>600</v>
+      </c>
+      <c r="O58">
+        <v>300</v>
+      </c>
+      <c r="V58" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22">
+      <c r="A59">
+        <v>22</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>104</v>
+      </c>
+      <c r="D59" t="s">
+        <v>118</v>
+      </c>
+      <c r="E59" t="s">
+        <v>118</v>
+      </c>
+      <c r="F59">
+        <v>350</v>
+      </c>
+      <c r="G59" s="43">
+        <v>4</v>
+      </c>
+      <c r="H59" s="66"/>
+      <c r="I59">
+        <v>430</v>
+      </c>
+      <c r="J59" s="43">
+        <v>13</v>
+      </c>
+      <c r="K59" s="66"/>
+      <c r="L59">
+        <v>430</v>
+      </c>
+      <c r="M59">
+        <v>27</v>
+      </c>
+      <c r="N59">
+        <v>1200</v>
+      </c>
+      <c r="O59">
+        <v>300</v>
+      </c>
+      <c r="V59" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22">
+      <c r="A60">
+        <v>22</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>104</v>
+      </c>
+      <c r="D60" t="s">
+        <v>118</v>
+      </c>
+      <c r="E60" t="s">
+        <v>118</v>
+      </c>
+      <c r="F60">
+        <v>490</v>
+      </c>
+      <c r="G60" s="43">
+        <v>2</v>
+      </c>
+      <c r="H60" s="66"/>
+      <c r="I60">
+        <v>700</v>
+      </c>
+      <c r="J60" s="43">
+        <v>18</v>
+      </c>
+      <c r="K60" s="66"/>
+      <c r="L60">
+        <v>700</v>
+      </c>
+      <c r="M60">
+        <v>37</v>
+      </c>
+      <c r="N60">
+        <v>1200</v>
+      </c>
+      <c r="O60">
+        <v>300</v>
+      </c>
+      <c r="V60" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22">
+      <c r="A61">
+        <v>22</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+      <c r="C61" t="s">
+        <v>104</v>
+      </c>
+      <c r="D61" t="s">
+        <v>118</v>
+      </c>
+      <c r="E61" t="s">
+        <v>118</v>
+      </c>
+      <c r="F61">
+        <f>720</f>
+        <v>720</v>
+      </c>
+      <c r="G61" s="43">
+        <v>6</v>
+      </c>
+      <c r="H61" s="66"/>
+      <c r="I61">
+        <v>1390</v>
+      </c>
+      <c r="J61" s="43">
+        <v>24</v>
+      </c>
+      <c r="K61" s="66"/>
+      <c r="L61">
+        <v>1390</v>
+      </c>
+      <c r="M61">
+        <v>49</v>
+      </c>
+      <c r="N61">
+        <v>1200</v>
+      </c>
+      <c r="O61">
+        <v>300</v>
+      </c>
+      <c r="V61" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22">
+      <c r="A62">
+        <v>22</v>
+      </c>
+      <c r="B62">
+        <v>4</v>
+      </c>
+      <c r="C62" t="s">
+        <v>104</v>
+      </c>
+      <c r="D62" t="s">
+        <v>118</v>
+      </c>
+      <c r="E62" t="s">
+        <v>118</v>
+      </c>
+      <c r="F62">
+        <v>840</v>
+      </c>
+      <c r="G62" s="43">
+        <v>3</v>
+      </c>
+      <c r="H62" s="66"/>
+      <c r="I62">
+        <v>1120</v>
+      </c>
+      <c r="J62" s="43">
+        <v>16</v>
+      </c>
+      <c r="K62" s="66"/>
+      <c r="L62">
+        <v>1120</v>
+      </c>
+      <c r="M62">
+        <v>33</v>
+      </c>
+      <c r="N62">
+        <v>1200</v>
+      </c>
+      <c r="O62">
+        <v>300</v>
+      </c>
+      <c r="V62" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22">
+      <c r="A63">
+        <v>22</v>
+      </c>
+      <c r="B63">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>104</v>
+      </c>
+      <c r="D63" t="s">
+        <v>118</v>
+      </c>
+      <c r="E63" t="s">
+        <v>118</v>
+      </c>
+      <c r="F63" s="37">
+        <v>31.714285714285715</v>
+      </c>
+      <c r="G63" s="43">
+        <v>4</v>
+      </c>
+      <c r="H63" s="66"/>
+      <c r="I63" s="37">
+        <v>39</v>
+      </c>
+      <c r="J63" s="43">
+        <v>13</v>
+      </c>
+      <c r="K63" s="66"/>
+      <c r="L63">
+        <v>40</v>
+      </c>
+      <c r="M63">
+        <v>27</v>
+      </c>
+      <c r="N63">
+        <v>1200</v>
+      </c>
+      <c r="O63">
+        <v>300</v>
+      </c>
+      <c r="V63" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22">
+      <c r="A64">
+        <v>22</v>
+      </c>
+      <c r="B64">
+        <v>6</v>
+      </c>
+      <c r="C64" t="s">
+        <v>104</v>
+      </c>
+      <c r="D64" t="s">
+        <v>118</v>
+      </c>
+      <c r="E64" t="s">
+        <v>118</v>
+      </c>
+      <c r="F64" s="37">
+        <v>44.571428571428569</v>
+      </c>
+      <c r="G64" s="43">
+        <v>2</v>
+      </c>
+      <c r="H64" s="66"/>
+      <c r="I64" s="37">
+        <v>70</v>
+      </c>
+      <c r="J64" s="43">
+        <v>18</v>
+      </c>
+      <c r="K64" s="66"/>
+      <c r="L64">
+        <v>70</v>
+      </c>
+      <c r="M64">
+        <v>37</v>
+      </c>
+      <c r="N64">
+        <v>1200</v>
+      </c>
+      <c r="O64">
+        <v>300</v>
+      </c>
+      <c r="V64" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22">
+      <c r="A65">
+        <v>22</v>
+      </c>
+      <c r="B65">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s">
+        <v>104</v>
+      </c>
+      <c r="D65" t="s">
+        <v>118</v>
+      </c>
+      <c r="E65" t="s">
+        <v>118</v>
+      </c>
+      <c r="F65" s="37">
+        <v>66</v>
+      </c>
+      <c r="G65" s="43">
+        <v>6</v>
+      </c>
+      <c r="H65" s="66"/>
+      <c r="I65" s="37">
+        <v>110</v>
+      </c>
+      <c r="J65" s="43">
+        <v>24</v>
+      </c>
+      <c r="K65" s="66"/>
+      <c r="L65">
+        <v>110</v>
+      </c>
+      <c r="M65">
+        <v>49</v>
+      </c>
+      <c r="N65">
+        <v>1200</v>
+      </c>
+      <c r="O65">
+        <v>300</v>
+      </c>
+      <c r="V65" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22">
+      <c r="A66">
+        <v>22</v>
+      </c>
+      <c r="B66">
+        <v>8</v>
+      </c>
+      <c r="C66" t="s">
+        <v>104</v>
+      </c>
+      <c r="D66" t="s">
+        <v>118</v>
+      </c>
+      <c r="E66" t="s">
+        <v>118</v>
+      </c>
+      <c r="F66" s="37">
+        <v>77.142857142857139</v>
+      </c>
+      <c r="G66" s="43">
+        <v>3</v>
+      </c>
+      <c r="H66" s="66"/>
+      <c r="I66" s="37">
+        <v>118</v>
+      </c>
+      <c r="J66" s="43">
+        <v>16</v>
+      </c>
+      <c r="K66" s="66"/>
+      <c r="L66">
+        <v>120</v>
+      </c>
+      <c r="M66">
+        <v>33</v>
+      </c>
+      <c r="N66">
+        <v>1200</v>
+      </c>
+      <c r="O66">
+        <v>300</v>
+      </c>
+      <c r="V66" t="s">
+        <v>187</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6805,7 +7321,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.97757786624641418</v>
+        <v>0.86579947576232363</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -6825,7 +7341,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f t="shared" ref="G3:G5" ca="1" si="0">RAND()</f>
-        <v>0.43045682736051805</v>
+        <v>0.23712147014348073</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6846,7 +7362,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12566478391209812</v>
+        <v>0.15042399061412903</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6866,7 +7382,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53141155750190505</v>
+        <v>0.75310467193325614</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -6942,8 +7458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F6B51D-A4A1-6D46-8F47-1EE4F323E4DF}">
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6957,7 +7473,7 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:24">
@@ -6965,48 +7481,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="69" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="68" t="s">
+      <c r="D3" s="70"/>
+      <c r="E3" s="69" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="69"/>
-      <c r="G3" s="68" t="s">
+      <c r="F3" s="70"/>
+      <c r="G3" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="69"/>
-      <c r="I3" s="68" t="s">
+      <c r="H3" s="70"/>
+      <c r="I3" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="69"/>
+      <c r="J3" s="70"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="70" t="s">
+      <c r="M3" s="71" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="71"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="70" t="s">
+      <c r="N3" s="72"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="71" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="72"/>
-      <c r="S3" s="70" t="s">
+      <c r="Q3" s="72"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="71"/>
-      <c r="U3" s="71"/>
-      <c r="V3" s="73" t="s">
+      <c r="T3" s="72"/>
+      <c r="U3" s="72"/>
+      <c r="V3" s="74" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="73"/>
-      <c r="X3" s="73"/>
+      <c r="W3" s="74"/>
+      <c r="X3" s="74"/>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="50"/>
@@ -7833,16 +8349,16 @@
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="C29" s="74" t="s">
+      <c r="C29" s="68" t="s">
         <v>169</v>
       </c>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74" t="s">
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="G29" s="74"/>
-      <c r="H29" s="74"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
       <c r="J29" t="s">
         <v>170</v>
       </c>
@@ -8462,16 +8978,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8508,105 +9024,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="75" t="s">
+      <c r="A2" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="75" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="76"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="84" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="82"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="90" t="s">
+      <c r="I2" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="90" t="s">
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="90"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="84" t="s">
+      <c r="S2" s="93"/>
+      <c r="T2" s="93"/>
+      <c r="U2" s="93"/>
+      <c r="V2" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="84" t="s">
+      <c r="W2" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="92" t="s">
+      <c r="X2" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="92" t="s">
+      <c r="Y2" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="92" t="s">
+      <c r="Z2" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="92" t="s">
+      <c r="AA2" s="75" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="82"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="91" t="s">
+      <c r="A3" s="88"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89" t="s">
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89" t="s">
+      <c r="M3" s="92"/>
+      <c r="N3" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89" t="s">
+      <c r="O3" s="92"/>
+      <c r="P3" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="87" t="s">
+      <c r="Q3" s="92"/>
+      <c r="R3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="87" t="s">
+      <c r="S3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="87" t="s">
+      <c r="T3" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="87" t="s">
+      <c r="U3" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="85"/>
-      <c r="W3" s="85"/>
-      <c r="X3" s="93"/>
-      <c r="Y3" s="93"/>
-      <c r="Z3" s="93"/>
-      <c r="AA3" s="93"/>
+      <c r="V3" s="79"/>
+      <c r="W3" s="79"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="76"/>
+      <c r="Z3" s="76"/>
+      <c r="AA3" s="76"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="83"/>
+      <c r="A4" s="89"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -8625,7 +9141,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="86"/>
+      <c r="H4" s="80"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -8653,16 +9169,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="86"/>
-      <c r="X4" s="94"/>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="94"/>
-      <c r="AA4" s="93"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="80"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="77"/>
+      <c r="Z4" s="77"/>
+      <c r="AA4" s="76"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -9163,11 +9679,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -9183,6 +9694,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updated instruction text to be parameterized.
Parameterized the introduction text based on the visualization (i.e. worded vs bar chart).  Fixed the issue with .env file having non escaped $ for compensation setting.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D8BB13-F5EA-DB4F-9ABD-4B69DCAC8AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5F0C5C-D8DD-7641-B5E8-2AAEA7F9D8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="1" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -982,6 +982,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1000,8 +1003,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1031,15 +1049,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1053,15 +1062,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4250,7 +4250,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M15" sqref="M15"/>
+      <selection pane="bottomLeft" activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -7456,7 +7456,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.59007458599140183</v>
+        <v>0.1319386425572403</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -7476,7 +7476,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f t="shared" ref="G3:G5" ca="1" si="0">RAND()</f>
-        <v>0.16444098806801022</v>
+        <v>0.38138160498094809</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -7497,7 +7497,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6898002662919297</v>
+        <v>0.98923239793536477</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7517,7 +7517,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70501408511060593</v>
+        <v>3.0710738273614369E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -7616,48 +7616,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="69" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="68" t="s">
+      <c r="D3" s="70"/>
+      <c r="E3" s="69" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="69"/>
-      <c r="G3" s="68" t="s">
+      <c r="F3" s="70"/>
+      <c r="G3" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="69"/>
-      <c r="I3" s="68" t="s">
+      <c r="H3" s="70"/>
+      <c r="I3" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="69"/>
+      <c r="J3" s="70"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="70" t="s">
+      <c r="M3" s="71" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="71"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="70" t="s">
+      <c r="N3" s="72"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="71" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="72"/>
-      <c r="S3" s="70" t="s">
+      <c r="Q3" s="72"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="71"/>
-      <c r="U3" s="71"/>
-      <c r="V3" s="73" t="s">
+      <c r="T3" s="72"/>
+      <c r="U3" s="72"/>
+      <c r="V3" s="74" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="73"/>
-      <c r="X3" s="73"/>
+      <c r="W3" s="74"/>
+      <c r="X3" s="74"/>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="50"/>
@@ -8484,16 +8484,16 @@
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="C29" s="74" t="s">
+      <c r="C29" s="68" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74" t="s">
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68" t="s">
         <v>169</v>
       </c>
-      <c r="G29" s="74"/>
-      <c r="H29" s="74"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
       <c r="J29" t="s">
         <v>168</v>
       </c>
@@ -9113,16 +9113,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9159,105 +9159,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="75" t="s">
+      <c r="A2" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="75" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="76"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="84" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="82"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="90" t="s">
+      <c r="I2" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="90" t="s">
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="90"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="84" t="s">
+      <c r="S2" s="93"/>
+      <c r="T2" s="93"/>
+      <c r="U2" s="93"/>
+      <c r="V2" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="84" t="s">
+      <c r="W2" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="92" t="s">
+      <c r="X2" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="92" t="s">
+      <c r="Y2" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="92" t="s">
+      <c r="Z2" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="92" t="s">
+      <c r="AA2" s="75" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="82"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="91" t="s">
+      <c r="A3" s="88"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89" t="s">
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89" t="s">
+      <c r="M3" s="92"/>
+      <c r="N3" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89" t="s">
+      <c r="O3" s="92"/>
+      <c r="P3" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="87" t="s">
+      <c r="Q3" s="92"/>
+      <c r="R3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="87" t="s">
+      <c r="S3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="87" t="s">
+      <c r="T3" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="87" t="s">
+      <c r="U3" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="85"/>
-      <c r="W3" s="85"/>
-      <c r="X3" s="93"/>
-      <c r="Y3" s="93"/>
-      <c r="Z3" s="93"/>
-      <c r="AA3" s="93"/>
+      <c r="V3" s="79"/>
+      <c r="W3" s="79"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="76"/>
+      <c r="Z3" s="76"/>
+      <c r="AA3" s="76"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="83"/>
+      <c r="A4" s="89"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -9276,7 +9276,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="86"/>
+      <c r="H4" s="80"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -9304,16 +9304,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="86"/>
-      <c r="X4" s="94"/>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="94"/>
-      <c r="AA4" s="93"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="80"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="77"/>
+      <c r="Z4" s="77"/>
+      <c r="AA4" s="76"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -9814,11 +9814,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -9834,6 +9829,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Not sure what changes these were if any. Didn't change treatment values.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5F0C5C-D8DD-7641-B5E8-2AAEA7F9D8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4D59FFA-5CED-9B4A-948C-83646D99120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="1" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="MCL questions prod" sheetId="10" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Web Parameters v1" sheetId="1" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1081,7 +1082,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1369,7 +1370,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1379,7 +1380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6462F7B1-F956-1241-A84D-BB94A5075354}">
   <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="V1" sqref="V1"/>
     </sheetView>
@@ -4248,7 +4249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
   <dimension ref="A1:W66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="X5" sqref="X5"/>
     </sheetView>
@@ -7411,7 +7412,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7456,7 +7457,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.1319386425572403</v>
+        <v>0.85672864624929124</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -7475,8 +7476,8 @@
       </c>
       <c r="F3" s="66"/>
       <c r="G3">
-        <f t="shared" ref="G3:G5" ca="1" si="0">RAND()</f>
-        <v>0.38138160498094809</v>
+        <f ca="1">RAND()</f>
+        <v>7.1221422827264957E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -7496,8 +7497,8 @@
       </c>
       <c r="F4" s="66"/>
       <c r="G4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.98923239793536477</v>
+        <f ca="1">RAND()</f>
+        <v>3.3321846748652795E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7516,8 +7517,8 @@
       </c>
       <c r="F5" s="66"/>
       <c r="G5">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.0710738273614369E-2</v>
+        <f ca="1">RAND()</f>
+        <v>0.10258517007342238</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -8603,7 +8604,7 @@
         <v>13</v>
       </c>
       <c r="Q31" s="37">
-        <f>K31/$C$28</f>
+        <f t="shared" ref="Q31:Q42" si="0">K31/$C$28</f>
         <v>2.3648648648648649</v>
       </c>
       <c r="R31" s="37">
@@ -8624,7 +8625,7 @@
         <v>740</v>
       </c>
       <c r="E32">
-        <f t="shared" ref="E32:E34" si="0">D32-C32</f>
+        <f>D32-C32</f>
         <v>220</v>
       </c>
       <c r="F32" s="37">
@@ -8650,7 +8651,7 @@
         <v>700</v>
       </c>
       <c r="N32" s="37">
-        <f t="shared" ref="N32:N34" si="1">M32-L32</f>
+        <f>M32-L32</f>
         <v>3.75</v>
       </c>
       <c r="O32" s="8">
@@ -8662,7 +8663,7 @@
         <v>18</v>
       </c>
       <c r="Q32" s="37">
-        <f>K32/$C$28</f>
+        <f t="shared" si="0"/>
         <v>3.310810810810811</v>
       </c>
       <c r="R32" s="37">
@@ -8683,7 +8684,7 @@
         <v>1480</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
+        <f>D33-C33</f>
         <v>710</v>
       </c>
       <c r="F33" s="37">
@@ -8710,7 +8711,7 @@
         <v>1390</v>
       </c>
       <c r="N33" s="37">
-        <f t="shared" si="1"/>
+        <f>M33-L33</f>
         <v>4.375</v>
       </c>
       <c r="O33" s="8">
@@ -8722,7 +8723,7 @@
         <v>36</v>
       </c>
       <c r="Q33" s="37">
-        <f>K33/$C$28</f>
+        <f t="shared" si="0"/>
         <v>4.8648648648648649</v>
       </c>
       <c r="R33" s="37">
@@ -8743,7 +8744,7 @@
         <v>1200</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
+        <f>D34-C34</f>
         <v>300</v>
       </c>
       <c r="F34" s="37">
@@ -8769,7 +8770,7 @@
         <v>1120</v>
       </c>
       <c r="N34" s="37">
-        <f t="shared" si="1"/>
+        <f>M34-L34</f>
         <v>-1.25</v>
       </c>
       <c r="O34" s="8">
@@ -8781,7 +8782,7 @@
         <v>16</v>
       </c>
       <c r="Q34" s="37">
-        <f>K34/$C$28</f>
+        <f t="shared" si="0"/>
         <v>5.6756756756756754</v>
       </c>
       <c r="R34" s="37">
@@ -8818,7 +8819,7 @@
         <v>13</v>
       </c>
       <c r="Q35" s="11">
-        <f>K35/$C$28</f>
+        <f t="shared" si="0"/>
         <v>78.378378378378372</v>
       </c>
       <c r="R35" s="11">
@@ -8854,7 +8855,7 @@
         <v>18</v>
       </c>
       <c r="Q36" s="11">
-        <f t="shared" ref="Q36:Q38" si="2">K36/$C$28</f>
+        <f t="shared" si="0"/>
         <v>110.13513513513513</v>
       </c>
       <c r="R36" s="11">
@@ -8890,7 +8891,7 @@
         <v>36</v>
       </c>
       <c r="Q37" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>162.16216216216216</v>
       </c>
       <c r="R37" s="11">
@@ -8926,7 +8927,7 @@
         <v>16</v>
       </c>
       <c r="Q38" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>189.18918918918919</v>
       </c>
       <c r="R38" s="11">
@@ -8970,7 +8971,7 @@
         <v>13</v>
       </c>
       <c r="Q39" s="11">
-        <f>K39/$C$28</f>
+        <f t="shared" si="0"/>
         <v>0.21621621621621623</v>
       </c>
       <c r="R39" s="11">
@@ -9015,7 +9016,7 @@
         <v>18</v>
       </c>
       <c r="Q40" s="11">
-        <f>K40/$C$28</f>
+        <f t="shared" si="0"/>
         <v>0.30405405405405406</v>
       </c>
       <c r="R40" s="11">
@@ -9059,7 +9060,7 @@
         <v>23</v>
       </c>
       <c r="Q41" s="11">
-        <f>K41/$C$28</f>
+        <f t="shared" si="0"/>
         <v>0.44594594594594594</v>
       </c>
       <c r="R41" s="11">
@@ -9103,7 +9104,7 @@
         <v>16</v>
       </c>
       <c r="Q42" s="11">
-        <f>K42/$C$28</f>
+        <f t="shared" si="0"/>
         <v>0.52027027027027029</v>
       </c>
       <c r="R42" s="11">
@@ -10225,19 +10226,19 @@
         <v>54</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" ref="D16:D18" si="4">AVERAGE(A16:B16)/365</f>
+        <f>AVERAGE(A16:B16)/365</f>
         <v>102.73835616438356</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" ref="E16:E18" si="5">3.3*D16</f>
+        <f>3.3*D16</f>
         <v>339.03657534246571</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" ref="F16:F18" si="6">16.7*D16</f>
+        <f>16.7*D16</f>
         <v>1715.7305479452054</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" ref="G16:G18" si="7">33.3*D16</f>
+        <f>33.3*D16</f>
         <v>3421.1872602739722</v>
       </c>
     </row>
@@ -10252,19 +10253,19 @@
         <v>54</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(A17:B17)/365</f>
         <v>171.23150684931508</v>
       </c>
       <c r="E17" s="4">
-        <f t="shared" si="5"/>
+        <f>3.3*D17</f>
         <v>565.0639726027398</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" si="6"/>
+        <f>16.7*D17</f>
         <v>2859.566164383562</v>
       </c>
       <c r="G17" s="4">
-        <f t="shared" si="7"/>
+        <f>33.3*D17</f>
         <v>5702.0091780821913</v>
       </c>
       <c r="H17" t="s">
@@ -10282,19 +10283,19 @@
         <v>54</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(A18:B18)/365</f>
         <v>239.72465753424657</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="5"/>
+        <f>3.3*D18</f>
         <v>791.09136986301371</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="6"/>
+        <f>16.7*D18</f>
         <v>4003.4017808219178</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="7"/>
+        <f>33.3*D18</f>
         <v>7982.8310958904103</v>
       </c>
     </row>

</xml_diff>

<commit_message>
merge latest of main to release
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D365563-D7E2-3242-933F-78A0B92D54F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4D59FFA-5CED-9B4A-948C-83646D99120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="3" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Web Parameters Prod" sheetId="10" r:id="rId1"/>
+    <sheet name="MCL questions prod" sheetId="10" r:id="rId1"/>
     <sheet name="Web Parameters Dev" sheetId="8" r:id="rId2"/>
     <sheet name="Web Parameters Random" sheetId="11" r:id="rId3"/>
     <sheet name="Date Delay Paper" sheetId="9" r:id="rId4"/>
@@ -25,6 +25,7 @@
     <sheet name="Web Parameters v1" sheetId="1" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="192">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -566,12 +567,6 @@
     <t>Question 4 (USD)</t>
   </si>
   <si>
-    <t>Barchart MEL question with no interaction inches.</t>
-  </si>
-  <si>
-    <t>Barchart with no interaction inches.</t>
-  </si>
-  <si>
     <t>Barchart MEL question with no interaction pixels.</t>
   </si>
   <si>
@@ -620,9 +615,6 @@
     <t>Worded MEL question experiment 1 date/delay paper.</t>
   </si>
   <si>
-    <t>Worded MEL question 33.3 DWR of experiment 1 to test magnitude effect.</t>
-  </si>
-  <si>
     <t>Worded MEL question experiment 3 of date/delay paper.</t>
   </si>
   <si>
@@ -632,22 +624,31 @@
     <t>Barchart MEL question experiment 1 date/delay paper half the screen.</t>
   </si>
   <si>
-    <t>Barchart MEL question 33.3 DWR of experiment 1 to test magnitude effect half the screen.</t>
-  </si>
-  <si>
     <t>Barchart MEL question experiment 3 of date/delay paper half the screen.</t>
   </si>
   <si>
     <t>Barchart MEL question experiment 1 date/delay paper full screen.</t>
   </si>
   <si>
-    <t>Barchart MEL question 33.3 DWR of experiment 1 to test magnitude effect full screen.</t>
-  </si>
-  <si>
     <t>Barchart MEL question experiment 3 of date/delay paper full screen.</t>
   </si>
   <si>
     <t>Amounts were used from Four Score and Seven Years from Now: The Date/Delay Effect in Temporal Discounting paper and converted from british pounds to USD using the conversion rate in the year the experiment was done and adjusting those amounts for inflation.</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Barchart with no interaction inches and minor tick marks.</t>
+  </si>
+  <si>
+    <t>Barchart MEL question with no interaction inches and minor tick marks.</t>
+  </si>
+  <si>
+    <t>show_minor_ticks</t>
   </si>
 </sst>
 </file>
@@ -982,6 +983,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1000,8 +1004,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1031,15 +1050,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1053,15 +1063,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1081,7 +1082,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1369,7 +1370,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1377,11 +1378,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6462F7B1-F956-1241-A84D-BB94A5075354}">
-  <dimension ref="A1:V37"/>
+  <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomLeft" activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1400,10 +1401,10 @@
     <col min="18" max="18" width="14.5" customWidth="1"/>
     <col min="19" max="19" width="14.83203125" customWidth="1"/>
     <col min="20" max="20" width="13.1640625" customWidth="1"/>
-    <col min="21" max="21" width="13.83203125" customWidth="1"/>
+    <col min="21" max="22" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -1468,10 +1469,13 @@
         <v>102</v>
       </c>
       <c r="V1" t="s">
+        <v>191</v>
+      </c>
+      <c r="W1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:23">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1504,11 +1508,11 @@
       <c r="L2">
         <v>430</v>
       </c>
-      <c r="V2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="W2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1541,11 +1545,11 @@
       <c r="L3">
         <v>700</v>
       </c>
-      <c r="V3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="W3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1579,11 +1583,11 @@
       <c r="L4">
         <v>1390</v>
       </c>
-      <c r="V4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="W4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1616,11 +1620,11 @@
       <c r="L5">
         <v>1120</v>
       </c>
-      <c r="V5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
+      <c r="W5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1636,28 +1640,28 @@
       <c r="E6" t="s">
         <v>118</v>
       </c>
-      <c r="F6">
-        <v>11600</v>
+      <c r="F6" s="37">
+        <v>31.714285714285715</v>
       </c>
       <c r="G6" s="43">
         <v>4</v>
       </c>
       <c r="H6" s="66"/>
-      <c r="I6">
-        <v>14000</v>
+      <c r="I6" s="37">
+        <v>39</v>
       </c>
       <c r="J6" s="43">
         <v>13</v>
       </c>
       <c r="K6" s="66"/>
       <c r="L6">
-        <v>14000</v>
-      </c>
-      <c r="V6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
+        <v>40</v>
+      </c>
+      <c r="W6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1673,28 +1677,28 @@
       <c r="E7" t="s">
         <v>118</v>
       </c>
-      <c r="F7">
-        <v>16300</v>
+      <c r="F7" s="37">
+        <v>44.571428571428569</v>
       </c>
       <c r="G7" s="43">
         <v>2</v>
       </c>
       <c r="H7" s="66"/>
-      <c r="I7">
-        <v>23000</v>
+      <c r="I7" s="37">
+        <v>70</v>
       </c>
       <c r="J7" s="43">
         <v>18</v>
       </c>
       <c r="K7" s="66"/>
       <c r="L7">
-        <v>23000</v>
-      </c>
-      <c r="V7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
+        <v>70</v>
+      </c>
+      <c r="W7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1710,28 +1714,28 @@
       <c r="E8" t="s">
         <v>118</v>
       </c>
-      <c r="F8">
-        <v>24000</v>
+      <c r="F8" s="37">
+        <v>66</v>
       </c>
       <c r="G8" s="43">
         <v>6</v>
       </c>
       <c r="H8" s="66"/>
-      <c r="I8">
-        <v>46000</v>
+      <c r="I8" s="37">
+        <v>110</v>
       </c>
       <c r="J8" s="43">
         <v>24</v>
       </c>
       <c r="K8" s="66"/>
       <c r="L8">
-        <v>46000</v>
-      </c>
-      <c r="V8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
+        <v>110</v>
+      </c>
+      <c r="W8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1747,36 +1751,42 @@
       <c r="E9" t="s">
         <v>118</v>
       </c>
-      <c r="F9">
-        <v>28000</v>
+      <c r="F9" s="37">
+        <v>77.142857142857139</v>
       </c>
       <c r="G9" s="43">
         <v>3</v>
       </c>
       <c r="H9" s="66"/>
-      <c r="I9">
-        <v>37000</v>
+      <c r="I9" s="37">
+        <v>118</v>
       </c>
       <c r="J9" s="43">
         <v>16</v>
       </c>
       <c r="K9" s="66"/>
       <c r="L9">
-        <v>37000</v>
-      </c>
-      <c r="V9" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
+        <v>120</v>
+      </c>
+      <c r="N9">
+        <v>600</v>
+      </c>
+      <c r="O9">
+        <v>300</v>
+      </c>
+      <c r="W9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D10" t="s">
         <v>118</v>
@@ -1784,36 +1794,48 @@
       <c r="E10" t="s">
         <v>118</v>
       </c>
-      <c r="F10" s="37">
-        <v>31.714285714285715</v>
+      <c r="F10">
+        <v>350</v>
       </c>
       <c r="G10" s="43">
         <v>4</v>
       </c>
       <c r="H10" s="66"/>
-      <c r="I10" s="37">
-        <v>39</v>
+      <c r="I10">
+        <v>430</v>
       </c>
       <c r="J10" s="43">
         <v>13</v>
       </c>
       <c r="K10" s="66"/>
       <c r="L10">
-        <v>40</v>
+        <v>430</v>
+      </c>
+      <c r="M10">
+        <v>14</v>
+      </c>
+      <c r="N10">
+        <v>600</v>
+      </c>
+      <c r="O10">
+        <v>300</v>
       </c>
       <c r="V10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
+        <v>187</v>
+      </c>
+      <c r="W10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D11" t="s">
         <v>118</v>
@@ -1821,36 +1843,48 @@
       <c r="E11" t="s">
         <v>118</v>
       </c>
-      <c r="F11" s="37">
-        <v>44.571428571428569</v>
+      <c r="F11">
+        <v>490</v>
       </c>
       <c r="G11" s="43">
         <v>2</v>
       </c>
       <c r="H11" s="66"/>
-      <c r="I11" s="37">
-        <v>70</v>
+      <c r="I11">
+        <v>700</v>
       </c>
       <c r="J11" s="43">
         <v>18</v>
       </c>
       <c r="K11" s="66"/>
       <c r="L11">
-        <v>70</v>
+        <v>700</v>
+      </c>
+      <c r="M11">
+        <v>19</v>
+      </c>
+      <c r="N11">
+        <v>600</v>
+      </c>
+      <c r="O11">
+        <v>300</v>
       </c>
       <c r="V11" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22">
+        <v>187</v>
+      </c>
+      <c r="W11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D12" t="s">
         <v>118</v>
@@ -1858,36 +1892,49 @@
       <c r="E12" t="s">
         <v>118</v>
       </c>
-      <c r="F12" s="37">
-        <v>66</v>
+      <c r="F12">
+        <f>720</f>
+        <v>720</v>
       </c>
       <c r="G12" s="43">
         <v>6</v>
       </c>
       <c r="H12" s="66"/>
-      <c r="I12" s="37">
-        <v>110</v>
+      <c r="I12">
+        <v>1390</v>
       </c>
       <c r="J12" s="43">
         <v>24</v>
       </c>
       <c r="K12" s="66"/>
       <c r="L12">
-        <v>110</v>
+        <v>1390</v>
+      </c>
+      <c r="M12">
+        <v>25</v>
+      </c>
+      <c r="N12">
+        <v>600</v>
+      </c>
+      <c r="O12">
+        <v>300</v>
       </c>
       <c r="V12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
+        <v>187</v>
+      </c>
+      <c r="W12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D13" t="s">
         <v>118</v>
@@ -1895,22 +1942,25 @@
       <c r="E13" t="s">
         <v>118</v>
       </c>
-      <c r="F13" s="37">
-        <v>77.142857142857139</v>
+      <c r="F13">
+        <v>840</v>
       </c>
       <c r="G13" s="43">
         <v>3</v>
       </c>
       <c r="H13" s="66"/>
-      <c r="I13" s="37">
-        <v>118</v>
+      <c r="I13">
+        <v>1120</v>
       </c>
       <c r="J13" s="43">
         <v>16</v>
       </c>
       <c r="K13" s="66"/>
       <c r="L13">
-        <v>120</v>
+        <v>1120</v>
+      </c>
+      <c r="M13">
+        <v>17</v>
       </c>
       <c r="N13">
         <v>600</v>
@@ -1919,15 +1969,18 @@
         <v>300</v>
       </c>
       <c r="V13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
+        <v>187</v>
+      </c>
+      <c r="W13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
         <v>104</v>
@@ -1938,22 +1991,22 @@
       <c r="E14" t="s">
         <v>118</v>
       </c>
-      <c r="F14">
-        <v>350</v>
+      <c r="F14" s="37">
+        <v>31.714285714285715</v>
       </c>
       <c r="G14" s="43">
         <v>4</v>
       </c>
       <c r="H14" s="66"/>
-      <c r="I14">
-        <v>430</v>
+      <c r="I14" s="37">
+        <v>39</v>
       </c>
       <c r="J14" s="43">
         <v>13</v>
       </c>
       <c r="K14" s="66"/>
       <c r="L14">
-        <v>430</v>
+        <v>40</v>
       </c>
       <c r="M14">
         <v>14</v>
@@ -1965,15 +2018,18 @@
         <v>300</v>
       </c>
       <c r="V14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22">
+        <v>187</v>
+      </c>
+      <c r="W14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
         <v>104</v>
@@ -1984,22 +2040,22 @@
       <c r="E15" t="s">
         <v>118</v>
       </c>
-      <c r="F15">
-        <v>490</v>
+      <c r="F15" s="37">
+        <v>44.571428571428569</v>
       </c>
       <c r="G15" s="43">
         <v>2</v>
       </c>
       <c r="H15" s="66"/>
-      <c r="I15">
-        <v>700</v>
+      <c r="I15" s="37">
+        <v>70</v>
       </c>
       <c r="J15" s="43">
         <v>18</v>
       </c>
       <c r="K15" s="66"/>
       <c r="L15">
-        <v>700</v>
+        <v>70</v>
       </c>
       <c r="M15">
         <v>19</v>
@@ -2011,15 +2067,18 @@
         <v>300</v>
       </c>
       <c r="V15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22">
+        <v>187</v>
+      </c>
+      <c r="W15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
         <v>104</v>
@@ -2030,227 +2089,242 @@
       <c r="E16" t="s">
         <v>118</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="37">
+        <v>66</v>
+      </c>
+      <c r="G16" s="43">
+        <v>6</v>
+      </c>
+      <c r="H16" s="66"/>
+      <c r="I16" s="37">
+        <v>110</v>
+      </c>
+      <c r="J16" s="43">
+        <v>24</v>
+      </c>
+      <c r="K16" s="66"/>
+      <c r="L16">
+        <v>110</v>
+      </c>
+      <c r="M16">
+        <v>25</v>
+      </c>
+      <c r="N16">
+        <v>600</v>
+      </c>
+      <c r="O16">
+        <v>300</v>
+      </c>
+      <c r="V16" t="s">
+        <v>187</v>
+      </c>
+      <c r="W16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" s="37">
+        <v>77.142857142857139</v>
+      </c>
+      <c r="G17" s="43">
+        <v>3</v>
+      </c>
+      <c r="H17" s="66"/>
+      <c r="I17" s="37">
+        <v>118</v>
+      </c>
+      <c r="J17" s="43">
+        <v>16</v>
+      </c>
+      <c r="K17" s="66"/>
+      <c r="L17">
+        <v>120</v>
+      </c>
+      <c r="M17">
+        <v>17</v>
+      </c>
+      <c r="N17">
+        <v>600</v>
+      </c>
+      <c r="O17">
+        <v>300</v>
+      </c>
+      <c r="V17" t="s">
+        <v>187</v>
+      </c>
+      <c r="W17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18">
+        <v>350</v>
+      </c>
+      <c r="G18" s="43">
+        <v>4</v>
+      </c>
+      <c r="H18" s="66"/>
+      <c r="I18">
+        <v>430</v>
+      </c>
+      <c r="J18" s="43">
+        <v>13</v>
+      </c>
+      <c r="K18" s="66"/>
+      <c r="L18">
+        <v>430</v>
+      </c>
+      <c r="M18">
+        <v>27</v>
+      </c>
+      <c r="N18">
+        <v>1200</v>
+      </c>
+      <c r="O18">
+        <v>300</v>
+      </c>
+      <c r="V18" t="s">
+        <v>187</v>
+      </c>
+      <c r="W18" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19">
+        <v>490</v>
+      </c>
+      <c r="G19" s="43">
+        <v>2</v>
+      </c>
+      <c r="H19" s="66"/>
+      <c r="I19">
+        <v>700</v>
+      </c>
+      <c r="J19" s="43">
+        <v>18</v>
+      </c>
+      <c r="K19" s="66"/>
+      <c r="L19">
+        <v>700</v>
+      </c>
+      <c r="M19">
+        <v>37</v>
+      </c>
+      <c r="N19">
+        <v>1200</v>
+      </c>
+      <c r="O19">
+        <v>300</v>
+      </c>
+      <c r="V19" t="s">
+        <v>187</v>
+      </c>
+      <c r="W19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F20">
         <f>720</f>
         <v>720</v>
       </c>
-      <c r="G16" s="43">
-        <v>6</v>
-      </c>
-      <c r="H16" s="66"/>
-      <c r="I16">
-        <v>1390</v>
-      </c>
-      <c r="J16" s="43">
-        <v>24</v>
-      </c>
-      <c r="K16" s="66"/>
-      <c r="L16">
-        <v>1390</v>
-      </c>
-      <c r="M16">
-        <v>25</v>
-      </c>
-      <c r="N16">
-        <v>600</v>
-      </c>
-      <c r="O16">
-        <v>300</v>
-      </c>
-      <c r="V16" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22">
-      <c r="A17">
-        <v>2</v>
-      </c>
-      <c r="B17">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>104</v>
-      </c>
-      <c r="D17" t="s">
-        <v>118</v>
-      </c>
-      <c r="E17" t="s">
-        <v>118</v>
-      </c>
-      <c r="F17">
-        <v>840</v>
-      </c>
-      <c r="G17" s="43">
-        <v>3</v>
-      </c>
-      <c r="H17" s="66"/>
-      <c r="I17">
-        <v>1120</v>
-      </c>
-      <c r="J17" s="43">
-        <v>16</v>
-      </c>
-      <c r="K17" s="66"/>
-      <c r="L17">
-        <v>1120</v>
-      </c>
-      <c r="M17">
-        <v>17</v>
-      </c>
-      <c r="N17">
-        <v>600</v>
-      </c>
-      <c r="O17">
-        <v>300</v>
-      </c>
-      <c r="V17" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22">
-      <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>104</v>
-      </c>
-      <c r="D18" t="s">
-        <v>118</v>
-      </c>
-      <c r="E18" t="s">
-        <v>118</v>
-      </c>
-      <c r="F18">
-        <v>11600</v>
-      </c>
-      <c r="G18" s="43">
-        <v>4</v>
-      </c>
-      <c r="H18" s="66"/>
-      <c r="I18">
-        <v>14000</v>
-      </c>
-      <c r="J18" s="43">
-        <v>13</v>
-      </c>
-      <c r="K18" s="66"/>
-      <c r="L18">
-        <v>14000</v>
-      </c>
-      <c r="M18">
-        <v>14</v>
-      </c>
-      <c r="N18">
-        <v>600</v>
-      </c>
-      <c r="O18">
-        <v>300</v>
-      </c>
-      <c r="V18" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D19" t="s">
-        <v>118</v>
-      </c>
-      <c r="E19" t="s">
-        <v>118</v>
-      </c>
-      <c r="F19">
-        <v>16300</v>
-      </c>
-      <c r="G19" s="43">
-        <v>2</v>
-      </c>
-      <c r="H19" s="66"/>
-      <c r="I19">
-        <v>23000</v>
-      </c>
-      <c r="J19" s="43">
-        <v>18</v>
-      </c>
-      <c r="K19" s="66"/>
-      <c r="L19">
-        <v>23000</v>
-      </c>
-      <c r="M19">
-        <v>19</v>
-      </c>
-      <c r="N19">
-        <v>600</v>
-      </c>
-      <c r="O19">
-        <v>300</v>
-      </c>
-      <c r="V19" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22">
-      <c r="A20">
-        <v>2</v>
-      </c>
-      <c r="B20">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E20" t="s">
-        <v>118</v>
-      </c>
-      <c r="F20">
-        <v>24000</v>
-      </c>
       <c r="G20" s="43">
         <v>6</v>
       </c>
       <c r="H20" s="66"/>
       <c r="I20">
-        <v>46000</v>
+        <v>1390</v>
       </c>
       <c r="J20" s="43">
         <v>24</v>
       </c>
       <c r="K20" s="66"/>
       <c r="L20">
-        <v>46000</v>
+        <v>1390</v>
       </c>
       <c r="M20">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="N20">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="O20">
         <v>300</v>
       </c>
       <c r="V20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22">
+        <v>187</v>
+      </c>
+      <c r="W20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
         <v>104</v>
@@ -2262,41 +2336,44 @@
         <v>118</v>
       </c>
       <c r="F21">
-        <v>28000</v>
+        <v>840</v>
       </c>
       <c r="G21" s="43">
         <v>3</v>
       </c>
       <c r="H21" s="66"/>
       <c r="I21">
-        <v>37000</v>
+        <v>1120</v>
       </c>
       <c r="J21" s="43">
         <v>16</v>
       </c>
       <c r="K21" s="66"/>
       <c r="L21">
-        <v>37000</v>
+        <v>1120</v>
       </c>
       <c r="M21">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="N21">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="O21">
         <v>300</v>
       </c>
       <c r="V21" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22">
+        <v>187</v>
+      </c>
+      <c r="W21" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
         <v>104</v>
@@ -2325,10 +2402,10 @@
         <v>40</v>
       </c>
       <c r="M22">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="N22">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="O22">
         <v>300</v>
@@ -2336,13 +2413,16 @@
       <c r="V22" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="23" spans="1:22">
+      <c r="W22" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B23">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
         <v>104</v>
@@ -2371,10 +2451,10 @@
         <v>70</v>
       </c>
       <c r="M23">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="N23">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="O23">
         <v>300</v>
@@ -2382,13 +2462,16 @@
       <c r="V23" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="24" spans="1:22">
+      <c r="W23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
       <c r="A24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B24">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
         <v>104</v>
@@ -2417,24 +2500,27 @@
         <v>110</v>
       </c>
       <c r="M24">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="N24">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="O24">
         <v>300</v>
       </c>
       <c r="V24" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22">
+        <v>187</v>
+      </c>
+      <c r="W24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B25">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
         <v>104</v>
@@ -2463,10 +2549,10 @@
         <v>120</v>
       </c>
       <c r="M25">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="N25">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="O25">
         <v>300</v>
@@ -2474,558 +2560,8 @@
       <c r="V25" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="26" spans="1:22">
-      <c r="A26">
-        <v>3</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>104</v>
-      </c>
-      <c r="D26" t="s">
-        <v>118</v>
-      </c>
-      <c r="E26" t="s">
-        <v>118</v>
-      </c>
-      <c r="F26">
-        <v>350</v>
-      </c>
-      <c r="G26" s="43">
-        <v>4</v>
-      </c>
-      <c r="H26" s="66"/>
-      <c r="I26">
-        <v>430</v>
-      </c>
-      <c r="J26" s="43">
-        <v>13</v>
-      </c>
-      <c r="K26" s="66"/>
-      <c r="L26">
-        <v>430</v>
-      </c>
-      <c r="M26">
-        <v>27</v>
-      </c>
-      <c r="N26">
-        <v>1200</v>
-      </c>
-      <c r="O26">
-        <v>300</v>
-      </c>
-      <c r="V26" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22">
-      <c r="A27">
-        <v>3</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>104</v>
-      </c>
-      <c r="D27" t="s">
-        <v>118</v>
-      </c>
-      <c r="E27" t="s">
-        <v>118</v>
-      </c>
-      <c r="F27">
-        <v>490</v>
-      </c>
-      <c r="G27" s="43">
-        <v>2</v>
-      </c>
-      <c r="H27" s="66"/>
-      <c r="I27">
-        <v>700</v>
-      </c>
-      <c r="J27" s="43">
-        <v>18</v>
-      </c>
-      <c r="K27" s="66"/>
-      <c r="L27">
-        <v>700</v>
-      </c>
-      <c r="M27">
-        <v>37</v>
-      </c>
-      <c r="N27">
-        <v>1200</v>
-      </c>
-      <c r="O27">
-        <v>300</v>
-      </c>
-      <c r="V27" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22">
-      <c r="A28">
-        <v>3</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>104</v>
-      </c>
-      <c r="D28" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" t="s">
-        <v>118</v>
-      </c>
-      <c r="F28">
-        <f>720</f>
-        <v>720</v>
-      </c>
-      <c r="G28" s="43">
-        <v>6</v>
-      </c>
-      <c r="H28" s="66"/>
-      <c r="I28">
-        <v>1390</v>
-      </c>
-      <c r="J28" s="43">
-        <v>24</v>
-      </c>
-      <c r="K28" s="66"/>
-      <c r="L28">
-        <v>1390</v>
-      </c>
-      <c r="M28">
-        <v>49</v>
-      </c>
-      <c r="N28">
-        <v>1200</v>
-      </c>
-      <c r="O28">
-        <v>300</v>
-      </c>
-      <c r="V28" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22">
-      <c r="A29">
-        <v>3</v>
-      </c>
-      <c r="B29">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>104</v>
-      </c>
-      <c r="D29" t="s">
-        <v>118</v>
-      </c>
-      <c r="E29" t="s">
-        <v>118</v>
-      </c>
-      <c r="F29">
-        <v>840</v>
-      </c>
-      <c r="G29" s="43">
-        <v>3</v>
-      </c>
-      <c r="H29" s="66"/>
-      <c r="I29">
-        <v>1120</v>
-      </c>
-      <c r="J29" s="43">
-        <v>16</v>
-      </c>
-      <c r="K29" s="66"/>
-      <c r="L29">
-        <v>1120</v>
-      </c>
-      <c r="M29">
-        <v>33</v>
-      </c>
-      <c r="N29">
-        <v>1200</v>
-      </c>
-      <c r="O29">
-        <v>300</v>
-      </c>
-      <c r="V29" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22">
-      <c r="A30">
-        <v>3</v>
-      </c>
-      <c r="B30">
-        <v>5</v>
-      </c>
-      <c r="C30" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" t="s">
-        <v>118</v>
-      </c>
-      <c r="E30" t="s">
-        <v>118</v>
-      </c>
-      <c r="F30">
-        <v>11600</v>
-      </c>
-      <c r="G30" s="43">
-        <v>4</v>
-      </c>
-      <c r="H30" s="66"/>
-      <c r="I30">
-        <v>14000</v>
-      </c>
-      <c r="J30" s="43">
-        <v>13</v>
-      </c>
-      <c r="K30" s="66"/>
-      <c r="L30">
-        <v>14000</v>
-      </c>
-      <c r="M30">
-        <v>37</v>
-      </c>
-      <c r="N30">
-        <v>1200</v>
-      </c>
-      <c r="O30">
-        <v>300</v>
-      </c>
-      <c r="V30" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22">
-      <c r="A31">
-        <v>3</v>
-      </c>
-      <c r="B31">
-        <v>6</v>
-      </c>
-      <c r="C31" t="s">
-        <v>104</v>
-      </c>
-      <c r="D31" t="s">
-        <v>118</v>
-      </c>
-      <c r="E31" t="s">
-        <v>118</v>
-      </c>
-      <c r="F31">
-        <v>16300</v>
-      </c>
-      <c r="G31" s="43">
-        <v>2</v>
-      </c>
-      <c r="H31" s="66"/>
-      <c r="I31">
-        <v>23000</v>
-      </c>
-      <c r="J31" s="43">
-        <v>18</v>
-      </c>
-      <c r="K31" s="66"/>
-      <c r="L31">
-        <v>23000</v>
-      </c>
-      <c r="M31">
-        <v>37</v>
-      </c>
-      <c r="N31">
-        <v>1200</v>
-      </c>
-      <c r="O31">
-        <v>300</v>
-      </c>
-      <c r="V31" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22">
-      <c r="A32">
-        <v>3</v>
-      </c>
-      <c r="B32">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>104</v>
-      </c>
-      <c r="D32" t="s">
-        <v>118</v>
-      </c>
-      <c r="E32" t="s">
-        <v>118</v>
-      </c>
-      <c r="F32">
-        <v>24000</v>
-      </c>
-      <c r="G32" s="43">
-        <v>6</v>
-      </c>
-      <c r="H32" s="66"/>
-      <c r="I32">
-        <v>46000</v>
-      </c>
-      <c r="J32" s="43">
-        <v>24</v>
-      </c>
-      <c r="K32" s="66"/>
-      <c r="L32">
-        <v>46000</v>
-      </c>
-      <c r="M32">
-        <v>49</v>
-      </c>
-      <c r="N32">
-        <v>1200</v>
-      </c>
-      <c r="O32">
-        <v>300</v>
-      </c>
-      <c r="V32" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22">
-      <c r="A33">
-        <v>3</v>
-      </c>
-      <c r="B33">
-        <v>8</v>
-      </c>
-      <c r="C33" t="s">
-        <v>104</v>
-      </c>
-      <c r="D33" t="s">
-        <v>118</v>
-      </c>
-      <c r="E33" t="s">
-        <v>118</v>
-      </c>
-      <c r="F33">
-        <v>28000</v>
-      </c>
-      <c r="G33" s="43">
-        <v>3</v>
-      </c>
-      <c r="H33" s="66"/>
-      <c r="I33">
-        <v>37000</v>
-      </c>
-      <c r="J33" s="43">
-        <v>16</v>
-      </c>
-      <c r="K33" s="66"/>
-      <c r="L33">
-        <v>37000</v>
-      </c>
-      <c r="M33">
-        <v>33</v>
-      </c>
-      <c r="N33">
-        <v>1200</v>
-      </c>
-      <c r="O33">
-        <v>300</v>
-      </c>
-      <c r="V33" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22">
-      <c r="A34">
-        <v>3</v>
-      </c>
-      <c r="B34">
-        <v>9</v>
-      </c>
-      <c r="C34" t="s">
-        <v>104</v>
-      </c>
-      <c r="D34" t="s">
-        <v>118</v>
-      </c>
-      <c r="E34" t="s">
-        <v>118</v>
-      </c>
-      <c r="F34" s="37">
-        <v>31.714285714285715</v>
-      </c>
-      <c r="G34" s="43">
-        <v>4</v>
-      </c>
-      <c r="H34" s="66"/>
-      <c r="I34" s="37">
-        <v>39</v>
-      </c>
-      <c r="J34" s="43">
-        <v>13</v>
-      </c>
-      <c r="K34" s="66"/>
-      <c r="L34">
-        <v>40</v>
-      </c>
-      <c r="M34">
-        <v>27</v>
-      </c>
-      <c r="N34">
-        <v>1200</v>
-      </c>
-      <c r="O34">
-        <v>300</v>
-      </c>
-      <c r="V34" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22">
-      <c r="A35">
-        <v>3</v>
-      </c>
-      <c r="B35">
-        <v>10</v>
-      </c>
-      <c r="C35" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" t="s">
-        <v>118</v>
-      </c>
-      <c r="E35" t="s">
-        <v>118</v>
-      </c>
-      <c r="F35" s="37">
-        <v>44.571428571428569</v>
-      </c>
-      <c r="G35" s="43">
-        <v>2</v>
-      </c>
-      <c r="H35" s="66"/>
-      <c r="I35" s="37">
-        <v>70</v>
-      </c>
-      <c r="J35" s="43">
-        <v>18</v>
-      </c>
-      <c r="K35" s="66"/>
-      <c r="L35">
-        <v>70</v>
-      </c>
-      <c r="M35">
-        <v>37</v>
-      </c>
-      <c r="N35">
-        <v>1200</v>
-      </c>
-      <c r="O35">
-        <v>300</v>
-      </c>
-      <c r="V35" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22">
-      <c r="A36">
-        <v>3</v>
-      </c>
-      <c r="B36">
-        <v>11</v>
-      </c>
-      <c r="C36" t="s">
-        <v>104</v>
-      </c>
-      <c r="D36" t="s">
-        <v>118</v>
-      </c>
-      <c r="E36" t="s">
-        <v>118</v>
-      </c>
-      <c r="F36" s="37">
-        <v>66</v>
-      </c>
-      <c r="G36" s="43">
-        <v>6</v>
-      </c>
-      <c r="H36" s="66"/>
-      <c r="I36" s="37">
-        <v>110</v>
-      </c>
-      <c r="J36" s="43">
-        <v>24</v>
-      </c>
-      <c r="K36" s="66"/>
-      <c r="L36">
-        <v>110</v>
-      </c>
-      <c r="M36">
-        <v>49</v>
-      </c>
-      <c r="N36">
-        <v>1200</v>
-      </c>
-      <c r="O36">
-        <v>300</v>
-      </c>
-      <c r="V36" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22">
-      <c r="A37">
-        <v>3</v>
-      </c>
-      <c r="B37">
-        <v>12</v>
-      </c>
-      <c r="C37" t="s">
-        <v>104</v>
-      </c>
-      <c r="D37" t="s">
-        <v>118</v>
-      </c>
-      <c r="E37" t="s">
-        <v>118</v>
-      </c>
-      <c r="F37" s="37">
-        <v>77.142857142857139</v>
-      </c>
-      <c r="G37" s="43">
-        <v>3</v>
-      </c>
-      <c r="H37" s="66"/>
-      <c r="I37" s="37">
-        <v>118</v>
-      </c>
-      <c r="J37" s="43">
-        <v>16</v>
-      </c>
-      <c r="K37" s="66"/>
-      <c r="L37">
-        <v>120</v>
-      </c>
-      <c r="M37">
-        <v>33</v>
-      </c>
-      <c r="N37">
-        <v>1200</v>
-      </c>
-      <c r="O37">
-        <v>300</v>
-      </c>
-      <c r="V37" t="s">
-        <v>190</v>
+      <c r="W25" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -4711,11 +4247,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:W66"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -4734,10 +4270,10 @@
     <col min="18" max="18" width="14.5" customWidth="1"/>
     <col min="19" max="19" width="14.83203125" customWidth="1"/>
     <col min="20" max="20" width="13.1640625" customWidth="1"/>
-    <col min="21" max="21" width="13.83203125" customWidth="1"/>
+    <col min="21" max="22" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -4802,10 +4338,13 @@
         <v>102</v>
       </c>
       <c r="V1" t="s">
+        <v>191</v>
+      </c>
+      <c r="W1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:23">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4842,11 +4381,11 @@
       <c r="U2">
         <v>4</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:23">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4883,11 +4422,11 @@
       <c r="U3">
         <v>8</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:23">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4924,11 +4463,11 @@
       <c r="U4">
         <v>8</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:23">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4981,10 +4520,13 @@
         <v>8.5</v>
       </c>
       <c r="V5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
+        <v>188</v>
+      </c>
+      <c r="W5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6">
         <v>2</v>
       </c>
@@ -5037,10 +4579,13 @@
         <v>8.5</v>
       </c>
       <c r="V6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
+        <v>188</v>
+      </c>
+      <c r="W6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7">
         <v>2</v>
       </c>
@@ -5093,10 +4638,13 @@
         <v>4.5</v>
       </c>
       <c r="V7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
+        <v>188</v>
+      </c>
+      <c r="W7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8">
         <v>3</v>
       </c>
@@ -5137,10 +4685,13 @@
         <v>300</v>
       </c>
       <c r="V8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
+        <v>187</v>
+      </c>
+      <c r="W8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9">
         <v>3</v>
       </c>
@@ -5181,10 +4732,13 @@
         <v>300</v>
       </c>
       <c r="V9" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
+        <v>187</v>
+      </c>
+      <c r="W9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10">
         <v>3</v>
       </c>
@@ -5225,10 +4779,13 @@
         <v>300</v>
       </c>
       <c r="V10" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
+        <v>187</v>
+      </c>
+      <c r="W10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11">
         <v>3</v>
       </c>
@@ -5269,10 +4826,13 @@
         <v>300</v>
       </c>
       <c r="V11" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22">
+        <v>187</v>
+      </c>
+      <c r="W11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12">
         <v>3</v>
       </c>
@@ -5313,10 +4873,13 @@
         <v>300</v>
       </c>
       <c r="V12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
+        <v>187</v>
+      </c>
+      <c r="W12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13">
         <v>4</v>
       </c>
@@ -5359,11 +4922,11 @@
       <c r="U13">
         <v>8</v>
       </c>
-      <c r="V13" t="s">
+      <c r="W13" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:23">
       <c r="A14">
         <v>4</v>
       </c>
@@ -5406,11 +4969,11 @@
       <c r="U14">
         <v>8</v>
       </c>
-      <c r="V14" t="s">
+      <c r="W14" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:23">
       <c r="A15">
         <v>4</v>
       </c>
@@ -5453,11 +5016,11 @@
       <c r="U15">
         <v>8</v>
       </c>
-      <c r="V15" t="s">
+      <c r="W15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:23">
       <c r="A16">
         <v>5</v>
       </c>
@@ -5500,11 +5063,11 @@
       <c r="U16">
         <v>8</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:23">
       <c r="A17">
         <v>5</v>
       </c>
@@ -5547,11 +5110,11 @@
       <c r="U17">
         <v>8</v>
       </c>
-      <c r="V17" t="s">
+      <c r="W17" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:23">
       <c r="A18">
         <v>5</v>
       </c>
@@ -5594,11 +5157,11 @@
       <c r="U18">
         <v>8</v>
       </c>
-      <c r="V18" t="s">
+      <c r="W18" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:23">
       <c r="A19">
         <v>6</v>
       </c>
@@ -5656,11 +5219,11 @@
       <c r="U19">
         <v>8.5</v>
       </c>
-      <c r="V19" t="s">
+      <c r="W19" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:23">
       <c r="A20">
         <v>7</v>
       </c>
@@ -5703,11 +5266,11 @@
       <c r="U20">
         <v>8</v>
       </c>
-      <c r="V20" t="s">
+      <c r="W20" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:23">
       <c r="A21">
         <v>8</v>
       </c>
@@ -5744,11 +5307,11 @@
       <c r="U21">
         <v>8</v>
       </c>
-      <c r="V21" t="s">
+      <c r="W21" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:23">
       <c r="A22">
         <v>9</v>
       </c>
@@ -5806,11 +5369,11 @@
       <c r="U22">
         <v>8.5</v>
       </c>
-      <c r="V22" t="s">
+      <c r="W22" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:23">
       <c r="A23">
         <v>10</v>
       </c>
@@ -5853,11 +5416,11 @@
       <c r="U23">
         <v>8</v>
       </c>
-      <c r="V23" t="s">
+      <c r="W23" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:23">
       <c r="A24">
         <v>11</v>
       </c>
@@ -5900,11 +5463,11 @@
       <c r="U24">
         <v>8</v>
       </c>
-      <c r="V24" t="s">
+      <c r="W24" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:23">
       <c r="A25">
         <v>12</v>
       </c>
@@ -5947,11 +5510,11 @@
       <c r="U25">
         <v>8</v>
       </c>
-      <c r="V25" t="s">
+      <c r="W25" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:23">
       <c r="A26">
         <v>13</v>
       </c>
@@ -5994,11 +5557,11 @@
       <c r="U26">
         <v>8</v>
       </c>
-      <c r="V26" t="s">
+      <c r="W26" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:23">
       <c r="A27">
         <v>14</v>
       </c>
@@ -6041,11 +5604,11 @@
       <c r="U27">
         <v>8</v>
       </c>
-      <c r="V27" t="s">
+      <c r="W27" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:23">
       <c r="A28">
         <v>15</v>
       </c>
@@ -6088,11 +5651,11 @@
       <c r="U28">
         <v>8</v>
       </c>
-      <c r="V28" t="s">
+      <c r="W28" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:23">
       <c r="A29">
         <v>15</v>
       </c>
@@ -6135,11 +5698,11 @@
       <c r="U29">
         <v>8</v>
       </c>
-      <c r="V29" t="s">
+      <c r="W29" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:23">
       <c r="A30">
         <v>15</v>
       </c>
@@ -6182,11 +5745,11 @@
       <c r="U30">
         <v>8</v>
       </c>
-      <c r="V30" t="s">
+      <c r="W30" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:23">
       <c r="A31">
         <v>16</v>
       </c>
@@ -6229,11 +5792,11 @@
       <c r="U31">
         <v>8</v>
       </c>
-      <c r="V31" t="s">
+      <c r="W31" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:23">
       <c r="A32">
         <v>16</v>
       </c>
@@ -6276,11 +5839,11 @@
       <c r="U32">
         <v>8</v>
       </c>
-      <c r="V32" t="s">
+      <c r="W32" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:22">
+    <row r="33" spans="1:23">
       <c r="A33">
         <v>16</v>
       </c>
@@ -6323,11 +5886,11 @@
       <c r="U33">
         <v>8</v>
       </c>
-      <c r="V33" t="s">
+      <c r="W33" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:22">
+    <row r="34" spans="1:23">
       <c r="A34">
         <v>17</v>
       </c>
@@ -6370,11 +5933,11 @@
       <c r="U34">
         <v>8</v>
       </c>
-      <c r="V34" t="s">
+      <c r="W34" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:22">
+    <row r="35" spans="1:23">
       <c r="A35">
         <v>17</v>
       </c>
@@ -6417,11 +5980,11 @@
       <c r="U35">
         <v>8</v>
       </c>
-      <c r="V35" t="s">
+      <c r="W35" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:22">
+    <row r="36" spans="1:23">
       <c r="A36">
         <v>17</v>
       </c>
@@ -6464,11 +6027,11 @@
       <c r="U36">
         <v>8</v>
       </c>
-      <c r="V36" t="s">
+      <c r="W36" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:22">
+    <row r="37" spans="1:23">
       <c r="A37">
         <v>18</v>
       </c>
@@ -6511,11 +6074,11 @@
       <c r="U37">
         <v>8</v>
       </c>
-      <c r="V37" t="s">
+      <c r="W37" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="1:22">
+    <row r="38" spans="1:23">
       <c r="A38">
         <v>18</v>
       </c>
@@ -6558,11 +6121,11 @@
       <c r="U38">
         <v>8</v>
       </c>
-      <c r="V38" t="s">
+      <c r="W38" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:22">
+    <row r="39" spans="1:23">
       <c r="A39">
         <v>18</v>
       </c>
@@ -6605,11 +6168,11 @@
       <c r="U39">
         <v>8</v>
       </c>
-      <c r="V39" t="s">
+      <c r="W39" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:22">
+    <row r="40" spans="1:23">
       <c r="A40">
         <v>19</v>
       </c>
@@ -6652,11 +6215,11 @@
       <c r="U40">
         <v>8</v>
       </c>
-      <c r="V40" t="s">
+      <c r="W40" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:22">
+    <row r="41" spans="1:23">
       <c r="A41">
         <v>19</v>
       </c>
@@ -6699,11 +6262,11 @@
       <c r="U41">
         <v>8</v>
       </c>
-      <c r="V41" t="s">
+      <c r="W41" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="1:22">
+    <row r="42" spans="1:23">
       <c r="A42">
         <v>19</v>
       </c>
@@ -6746,8 +6309,1097 @@
       <c r="U42">
         <v>8</v>
       </c>
-      <c r="V42" t="s">
+      <c r="W42" t="s">
         <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23">
+      <c r="A43">
+        <v>20</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43" t="s">
+        <v>118</v>
+      </c>
+      <c r="E43" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43">
+        <v>350</v>
+      </c>
+      <c r="G43" s="43">
+        <v>4</v>
+      </c>
+      <c r="H43" s="66"/>
+      <c r="I43">
+        <v>430</v>
+      </c>
+      <c r="J43" s="43">
+        <v>13</v>
+      </c>
+      <c r="K43" s="66"/>
+      <c r="L43">
+        <v>430</v>
+      </c>
+      <c r="W43" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23">
+      <c r="A44">
+        <v>20</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" t="s">
+        <v>118</v>
+      </c>
+      <c r="E44" t="s">
+        <v>118</v>
+      </c>
+      <c r="F44">
+        <v>490</v>
+      </c>
+      <c r="G44" s="43">
+        <v>2</v>
+      </c>
+      <c r="H44" s="66"/>
+      <c r="I44">
+        <v>700</v>
+      </c>
+      <c r="J44" s="43">
+        <v>18</v>
+      </c>
+      <c r="K44" s="66"/>
+      <c r="L44">
+        <v>700</v>
+      </c>
+      <c r="W44" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23">
+      <c r="A45">
+        <v>20</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>120</v>
+      </c>
+      <c r="D45" t="s">
+        <v>118</v>
+      </c>
+      <c r="E45" t="s">
+        <v>118</v>
+      </c>
+      <c r="F45">
+        <f>720</f>
+        <v>720</v>
+      </c>
+      <c r="G45" s="43">
+        <v>6</v>
+      </c>
+      <c r="H45" s="66"/>
+      <c r="I45">
+        <v>1390</v>
+      </c>
+      <c r="J45" s="43">
+        <v>24</v>
+      </c>
+      <c r="K45" s="66"/>
+      <c r="L45">
+        <v>1390</v>
+      </c>
+      <c r="W45" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23">
+      <c r="A46">
+        <v>20</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" t="s">
+        <v>118</v>
+      </c>
+      <c r="E46" t="s">
+        <v>118</v>
+      </c>
+      <c r="F46">
+        <v>840</v>
+      </c>
+      <c r="G46" s="43">
+        <v>3</v>
+      </c>
+      <c r="H46" s="66"/>
+      <c r="I46">
+        <v>1120</v>
+      </c>
+      <c r="J46" s="43">
+        <v>16</v>
+      </c>
+      <c r="K46" s="66"/>
+      <c r="L46">
+        <v>1120</v>
+      </c>
+      <c r="W46" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23">
+      <c r="A47">
+        <v>20</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" t="s">
+        <v>118</v>
+      </c>
+      <c r="E47" t="s">
+        <v>118</v>
+      </c>
+      <c r="F47" s="37">
+        <v>31.714285714285715</v>
+      </c>
+      <c r="G47" s="43">
+        <v>4</v>
+      </c>
+      <c r="H47" s="66"/>
+      <c r="I47" s="37">
+        <v>39</v>
+      </c>
+      <c r="J47" s="43">
+        <v>13</v>
+      </c>
+      <c r="K47" s="66"/>
+      <c r="L47">
+        <v>40</v>
+      </c>
+      <c r="W47" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23">
+      <c r="A48">
+        <v>20</v>
+      </c>
+      <c r="B48">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>120</v>
+      </c>
+      <c r="D48" t="s">
+        <v>118</v>
+      </c>
+      <c r="E48" t="s">
+        <v>118</v>
+      </c>
+      <c r="F48" s="37">
+        <v>44.571428571428569</v>
+      </c>
+      <c r="G48" s="43">
+        <v>2</v>
+      </c>
+      <c r="H48" s="66"/>
+      <c r="I48" s="37">
+        <v>70</v>
+      </c>
+      <c r="J48" s="43">
+        <v>18</v>
+      </c>
+      <c r="K48" s="66"/>
+      <c r="L48">
+        <v>70</v>
+      </c>
+      <c r="W48" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23">
+      <c r="A49">
+        <v>20</v>
+      </c>
+      <c r="B49">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" t="s">
+        <v>118</v>
+      </c>
+      <c r="E49" t="s">
+        <v>118</v>
+      </c>
+      <c r="F49" s="37">
+        <v>66</v>
+      </c>
+      <c r="G49" s="43">
+        <v>6</v>
+      </c>
+      <c r="H49" s="66"/>
+      <c r="I49" s="37">
+        <v>110</v>
+      </c>
+      <c r="J49" s="43">
+        <v>24</v>
+      </c>
+      <c r="K49" s="66"/>
+      <c r="L49">
+        <v>110</v>
+      </c>
+      <c r="W49" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23">
+      <c r="A50">
+        <v>20</v>
+      </c>
+      <c r="B50">
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" t="s">
+        <v>118</v>
+      </c>
+      <c r="E50" t="s">
+        <v>118</v>
+      </c>
+      <c r="F50" s="37">
+        <v>77.142857142857139</v>
+      </c>
+      <c r="G50" s="43">
+        <v>3</v>
+      </c>
+      <c r="H50" s="66"/>
+      <c r="I50" s="37">
+        <v>118</v>
+      </c>
+      <c r="J50" s="43">
+        <v>16</v>
+      </c>
+      <c r="K50" s="66"/>
+      <c r="L50">
+        <v>120</v>
+      </c>
+      <c r="N50">
+        <v>600</v>
+      </c>
+      <c r="O50">
+        <v>300</v>
+      </c>
+      <c r="W50" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23">
+      <c r="A51">
+        <v>21</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>104</v>
+      </c>
+      <c r="D51" t="s">
+        <v>118</v>
+      </c>
+      <c r="E51" t="s">
+        <v>118</v>
+      </c>
+      <c r="F51">
+        <v>350</v>
+      </c>
+      <c r="G51" s="43">
+        <v>4</v>
+      </c>
+      <c r="H51" s="66"/>
+      <c r="I51">
+        <v>430</v>
+      </c>
+      <c r="J51" s="43">
+        <v>13</v>
+      </c>
+      <c r="K51" s="66"/>
+      <c r="L51">
+        <v>430</v>
+      </c>
+      <c r="M51">
+        <v>14</v>
+      </c>
+      <c r="N51">
+        <v>600</v>
+      </c>
+      <c r="O51">
+        <v>300</v>
+      </c>
+      <c r="V51" t="s">
+        <v>187</v>
+      </c>
+      <c r="W51" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23">
+      <c r="A52">
+        <v>21</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>104</v>
+      </c>
+      <c r="D52" t="s">
+        <v>118</v>
+      </c>
+      <c r="E52" t="s">
+        <v>118</v>
+      </c>
+      <c r="F52">
+        <v>490</v>
+      </c>
+      <c r="G52" s="43">
+        <v>2</v>
+      </c>
+      <c r="H52" s="66"/>
+      <c r="I52">
+        <v>700</v>
+      </c>
+      <c r="J52" s="43">
+        <v>18</v>
+      </c>
+      <c r="K52" s="66"/>
+      <c r="L52">
+        <v>700</v>
+      </c>
+      <c r="M52">
+        <v>19</v>
+      </c>
+      <c r="N52">
+        <v>600</v>
+      </c>
+      <c r="O52">
+        <v>300</v>
+      </c>
+      <c r="V52" t="s">
+        <v>187</v>
+      </c>
+      <c r="W52" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23">
+      <c r="A53">
+        <v>21</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>104</v>
+      </c>
+      <c r="D53" t="s">
+        <v>118</v>
+      </c>
+      <c r="E53" t="s">
+        <v>118</v>
+      </c>
+      <c r="F53">
+        <f>720</f>
+        <v>720</v>
+      </c>
+      <c r="G53" s="43">
+        <v>6</v>
+      </c>
+      <c r="H53" s="66"/>
+      <c r="I53">
+        <v>1390</v>
+      </c>
+      <c r="J53" s="43">
+        <v>24</v>
+      </c>
+      <c r="K53" s="66"/>
+      <c r="L53">
+        <v>1390</v>
+      </c>
+      <c r="M53">
+        <v>25</v>
+      </c>
+      <c r="N53">
+        <v>600</v>
+      </c>
+      <c r="O53">
+        <v>300</v>
+      </c>
+      <c r="V53" t="s">
+        <v>187</v>
+      </c>
+      <c r="W53" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23">
+      <c r="A54">
+        <v>21</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" t="s">
+        <v>118</v>
+      </c>
+      <c r="E54" t="s">
+        <v>118</v>
+      </c>
+      <c r="F54">
+        <v>840</v>
+      </c>
+      <c r="G54" s="43">
+        <v>3</v>
+      </c>
+      <c r="H54" s="66"/>
+      <c r="I54">
+        <v>1120</v>
+      </c>
+      <c r="J54" s="43">
+        <v>16</v>
+      </c>
+      <c r="K54" s="66"/>
+      <c r="L54">
+        <v>1120</v>
+      </c>
+      <c r="M54">
+        <v>17</v>
+      </c>
+      <c r="N54">
+        <v>600</v>
+      </c>
+      <c r="O54">
+        <v>300</v>
+      </c>
+      <c r="V54" t="s">
+        <v>187</v>
+      </c>
+      <c r="W54" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23">
+      <c r="A55">
+        <v>21</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" t="s">
+        <v>118</v>
+      </c>
+      <c r="E55" t="s">
+        <v>118</v>
+      </c>
+      <c r="F55" s="37">
+        <v>31.714285714285715</v>
+      </c>
+      <c r="G55" s="43">
+        <v>4</v>
+      </c>
+      <c r="H55" s="66"/>
+      <c r="I55" s="37">
+        <v>39</v>
+      </c>
+      <c r="J55" s="43">
+        <v>13</v>
+      </c>
+      <c r="K55" s="66"/>
+      <c r="L55">
+        <v>40</v>
+      </c>
+      <c r="M55">
+        <v>14</v>
+      </c>
+      <c r="N55">
+        <v>600</v>
+      </c>
+      <c r="O55">
+        <v>300</v>
+      </c>
+      <c r="V55" t="s">
+        <v>187</v>
+      </c>
+      <c r="W55" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23">
+      <c r="A56">
+        <v>21</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+      <c r="C56" t="s">
+        <v>104</v>
+      </c>
+      <c r="D56" t="s">
+        <v>118</v>
+      </c>
+      <c r="E56" t="s">
+        <v>118</v>
+      </c>
+      <c r="F56" s="37">
+        <v>44.571428571428569</v>
+      </c>
+      <c r="G56" s="43">
+        <v>2</v>
+      </c>
+      <c r="H56" s="66"/>
+      <c r="I56" s="37">
+        <v>70</v>
+      </c>
+      <c r="J56" s="43">
+        <v>18</v>
+      </c>
+      <c r="K56" s="66"/>
+      <c r="L56">
+        <v>70</v>
+      </c>
+      <c r="M56">
+        <v>19</v>
+      </c>
+      <c r="N56">
+        <v>600</v>
+      </c>
+      <c r="O56">
+        <v>300</v>
+      </c>
+      <c r="V56" t="s">
+        <v>187</v>
+      </c>
+      <c r="W56" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23">
+      <c r="A57">
+        <v>21</v>
+      </c>
+      <c r="B57">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>104</v>
+      </c>
+      <c r="D57" t="s">
+        <v>118</v>
+      </c>
+      <c r="E57" t="s">
+        <v>118</v>
+      </c>
+      <c r="F57" s="37">
+        <v>66</v>
+      </c>
+      <c r="G57" s="43">
+        <v>6</v>
+      </c>
+      <c r="H57" s="66"/>
+      <c r="I57" s="37">
+        <v>110</v>
+      </c>
+      <c r="J57" s="43">
+        <v>24</v>
+      </c>
+      <c r="K57" s="66"/>
+      <c r="L57">
+        <v>110</v>
+      </c>
+      <c r="M57">
+        <v>25</v>
+      </c>
+      <c r="N57">
+        <v>600</v>
+      </c>
+      <c r="O57">
+        <v>300</v>
+      </c>
+      <c r="V57" t="s">
+        <v>187</v>
+      </c>
+      <c r="W57" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23">
+      <c r="A58">
+        <v>21</v>
+      </c>
+      <c r="B58">
+        <v>8</v>
+      </c>
+      <c r="C58" t="s">
+        <v>104</v>
+      </c>
+      <c r="D58" t="s">
+        <v>118</v>
+      </c>
+      <c r="E58" t="s">
+        <v>118</v>
+      </c>
+      <c r="F58" s="37">
+        <v>77.142857142857139</v>
+      </c>
+      <c r="G58" s="43">
+        <v>3</v>
+      </c>
+      <c r="H58" s="66"/>
+      <c r="I58" s="37">
+        <v>118</v>
+      </c>
+      <c r="J58" s="43">
+        <v>16</v>
+      </c>
+      <c r="K58" s="66"/>
+      <c r="L58">
+        <v>120</v>
+      </c>
+      <c r="M58">
+        <v>17</v>
+      </c>
+      <c r="N58">
+        <v>600</v>
+      </c>
+      <c r="O58">
+        <v>300</v>
+      </c>
+      <c r="V58" t="s">
+        <v>187</v>
+      </c>
+      <c r="W58" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23">
+      <c r="A59">
+        <v>22</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>104</v>
+      </c>
+      <c r="D59" t="s">
+        <v>118</v>
+      </c>
+      <c r="E59" t="s">
+        <v>118</v>
+      </c>
+      <c r="F59">
+        <v>350</v>
+      </c>
+      <c r="G59" s="43">
+        <v>4</v>
+      </c>
+      <c r="H59" s="66"/>
+      <c r="I59">
+        <v>430</v>
+      </c>
+      <c r="J59" s="43">
+        <v>13</v>
+      </c>
+      <c r="K59" s="66"/>
+      <c r="L59">
+        <v>430</v>
+      </c>
+      <c r="M59">
+        <v>27</v>
+      </c>
+      <c r="N59">
+        <v>1200</v>
+      </c>
+      <c r="O59">
+        <v>300</v>
+      </c>
+      <c r="V59" t="s">
+        <v>187</v>
+      </c>
+      <c r="W59" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23">
+      <c r="A60">
+        <v>22</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>104</v>
+      </c>
+      <c r="D60" t="s">
+        <v>118</v>
+      </c>
+      <c r="E60" t="s">
+        <v>118</v>
+      </c>
+      <c r="F60">
+        <v>490</v>
+      </c>
+      <c r="G60" s="43">
+        <v>2</v>
+      </c>
+      <c r="H60" s="66"/>
+      <c r="I60">
+        <v>700</v>
+      </c>
+      <c r="J60" s="43">
+        <v>18</v>
+      </c>
+      <c r="K60" s="66"/>
+      <c r="L60">
+        <v>700</v>
+      </c>
+      <c r="M60">
+        <v>37</v>
+      </c>
+      <c r="N60">
+        <v>1200</v>
+      </c>
+      <c r="O60">
+        <v>300</v>
+      </c>
+      <c r="V60" t="s">
+        <v>187</v>
+      </c>
+      <c r="W60" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23">
+      <c r="A61">
+        <v>22</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+      <c r="C61" t="s">
+        <v>104</v>
+      </c>
+      <c r="D61" t="s">
+        <v>118</v>
+      </c>
+      <c r="E61" t="s">
+        <v>118</v>
+      </c>
+      <c r="F61">
+        <f>720</f>
+        <v>720</v>
+      </c>
+      <c r="G61" s="43">
+        <v>6</v>
+      </c>
+      <c r="H61" s="66"/>
+      <c r="I61">
+        <v>1390</v>
+      </c>
+      <c r="J61" s="43">
+        <v>24</v>
+      </c>
+      <c r="K61" s="66"/>
+      <c r="L61">
+        <v>1390</v>
+      </c>
+      <c r="M61">
+        <v>49</v>
+      </c>
+      <c r="N61">
+        <v>1200</v>
+      </c>
+      <c r="O61">
+        <v>300</v>
+      </c>
+      <c r="V61" t="s">
+        <v>187</v>
+      </c>
+      <c r="W61" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23">
+      <c r="A62">
+        <v>22</v>
+      </c>
+      <c r="B62">
+        <v>4</v>
+      </c>
+      <c r="C62" t="s">
+        <v>104</v>
+      </c>
+      <c r="D62" t="s">
+        <v>118</v>
+      </c>
+      <c r="E62" t="s">
+        <v>118</v>
+      </c>
+      <c r="F62">
+        <v>840</v>
+      </c>
+      <c r="G62" s="43">
+        <v>3</v>
+      </c>
+      <c r="H62" s="66"/>
+      <c r="I62">
+        <v>1120</v>
+      </c>
+      <c r="J62" s="43">
+        <v>16</v>
+      </c>
+      <c r="K62" s="66"/>
+      <c r="L62">
+        <v>1120</v>
+      </c>
+      <c r="M62">
+        <v>33</v>
+      </c>
+      <c r="N62">
+        <v>1200</v>
+      </c>
+      <c r="O62">
+        <v>300</v>
+      </c>
+      <c r="V62" t="s">
+        <v>187</v>
+      </c>
+      <c r="W62" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23">
+      <c r="A63">
+        <v>22</v>
+      </c>
+      <c r="B63">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>104</v>
+      </c>
+      <c r="D63" t="s">
+        <v>118</v>
+      </c>
+      <c r="E63" t="s">
+        <v>118</v>
+      </c>
+      <c r="F63" s="37">
+        <v>31.714285714285715</v>
+      </c>
+      <c r="G63" s="43">
+        <v>4</v>
+      </c>
+      <c r="H63" s="66"/>
+      <c r="I63" s="37">
+        <v>39</v>
+      </c>
+      <c r="J63" s="43">
+        <v>13</v>
+      </c>
+      <c r="K63" s="66"/>
+      <c r="L63">
+        <v>40</v>
+      </c>
+      <c r="M63">
+        <v>27</v>
+      </c>
+      <c r="N63">
+        <v>1200</v>
+      </c>
+      <c r="O63">
+        <v>300</v>
+      </c>
+      <c r="V63" t="s">
+        <v>187</v>
+      </c>
+      <c r="W63" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23">
+      <c r="A64">
+        <v>22</v>
+      </c>
+      <c r="B64">
+        <v>6</v>
+      </c>
+      <c r="C64" t="s">
+        <v>104</v>
+      </c>
+      <c r="D64" t="s">
+        <v>118</v>
+      </c>
+      <c r="E64" t="s">
+        <v>118</v>
+      </c>
+      <c r="F64" s="37">
+        <v>44.571428571428569</v>
+      </c>
+      <c r="G64" s="43">
+        <v>2</v>
+      </c>
+      <c r="H64" s="66"/>
+      <c r="I64" s="37">
+        <v>70</v>
+      </c>
+      <c r="J64" s="43">
+        <v>18</v>
+      </c>
+      <c r="K64" s="66"/>
+      <c r="L64">
+        <v>70</v>
+      </c>
+      <c r="M64">
+        <v>37</v>
+      </c>
+      <c r="N64">
+        <v>1200</v>
+      </c>
+      <c r="O64">
+        <v>300</v>
+      </c>
+      <c r="V64" t="s">
+        <v>187</v>
+      </c>
+      <c r="W64" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23">
+      <c r="A65">
+        <v>22</v>
+      </c>
+      <c r="B65">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s">
+        <v>104</v>
+      </c>
+      <c r="D65" t="s">
+        <v>118</v>
+      </c>
+      <c r="E65" t="s">
+        <v>118</v>
+      </c>
+      <c r="F65" s="37">
+        <v>66</v>
+      </c>
+      <c r="G65" s="43">
+        <v>6</v>
+      </c>
+      <c r="H65" s="66"/>
+      <c r="I65" s="37">
+        <v>110</v>
+      </c>
+      <c r="J65" s="43">
+        <v>24</v>
+      </c>
+      <c r="K65" s="66"/>
+      <c r="L65">
+        <v>110</v>
+      </c>
+      <c r="M65">
+        <v>49</v>
+      </c>
+      <c r="N65">
+        <v>1200</v>
+      </c>
+      <c r="O65">
+        <v>300</v>
+      </c>
+      <c r="V65" t="s">
+        <v>187</v>
+      </c>
+      <c r="W65" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23">
+      <c r="A66">
+        <v>22</v>
+      </c>
+      <c r="B66">
+        <v>8</v>
+      </c>
+      <c r="C66" t="s">
+        <v>104</v>
+      </c>
+      <c r="D66" t="s">
+        <v>118</v>
+      </c>
+      <c r="E66" t="s">
+        <v>118</v>
+      </c>
+      <c r="F66" s="37">
+        <v>77.142857142857139</v>
+      </c>
+      <c r="G66" s="43">
+        <v>3</v>
+      </c>
+      <c r="H66" s="66"/>
+      <c r="I66" s="37">
+        <v>118</v>
+      </c>
+      <c r="J66" s="43">
+        <v>16</v>
+      </c>
+      <c r="K66" s="66"/>
+      <c r="L66">
+        <v>120</v>
+      </c>
+      <c r="M66">
+        <v>33</v>
+      </c>
+      <c r="N66">
+        <v>1200</v>
+      </c>
+      <c r="O66">
+        <v>300</v>
+      </c>
+      <c r="V66" t="s">
+        <v>187</v>
+      </c>
+      <c r="W66" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -6760,7 +7412,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6785,7 +7437,7 @@
         <v>92</v>
       </c>
       <c r="G1" s="43" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -6805,7 +7457,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.97757786624641418</v>
+        <v>0.85672864624929124</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -6824,8 +7476,8 @@
       </c>
       <c r="F3" s="66"/>
       <c r="G3">
-        <f t="shared" ref="G3:G5" ca="1" si="0">RAND()</f>
-        <v>0.43045682736051805</v>
+        <f ca="1">RAND()</f>
+        <v>7.1221422827264957E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6845,8 +7497,8 @@
       </c>
       <c r="F4" s="66"/>
       <c r="G4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.12566478391209812</v>
+        <f ca="1">RAND()</f>
+        <v>3.3321846748652795E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6865,8 +7517,8 @@
       </c>
       <c r="F5" s="66"/>
       <c r="G5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.53141155750190505</v>
+        <f ca="1">RAND()</f>
+        <v>0.10258517007342238</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -6942,8 +7594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F6B51D-A4A1-6D46-8F47-1EE4F323E4DF}">
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6957,7 +7609,7 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:24">
@@ -6965,48 +7617,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="69" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="68" t="s">
+      <c r="D3" s="70"/>
+      <c r="E3" s="69" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="69"/>
-      <c r="G3" s="68" t="s">
+      <c r="F3" s="70"/>
+      <c r="G3" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="69"/>
-      <c r="I3" s="68" t="s">
+      <c r="H3" s="70"/>
+      <c r="I3" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="69"/>
+      <c r="J3" s="70"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="70" t="s">
+      <c r="M3" s="71" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="71"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="70" t="s">
+      <c r="N3" s="72"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="71" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="72"/>
-      <c r="S3" s="70" t="s">
+      <c r="Q3" s="72"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="71"/>
-      <c r="U3" s="71"/>
-      <c r="V3" s="73" t="s">
+      <c r="T3" s="72"/>
+      <c r="U3" s="72"/>
+      <c r="V3" s="74" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="73"/>
-      <c r="X3" s="73"/>
+      <c r="W3" s="74"/>
+      <c r="X3" s="74"/>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="50"/>
@@ -7823,34 +8475,34 @@
     </row>
     <row r="28" spans="1:24">
       <c r="B28" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C28" s="2">
         <v>148</v>
       </c>
       <c r="D28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="C29" s="74" t="s">
+      <c r="C29" s="68" t="s">
+        <v>167</v>
+      </c>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68" t="s">
         <v>169</v>
       </c>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74" t="s">
-        <v>171</v>
-      </c>
-      <c r="G29" s="74"/>
-      <c r="H29" s="74"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
       <c r="J29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M29"/>
     </row>
     <row r="30" spans="1:24">
       <c r="B30" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C30" t="s">
         <v>146</v>
@@ -7859,7 +8511,7 @@
         <v>147</v>
       </c>
       <c r="E30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F30" t="s">
         <v>146</v>
@@ -7868,10 +8520,10 @@
         <v>147</v>
       </c>
       <c r="H30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I30" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J30" t="s">
         <v>146</v>
@@ -7886,19 +8538,19 @@
         <v>147</v>
       </c>
       <c r="N30" t="s">
+        <v>172</v>
+      </c>
+      <c r="O30" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="P30" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q30" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="R30" s="37" t="s">
         <v>174</v>
-      </c>
-      <c r="O30" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="P30" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q30" s="37" t="s">
-        <v>175</v>
-      </c>
-      <c r="R30" s="37" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:24">
@@ -7952,7 +8604,7 @@
         <v>13</v>
       </c>
       <c r="Q31" s="37">
-        <f>K31/$C$28</f>
+        <f t="shared" ref="Q31:Q42" si="0">K31/$C$28</f>
         <v>2.3648648648648649</v>
       </c>
       <c r="R31" s="37">
@@ -7973,7 +8625,7 @@
         <v>740</v>
       </c>
       <c r="E32">
-        <f t="shared" ref="E32:E34" si="0">D32-C32</f>
+        <f>D32-C32</f>
         <v>220</v>
       </c>
       <c r="F32" s="37">
@@ -7999,7 +8651,7 @@
         <v>700</v>
       </c>
       <c r="N32" s="37">
-        <f t="shared" ref="N32:N34" si="1">M32-L32</f>
+        <f>M32-L32</f>
         <v>3.75</v>
       </c>
       <c r="O32" s="8">
@@ -8011,7 +8663,7 @@
         <v>18</v>
       </c>
       <c r="Q32" s="37">
-        <f>K32/$C$28</f>
+        <f t="shared" si="0"/>
         <v>3.310810810810811</v>
       </c>
       <c r="R32" s="37">
@@ -8032,7 +8684,7 @@
         <v>1480</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
+        <f>D33-C33</f>
         <v>710</v>
       </c>
       <c r="F33" s="37">
@@ -8059,7 +8711,7 @@
         <v>1390</v>
       </c>
       <c r="N33" s="37">
-        <f t="shared" si="1"/>
+        <f>M33-L33</f>
         <v>4.375</v>
       </c>
       <c r="O33" s="8">
@@ -8071,7 +8723,7 @@
         <v>36</v>
       </c>
       <c r="Q33" s="37">
-        <f>K33/$C$28</f>
+        <f t="shared" si="0"/>
         <v>4.8648648648648649</v>
       </c>
       <c r="R33" s="37">
@@ -8092,7 +8744,7 @@
         <v>1200</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
+        <f>D34-C34</f>
         <v>300</v>
       </c>
       <c r="F34" s="37">
@@ -8118,7 +8770,7 @@
         <v>1120</v>
       </c>
       <c r="N34" s="37">
-        <f t="shared" si="1"/>
+        <f>M34-L34</f>
         <v>-1.25</v>
       </c>
       <c r="O34" s="8">
@@ -8130,7 +8782,7 @@
         <v>16</v>
       </c>
       <c r="Q34" s="37">
-        <f>K34/$C$28</f>
+        <f t="shared" si="0"/>
         <v>5.6756756756756754</v>
       </c>
       <c r="R34" s="37">
@@ -8167,7 +8819,7 @@
         <v>13</v>
       </c>
       <c r="Q35" s="11">
-        <f>K35/$C$28</f>
+        <f t="shared" si="0"/>
         <v>78.378378378378372</v>
       </c>
       <c r="R35" s="11">
@@ -8203,7 +8855,7 @@
         <v>18</v>
       </c>
       <c r="Q36" s="11">
-        <f t="shared" ref="Q36:Q38" si="2">K36/$C$28</f>
+        <f t="shared" si="0"/>
         <v>110.13513513513513</v>
       </c>
       <c r="R36" s="11">
@@ -8239,7 +8891,7 @@
         <v>36</v>
       </c>
       <c r="Q37" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>162.16216216216216</v>
       </c>
       <c r="R37" s="11">
@@ -8275,7 +8927,7 @@
         <v>16</v>
       </c>
       <c r="Q38" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>189.18918918918919</v>
       </c>
       <c r="R38" s="11">
@@ -8319,7 +8971,7 @@
         <v>13</v>
       </c>
       <c r="Q39" s="11">
-        <f>K39/$C$28</f>
+        <f t="shared" si="0"/>
         <v>0.21621621621621623</v>
       </c>
       <c r="R39" s="11">
@@ -8364,7 +9016,7 @@
         <v>18</v>
       </c>
       <c r="Q40" s="11">
-        <f>K40/$C$28</f>
+        <f t="shared" si="0"/>
         <v>0.30405405405405406</v>
       </c>
       <c r="R40" s="11">
@@ -8408,7 +9060,7 @@
         <v>23</v>
       </c>
       <c r="Q41" s="11">
-        <f>K41/$C$28</f>
+        <f t="shared" si="0"/>
         <v>0.44594594594594594</v>
       </c>
       <c r="R41" s="11">
@@ -8452,7 +9104,7 @@
         <v>16</v>
       </c>
       <c r="Q42" s="11">
-        <f>K42/$C$28</f>
+        <f t="shared" si="0"/>
         <v>0.52027027027027029</v>
       </c>
       <c r="R42" s="11">
@@ -8462,16 +9114,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8508,105 +9160,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="75" t="s">
+      <c r="A2" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="75" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="76"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="84" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="82"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="90" t="s">
+      <c r="I2" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="90" t="s">
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="90"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="84" t="s">
+      <c r="S2" s="93"/>
+      <c r="T2" s="93"/>
+      <c r="U2" s="93"/>
+      <c r="V2" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="84" t="s">
+      <c r="W2" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="92" t="s">
+      <c r="X2" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="92" t="s">
+      <c r="Y2" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="92" t="s">
+      <c r="Z2" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="92" t="s">
+      <c r="AA2" s="75" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="82"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="91" t="s">
+      <c r="A3" s="88"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89" t="s">
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89" t="s">
+      <c r="M3" s="92"/>
+      <c r="N3" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89" t="s">
+      <c r="O3" s="92"/>
+      <c r="P3" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="87" t="s">
+      <c r="Q3" s="92"/>
+      <c r="R3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="87" t="s">
+      <c r="S3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="87" t="s">
+      <c r="T3" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="87" t="s">
+      <c r="U3" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="85"/>
-      <c r="W3" s="85"/>
-      <c r="X3" s="93"/>
-      <c r="Y3" s="93"/>
-      <c r="Z3" s="93"/>
-      <c r="AA3" s="93"/>
+      <c r="V3" s="79"/>
+      <c r="W3" s="79"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="76"/>
+      <c r="Z3" s="76"/>
+      <c r="AA3" s="76"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="83"/>
+      <c r="A4" s="89"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -8625,7 +9277,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="86"/>
+      <c r="H4" s="80"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -8653,16 +9305,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="86"/>
-      <c r="X4" s="94"/>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="94"/>
-      <c r="AA4" s="93"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="80"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="77"/>
+      <c r="Z4" s="77"/>
+      <c r="AA4" s="76"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -9163,11 +9815,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -9183,6 +9830,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -9574,19 +10226,19 @@
         <v>54</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" ref="D16:D18" si="4">AVERAGE(A16:B16)/365</f>
+        <f>AVERAGE(A16:B16)/365</f>
         <v>102.73835616438356</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" ref="E16:E18" si="5">3.3*D16</f>
+        <f>3.3*D16</f>
         <v>339.03657534246571</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" ref="F16:F18" si="6">16.7*D16</f>
+        <f>16.7*D16</f>
         <v>1715.7305479452054</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" ref="G16:G18" si="7">33.3*D16</f>
+        <f>33.3*D16</f>
         <v>3421.1872602739722</v>
       </c>
     </row>
@@ -9601,19 +10253,19 @@
         <v>54</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(A17:B17)/365</f>
         <v>171.23150684931508</v>
       </c>
       <c r="E17" s="4">
-        <f t="shared" si="5"/>
+        <f>3.3*D17</f>
         <v>565.0639726027398</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" si="6"/>
+        <f>16.7*D17</f>
         <v>2859.566164383562</v>
       </c>
       <c r="G17" s="4">
-        <f t="shared" si="7"/>
+        <f>33.3*D17</f>
         <v>5702.0091780821913</v>
       </c>
       <c r="H17" t="s">
@@ -9631,19 +10283,19 @@
         <v>54</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(A18:B18)/365</f>
         <v>239.72465753424657</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="5"/>
+        <f>3.3*D18</f>
         <v>791.09136986301371</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="6"/>
+        <f>16.7*D18</f>
         <v>4003.4017808219178</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="7"/>
+        <f>33.3*D18</f>
         <v>7982.8310958904103</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added capturing user agent string
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4D59FFA-5CED-9B4A-948C-83646D99120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C8A9CA-A2EF-D54D-872E-DBF3FCBB57B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
-    <sheet name="MCL questions prod" sheetId="10" r:id="rId1"/>
-    <sheet name="Web Parameters Dev" sheetId="8" r:id="rId2"/>
-    <sheet name="Web Parameters Random" sheetId="11" r:id="rId3"/>
-    <sheet name="Date Delay Paper" sheetId="9" r:id="rId4"/>
-    <sheet name="MCL" sheetId="2" r:id="rId5"/>
-    <sheet name="CL LL Amounts" sheetId="3" r:id="rId6"/>
-    <sheet name="Holden et al." sheetId="4" r:id="rId7"/>
-    <sheet name="Screen Size Zooming" sheetId="5" r:id="rId8"/>
-    <sheet name="Worker Rate" sheetId="7" r:id="rId9"/>
-    <sheet name="Web Parameters v1" sheetId="1" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
+    <sheet name="MCL questions prod" sheetId="10" r:id="rId2"/>
+    <sheet name="Web Parameters Dev" sheetId="8" r:id="rId3"/>
+    <sheet name="Web Parameters Random" sheetId="11" r:id="rId4"/>
+    <sheet name="Date Delay Paper" sheetId="9" r:id="rId5"/>
+    <sheet name="MCL" sheetId="2" r:id="rId6"/>
+    <sheet name="CL LL Amounts" sheetId="3" r:id="rId7"/>
+    <sheet name="Holden et al." sheetId="4" r:id="rId8"/>
+    <sheet name="Screen Size Zooming" sheetId="5" r:id="rId9"/>
+    <sheet name="Worker Rate" sheetId="7" r:id="rId10"/>
+    <sheet name="Web Parameters v1" sheetId="1" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="194">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -649,6 +649,13 @@
   </si>
   <si>
     <t>show_minor_ticks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title: Choices about money.
+</t>
+  </si>
+  <si>
+    <t>Description: The purpose of this research is to get a better understanding of how people make choices about money.  You will be asked some background information about yourself and then presented with a series of questions to make choices about when to receive money of different amounts.  There are two short surveys at the end.  The survey should take no longer than 10 minutes to complete and is designed to be performed on a computer screen and not a mobile devices.</t>
   </si>
 </sst>
 </file>
@@ -894,7 +901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -983,9 +990,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1004,23 +1008,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1050,6 +1039,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1064,6 +1062,16 @@
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1377,1191 +1385,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6462F7B1-F956-1241-A84D-BB94A5075354}">
-  <dimension ref="A1:W25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A1C2A0-9A4B-1A4B-A6D5-91595022903D}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V1" sqref="V1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11" style="36"/>
-    <col min="9" max="9" width="19.1640625" customWidth="1"/>
-    <col min="11" max="11" width="11" style="36"/>
-    <col min="14" max="14" width="19.5" customWidth="1"/>
-    <col min="15" max="15" width="24.5" customWidth="1"/>
-    <col min="16" max="16" width="19.1640625" customWidth="1"/>
-    <col min="17" max="17" width="22.83203125" customWidth="1"/>
-    <col min="18" max="18" width="14.5" customWidth="1"/>
-    <col min="19" max="19" width="14.83203125" customWidth="1"/>
-    <col min="20" max="20" width="13.1640625" customWidth="1"/>
-    <col min="21" max="22" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="95"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
-      <c r="A1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" s="66" t="s">
-        <v>89</v>
-      </c>
-      <c r="I1" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="J1" s="43" t="s">
-        <v>91</v>
-      </c>
-      <c r="K1" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="L1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M1" t="s">
-        <v>94</v>
-      </c>
-      <c r="N1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O1" t="s">
-        <v>96</v>
-      </c>
-      <c r="P1" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>98</v>
-      </c>
-      <c r="R1" t="s">
-        <v>99</v>
-      </c>
-      <c r="S1" t="s">
-        <v>100</v>
-      </c>
-      <c r="T1" t="s">
-        <v>101</v>
-      </c>
-      <c r="U1" t="s">
-        <v>102</v>
-      </c>
-      <c r="V1" t="s">
-        <v>191</v>
-      </c>
-      <c r="W1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F2">
-        <v>350</v>
-      </c>
-      <c r="G2" s="43">
-        <v>4</v>
-      </c>
-      <c r="H2" s="66"/>
-      <c r="I2">
-        <v>430</v>
-      </c>
-      <c r="J2" s="43">
-        <v>13</v>
-      </c>
-      <c r="K2" s="66"/>
-      <c r="L2">
-        <v>430</v>
-      </c>
-      <c r="W2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F3">
-        <v>490</v>
-      </c>
-      <c r="G3" s="43">
-        <v>2</v>
-      </c>
-      <c r="H3" s="66"/>
-      <c r="I3">
-        <v>700</v>
-      </c>
-      <c r="J3" s="43">
-        <v>18</v>
-      </c>
-      <c r="K3" s="66"/>
-      <c r="L3">
-        <v>700</v>
-      </c>
-      <c r="W3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F4">
-        <f>720</f>
-        <v>720</v>
-      </c>
-      <c r="G4" s="43">
-        <v>6</v>
-      </c>
-      <c r="H4" s="66"/>
-      <c r="I4">
-        <v>1390</v>
-      </c>
-      <c r="J4" s="43">
-        <v>24</v>
-      </c>
-      <c r="K4" s="66"/>
-      <c r="L4">
-        <v>1390</v>
-      </c>
-      <c r="W4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" t="s">
-        <v>118</v>
-      </c>
-      <c r="F5">
-        <v>840</v>
-      </c>
-      <c r="G5" s="43">
-        <v>3</v>
-      </c>
-      <c r="H5" s="66"/>
-      <c r="I5">
-        <v>1120</v>
-      </c>
-      <c r="J5" s="43">
-        <v>16</v>
-      </c>
-      <c r="K5" s="66"/>
-      <c r="L5">
-        <v>1120</v>
-      </c>
-      <c r="W5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6" t="s">
-        <v>118</v>
-      </c>
-      <c r="E6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F6" s="37">
-        <v>31.714285714285715</v>
-      </c>
-      <c r="G6" s="43">
-        <v>4</v>
-      </c>
-      <c r="H6" s="66"/>
-      <c r="I6" s="37">
-        <v>39</v>
-      </c>
-      <c r="J6" s="43">
-        <v>13</v>
-      </c>
-      <c r="K6" s="66"/>
-      <c r="L6">
-        <v>40</v>
-      </c>
-      <c r="W6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F7" s="37">
-        <v>44.571428571428569</v>
-      </c>
-      <c r="G7" s="43">
-        <v>2</v>
-      </c>
-      <c r="H7" s="66"/>
-      <c r="I7" s="37">
-        <v>70</v>
-      </c>
-      <c r="J7" s="43">
-        <v>18</v>
-      </c>
-      <c r="K7" s="66"/>
-      <c r="L7">
-        <v>70</v>
-      </c>
-      <c r="W7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" t="s">
-        <v>118</v>
-      </c>
-      <c r="E8" t="s">
-        <v>118</v>
-      </c>
-      <c r="F8" s="37">
-        <v>66</v>
-      </c>
-      <c r="G8" s="43">
-        <v>6</v>
-      </c>
-      <c r="H8" s="66"/>
-      <c r="I8" s="37">
-        <v>110</v>
-      </c>
-      <c r="J8" s="43">
-        <v>24</v>
-      </c>
-      <c r="K8" s="66"/>
-      <c r="L8">
-        <v>110</v>
-      </c>
-      <c r="W8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E9" t="s">
-        <v>118</v>
-      </c>
-      <c r="F9" s="37">
-        <v>77.142857142857139</v>
-      </c>
-      <c r="G9" s="43">
-        <v>3</v>
-      </c>
-      <c r="H9" s="66"/>
-      <c r="I9" s="37">
-        <v>118</v>
-      </c>
-      <c r="J9" s="43">
-        <v>16</v>
-      </c>
-      <c r="K9" s="66"/>
-      <c r="L9">
-        <v>120</v>
-      </c>
-      <c r="N9">
-        <v>600</v>
-      </c>
-      <c r="O9">
-        <v>300</v>
-      </c>
-      <c r="W9" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" t="s">
-        <v>118</v>
-      </c>
-      <c r="E10" t="s">
-        <v>118</v>
-      </c>
-      <c r="F10">
-        <v>350</v>
-      </c>
-      <c r="G10" s="43">
-        <v>4</v>
-      </c>
-      <c r="H10" s="66"/>
-      <c r="I10">
-        <v>430</v>
-      </c>
-      <c r="J10" s="43">
-        <v>13</v>
-      </c>
-      <c r="K10" s="66"/>
-      <c r="L10">
-        <v>430</v>
-      </c>
-      <c r="M10">
-        <v>14</v>
-      </c>
-      <c r="N10">
-        <v>600</v>
-      </c>
-      <c r="O10">
-        <v>300</v>
-      </c>
-      <c r="V10" t="s">
-        <v>187</v>
-      </c>
-      <c r="W10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" t="s">
-        <v>118</v>
-      </c>
-      <c r="E11" t="s">
-        <v>118</v>
-      </c>
-      <c r="F11">
-        <v>490</v>
-      </c>
-      <c r="G11" s="43">
-        <v>2</v>
-      </c>
-      <c r="H11" s="66"/>
-      <c r="I11">
-        <v>700</v>
-      </c>
-      <c r="J11" s="43">
-        <v>18</v>
-      </c>
-      <c r="K11" s="66"/>
-      <c r="L11">
-        <v>700</v>
-      </c>
-      <c r="M11">
-        <v>19</v>
-      </c>
-      <c r="N11">
-        <v>600</v>
-      </c>
-      <c r="O11">
-        <v>300</v>
-      </c>
-      <c r="V11" t="s">
-        <v>187</v>
-      </c>
-      <c r="W11" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D12" t="s">
-        <v>118</v>
-      </c>
-      <c r="E12" t="s">
-        <v>118</v>
-      </c>
-      <c r="F12">
-        <f>720</f>
-        <v>720</v>
-      </c>
-      <c r="G12" s="43">
-        <v>6</v>
-      </c>
-      <c r="H12" s="66"/>
-      <c r="I12">
-        <v>1390</v>
-      </c>
-      <c r="J12" s="43">
-        <v>24</v>
-      </c>
-      <c r="K12" s="66"/>
-      <c r="L12">
-        <v>1390</v>
-      </c>
-      <c r="M12">
-        <v>25</v>
-      </c>
-      <c r="N12">
-        <v>600</v>
-      </c>
-      <c r="O12">
-        <v>300</v>
-      </c>
-      <c r="V12" t="s">
-        <v>187</v>
-      </c>
-      <c r="W12" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>104</v>
-      </c>
-      <c r="D13" t="s">
-        <v>118</v>
-      </c>
-      <c r="E13" t="s">
-        <v>118</v>
-      </c>
-      <c r="F13">
-        <v>840</v>
-      </c>
-      <c r="G13" s="43">
-        <v>3</v>
-      </c>
-      <c r="H13" s="66"/>
-      <c r="I13">
-        <v>1120</v>
-      </c>
-      <c r="J13" s="43">
-        <v>16</v>
-      </c>
-      <c r="K13" s="66"/>
-      <c r="L13">
-        <v>1120</v>
-      </c>
-      <c r="M13">
-        <v>17</v>
-      </c>
-      <c r="N13">
-        <v>600</v>
-      </c>
-      <c r="O13">
-        <v>300</v>
-      </c>
-      <c r="V13" t="s">
-        <v>187</v>
-      </c>
-      <c r="W13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D14" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" t="s">
-        <v>118</v>
-      </c>
-      <c r="F14" s="37">
-        <v>31.714285714285715</v>
-      </c>
-      <c r="G14" s="43">
-        <v>4</v>
-      </c>
-      <c r="H14" s="66"/>
-      <c r="I14" s="37">
-        <v>39</v>
-      </c>
-      <c r="J14" s="43">
-        <v>13</v>
-      </c>
-      <c r="K14" s="66"/>
-      <c r="L14">
-        <v>40</v>
-      </c>
-      <c r="M14">
-        <v>14</v>
-      </c>
-      <c r="N14">
-        <v>600</v>
-      </c>
-      <c r="O14">
-        <v>300</v>
-      </c>
-      <c r="V14" t="s">
-        <v>187</v>
-      </c>
-      <c r="W14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>104</v>
-      </c>
-      <c r="D15" t="s">
-        <v>118</v>
-      </c>
-      <c r="E15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F15" s="37">
-        <v>44.571428571428569</v>
-      </c>
-      <c r="G15" s="43">
-        <v>2</v>
-      </c>
-      <c r="H15" s="66"/>
-      <c r="I15" s="37">
-        <v>70</v>
-      </c>
-      <c r="J15" s="43">
-        <v>18</v>
-      </c>
-      <c r="K15" s="66"/>
-      <c r="L15">
-        <v>70</v>
-      </c>
-      <c r="M15">
-        <v>19</v>
-      </c>
-      <c r="N15">
-        <v>600</v>
-      </c>
-      <c r="O15">
-        <v>300</v>
-      </c>
-      <c r="V15" t="s">
-        <v>187</v>
-      </c>
-      <c r="W15" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" t="s">
-        <v>118</v>
-      </c>
-      <c r="E16" t="s">
-        <v>118</v>
-      </c>
-      <c r="F16" s="37">
-        <v>66</v>
-      </c>
-      <c r="G16" s="43">
-        <v>6</v>
-      </c>
-      <c r="H16" s="66"/>
-      <c r="I16" s="37">
-        <v>110</v>
-      </c>
-      <c r="J16" s="43">
-        <v>24</v>
-      </c>
-      <c r="K16" s="66"/>
-      <c r="L16">
-        <v>110</v>
-      </c>
-      <c r="M16">
-        <v>25</v>
-      </c>
-      <c r="N16">
-        <v>600</v>
-      </c>
-      <c r="O16">
-        <v>300</v>
-      </c>
-      <c r="V16" t="s">
-        <v>187</v>
-      </c>
-      <c r="W16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23">
-      <c r="A17">
-        <v>2</v>
-      </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>104</v>
-      </c>
-      <c r="D17" t="s">
-        <v>118</v>
-      </c>
-      <c r="E17" t="s">
-        <v>118</v>
-      </c>
-      <c r="F17" s="37">
-        <v>77.142857142857139</v>
-      </c>
-      <c r="G17" s="43">
-        <v>3</v>
-      </c>
-      <c r="H17" s="66"/>
-      <c r="I17" s="37">
-        <v>118</v>
-      </c>
-      <c r="J17" s="43">
-        <v>16</v>
-      </c>
-      <c r="K17" s="66"/>
-      <c r="L17">
-        <v>120</v>
-      </c>
-      <c r="M17">
-        <v>17</v>
-      </c>
-      <c r="N17">
-        <v>600</v>
-      </c>
-      <c r="O17">
-        <v>300</v>
-      </c>
-      <c r="V17" t="s">
-        <v>187</v>
-      </c>
-      <c r="W17" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23">
-      <c r="A18">
-        <v>3</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>104</v>
-      </c>
-      <c r="D18" t="s">
-        <v>118</v>
-      </c>
-      <c r="E18" t="s">
-        <v>118</v>
-      </c>
-      <c r="F18">
-        <v>350</v>
-      </c>
-      <c r="G18" s="43">
-        <v>4</v>
-      </c>
-      <c r="H18" s="66"/>
-      <c r="I18">
-        <v>430</v>
-      </c>
-      <c r="J18" s="43">
-        <v>13</v>
-      </c>
-      <c r="K18" s="66"/>
-      <c r="L18">
-        <v>430</v>
-      </c>
-      <c r="M18">
-        <v>27</v>
-      </c>
-      <c r="N18">
-        <v>1200</v>
-      </c>
-      <c r="O18">
-        <v>300</v>
-      </c>
-      <c r="V18" t="s">
-        <v>187</v>
-      </c>
-      <c r="W18" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23">
-      <c r="A19">
-        <v>3</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D19" t="s">
-        <v>118</v>
-      </c>
-      <c r="E19" t="s">
-        <v>118</v>
-      </c>
-      <c r="F19">
-        <v>490</v>
-      </c>
-      <c r="G19" s="43">
-        <v>2</v>
-      </c>
-      <c r="H19" s="66"/>
-      <c r="I19">
-        <v>700</v>
-      </c>
-      <c r="J19" s="43">
-        <v>18</v>
-      </c>
-      <c r="K19" s="66"/>
-      <c r="L19">
-        <v>700</v>
-      </c>
-      <c r="M19">
-        <v>37</v>
-      </c>
-      <c r="N19">
-        <v>1200</v>
-      </c>
-      <c r="O19">
-        <v>300</v>
-      </c>
-      <c r="V19" t="s">
-        <v>187</v>
-      </c>
-      <c r="W19" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E20" t="s">
-        <v>118</v>
-      </c>
-      <c r="F20">
-        <f>720</f>
-        <v>720</v>
-      </c>
-      <c r="G20" s="43">
-        <v>6</v>
-      </c>
-      <c r="H20" s="66"/>
-      <c r="I20">
-        <v>1390</v>
-      </c>
-      <c r="J20" s="43">
-        <v>24</v>
-      </c>
-      <c r="K20" s="66"/>
-      <c r="L20">
-        <v>1390</v>
-      </c>
-      <c r="M20">
-        <v>49</v>
-      </c>
-      <c r="N20">
-        <v>1200</v>
-      </c>
-      <c r="O20">
-        <v>300</v>
-      </c>
-      <c r="V20" t="s">
-        <v>187</v>
-      </c>
-      <c r="W20" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23">
-      <c r="A21">
-        <v>3</v>
-      </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>104</v>
-      </c>
-      <c r="D21" t="s">
-        <v>118</v>
-      </c>
-      <c r="E21" t="s">
-        <v>118</v>
-      </c>
-      <c r="F21">
-        <v>840</v>
-      </c>
-      <c r="G21" s="43">
-        <v>3</v>
-      </c>
-      <c r="H21" s="66"/>
-      <c r="I21">
-        <v>1120</v>
-      </c>
-      <c r="J21" s="43">
-        <v>16</v>
-      </c>
-      <c r="K21" s="66"/>
-      <c r="L21">
-        <v>1120</v>
-      </c>
-      <c r="M21">
-        <v>33</v>
-      </c>
-      <c r="N21">
-        <v>1200</v>
-      </c>
-      <c r="O21">
-        <v>300</v>
-      </c>
-      <c r="V21" t="s">
-        <v>187</v>
-      </c>
-      <c r="W21" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23">
-      <c r="A22">
-        <v>3</v>
-      </c>
-      <c r="B22">
-        <v>5</v>
-      </c>
-      <c r="C22" t="s">
-        <v>104</v>
-      </c>
-      <c r="D22" t="s">
-        <v>118</v>
-      </c>
-      <c r="E22" t="s">
-        <v>118</v>
-      </c>
-      <c r="F22" s="37">
-        <v>31.714285714285715</v>
-      </c>
-      <c r="G22" s="43">
-        <v>4</v>
-      </c>
-      <c r="H22" s="66"/>
-      <c r="I22" s="37">
-        <v>39</v>
-      </c>
-      <c r="J22" s="43">
-        <v>13</v>
-      </c>
-      <c r="K22" s="66"/>
-      <c r="L22">
-        <v>40</v>
-      </c>
-      <c r="M22">
-        <v>27</v>
-      </c>
-      <c r="N22">
-        <v>1200</v>
-      </c>
-      <c r="O22">
-        <v>300</v>
-      </c>
-      <c r="V22" t="s">
-        <v>187</v>
-      </c>
-      <c r="W22" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
-        <v>104</v>
-      </c>
-      <c r="D23" t="s">
-        <v>118</v>
-      </c>
-      <c r="E23" t="s">
-        <v>118</v>
-      </c>
-      <c r="F23" s="37">
-        <v>44.571428571428569</v>
-      </c>
-      <c r="G23" s="43">
-        <v>2</v>
-      </c>
-      <c r="H23" s="66"/>
-      <c r="I23" s="37">
-        <v>70</v>
-      </c>
-      <c r="J23" s="43">
-        <v>18</v>
-      </c>
-      <c r="K23" s="66"/>
-      <c r="L23">
-        <v>70</v>
-      </c>
-      <c r="M23">
-        <v>37</v>
-      </c>
-      <c r="N23">
-        <v>1200</v>
-      </c>
-      <c r="O23">
-        <v>300</v>
-      </c>
-      <c r="V23" t="s">
-        <v>187</v>
-      </c>
-      <c r="W23" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23">
-      <c r="A24">
-        <v>3</v>
-      </c>
-      <c r="B24">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>104</v>
-      </c>
-      <c r="D24" t="s">
-        <v>118</v>
-      </c>
-      <c r="E24" t="s">
-        <v>118</v>
-      </c>
-      <c r="F24" s="37">
-        <v>66</v>
-      </c>
-      <c r="G24" s="43">
-        <v>6</v>
-      </c>
-      <c r="H24" s="66"/>
-      <c r="I24" s="37">
-        <v>110</v>
-      </c>
-      <c r="J24" s="43">
-        <v>24</v>
-      </c>
-      <c r="K24" s="66"/>
-      <c r="L24">
-        <v>110</v>
-      </c>
-      <c r="M24">
-        <v>49</v>
-      </c>
-      <c r="N24">
-        <v>1200</v>
-      </c>
-      <c r="O24">
-        <v>300</v>
-      </c>
-      <c r="V24" t="s">
-        <v>187</v>
-      </c>
-      <c r="W24" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23">
-      <c r="A25">
-        <v>3</v>
-      </c>
-      <c r="B25">
-        <v>8</v>
-      </c>
-      <c r="C25" t="s">
-        <v>104</v>
-      </c>
-      <c r="D25" t="s">
-        <v>118</v>
-      </c>
-      <c r="E25" t="s">
-        <v>118</v>
-      </c>
-      <c r="F25" s="37">
-        <v>77.142857142857139</v>
-      </c>
-      <c r="G25" s="43">
-        <v>3</v>
-      </c>
-      <c r="H25" s="66"/>
-      <c r="I25" s="37">
-        <v>118</v>
-      </c>
-      <c r="J25" s="43">
-        <v>16</v>
-      </c>
-      <c r="K25" s="66"/>
-      <c r="L25">
-        <v>120</v>
-      </c>
-      <c r="M25">
-        <v>33</v>
-      </c>
-      <c r="N25">
-        <v>1200</v>
-      </c>
-      <c r="O25">
-        <v>300</v>
-      </c>
-      <c r="V25" t="s">
-        <v>187</v>
-      </c>
-      <c r="W25" t="s">
-        <v>185</v>
+    <row r="1" spans="1:1">
+      <c r="A1" s="95" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="95" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2570,6 +1413,71 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CC848A2-46C4-BD4C-AFD2-CF7F6FD4ADEE}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="12">
+        <v>15</v>
+      </c>
+      <c r="C1" s="12">
+        <v>10</v>
+      </c>
+      <c r="D1" s="12">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="12">
+        <f>B1/60</f>
+        <v>0.25</v>
+      </c>
+      <c r="C2" s="12">
+        <f>C1/60</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D2" s="12">
+        <f>D1/60</f>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="12">
+        <f xml:space="preserve"> B2*5</f>
+        <v>1.25</v>
+      </c>
+      <c r="C3" s="12">
+        <f xml:space="preserve"> C2*5</f>
+        <v>0.83333333333333326</v>
+      </c>
+      <c r="D3" s="12">
+        <f xml:space="preserve"> D2*5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86262417-1283-894E-BFF0-F5DD2E135B8D}">
   <dimension ref="A1:V40"/>
   <sheetViews>
@@ -4246,6 +3154,1199 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6462F7B1-F956-1241-A84D-BB94A5075354}">
+  <dimension ref="A1:W25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V1" sqref="V1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11" style="36"/>
+    <col min="9" max="9" width="19.1640625" customWidth="1"/>
+    <col min="11" max="11" width="11" style="36"/>
+    <col min="14" max="14" width="19.5" customWidth="1"/>
+    <col min="15" max="15" width="24.5" customWidth="1"/>
+    <col min="16" max="16" width="19.1640625" customWidth="1"/>
+    <col min="17" max="17" width="22.83203125" customWidth="1"/>
+    <col min="18" max="18" width="14.5" customWidth="1"/>
+    <col min="19" max="19" width="14.83203125" customWidth="1"/>
+    <col min="20" max="20" width="13.1640625" customWidth="1"/>
+    <col min="21" max="22" width="13.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="66" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="K1" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O1" t="s">
+        <v>96</v>
+      </c>
+      <c r="P1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S1" t="s">
+        <v>100</v>
+      </c>
+      <c r="T1" t="s">
+        <v>101</v>
+      </c>
+      <c r="U1" t="s">
+        <v>102</v>
+      </c>
+      <c r="V1" t="s">
+        <v>191</v>
+      </c>
+      <c r="W1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2">
+        <v>350</v>
+      </c>
+      <c r="G2" s="43">
+        <v>4</v>
+      </c>
+      <c r="H2" s="66"/>
+      <c r="I2">
+        <v>430</v>
+      </c>
+      <c r="J2" s="43">
+        <v>13</v>
+      </c>
+      <c r="K2" s="66"/>
+      <c r="L2">
+        <v>430</v>
+      </c>
+      <c r="W2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3">
+        <v>490</v>
+      </c>
+      <c r="G3" s="43">
+        <v>2</v>
+      </c>
+      <c r="H3" s="66"/>
+      <c r="I3">
+        <v>700</v>
+      </c>
+      <c r="J3" s="43">
+        <v>18</v>
+      </c>
+      <c r="K3" s="66"/>
+      <c r="L3">
+        <v>700</v>
+      </c>
+      <c r="W3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4">
+        <f>720</f>
+        <v>720</v>
+      </c>
+      <c r="G4" s="43">
+        <v>6</v>
+      </c>
+      <c r="H4" s="66"/>
+      <c r="I4">
+        <v>1390</v>
+      </c>
+      <c r="J4" s="43">
+        <v>24</v>
+      </c>
+      <c r="K4" s="66"/>
+      <c r="L4">
+        <v>1390</v>
+      </c>
+      <c r="W4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5">
+        <v>840</v>
+      </c>
+      <c r="G5" s="43">
+        <v>3</v>
+      </c>
+      <c r="H5" s="66"/>
+      <c r="I5">
+        <v>1120</v>
+      </c>
+      <c r="J5" s="43">
+        <v>16</v>
+      </c>
+      <c r="K5" s="66"/>
+      <c r="L5">
+        <v>1120</v>
+      </c>
+      <c r="W5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6" s="37">
+        <v>31.714285714285715</v>
+      </c>
+      <c r="G6" s="43">
+        <v>4</v>
+      </c>
+      <c r="H6" s="66"/>
+      <c r="I6" s="37">
+        <v>39</v>
+      </c>
+      <c r="J6" s="43">
+        <v>13</v>
+      </c>
+      <c r="K6" s="66"/>
+      <c r="L6">
+        <v>40</v>
+      </c>
+      <c r="W6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" s="37">
+        <v>44.571428571428569</v>
+      </c>
+      <c r="G7" s="43">
+        <v>2</v>
+      </c>
+      <c r="H7" s="66"/>
+      <c r="I7" s="37">
+        <v>70</v>
+      </c>
+      <c r="J7" s="43">
+        <v>18</v>
+      </c>
+      <c r="K7" s="66"/>
+      <c r="L7">
+        <v>70</v>
+      </c>
+      <c r="W7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="37">
+        <v>66</v>
+      </c>
+      <c r="G8" s="43">
+        <v>6</v>
+      </c>
+      <c r="H8" s="66"/>
+      <c r="I8" s="37">
+        <v>110</v>
+      </c>
+      <c r="J8" s="43">
+        <v>24</v>
+      </c>
+      <c r="K8" s="66"/>
+      <c r="L8">
+        <v>110</v>
+      </c>
+      <c r="W8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" s="37">
+        <v>77.142857142857139</v>
+      </c>
+      <c r="G9" s="43">
+        <v>3</v>
+      </c>
+      <c r="H9" s="66"/>
+      <c r="I9" s="37">
+        <v>118</v>
+      </c>
+      <c r="J9" s="43">
+        <v>16</v>
+      </c>
+      <c r="K9" s="66"/>
+      <c r="L9">
+        <v>120</v>
+      </c>
+      <c r="N9">
+        <v>600</v>
+      </c>
+      <c r="O9">
+        <v>300</v>
+      </c>
+      <c r="W9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10">
+        <v>350</v>
+      </c>
+      <c r="G10" s="43">
+        <v>4</v>
+      </c>
+      <c r="H10" s="66"/>
+      <c r="I10">
+        <v>430</v>
+      </c>
+      <c r="J10" s="43">
+        <v>13</v>
+      </c>
+      <c r="K10" s="66"/>
+      <c r="L10">
+        <v>430</v>
+      </c>
+      <c r="M10">
+        <v>14</v>
+      </c>
+      <c r="N10">
+        <v>600</v>
+      </c>
+      <c r="O10">
+        <v>300</v>
+      </c>
+      <c r="V10" t="s">
+        <v>187</v>
+      </c>
+      <c r="W10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11">
+        <v>490</v>
+      </c>
+      <c r="G11" s="43">
+        <v>2</v>
+      </c>
+      <c r="H11" s="66"/>
+      <c r="I11">
+        <v>700</v>
+      </c>
+      <c r="J11" s="43">
+        <v>18</v>
+      </c>
+      <c r="K11" s="66"/>
+      <c r="L11">
+        <v>700</v>
+      </c>
+      <c r="M11">
+        <v>19</v>
+      </c>
+      <c r="N11">
+        <v>600</v>
+      </c>
+      <c r="O11">
+        <v>300</v>
+      </c>
+      <c r="V11" t="s">
+        <v>187</v>
+      </c>
+      <c r="W11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12">
+        <f>720</f>
+        <v>720</v>
+      </c>
+      <c r="G12" s="43">
+        <v>6</v>
+      </c>
+      <c r="H12" s="66"/>
+      <c r="I12">
+        <v>1390</v>
+      </c>
+      <c r="J12" s="43">
+        <v>24</v>
+      </c>
+      <c r="K12" s="66"/>
+      <c r="L12">
+        <v>1390</v>
+      </c>
+      <c r="M12">
+        <v>25</v>
+      </c>
+      <c r="N12">
+        <v>600</v>
+      </c>
+      <c r="O12">
+        <v>300</v>
+      </c>
+      <c r="V12" t="s">
+        <v>187</v>
+      </c>
+      <c r="W12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13">
+        <v>840</v>
+      </c>
+      <c r="G13" s="43">
+        <v>3</v>
+      </c>
+      <c r="H13" s="66"/>
+      <c r="I13">
+        <v>1120</v>
+      </c>
+      <c r="J13" s="43">
+        <v>16</v>
+      </c>
+      <c r="K13" s="66"/>
+      <c r="L13">
+        <v>1120</v>
+      </c>
+      <c r="M13">
+        <v>17</v>
+      </c>
+      <c r="N13">
+        <v>600</v>
+      </c>
+      <c r="O13">
+        <v>300</v>
+      </c>
+      <c r="V13" t="s">
+        <v>187</v>
+      </c>
+      <c r="W13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" s="37">
+        <v>31.714285714285715</v>
+      </c>
+      <c r="G14" s="43">
+        <v>4</v>
+      </c>
+      <c r="H14" s="66"/>
+      <c r="I14" s="37">
+        <v>39</v>
+      </c>
+      <c r="J14" s="43">
+        <v>13</v>
+      </c>
+      <c r="K14" s="66"/>
+      <c r="L14">
+        <v>40</v>
+      </c>
+      <c r="M14">
+        <v>14</v>
+      </c>
+      <c r="N14">
+        <v>600</v>
+      </c>
+      <c r="O14">
+        <v>300</v>
+      </c>
+      <c r="V14" t="s">
+        <v>187</v>
+      </c>
+      <c r="W14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F15" s="37">
+        <v>44.571428571428569</v>
+      </c>
+      <c r="G15" s="43">
+        <v>2</v>
+      </c>
+      <c r="H15" s="66"/>
+      <c r="I15" s="37">
+        <v>70</v>
+      </c>
+      <c r="J15" s="43">
+        <v>18</v>
+      </c>
+      <c r="K15" s="66"/>
+      <c r="L15">
+        <v>70</v>
+      </c>
+      <c r="M15">
+        <v>19</v>
+      </c>
+      <c r="N15">
+        <v>600</v>
+      </c>
+      <c r="O15">
+        <v>300</v>
+      </c>
+      <c r="V15" t="s">
+        <v>187</v>
+      </c>
+      <c r="W15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F16" s="37">
+        <v>66</v>
+      </c>
+      <c r="G16" s="43">
+        <v>6</v>
+      </c>
+      <c r="H16" s="66"/>
+      <c r="I16" s="37">
+        <v>110</v>
+      </c>
+      <c r="J16" s="43">
+        <v>24</v>
+      </c>
+      <c r="K16" s="66"/>
+      <c r="L16">
+        <v>110</v>
+      </c>
+      <c r="M16">
+        <v>25</v>
+      </c>
+      <c r="N16">
+        <v>600</v>
+      </c>
+      <c r="O16">
+        <v>300</v>
+      </c>
+      <c r="V16" t="s">
+        <v>187</v>
+      </c>
+      <c r="W16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" s="37">
+        <v>77.142857142857139</v>
+      </c>
+      <c r="G17" s="43">
+        <v>3</v>
+      </c>
+      <c r="H17" s="66"/>
+      <c r="I17" s="37">
+        <v>118</v>
+      </c>
+      <c r="J17" s="43">
+        <v>16</v>
+      </c>
+      <c r="K17" s="66"/>
+      <c r="L17">
+        <v>120</v>
+      </c>
+      <c r="M17">
+        <v>17</v>
+      </c>
+      <c r="N17">
+        <v>600</v>
+      </c>
+      <c r="O17">
+        <v>300</v>
+      </c>
+      <c r="V17" t="s">
+        <v>187</v>
+      </c>
+      <c r="W17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18">
+        <v>350</v>
+      </c>
+      <c r="G18" s="43">
+        <v>4</v>
+      </c>
+      <c r="H18" s="66"/>
+      <c r="I18">
+        <v>430</v>
+      </c>
+      <c r="J18" s="43">
+        <v>13</v>
+      </c>
+      <c r="K18" s="66"/>
+      <c r="L18">
+        <v>430</v>
+      </c>
+      <c r="M18">
+        <v>27</v>
+      </c>
+      <c r="N18">
+        <v>1200</v>
+      </c>
+      <c r="O18">
+        <v>300</v>
+      </c>
+      <c r="V18" t="s">
+        <v>187</v>
+      </c>
+      <c r="W18" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19">
+        <v>490</v>
+      </c>
+      <c r="G19" s="43">
+        <v>2</v>
+      </c>
+      <c r="H19" s="66"/>
+      <c r="I19">
+        <v>700</v>
+      </c>
+      <c r="J19" s="43">
+        <v>18</v>
+      </c>
+      <c r="K19" s="66"/>
+      <c r="L19">
+        <v>700</v>
+      </c>
+      <c r="M19">
+        <v>37</v>
+      </c>
+      <c r="N19">
+        <v>1200</v>
+      </c>
+      <c r="O19">
+        <v>300</v>
+      </c>
+      <c r="V19" t="s">
+        <v>187</v>
+      </c>
+      <c r="W19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F20">
+        <f>720</f>
+        <v>720</v>
+      </c>
+      <c r="G20" s="43">
+        <v>6</v>
+      </c>
+      <c r="H20" s="66"/>
+      <c r="I20">
+        <v>1390</v>
+      </c>
+      <c r="J20" s="43">
+        <v>24</v>
+      </c>
+      <c r="K20" s="66"/>
+      <c r="L20">
+        <v>1390</v>
+      </c>
+      <c r="M20">
+        <v>49</v>
+      </c>
+      <c r="N20">
+        <v>1200</v>
+      </c>
+      <c r="O20">
+        <v>300</v>
+      </c>
+      <c r="V20" t="s">
+        <v>187</v>
+      </c>
+      <c r="W20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21">
+        <v>840</v>
+      </c>
+      <c r="G21" s="43">
+        <v>3</v>
+      </c>
+      <c r="H21" s="66"/>
+      <c r="I21">
+        <v>1120</v>
+      </c>
+      <c r="J21" s="43">
+        <v>16</v>
+      </c>
+      <c r="K21" s="66"/>
+      <c r="L21">
+        <v>1120</v>
+      </c>
+      <c r="M21">
+        <v>33</v>
+      </c>
+      <c r="N21">
+        <v>1200</v>
+      </c>
+      <c r="O21">
+        <v>300</v>
+      </c>
+      <c r="V21" t="s">
+        <v>187</v>
+      </c>
+      <c r="W21" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" s="37">
+        <v>31.714285714285715</v>
+      </c>
+      <c r="G22" s="43">
+        <v>4</v>
+      </c>
+      <c r="H22" s="66"/>
+      <c r="I22" s="37">
+        <v>39</v>
+      </c>
+      <c r="J22" s="43">
+        <v>13</v>
+      </c>
+      <c r="K22" s="66"/>
+      <c r="L22">
+        <v>40</v>
+      </c>
+      <c r="M22">
+        <v>27</v>
+      </c>
+      <c r="N22">
+        <v>1200</v>
+      </c>
+      <c r="O22">
+        <v>300</v>
+      </c>
+      <c r="V22" t="s">
+        <v>187</v>
+      </c>
+      <c r="W22" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23" s="37">
+        <v>44.571428571428569</v>
+      </c>
+      <c r="G23" s="43">
+        <v>2</v>
+      </c>
+      <c r="H23" s="66"/>
+      <c r="I23" s="37">
+        <v>70</v>
+      </c>
+      <c r="J23" s="43">
+        <v>18</v>
+      </c>
+      <c r="K23" s="66"/>
+      <c r="L23">
+        <v>70</v>
+      </c>
+      <c r="M23">
+        <v>37</v>
+      </c>
+      <c r="N23">
+        <v>1200</v>
+      </c>
+      <c r="O23">
+        <v>300</v>
+      </c>
+      <c r="V23" t="s">
+        <v>187</v>
+      </c>
+      <c r="W23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" s="37">
+        <v>66</v>
+      </c>
+      <c r="G24" s="43">
+        <v>6</v>
+      </c>
+      <c r="H24" s="66"/>
+      <c r="I24" s="37">
+        <v>110</v>
+      </c>
+      <c r="J24" s="43">
+        <v>24</v>
+      </c>
+      <c r="K24" s="66"/>
+      <c r="L24">
+        <v>110</v>
+      </c>
+      <c r="M24">
+        <v>49</v>
+      </c>
+      <c r="N24">
+        <v>1200</v>
+      </c>
+      <c r="O24">
+        <v>300</v>
+      </c>
+      <c r="V24" t="s">
+        <v>187</v>
+      </c>
+      <c r="W24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="37">
+        <v>77.142857142857139</v>
+      </c>
+      <c r="G25" s="43">
+        <v>3</v>
+      </c>
+      <c r="H25" s="66"/>
+      <c r="I25" s="37">
+        <v>118</v>
+      </c>
+      <c r="J25" s="43">
+        <v>16</v>
+      </c>
+      <c r="K25" s="66"/>
+      <c r="L25">
+        <v>120</v>
+      </c>
+      <c r="M25">
+        <v>33</v>
+      </c>
+      <c r="N25">
+        <v>1200</v>
+      </c>
+      <c r="O25">
+        <v>300</v>
+      </c>
+      <c r="V25" t="s">
+        <v>187</v>
+      </c>
+      <c r="W25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
   <dimension ref="A1:W66"/>
   <sheetViews>
@@ -7407,7 +7508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B880D5D-98F5-BA4D-B0BB-6D687A1CAC9F}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -7457,7 +7558,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.85672864624929124</v>
+        <v>0.621344986971617</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -7477,7 +7578,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>7.1221422827264957E-2</v>
+        <v>3.9735454105311097E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -7498,7 +7599,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>3.3321846748652795E-2</v>
+        <v>0.4682789491777678</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7518,7 +7619,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.10258517007342238</v>
+        <v>0.17007126783934279</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -7590,7 +7691,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F6B51D-A4A1-6D46-8F47-1EE4F323E4DF}">
   <dimension ref="A1:X42"/>
   <sheetViews>
@@ -7617,48 +7718,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="68" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="70"/>
-      <c r="E3" s="69" t="s">
+      <c r="D3" s="69"/>
+      <c r="E3" s="68" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="70"/>
-      <c r="G3" s="69" t="s">
+      <c r="F3" s="69"/>
+      <c r="G3" s="68" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="70"/>
-      <c r="I3" s="69" t="s">
+      <c r="H3" s="69"/>
+      <c r="I3" s="68" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="70"/>
+      <c r="J3" s="69"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="71" t="s">
+      <c r="M3" s="70" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="72"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="71" t="s">
+      <c r="N3" s="71"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="70" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="72"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="71" t="s">
+      <c r="Q3" s="71"/>
+      <c r="R3" s="72"/>
+      <c r="S3" s="70" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="72"/>
-      <c r="U3" s="72"/>
-      <c r="V3" s="74" t="s">
+      <c r="T3" s="71"/>
+      <c r="U3" s="71"/>
+      <c r="V3" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="74"/>
-      <c r="X3" s="74"/>
+      <c r="W3" s="73"/>
+      <c r="X3" s="73"/>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="50"/>
@@ -8485,16 +8586,16 @@
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="C29" s="68" t="s">
+      <c r="C29" s="74" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="68"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="68" t="s">
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74" t="s">
         <v>169</v>
       </c>
-      <c r="G29" s="68"/>
-      <c r="H29" s="68"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
       <c r="J29" t="s">
         <v>168</v>
       </c>
@@ -9114,22 +9215,22 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="P3:R3"/>
     <mergeCell ref="S3:U3"/>
     <mergeCell ref="V3:X3"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172F3C91-0245-C642-8607-0C1863490763}">
   <dimension ref="A1:AA22"/>
   <sheetViews>
@@ -9160,105 +9261,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="87" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="81" t="s">
+      <c r="A2" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="81" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="82"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="78" t="s">
+      <c r="C2" s="76"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="75" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="76"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="93" t="s">
+      <c r="I2" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="93"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="93"/>
-      <c r="P2" s="93"/>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="93" t="s">
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="93"/>
-      <c r="T2" s="93"/>
-      <c r="U2" s="93"/>
-      <c r="V2" s="78" t="s">
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="78" t="s">
+      <c r="W2" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="75" t="s">
+      <c r="X2" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="75" t="s">
+      <c r="Y2" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="75" t="s">
+      <c r="Z2" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="75" t="s">
+      <c r="AA2" s="92" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="88"/>
-      <c r="B3" s="84"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="94" t="s">
+      <c r="A3" s="82"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92" t="s">
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92" t="s">
+      <c r="M3" s="89"/>
+      <c r="N3" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92" t="s">
+      <c r="O3" s="89"/>
+      <c r="P3" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="90" t="s">
+      <c r="Q3" s="89"/>
+      <c r="R3" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="90" t="s">
+      <c r="S3" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="90" t="s">
+      <c r="T3" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="90" t="s">
+      <c r="U3" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="79"/>
-      <c r="W3" s="79"/>
-      <c r="X3" s="76"/>
-      <c r="Y3" s="76"/>
-      <c r="Z3" s="76"/>
-      <c r="AA3" s="76"/>
+      <c r="V3" s="85"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="93"/>
+      <c r="Y3" s="93"/>
+      <c r="Z3" s="93"/>
+      <c r="AA3" s="93"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="89"/>
+      <c r="A4" s="83"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -9277,7 +9378,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="80"/>
+      <c r="H4" s="86"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -9305,16 +9406,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="91"/>
-      <c r="S4" s="91"/>
-      <c r="T4" s="91"/>
-      <c r="U4" s="91"/>
-      <c r="V4" s="80"/>
-      <c r="W4" s="80"/>
-      <c r="X4" s="77"/>
-      <c r="Y4" s="77"/>
-      <c r="Z4" s="77"/>
-      <c r="AA4" s="76"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="88"/>
+      <c r="V4" s="86"/>
+      <c r="W4" s="86"/>
+      <c r="X4" s="94"/>
+      <c r="Y4" s="94"/>
+      <c r="Z4" s="94"/>
+      <c r="AA4" s="93"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -9815,6 +9916,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -9830,18 +9936,13 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE45FD6-E248-1447-95F1-A5D07360E1EE}">
   <dimension ref="A1:H19"/>
   <sheetViews>
@@ -10312,7 +10413,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E1E67AD-5D17-8649-BBCA-56D0D08542BD}">
   <dimension ref="A1:O38"/>
   <sheetViews>
@@ -10704,7 +10805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2E945CF-9189-764F-9A6E-0EEEF9828B80}">
   <dimension ref="A1:I10"/>
   <sheetViews>
@@ -10925,69 +11026,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CC848A2-46C4-BD4C-AFD2-CF7F6FD4ADEE}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="12">
-        <v>15</v>
-      </c>
-      <c r="C1" s="12">
-        <v>10</v>
-      </c>
-      <c r="D1" s="12">
-        <v>9.6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="12">
-        <f>B1/60</f>
-        <v>0.25</v>
-      </c>
-      <c r="C2" s="12">
-        <f>C1/60</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="D2" s="12">
-        <f>D1/60</f>
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="12">
-        <f xml:space="preserve"> B2*5</f>
-        <v>1.25</v>
-      </c>
-      <c r="C3" s="12">
-        <f xml:space="preserve"> C2*5</f>
-        <v>0.83333333333333326</v>
-      </c>
-      <c r="D3" s="12">
-        <f xml:space="preserve"> D2*5</f>
-        <v>0.8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated screen shot of answer submission.
Also added more text in the instructions that explained the research.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C8A9CA-A2EF-D54D-872E-DBF3FCBB57B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83B2C00-7F32-7040-9FED-721DA0BFE1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -1389,7 +1389,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Implemented animated gifs with space to the right.  Fixed treatment configurations.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41BC453-FEC2-724E-BD99-4BB21E0CAB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FB130F-4EFC-1D4A-AAAF-6EC6319BF07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="2" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="2" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
@@ -4060,7 +4060,7 @@
         <v>1000</v>
       </c>
       <c r="M19">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N19">
         <v>600</v>
@@ -4505,7 +4505,7 @@
         <v>1000</v>
       </c>
       <c r="M28">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="N28">
         <v>1200</v>
@@ -4534,8 +4534,8 @@
   <dimension ref="A1:X88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L65" sqref="L65"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -8345,7 +8345,7 @@
         <v>1000</v>
       </c>
       <c r="M79">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N79">
         <v>600</v>
@@ -8790,7 +8790,7 @@
         <v>1000</v>
       </c>
       <c r="M88">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="N88">
         <v>1200</v>
@@ -8864,7 +8864,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.18293354596429723</v>
+        <v>0.67959142066036216</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -8884,7 +8884,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.89456275502778526</v>
+        <v>0.27711612671485231</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -8905,7 +8905,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.1221776617226048</v>
+        <v>0.70408920160705324</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -8925,7 +8925,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.24915137371527207</v>
+        <v>0.17338255197206343</v>
       </c>
     </row>
     <row r="6" spans="1:7">

</xml_diff>

<commit_message>
Added 3rd survey of survey experience.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FB130F-4EFC-1D4A-AAAF-6EC6319BF07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E02C70-474B-8C49-8536-8286C02A858C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="2" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="1" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
@@ -1033,6 +1033,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1051,8 +1054,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1082,15 +1100,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1104,15 +1113,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3196,9 +3196,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6462F7B1-F956-1241-A84D-BB94A5075354}">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD28"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -4533,7 +4533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
   <dimension ref="A1:X88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I71" sqref="I71"/>
     </sheetView>
@@ -8864,7 +8864,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.67959142066036216</v>
+        <v>0.36913974170032826</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -8884,7 +8884,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.27711612671485231</v>
+        <v>0.95415812166791358</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -8905,7 +8905,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.70408920160705324</v>
+        <v>0.7954385491953494</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -8925,7 +8925,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.17338255197206343</v>
+        <v>0.73478724689999553</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -9024,48 +9024,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="69" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="68" t="s">
+      <c r="D3" s="70"/>
+      <c r="E3" s="69" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="69"/>
-      <c r="G3" s="68" t="s">
+      <c r="F3" s="70"/>
+      <c r="G3" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="69"/>
-      <c r="I3" s="68" t="s">
+      <c r="H3" s="70"/>
+      <c r="I3" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="69"/>
+      <c r="J3" s="70"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="70" t="s">
+      <c r="M3" s="71" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="71"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="70" t="s">
+      <c r="N3" s="72"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="71" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="72"/>
-      <c r="S3" s="70" t="s">
+      <c r="Q3" s="72"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="71"/>
-      <c r="U3" s="71"/>
-      <c r="V3" s="73" t="s">
+      <c r="T3" s="72"/>
+      <c r="U3" s="72"/>
+      <c r="V3" s="74" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="73"/>
-      <c r="X3" s="73"/>
+      <c r="W3" s="74"/>
+      <c r="X3" s="74"/>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="50"/>
@@ -9892,16 +9892,16 @@
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="C29" s="74" t="s">
+      <c r="C29" s="68" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74" t="s">
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68" t="s">
         <v>169</v>
       </c>
-      <c r="G29" s="74"/>
-      <c r="H29" s="74"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
       <c r="J29" t="s">
         <v>168</v>
       </c>
@@ -10521,16 +10521,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10567,105 +10567,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="75" t="s">
+      <c r="A2" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="75" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="76"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="84" t="s">
+      <c r="F2" s="82"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="90" t="s">
+      <c r="I2" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="90" t="s">
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="90"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="84" t="s">
+      <c r="S2" s="93"/>
+      <c r="T2" s="93"/>
+      <c r="U2" s="93"/>
+      <c r="V2" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="84" t="s">
+      <c r="W2" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="92" t="s">
+      <c r="X2" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="92" t="s">
+      <c r="Y2" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="92" t="s">
+      <c r="Z2" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="92" t="s">
+      <c r="AA2" s="75" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="82"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="91" t="s">
+      <c r="A3" s="88"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89" t="s">
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89" t="s">
+      <c r="M3" s="92"/>
+      <c r="N3" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89" t="s">
+      <c r="O3" s="92"/>
+      <c r="P3" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="87" t="s">
+      <c r="Q3" s="92"/>
+      <c r="R3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="87" t="s">
+      <c r="S3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="87" t="s">
+      <c r="T3" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="87" t="s">
+      <c r="U3" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="85"/>
-      <c r="W3" s="85"/>
-      <c r="X3" s="93"/>
-      <c r="Y3" s="93"/>
-      <c r="Z3" s="93"/>
-      <c r="AA3" s="93"/>
+      <c r="V3" s="79"/>
+      <c r="W3" s="79"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="76"/>
+      <c r="Z3" s="76"/>
+      <c r="AA3" s="76"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="83"/>
+      <c r="A4" s="89"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -10684,7 +10684,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="86"/>
+      <c r="H4" s="80"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -10712,16 +10712,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="86"/>
-      <c r="X4" s="94"/>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="94"/>
-      <c r="AA4" s="93"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="80"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="77"/>
+      <c r="Z4" s="77"/>
+      <c r="AA4" s="76"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -11222,11 +11222,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -11242,6 +11237,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Fixed split to write same columns and order as survey.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10202"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E02C70-474B-8C49-8536-8286C02A858C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F4A6ED-2C01-E447-88CD-572208E78C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="1" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -1033,9 +1033,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1054,23 +1051,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1100,6 +1082,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1113,6 +1104,15 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3198,7 +3198,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -8864,7 +8864,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.36913974170032826</v>
+        <v>0.88482329502001356</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -8884,7 +8884,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.95415812166791358</v>
+        <v>0.62467870304618489</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -8905,7 +8905,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.7954385491953494</v>
+        <v>0.92235916021921138</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -8925,7 +8925,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.73478724689999553</v>
+        <v>0.55094073365523555</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -9024,48 +9024,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="68" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="70"/>
-      <c r="E3" s="69" t="s">
+      <c r="D3" s="69"/>
+      <c r="E3" s="68" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="70"/>
-      <c r="G3" s="69" t="s">
+      <c r="F3" s="69"/>
+      <c r="G3" s="68" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="70"/>
-      <c r="I3" s="69" t="s">
+      <c r="H3" s="69"/>
+      <c r="I3" s="68" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="70"/>
+      <c r="J3" s="69"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="71" t="s">
+      <c r="M3" s="70" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="72"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="71" t="s">
+      <c r="N3" s="71"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="70" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="72"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="71" t="s">
+      <c r="Q3" s="71"/>
+      <c r="R3" s="72"/>
+      <c r="S3" s="70" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="72"/>
-      <c r="U3" s="72"/>
-      <c r="V3" s="74" t="s">
+      <c r="T3" s="71"/>
+      <c r="U3" s="71"/>
+      <c r="V3" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="74"/>
-      <c r="X3" s="74"/>
+      <c r="W3" s="73"/>
+      <c r="X3" s="73"/>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="50"/>
@@ -9892,16 +9892,16 @@
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="C29" s="68" t="s">
+      <c r="C29" s="74" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="68"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="68" t="s">
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74" t="s">
         <v>169</v>
       </c>
-      <c r="G29" s="68"/>
-      <c r="H29" s="68"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
       <c r="J29" t="s">
         <v>168</v>
       </c>
@@ -10521,16 +10521,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="P3:R3"/>
     <mergeCell ref="S3:U3"/>
     <mergeCell ref="V3:X3"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10567,105 +10567,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="87" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="81" t="s">
+      <c r="A2" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="81" t="s">
+      <c r="C2" s="76"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="82"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="78" t="s">
+      <c r="F2" s="76"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="93" t="s">
+      <c r="I2" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="93"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="93"/>
-      <c r="P2" s="93"/>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="93" t="s">
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="93"/>
-      <c r="T2" s="93"/>
-      <c r="U2" s="93"/>
-      <c r="V2" s="78" t="s">
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="78" t="s">
+      <c r="W2" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="75" t="s">
+      <c r="X2" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="75" t="s">
+      <c r="Y2" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="75" t="s">
+      <c r="Z2" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="75" t="s">
+      <c r="AA2" s="92" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="88"/>
-      <c r="B3" s="84"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="94" t="s">
+      <c r="A3" s="82"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92" t="s">
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92" t="s">
+      <c r="M3" s="89"/>
+      <c r="N3" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92" t="s">
+      <c r="O3" s="89"/>
+      <c r="P3" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="90" t="s">
+      <c r="Q3" s="89"/>
+      <c r="R3" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="90" t="s">
+      <c r="S3" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="90" t="s">
+      <c r="T3" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="90" t="s">
+      <c r="U3" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="79"/>
-      <c r="W3" s="79"/>
-      <c r="X3" s="76"/>
-      <c r="Y3" s="76"/>
-      <c r="Z3" s="76"/>
-      <c r="AA3" s="76"/>
+      <c r="V3" s="85"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="93"/>
+      <c r="Y3" s="93"/>
+      <c r="Z3" s="93"/>
+      <c r="AA3" s="93"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="89"/>
+      <c r="A4" s="83"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -10684,7 +10684,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="80"/>
+      <c r="H4" s="86"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -10712,16 +10712,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="91"/>
-      <c r="S4" s="91"/>
-      <c r="T4" s="91"/>
-      <c r="U4" s="91"/>
-      <c r="V4" s="80"/>
-      <c r="W4" s="80"/>
-      <c r="X4" s="77"/>
-      <c r="Y4" s="77"/>
-      <c r="Z4" s="77"/>
-      <c r="AA4" s="76"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="88"/>
+      <c r="V4" s="86"/>
+      <c r="W4" s="86"/>
+      <c r="X4" s="94"/>
+      <c r="Y4" s="94"/>
+      <c r="Z4" s="94"/>
+      <c r="AA4" s="93"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -11222,6 +11222,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -11237,11 +11242,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
merge latest of main-calendar to release-calendar
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10202"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FB130F-4EFC-1D4A-AAAF-6EC6319BF07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F4A6ED-2C01-E447-88CD-572208E78C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="2" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="1" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
@@ -3196,9 +3196,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6462F7B1-F956-1241-A84D-BB94A5075354}">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD28"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -4533,7 +4533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
   <dimension ref="A1:X88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I71" sqref="I71"/>
     </sheetView>
@@ -8864,7 +8864,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.67959142066036216</v>
+        <v>0.88482329502001356</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -8884,7 +8884,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.27711612671485231</v>
+        <v>0.62467870304618489</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -8905,7 +8905,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.70408920160705324</v>
+        <v>0.92235916021921138</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -8925,7 +8925,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.17338255197206343</v>
+        <v>0.55094073365523555</v>
       </c>
     </row>
     <row r="6" spans="1:7">

</xml_diff>

<commit_message>
Modified monitor util to show in progress.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10202"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F4A6ED-2C01-E447-88CD-572208E78C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C952DFB-4D64-A442-A765-4BFBB703547B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="1" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="4" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="221">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -699,6 +699,48 @@
   </si>
   <si>
     <t>introduction-calendarIcon</t>
+  </si>
+  <si>
+    <t>Final amounts and delays.</t>
+  </si>
+  <si>
+    <t>Below is my calcuatlions of the final amounts and delays which is below this.</t>
+  </si>
+  <si>
+    <t>SS months</t>
+  </si>
+  <si>
+    <t>LL months</t>
+  </si>
+  <si>
+    <t>SS USD</t>
+  </si>
+  <si>
+    <t>LL USD</t>
+  </si>
+  <si>
+    <t>Original Amounts</t>
+  </si>
+  <si>
+    <t>Recalced for 2023</t>
+  </si>
+  <si>
+    <t>2023 inflation factor</t>
+  </si>
+  <si>
+    <t>Question 1</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Question 2</t>
+  </si>
+  <si>
+    <t>Question 4</t>
+  </si>
+  <si>
+    <t>Question 3</t>
   </si>
 </sst>
 </file>
@@ -710,7 +752,7 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -753,6 +795,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -941,10 +999,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1114,8 +1173,25 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3196,9 +3272,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6462F7B1-F956-1241-A84D-BB94A5075354}">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -4534,7 +4610,7 @@
   <dimension ref="A1:X88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
@@ -8864,7 +8940,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.88482329502001356</v>
+        <v>0.70646306116546564</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -8884,7 +8960,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.62467870304618489</v>
+        <v>0.7849673602392585</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -8905,7 +8981,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.92235916021921138</v>
+        <v>0.85625026269514737</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -8925,7 +9001,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.55094073365523555</v>
+        <v>0.6706069433597549</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -8999,10 +9075,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F6B51D-A4A1-6D46-8F47-1EE4F323E4DF}">
-  <dimension ref="A1:X42"/>
+  <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9014,12 +9090,12 @@
     <col min="24" max="24" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:33">
       <c r="A3" s="49" t="s">
         <v>145</v>
       </c>
@@ -9066,8 +9142,27 @@
       </c>
       <c r="W3" s="73"/>
       <c r="X3" s="73"/>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="Y3" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z3" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA3" s="53"/>
+      <c r="AB3" s="41" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC3" s="53"/>
+      <c r="AD3" s="104" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE3" s="105"/>
+      <c r="AF3" s="104" t="s">
+        <v>219</v>
+      </c>
+      <c r="AG3" s="105"/>
+    </row>
+    <row r="4" spans="1:33">
       <c r="A4" s="50"/>
       <c r="B4" s="46"/>
       <c r="C4" s="44" t="s">
@@ -9123,8 +9218,32 @@
       <c r="W4" s="48" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="Z4" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="AA4" s="53" t="s">
+        <v>147</v>
+      </c>
+      <c r="AB4" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC4" s="53" t="s">
+        <v>147</v>
+      </c>
+      <c r="AD4" s="104" t="s">
+        <v>146</v>
+      </c>
+      <c r="AE4" s="105" t="s">
+        <v>147</v>
+      </c>
+      <c r="AF4" s="104" t="s">
+        <v>146</v>
+      </c>
+      <c r="AG4" s="105" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33">
       <c r="A5" s="51">
         <v>1</v>
       </c>
@@ -9209,8 +9328,43 @@
         <f>(W5-V5)/W5</f>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="Y5">
+        <v>1.63</v>
+      </c>
+      <c r="Z5" s="56">
+        <f>C5/$K$5*$Y$5</f>
+        <v>376.9375</v>
+      </c>
+      <c r="AA5" s="42">
+        <f>D5/$K$5*$Y$5</f>
+        <v>458.43749999999994</v>
+      </c>
+      <c r="AB5" s="37">
+        <f>E5/$K$5*$Y$5</f>
+        <v>529.75</v>
+      </c>
+      <c r="AC5" s="37">
+        <f>F5/$K$5*$Y$5</f>
+        <v>753.875</v>
+      </c>
+      <c r="AD5" s="56">
+        <f>G5/$K$5*$Y$5</f>
+        <v>784.4375</v>
+      </c>
+      <c r="AE5" s="42">
+        <f>H5/$K$5*$Y$5</f>
+        <v>1507.75</v>
+      </c>
+      <c r="AF5" s="106">
+        <f>I5/$K$5*$Y$5</f>
+        <v>916.87499999999989</v>
+      </c>
+      <c r="AG5" s="106">
+        <f>J5/$K$5*$Y$5</f>
+        <v>1222.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33">
       <c r="A6" s="51"/>
       <c r="B6" t="s">
         <v>149</v>
@@ -9246,8 +9400,16 @@
       <c r="S6" s="56"/>
       <c r="T6" s="42"/>
       <c r="W6" s="42"/>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="Z6" s="56"/>
+      <c r="AA6" s="42"/>
+      <c r="AB6" s="37"/>
+      <c r="AC6" s="37"/>
+      <c r="AD6" s="56"/>
+      <c r="AE6" s="42"/>
+      <c r="AF6" s="37"/>
+      <c r="AG6" s="37"/>
+    </row>
+    <row r="7" spans="1:33">
       <c r="A7" s="51"/>
       <c r="B7" t="s">
         <v>150</v>
@@ -9283,8 +9445,16 @@
       <c r="S7" s="56"/>
       <c r="T7" s="42"/>
       <c r="W7" s="42"/>
-    </row>
-    <row r="8" spans="1:24">
+      <c r="Z7" s="56"/>
+      <c r="AA7" s="42"/>
+      <c r="AB7" s="37"/>
+      <c r="AC7" s="37"/>
+      <c r="AD7" s="56"/>
+      <c r="AE7" s="42"/>
+      <c r="AF7" s="37"/>
+      <c r="AG7" s="37"/>
+    </row>
+    <row r="8" spans="1:33">
       <c r="A8" s="51"/>
       <c r="B8" t="s">
         <v>151</v>
@@ -9320,8 +9490,16 @@
       <c r="S8" s="56"/>
       <c r="T8" s="42"/>
       <c r="W8" s="42"/>
-    </row>
-    <row r="9" spans="1:24">
+      <c r="Z8" s="56"/>
+      <c r="AA8" s="42"/>
+      <c r="AB8" s="37"/>
+      <c r="AC8" s="37"/>
+      <c r="AD8" s="56"/>
+      <c r="AE8" s="42"/>
+      <c r="AF8" s="37"/>
+      <c r="AG8" s="37"/>
+    </row>
+    <row r="9" spans="1:33">
       <c r="A9" s="49">
         <v>2</v>
       </c>
@@ -9358,17 +9536,16 @@
       <c r="L9" s="39">
         <v>1.5</v>
       </c>
-      <c r="M9" s="59">
-        <f>C9/$K$9*$L$9</f>
-        <v>346.875</v>
+      <c r="M9" s="59" t="s">
+        <v>217</v>
       </c>
       <c r="N9" s="60">
         <f>D9/$K$9*$L$9</f>
         <v>421.875</v>
       </c>
-      <c r="O9" s="37">
+      <c r="O9" s="37" t="e">
         <f>(N9-M9)</f>
-        <v>75</v>
+        <v>#VALUE!</v>
       </c>
       <c r="P9" s="59">
         <f>E9/$K$9*$L$9</f>
@@ -9406,8 +9583,19 @@
         <f>(W9-V9)/W9</f>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="10" spans="1:24">
+      <c r="Y9">
+        <v>1.63</v>
+      </c>
+      <c r="Z9" s="56"/>
+      <c r="AA9" s="42"/>
+      <c r="AB9" s="37"/>
+      <c r="AC9" s="37"/>
+      <c r="AD9" s="56"/>
+      <c r="AE9" s="42"/>
+      <c r="AF9" s="37"/>
+      <c r="AG9" s="37"/>
+    </row>
+    <row r="10" spans="1:33">
       <c r="A10" s="51"/>
       <c r="B10" t="s">
         <v>149</v>
@@ -9443,8 +9631,16 @@
       <c r="S10" s="56"/>
       <c r="T10" s="42"/>
       <c r="W10" s="42"/>
-    </row>
-    <row r="11" spans="1:24">
+      <c r="Z10" s="56"/>
+      <c r="AA10" s="42"/>
+      <c r="AB10" s="37"/>
+      <c r="AC10" s="37"/>
+      <c r="AD10" s="56"/>
+      <c r="AE10" s="42"/>
+      <c r="AF10" s="37"/>
+      <c r="AG10" s="37"/>
+    </row>
+    <row r="11" spans="1:33">
       <c r="A11" s="51"/>
       <c r="B11" t="s">
         <v>150</v>
@@ -9480,8 +9676,16 @@
       <c r="S11" s="56"/>
       <c r="T11" s="42"/>
       <c r="W11" s="42"/>
-    </row>
-    <row r="12" spans="1:24">
+      <c r="Z11" s="56"/>
+      <c r="AA11" s="42"/>
+      <c r="AB11" s="37"/>
+      <c r="AC11" s="37"/>
+      <c r="AD11" s="56"/>
+      <c r="AE11" s="42"/>
+      <c r="AF11" s="37"/>
+      <c r="AG11" s="37"/>
+    </row>
+    <row r="12" spans="1:33">
       <c r="A12" s="51"/>
       <c r="B12" t="s">
         <v>151</v>
@@ -9501,8 +9705,16 @@
       <c r="S12" s="56"/>
       <c r="T12" s="42"/>
       <c r="W12" s="42"/>
-    </row>
-    <row r="13" spans="1:24">
+      <c r="Z12" s="56"/>
+      <c r="AA12" s="42"/>
+      <c r="AB12" s="37"/>
+      <c r="AC12" s="37"/>
+      <c r="AD12" s="56"/>
+      <c r="AE12" s="42"/>
+      <c r="AF12" s="37"/>
+      <c r="AG12" s="37"/>
+    </row>
+    <row r="13" spans="1:33">
       <c r="A13" s="49">
         <v>3</v>
       </c>
@@ -9587,8 +9799,43 @@
         <f>(W13-V13)/W13</f>
         <v>0.34782608695652178</v>
       </c>
-    </row>
-    <row r="14" spans="1:24">
+      <c r="Y13">
+        <v>1.63</v>
+      </c>
+      <c r="Z13" s="56">
+        <f>C13/$K$13*$Y$13</f>
+        <v>34.462857142857139</v>
+      </c>
+      <c r="AA13" s="42">
+        <f>D13/$K$13*$Y$13</f>
+        <v>42.84571428571428</v>
+      </c>
+      <c r="AB13" s="37">
+        <f>E13/$K$13*$Y$13</f>
+        <v>48.434285714285714</v>
+      </c>
+      <c r="AC13" s="37">
+        <f>F13/$K$13*$Y$13</f>
+        <v>76.377142857142843</v>
+      </c>
+      <c r="AD13" s="56">
+        <f>G13/$K$13*$Y$13</f>
+        <v>71.72</v>
+      </c>
+      <c r="AE13" s="42">
+        <f>H13/$K$13*$Y$13</f>
+        <v>119.22285714285712</v>
+      </c>
+      <c r="AF13" s="106">
+        <f>I13/$K$13*$Y$13</f>
+        <v>83.828571428571422</v>
+      </c>
+      <c r="AG13" s="106">
+        <f>J13/$K$13*$Y$13</f>
+        <v>128.53714285714287</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33">
       <c r="A14" s="51"/>
       <c r="B14" s="43" t="s">
         <v>149</v>
@@ -9624,8 +9871,16 @@
       <c r="S14" s="56"/>
       <c r="T14" s="42"/>
       <c r="W14" s="42"/>
-    </row>
-    <row r="15" spans="1:24">
+      <c r="Z14" s="56"/>
+      <c r="AA14" s="42"/>
+      <c r="AB14" s="37"/>
+      <c r="AC14" s="37"/>
+      <c r="AD14" s="56"/>
+      <c r="AE14" s="42"/>
+      <c r="AF14" s="37"/>
+      <c r="AG14" s="37"/>
+    </row>
+    <row r="15" spans="1:33">
       <c r="A15" s="51"/>
       <c r="B15" s="43" t="s">
         <v>150</v>
@@ -9661,8 +9916,16 @@
       <c r="S15" s="56"/>
       <c r="T15" s="42"/>
       <c r="W15" s="42"/>
-    </row>
-    <row r="16" spans="1:24">
+      <c r="Z15" s="56"/>
+      <c r="AA15" s="42"/>
+      <c r="AB15" s="37"/>
+      <c r="AC15" s="37"/>
+      <c r="AD15" s="56"/>
+      <c r="AE15" s="42"/>
+      <c r="AF15" s="37"/>
+      <c r="AG15" s="37"/>
+    </row>
+    <row r="16" spans="1:33">
       <c r="A16" s="51"/>
       <c r="B16" s="43" t="s">
         <v>151</v>
@@ -9682,8 +9945,16 @@
       <c r="S16" s="56"/>
       <c r="T16" s="42"/>
       <c r="W16" s="42"/>
-    </row>
-    <row r="17" spans="1:24">
+      <c r="Z16" s="56"/>
+      <c r="AA16" s="42"/>
+      <c r="AB16" s="37"/>
+      <c r="AC16" s="37"/>
+      <c r="AD16" s="56"/>
+      <c r="AE16" s="42"/>
+      <c r="AF16" s="37"/>
+      <c r="AG16" s="37"/>
+    </row>
+    <row r="17" spans="1:33">
       <c r="A17" s="49">
         <v>4</v>
       </c>
@@ -9760,16 +10031,50 @@
         <f>I17/$K$17*$L$17</f>
         <v>410.2941176470589</v>
       </c>
-      <c r="W17" s="60">
-        <f>J17/$K$17*$L$17</f>
-        <v>767.64705882352939</v>
-      </c>
-      <c r="X17" s="11">
+      <c r="W17" s="60" t="s">
+        <v>217</v>
+      </c>
+      <c r="X17" s="11" t="e">
         <f>(W17-V17)/W17</f>
-        <v>0.46551724137931022</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y17">
+        <v>1.63</v>
+      </c>
+      <c r="Z17" s="56">
+        <f>C17/$K$17*$Y$17</f>
+        <v>862.94117647058818</v>
+      </c>
+      <c r="AA17" s="42">
+        <f>D17/$K$17*$Y$17</f>
+        <v>1150.5882352941176</v>
+      </c>
+      <c r="AB17" s="37">
+        <f>E17/$K$17*$Y$17</f>
+        <v>719.11764705882354</v>
+      </c>
+      <c r="AC17" s="37">
+        <f>F17/$K$17*$Y$17</f>
+        <v>1917.6470588235293</v>
+      </c>
+      <c r="AD17" s="56">
+        <f>G17/$K$17*$Y$17</f>
+        <v>498.58823529411762</v>
+      </c>
+      <c r="AE17" s="42">
+        <f>H17/$K$17*$Y$17</f>
+        <v>747.88235294117635</v>
+      </c>
+      <c r="AF17" s="106">
+        <f>I17/$K$17*$Y$17</f>
+        <v>445.85294117647061</v>
+      </c>
+      <c r="AG17" s="37">
+        <f>J17/$K$17*$Y$17</f>
+        <v>834.17647058823525</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33">
       <c r="A18" s="51"/>
       <c r="B18" s="43" t="s">
         <v>149</v>
@@ -9805,8 +10110,14 @@
       <c r="S18" s="56"/>
       <c r="T18" s="42"/>
       <c r="W18" s="42"/>
-    </row>
-    <row r="19" spans="1:24">
+      <c r="Z18" s="56"/>
+      <c r="AA18" s="53"/>
+      <c r="AB18" s="37"/>
+      <c r="AC18" s="37"/>
+      <c r="AD18" s="56"/>
+      <c r="AE18" s="42"/>
+    </row>
+    <row r="19" spans="1:33">
       <c r="A19" s="51"/>
       <c r="B19" s="43" t="s">
         <v>150</v>
@@ -9842,8 +10153,14 @@
       <c r="S19" s="56"/>
       <c r="T19" s="42"/>
       <c r="W19" s="42"/>
-    </row>
-    <row r="20" spans="1:24">
+      <c r="Z19" s="56"/>
+      <c r="AA19" s="53"/>
+      <c r="AB19" s="37"/>
+      <c r="AC19" s="37"/>
+      <c r="AD19" s="56"/>
+      <c r="AE19" s="42"/>
+    </row>
+    <row r="20" spans="1:33">
       <c r="A20" s="50"/>
       <c r="B20" s="45" t="s">
         <v>151</v>
@@ -9869,18 +10186,29 @@
       <c r="U20" s="65"/>
       <c r="V20" s="47"/>
       <c r="W20" s="48"/>
-    </row>
-    <row r="25" spans="1:24">
+      <c r="Z20" s="56"/>
+      <c r="AA20" s="53"/>
+      <c r="AB20" s="37"/>
+      <c r="AC20" s="37"/>
+      <c r="AD20" s="56"/>
+      <c r="AE20" s="42"/>
+    </row>
+    <row r="25" spans="1:33">
       <c r="B25" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="26" spans="1:24">
-      <c r="B26" t="s">
+    <row r="26" spans="1:33">
+      <c r="B26" s="95" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="28" spans="1:24">
+    <row r="27" spans="1:33">
+      <c r="B27" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33">
       <c r="B28" t="s">
         <v>175</v>
       </c>
@@ -9891,7 +10219,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="29" spans="1:24">
+    <row r="29" spans="1:33">
       <c r="C29" s="74" t="s">
         <v>167</v>
       </c>
@@ -9907,7 +10235,7 @@
       </c>
       <c r="M29"/>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:33">
       <c r="B30" t="s">
         <v>166</v>
       </c>
@@ -9960,7 +10288,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:33">
       <c r="B31">
         <v>1</v>
       </c>
@@ -10019,7 +10347,7 @@
         <v>2.9054054054054053</v>
       </c>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:33">
       <c r="B32">
         <v>2</v>
       </c>
@@ -10518,6 +10846,291 @@
         <f>M42/$C$28</f>
         <v>0.79729729729729726</v>
       </c>
+    </row>
+    <row r="45" spans="2:18">
+      <c r="B45" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18">
+      <c r="B46" s="43"/>
+      <c r="C46" s="96"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="43"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="43"/>
+      <c r="M46" s="97"/>
+      <c r="N46" s="97"/>
+      <c r="O46" s="97"/>
+      <c r="P46" s="97"/>
+      <c r="Q46" s="97"/>
+      <c r="R46" s="97"/>
+    </row>
+    <row r="47" spans="2:18">
+      <c r="B47" s="43"/>
+      <c r="C47" s="99" t="s">
+        <v>213</v>
+      </c>
+      <c r="D47" s="99"/>
+      <c r="E47" s="101"/>
+      <c r="F47" s="98"/>
+      <c r="G47" s="103" t="s">
+        <v>214</v>
+      </c>
+      <c r="H47" s="98"/>
+      <c r="I47" s="43"/>
+      <c r="N47" s="97"/>
+      <c r="P47" s="97"/>
+      <c r="Q47" s="97"/>
+      <c r="R47" s="97"/>
+    </row>
+    <row r="48" spans="2:18">
+      <c r="B48" s="99" t="s">
+        <v>166</v>
+      </c>
+      <c r="C48" s="99" t="s">
+        <v>211</v>
+      </c>
+      <c r="D48" s="99" t="s">
+        <v>212</v>
+      </c>
+      <c r="E48" s="99" t="s">
+        <v>209</v>
+      </c>
+      <c r="F48" s="99" t="s">
+        <v>210</v>
+      </c>
+      <c r="G48" s="43" t="s">
+        <v>211</v>
+      </c>
+      <c r="H48" s="43" t="s">
+        <v>212</v>
+      </c>
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="Q48" s="97"/>
+      <c r="R48" s="97"/>
+    </row>
+    <row r="49" spans="2:18">
+      <c r="B49" s="99">
+        <v>1</v>
+      </c>
+      <c r="C49" s="102">
+        <v>350</v>
+      </c>
+      <c r="D49" s="102">
+        <v>430</v>
+      </c>
+      <c r="E49" s="99">
+        <v>4</v>
+      </c>
+      <c r="F49" s="99">
+        <v>13</v>
+      </c>
+      <c r="G49" s="97">
+        <v>380</v>
+      </c>
+      <c r="H49" s="97">
+        <v>460</v>
+      </c>
+      <c r="I49" s="43"/>
+      <c r="J49" s="43"/>
+      <c r="Q49" s="97"/>
+      <c r="R49" s="97"/>
+    </row>
+    <row r="50" spans="2:18">
+      <c r="B50" s="99">
+        <v>2</v>
+      </c>
+      <c r="C50" s="102">
+        <v>490</v>
+      </c>
+      <c r="D50" s="102">
+        <v>700</v>
+      </c>
+      <c r="E50" s="99">
+        <v>2</v>
+      </c>
+      <c r="F50" s="99">
+        <v>18</v>
+      </c>
+      <c r="G50" s="97">
+        <v>530</v>
+      </c>
+      <c r="H50" s="97">
+        <v>750</v>
+      </c>
+      <c r="I50" s="43"/>
+      <c r="J50" s="43"/>
+      <c r="Q50" s="97"/>
+      <c r="R50" s="97"/>
+    </row>
+    <row r="51" spans="2:18">
+      <c r="B51" s="99">
+        <v>3</v>
+      </c>
+      <c r="C51" s="102">
+        <v>720</v>
+      </c>
+      <c r="D51" s="102">
+        <v>1390</v>
+      </c>
+      <c r="E51" s="99">
+        <v>6</v>
+      </c>
+      <c r="F51" s="99">
+        <v>36</v>
+      </c>
+      <c r="G51" s="97">
+        <v>780</v>
+      </c>
+      <c r="H51" s="97">
+        <v>1510</v>
+      </c>
+      <c r="I51" s="43"/>
+      <c r="J51" s="43"/>
+      <c r="Q51" s="97"/>
+      <c r="R51" s="97"/>
+    </row>
+    <row r="52" spans="2:18">
+      <c r="B52" s="99">
+        <v>4</v>
+      </c>
+      <c r="C52" s="102">
+        <v>840</v>
+      </c>
+      <c r="D52" s="102">
+        <v>1120</v>
+      </c>
+      <c r="E52" s="99">
+        <v>3</v>
+      </c>
+      <c r="F52" s="99">
+        <v>16</v>
+      </c>
+      <c r="G52" s="97">
+        <v>920</v>
+      </c>
+      <c r="H52" s="97">
+        <v>1220</v>
+      </c>
+      <c r="I52" s="43"/>
+      <c r="J52" s="43"/>
+      <c r="Q52" s="97"/>
+      <c r="R52" s="97"/>
+    </row>
+    <row r="53" spans="2:18">
+      <c r="B53" s="99">
+        <v>5</v>
+      </c>
+      <c r="C53" s="102">
+        <v>32</v>
+      </c>
+      <c r="D53" s="102">
+        <v>39</v>
+      </c>
+      <c r="E53" s="99">
+        <v>4</v>
+      </c>
+      <c r="F53" s="99">
+        <v>13</v>
+      </c>
+      <c r="G53" s="43">
+        <v>35</v>
+      </c>
+      <c r="H53" s="97">
+        <v>45</v>
+      </c>
+      <c r="I53" s="43"/>
+      <c r="J53" s="97"/>
+      <c r="Q53" s="100"/>
+      <c r="R53" s="100"/>
+    </row>
+    <row r="54" spans="2:18">
+      <c r="B54" s="99">
+        <v>6</v>
+      </c>
+      <c r="C54" s="102">
+        <v>45</v>
+      </c>
+      <c r="D54" s="102">
+        <v>70</v>
+      </c>
+      <c r="E54" s="99">
+        <v>2</v>
+      </c>
+      <c r="F54" s="99">
+        <v>18</v>
+      </c>
+      <c r="G54" s="43">
+        <v>50</v>
+      </c>
+      <c r="H54" s="97">
+        <v>75</v>
+      </c>
+      <c r="I54" s="43"/>
+      <c r="J54" s="97"/>
+      <c r="Q54" s="100"/>
+      <c r="R54" s="100"/>
+    </row>
+    <row r="55" spans="2:18">
+      <c r="B55" s="99">
+        <v>7</v>
+      </c>
+      <c r="C55" s="102">
+        <v>66</v>
+      </c>
+      <c r="D55" s="102">
+        <v>110</v>
+      </c>
+      <c r="E55" s="99">
+        <v>6</v>
+      </c>
+      <c r="F55" s="99">
+        <v>23</v>
+      </c>
+      <c r="G55" s="43">
+        <v>70</v>
+      </c>
+      <c r="H55" s="43">
+        <v>120</v>
+      </c>
+      <c r="I55" s="43"/>
+      <c r="J55" s="97"/>
+      <c r="Q55" s="100"/>
+      <c r="R55" s="100"/>
+    </row>
+    <row r="56" spans="2:18">
+      <c r="B56" s="99">
+        <v>8</v>
+      </c>
+      <c r="C56" s="102">
+        <v>77</v>
+      </c>
+      <c r="D56" s="102">
+        <v>118</v>
+      </c>
+      <c r="E56" s="99">
+        <v>3</v>
+      </c>
+      <c r="F56" s="99">
+        <v>16</v>
+      </c>
+      <c r="G56" s="43">
+        <v>85</v>
+      </c>
+      <c r="H56" s="43">
+        <v>130</v>
+      </c>
+      <c r="I56" s="43"/>
+      <c r="J56" s="97"/>
+      <c r="Q56" s="100"/>
+      <c r="R56" s="100"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -10532,6 +11145,9 @@
     <mergeCell ref="S3:U3"/>
     <mergeCell ref="V3:X3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B26" r:id="rId1" xr:uid="{D2B54FA7-7284-A444-93E2-10BEB7DF1432}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Presenting of questions from all treatments.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C952DFB-4D64-A442-A765-4BFBB703547B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5829F7-270F-134B-B001-90539C3AAAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="4" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -8940,7 +8940,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.70646306116546564</v>
+        <v>0.31687036939276803</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -8960,7 +8960,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.7849673602392585</v>
+        <v>0.53539795407210711</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -8981,7 +8981,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.85625026269514737</v>
+        <v>2.2762603279323668E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -9001,7 +9001,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.6706069433597549</v>
+        <v>0.91985169916371712</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -9077,8 +9077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F6B51D-A4A1-6D46-8F47-1EE4F323E4DF}">
   <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Firebase transaction working to generate unique id.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5829F7-270F-134B-B001-90539C3AAAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F26887-8451-AC4D-8CC8-BD1B811A13AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="4" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -17,13 +17,14 @@
     <sheet name="MCL questions prod" sheetId="10" r:id="rId2"/>
     <sheet name="Web Parameters Dev" sheetId="8" r:id="rId3"/>
     <sheet name="Web Parameters Random" sheetId="11" r:id="rId4"/>
-    <sheet name="Date Delay Paper" sheetId="9" r:id="rId5"/>
-    <sheet name="MCL" sheetId="2" r:id="rId6"/>
-    <sheet name="CL LL Amounts" sheetId="3" r:id="rId7"/>
-    <sheet name="Holden et al." sheetId="4" r:id="rId8"/>
-    <sheet name="Screen Size Zooming" sheetId="5" r:id="rId9"/>
-    <sheet name="Worker Rate" sheetId="7" r:id="rId10"/>
-    <sheet name="Web Parameters v1" sheetId="1" r:id="rId11"/>
+    <sheet name="Latin Square Treatment Order" sheetId="13" r:id="rId5"/>
+    <sheet name="Date Delay Paper" sheetId="9" r:id="rId6"/>
+    <sheet name="MCL" sheetId="2" r:id="rId7"/>
+    <sheet name="CL LL Amounts" sheetId="3" r:id="rId8"/>
+    <sheet name="Holden et al." sheetId="4" r:id="rId9"/>
+    <sheet name="Screen Size Zooming" sheetId="5" r:id="rId10"/>
+    <sheet name="Worker Rate" sheetId="7" r:id="rId11"/>
+    <sheet name="Web Parameters v1" sheetId="1" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MCL questions prod'!$A$1:$X$28</definedName>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="226">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -741,6 +742,21 @@
   </si>
   <si>
     <t>Question 3</t>
+  </si>
+  <si>
+    <t>I used https://cs.uwaterloo.ca/~dmasson/tools/latin_square/ to produce</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>or with numbers</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1019,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1092,6 +1108,24 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1110,8 +1144,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1141,15 +1190,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1164,31 +1204,6 @@
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1528,6 +1543,229 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2E945CF-9189-764F-9A6E-0EEEF9828B80}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="H1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <f>I2/3</f>
+        <v>240</v>
+      </c>
+      <c r="E2">
+        <f>I2/3</f>
+        <v>240</v>
+      </c>
+      <c r="H2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3">
+        <f>I2/3</f>
+        <v>240</v>
+      </c>
+      <c r="E3">
+        <f>I2/3*2</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4">
+        <f>I2/3</f>
+        <v>240</v>
+      </c>
+      <c r="E4">
+        <f>I2/3*3</f>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5">
+        <f>I2/3*2</f>
+        <v>480</v>
+      </c>
+      <c r="E5">
+        <f>I2/3</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6">
+        <f>I2/3*2</f>
+        <v>480</v>
+      </c>
+      <c r="E6">
+        <f>I2/3*2</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7">
+        <f>I2/3*2</f>
+        <v>480</v>
+      </c>
+      <c r="E7">
+        <f>I2/3*3</f>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8">
+        <f>I2/3*3</f>
+        <v>720</v>
+      </c>
+      <c r="E8">
+        <f>I2/3</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9">
+        <f>I2/3*3</f>
+        <v>720</v>
+      </c>
+      <c r="E9">
+        <f>I2/3*2</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <f>I2/3*3</f>
+        <v>720</v>
+      </c>
+      <c r="E10">
+        <f>I2/3*3</f>
+        <v>720</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CC848A2-46C4-BD4C-AFD2-CF7F6FD4ADEE}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1592,7 +1830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86262417-1283-894E-BFF0-F5DD2E135B8D}">
   <dimension ref="A1:V40"/>
   <sheetViews>
@@ -8895,7 +9133,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8940,7 +9178,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.31687036939276803</v>
+        <v>0.37944992435215519</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -8960,7 +9198,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.53539795407210711</v>
+        <v>0.76695502669500826</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -8981,7 +9219,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>2.2762603279323668E-2</v>
+        <v>9.9745012579485204E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -9001,7 +9239,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.91985169916371712</v>
+        <v>3.1217811428308484E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -9074,10 +9312,172 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{804D0482-239B-8D47-86AB-9AF9ADA263D4}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="43">
+        <v>1</v>
+      </c>
+      <c r="B12" s="43">
+        <v>2</v>
+      </c>
+      <c r="C12" s="43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="43">
+        <v>1</v>
+      </c>
+      <c r="B13" s="43">
+        <v>3</v>
+      </c>
+      <c r="C13" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="43">
+        <v>3</v>
+      </c>
+      <c r="B14" s="43">
+        <v>1</v>
+      </c>
+      <c r="C14" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="43">
+        <v>3</v>
+      </c>
+      <c r="B15" s="43">
+        <v>2</v>
+      </c>
+      <c r="C15" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="43">
+        <v>2</v>
+      </c>
+      <c r="B16" s="43">
+        <v>3</v>
+      </c>
+      <c r="C16" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="43">
+        <v>2</v>
+      </c>
+      <c r="B17" s="43">
+        <v>1</v>
+      </c>
+      <c r="C17" s="43">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F6B51D-A4A1-6D46-8F47-1EE4F323E4DF}">
   <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
@@ -9100,48 +9500,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="80" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="68" t="s">
+      <c r="D3" s="81"/>
+      <c r="E3" s="80" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="69"/>
-      <c r="G3" s="68" t="s">
+      <c r="F3" s="81"/>
+      <c r="G3" s="80" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="69"/>
-      <c r="I3" s="68" t="s">
+      <c r="H3" s="81"/>
+      <c r="I3" s="80" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="69"/>
+      <c r="J3" s="81"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="70" t="s">
+      <c r="M3" s="82" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="71"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="70" t="s">
+      <c r="N3" s="83"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="82" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="72"/>
-      <c r="S3" s="70" t="s">
+      <c r="Q3" s="83"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="82" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="71"/>
-      <c r="U3" s="71"/>
-      <c r="V3" s="73" t="s">
+      <c r="T3" s="83"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="85" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="73"/>
-      <c r="X3" s="73"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="85"/>
       <c r="Y3" t="s">
         <v>215</v>
       </c>
@@ -9153,14 +9553,14 @@
         <v>218</v>
       </c>
       <c r="AC3" s="53"/>
-      <c r="AD3" s="104" t="s">
+      <c r="AD3" s="77" t="s">
         <v>220</v>
       </c>
-      <c r="AE3" s="105"/>
-      <c r="AF3" s="104" t="s">
+      <c r="AE3" s="78"/>
+      <c r="AF3" s="77" t="s">
         <v>219</v>
       </c>
-      <c r="AG3" s="105"/>
+      <c r="AG3" s="78"/>
     </row>
     <row r="4" spans="1:33">
       <c r="A4" s="50"/>
@@ -9230,16 +9630,16 @@
       <c r="AC4" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="AD4" s="104" t="s">
+      <c r="AD4" s="77" t="s">
         <v>146</v>
       </c>
-      <c r="AE4" s="105" t="s">
+      <c r="AE4" s="78" t="s">
         <v>147</v>
       </c>
-      <c r="AF4" s="104" t="s">
+      <c r="AF4" s="77" t="s">
         <v>146</v>
       </c>
-      <c r="AG4" s="105" t="s">
+      <c r="AG4" s="78" t="s">
         <v>147</v>
       </c>
     </row>
@@ -9332,35 +9732,35 @@
         <v>1.63</v>
       </c>
       <c r="Z5" s="56">
-        <f>C5/$K$5*$Y$5</f>
+        <f t="shared" ref="Z5:AG5" si="0">C5/$K$5*$Y$5</f>
         <v>376.9375</v>
       </c>
       <c r="AA5" s="42">
-        <f>D5/$K$5*$Y$5</f>
+        <f t="shared" si="0"/>
         <v>458.43749999999994</v>
       </c>
       <c r="AB5" s="37">
-        <f>E5/$K$5*$Y$5</f>
+        <f t="shared" si="0"/>
         <v>529.75</v>
       </c>
       <c r="AC5" s="37">
-        <f>F5/$K$5*$Y$5</f>
+        <f t="shared" si="0"/>
         <v>753.875</v>
       </c>
       <c r="AD5" s="56">
-        <f>G5/$K$5*$Y$5</f>
+        <f t="shared" si="0"/>
         <v>784.4375</v>
       </c>
       <c r="AE5" s="42">
-        <f>H5/$K$5*$Y$5</f>
+        <f t="shared" si="0"/>
         <v>1507.75</v>
       </c>
-      <c r="AF5" s="106">
-        <f>I5/$K$5*$Y$5</f>
+      <c r="AF5" s="37">
+        <f t="shared" si="0"/>
         <v>916.87499999999989</v>
       </c>
-      <c r="AG5" s="106">
-        <f>J5/$K$5*$Y$5</f>
+      <c r="AG5" s="37">
+        <f t="shared" si="0"/>
         <v>1222.5</v>
       </c>
     </row>
@@ -9803,35 +10203,35 @@
         <v>1.63</v>
       </c>
       <c r="Z13" s="56">
-        <f>C13/$K$13*$Y$13</f>
+        <f t="shared" ref="Z13:AG13" si="1">C13/$K$13*$Y$13</f>
         <v>34.462857142857139</v>
       </c>
       <c r="AA13" s="42">
-        <f>D13/$K$13*$Y$13</f>
+        <f t="shared" si="1"/>
         <v>42.84571428571428</v>
       </c>
       <c r="AB13" s="37">
-        <f>E13/$K$13*$Y$13</f>
+        <f t="shared" si="1"/>
         <v>48.434285714285714</v>
       </c>
       <c r="AC13" s="37">
-        <f>F13/$K$13*$Y$13</f>
+        <f t="shared" si="1"/>
         <v>76.377142857142843</v>
       </c>
       <c r="AD13" s="56">
-        <f>G13/$K$13*$Y$13</f>
+        <f t="shared" si="1"/>
         <v>71.72</v>
       </c>
       <c r="AE13" s="42">
-        <f>H13/$K$13*$Y$13</f>
+        <f t="shared" si="1"/>
         <v>119.22285714285712</v>
       </c>
-      <c r="AF13" s="106">
-        <f>I13/$K$13*$Y$13</f>
+      <c r="AF13" s="37">
+        <f t="shared" si="1"/>
         <v>83.828571428571422</v>
       </c>
-      <c r="AG13" s="106">
-        <f>J13/$K$13*$Y$13</f>
+      <c r="AG13" s="37">
+        <f t="shared" si="1"/>
         <v>128.53714285714287</v>
       </c>
     </row>
@@ -10042,35 +10442,35 @@
         <v>1.63</v>
       </c>
       <c r="Z17" s="56">
-        <f>C17/$K$17*$Y$17</f>
+        <f t="shared" ref="Z17:AG17" si="2">C17/$K$17*$Y$17</f>
         <v>862.94117647058818</v>
       </c>
       <c r="AA17" s="42">
-        <f>D17/$K$17*$Y$17</f>
+        <f t="shared" si="2"/>
         <v>1150.5882352941176</v>
       </c>
       <c r="AB17" s="37">
-        <f>E17/$K$17*$Y$17</f>
+        <f t="shared" si="2"/>
         <v>719.11764705882354</v>
       </c>
       <c r="AC17" s="37">
-        <f>F17/$K$17*$Y$17</f>
+        <f t="shared" si="2"/>
         <v>1917.6470588235293</v>
       </c>
       <c r="AD17" s="56">
-        <f>G17/$K$17*$Y$17</f>
+        <f t="shared" si="2"/>
         <v>498.58823529411762</v>
       </c>
       <c r="AE17" s="42">
-        <f>H17/$K$17*$Y$17</f>
+        <f t="shared" si="2"/>
         <v>747.88235294117635</v>
       </c>
-      <c r="AF17" s="106">
-        <f>I17/$K$17*$Y$17</f>
+      <c r="AF17" s="37">
+        <f t="shared" si="2"/>
         <v>445.85294117647061</v>
       </c>
       <c r="AG17" s="37">
-        <f>J17/$K$17*$Y$17</f>
+        <f t="shared" si="2"/>
         <v>834.17647058823525</v>
       </c>
     </row>
@@ -10199,7 +10599,7 @@
       </c>
     </row>
     <row r="26" spans="1:33">
-      <c r="B26" s="95" t="s">
+      <c r="B26" s="68" t="s">
         <v>155</v>
       </c>
     </row>
@@ -10220,16 +10620,16 @@
       </c>
     </row>
     <row r="29" spans="1:33">
-      <c r="C29" s="74" t="s">
+      <c r="C29" s="79" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74" t="s">
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="79" t="s">
         <v>169</v>
       </c>
-      <c r="G29" s="74"/>
-      <c r="H29" s="74"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="79"/>
       <c r="J29" t="s">
         <v>168</v>
       </c>
@@ -10339,7 +10739,7 @@
         <v>13</v>
       </c>
       <c r="Q31" s="37">
-        <f t="shared" ref="Q31:Q42" si="0">K31/$C$28</f>
+        <f t="shared" ref="Q31:Q42" si="3">K31/$C$28</f>
         <v>2.3648648648648649</v>
       </c>
       <c r="R31" s="37">
@@ -10398,7 +10798,7 @@
         <v>18</v>
       </c>
       <c r="Q32" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.310810810810811</v>
       </c>
       <c r="R32" s="37">
@@ -10458,7 +10858,7 @@
         <v>36</v>
       </c>
       <c r="Q33" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4.8648648648648649</v>
       </c>
       <c r="R33" s="37">
@@ -10517,7 +10917,7 @@
         <v>16</v>
       </c>
       <c r="Q34" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5.6756756756756754</v>
       </c>
       <c r="R34" s="37">
@@ -10554,7 +10954,7 @@
         <v>13</v>
       </c>
       <c r="Q35" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>78.378378378378372</v>
       </c>
       <c r="R35" s="11">
@@ -10590,7 +10990,7 @@
         <v>18</v>
       </c>
       <c r="Q36" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>110.13513513513513</v>
       </c>
       <c r="R36" s="11">
@@ -10626,7 +11026,7 @@
         <v>36</v>
       </c>
       <c r="Q37" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>162.16216216216216</v>
       </c>
       <c r="R37" s="11">
@@ -10662,7 +11062,7 @@
         <v>16</v>
       </c>
       <c r="Q38" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>189.18918918918919</v>
       </c>
       <c r="R38" s="11">
@@ -10706,7 +11106,7 @@
         <v>13</v>
       </c>
       <c r="Q39" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.21621621621621623</v>
       </c>
       <c r="R39" s="11">
@@ -10751,7 +11151,7 @@
         <v>18</v>
       </c>
       <c r="Q40" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.30405405405405406</v>
       </c>
       <c r="R40" s="11">
@@ -10795,7 +11195,7 @@
         <v>23</v>
       </c>
       <c r="Q41" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.44594594594594594</v>
       </c>
       <c r="R41" s="11">
@@ -10839,7 +11239,7 @@
         <v>16</v>
       </c>
       <c r="Q42" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.52027027027027029</v>
       </c>
       <c r="R42" s="11">
@@ -10854,7 +11254,7 @@
     </row>
     <row r="46" spans="2:18">
       <c r="B46" s="43"/>
-      <c r="C46" s="96"/>
+      <c r="C46" s="69"/>
       <c r="D46" s="43"/>
       <c r="E46" s="43"/>
       <c r="F46" s="43"/>
@@ -10864,45 +11264,45 @@
       <c r="J46" s="43"/>
       <c r="K46" s="43"/>
       <c r="L46" s="43"/>
-      <c r="M46" s="97"/>
-      <c r="N46" s="97"/>
-      <c r="O46" s="97"/>
-      <c r="P46" s="97"/>
-      <c r="Q46" s="97"/>
-      <c r="R46" s="97"/>
+      <c r="M46" s="70"/>
+      <c r="N46" s="70"/>
+      <c r="O46" s="70"/>
+      <c r="P46" s="70"/>
+      <c r="Q46" s="70"/>
+      <c r="R46" s="70"/>
     </row>
     <row r="47" spans="2:18">
       <c r="B47" s="43"/>
-      <c r="C47" s="99" t="s">
+      <c r="C47" s="72" t="s">
         <v>213</v>
       </c>
-      <c r="D47" s="99"/>
-      <c r="E47" s="101"/>
-      <c r="F47" s="98"/>
-      <c r="G47" s="103" t="s">
+      <c r="D47" s="72"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="71"/>
+      <c r="G47" s="76" t="s">
         <v>214</v>
       </c>
-      <c r="H47" s="98"/>
+      <c r="H47" s="71"/>
       <c r="I47" s="43"/>
-      <c r="N47" s="97"/>
-      <c r="P47" s="97"/>
-      <c r="Q47" s="97"/>
-      <c r="R47" s="97"/>
+      <c r="N47" s="70"/>
+      <c r="P47" s="70"/>
+      <c r="Q47" s="70"/>
+      <c r="R47" s="70"/>
     </row>
     <row r="48" spans="2:18">
-      <c r="B48" s="99" t="s">
+      <c r="B48" s="72" t="s">
         <v>166</v>
       </c>
-      <c r="C48" s="99" t="s">
+      <c r="C48" s="72" t="s">
         <v>211</v>
       </c>
-      <c r="D48" s="99" t="s">
+      <c r="D48" s="72" t="s">
         <v>212</v>
       </c>
-      <c r="E48" s="99" t="s">
+      <c r="E48" s="72" t="s">
         <v>209</v>
       </c>
-      <c r="F48" s="99" t="s">
+      <c r="F48" s="72" t="s">
         <v>210</v>
       </c>
       <c r="G48" s="43" t="s">
@@ -10913,185 +11313,185 @@
       </c>
       <c r="I48" s="43"/>
       <c r="J48" s="43"/>
-      <c r="Q48" s="97"/>
-      <c r="R48" s="97"/>
+      <c r="Q48" s="70"/>
+      <c r="R48" s="70"/>
     </row>
     <row r="49" spans="2:18">
-      <c r="B49" s="99">
-        <v>1</v>
-      </c>
-      <c r="C49" s="102">
+      <c r="B49" s="72">
+        <v>1</v>
+      </c>
+      <c r="C49" s="75">
         <v>350</v>
       </c>
-      <c r="D49" s="102">
+      <c r="D49" s="75">
         <v>430</v>
       </c>
-      <c r="E49" s="99">
+      <c r="E49" s="72">
         <v>4</v>
       </c>
-      <c r="F49" s="99">
+      <c r="F49" s="72">
         <v>13</v>
       </c>
-      <c r="G49" s="97">
+      <c r="G49" s="70">
         <v>380</v>
       </c>
-      <c r="H49" s="97">
+      <c r="H49" s="70">
         <v>460</v>
       </c>
       <c r="I49" s="43"/>
       <c r="J49" s="43"/>
-      <c r="Q49" s="97"/>
-      <c r="R49" s="97"/>
+      <c r="Q49" s="70"/>
+      <c r="R49" s="70"/>
     </row>
     <row r="50" spans="2:18">
-      <c r="B50" s="99">
+      <c r="B50" s="72">
         <v>2</v>
       </c>
-      <c r="C50" s="102">
+      <c r="C50" s="75">
         <v>490</v>
       </c>
-      <c r="D50" s="102">
+      <c r="D50" s="75">
         <v>700</v>
       </c>
-      <c r="E50" s="99">
+      <c r="E50" s="72">
         <v>2</v>
       </c>
-      <c r="F50" s="99">
+      <c r="F50" s="72">
         <v>18</v>
       </c>
-      <c r="G50" s="97">
+      <c r="G50" s="70">
         <v>530</v>
       </c>
-      <c r="H50" s="97">
+      <c r="H50" s="70">
         <v>750</v>
       </c>
       <c r="I50" s="43"/>
       <c r="J50" s="43"/>
-      <c r="Q50" s="97"/>
-      <c r="R50" s="97"/>
+      <c r="Q50" s="70"/>
+      <c r="R50" s="70"/>
     </row>
     <row r="51" spans="2:18">
-      <c r="B51" s="99">
+      <c r="B51" s="72">
         <v>3</v>
       </c>
-      <c r="C51" s="102">
+      <c r="C51" s="75">
         <v>720</v>
       </c>
-      <c r="D51" s="102">
+      <c r="D51" s="75">
         <v>1390</v>
       </c>
-      <c r="E51" s="99">
+      <c r="E51" s="72">
         <v>6</v>
       </c>
-      <c r="F51" s="99">
+      <c r="F51" s="72">
         <v>36</v>
       </c>
-      <c r="G51" s="97">
+      <c r="G51" s="70">
         <v>780</v>
       </c>
-      <c r="H51" s="97">
+      <c r="H51" s="70">
         <v>1510</v>
       </c>
       <c r="I51" s="43"/>
       <c r="J51" s="43"/>
-      <c r="Q51" s="97"/>
-      <c r="R51" s="97"/>
+      <c r="Q51" s="70"/>
+      <c r="R51" s="70"/>
     </row>
     <row r="52" spans="2:18">
-      <c r="B52" s="99">
+      <c r="B52" s="72">
         <v>4</v>
       </c>
-      <c r="C52" s="102">
+      <c r="C52" s="75">
         <v>840</v>
       </c>
-      <c r="D52" s="102">
+      <c r="D52" s="75">
         <v>1120</v>
       </c>
-      <c r="E52" s="99">
+      <c r="E52" s="72">
         <v>3</v>
       </c>
-      <c r="F52" s="99">
+      <c r="F52" s="72">
         <v>16</v>
       </c>
-      <c r="G52" s="97">
+      <c r="G52" s="70">
         <v>920</v>
       </c>
-      <c r="H52" s="97">
+      <c r="H52" s="70">
         <v>1220</v>
       </c>
       <c r="I52" s="43"/>
       <c r="J52" s="43"/>
-      <c r="Q52" s="97"/>
-      <c r="R52" s="97"/>
+      <c r="Q52" s="70"/>
+      <c r="R52" s="70"/>
     </row>
     <row r="53" spans="2:18">
-      <c r="B53" s="99">
+      <c r="B53" s="72">
         <v>5</v>
       </c>
-      <c r="C53" s="102">
+      <c r="C53" s="75">
         <v>32</v>
       </c>
-      <c r="D53" s="102">
+      <c r="D53" s="75">
         <v>39</v>
       </c>
-      <c r="E53" s="99">
+      <c r="E53" s="72">
         <v>4</v>
       </c>
-      <c r="F53" s="99">
+      <c r="F53" s="72">
         <v>13</v>
       </c>
       <c r="G53" s="43">
         <v>35</v>
       </c>
-      <c r="H53" s="97">
+      <c r="H53" s="70">
         <v>45</v>
       </c>
       <c r="I53" s="43"/>
-      <c r="J53" s="97"/>
-      <c r="Q53" s="100"/>
-      <c r="R53" s="100"/>
+      <c r="J53" s="70"/>
+      <c r="Q53" s="73"/>
+      <c r="R53" s="73"/>
     </row>
     <row r="54" spans="2:18">
-      <c r="B54" s="99">
+      <c r="B54" s="72">
         <v>6</v>
       </c>
-      <c r="C54" s="102">
+      <c r="C54" s="75">
         <v>45</v>
       </c>
-      <c r="D54" s="102">
+      <c r="D54" s="75">
         <v>70</v>
       </c>
-      <c r="E54" s="99">
+      <c r="E54" s="72">
         <v>2</v>
       </c>
-      <c r="F54" s="99">
+      <c r="F54" s="72">
         <v>18</v>
       </c>
       <c r="G54" s="43">
         <v>50</v>
       </c>
-      <c r="H54" s="97">
+      <c r="H54" s="70">
         <v>75</v>
       </c>
       <c r="I54" s="43"/>
-      <c r="J54" s="97"/>
-      <c r="Q54" s="100"/>
-      <c r="R54" s="100"/>
+      <c r="J54" s="70"/>
+      <c r="Q54" s="73"/>
+      <c r="R54" s="73"/>
     </row>
     <row r="55" spans="2:18">
-      <c r="B55" s="99">
+      <c r="B55" s="72">
         <v>7</v>
       </c>
-      <c r="C55" s="102">
+      <c r="C55" s="75">
         <v>66</v>
       </c>
-      <c r="D55" s="102">
+      <c r="D55" s="75">
         <v>110</v>
       </c>
-      <c r="E55" s="99">
+      <c r="E55" s="72">
         <v>6</v>
       </c>
-      <c r="F55" s="99">
+      <c r="F55" s="72">
         <v>23</v>
       </c>
       <c r="G55" s="43">
@@ -11101,24 +11501,24 @@
         <v>120</v>
       </c>
       <c r="I55" s="43"/>
-      <c r="J55" s="97"/>
-      <c r="Q55" s="100"/>
-      <c r="R55" s="100"/>
+      <c r="J55" s="70"/>
+      <c r="Q55" s="73"/>
+      <c r="R55" s="73"/>
     </row>
     <row r="56" spans="2:18">
-      <c r="B56" s="99">
+      <c r="B56" s="72">
         <v>8</v>
       </c>
-      <c r="C56" s="102">
+      <c r="C56" s="75">
         <v>77</v>
       </c>
-      <c r="D56" s="102">
-        <v>118</v>
-      </c>
-      <c r="E56" s="99">
+      <c r="D56" s="75">
+        <v>118</v>
+      </c>
+      <c r="E56" s="72">
         <v>3</v>
       </c>
-      <c r="F56" s="99">
+      <c r="F56" s="72">
         <v>16</v>
       </c>
       <c r="G56" s="43">
@@ -11128,22 +11528,22 @@
         <v>130</v>
       </c>
       <c r="I56" s="43"/>
-      <c r="J56" s="97"/>
-      <c r="Q56" s="100"/>
-      <c r="R56" s="100"/>
+      <c r="J56" s="70"/>
+      <c r="Q56" s="73"/>
+      <c r="R56" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B26" r:id="rId1" xr:uid="{D2B54FA7-7284-A444-93E2-10BEB7DF1432}"/>
@@ -11152,7 +11552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172F3C91-0245-C642-8607-0C1863490763}">
   <dimension ref="A1:AA22"/>
   <sheetViews>
@@ -11183,105 +11583,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="75" t="s">
+      <c r="A2" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="75" t="s">
+      <c r="C2" s="93"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="76"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="84" t="s">
+      <c r="F2" s="93"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="90" t="s">
+      <c r="I2" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="90" t="s">
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="90"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="84" t="s">
+      <c r="S2" s="104"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="84" t="s">
+      <c r="W2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="92" t="s">
+      <c r="X2" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="92" t="s">
+      <c r="Y2" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="92" t="s">
+      <c r="Z2" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="92" t="s">
+      <c r="AA2" s="86" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="82"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="91" t="s">
+      <c r="A3" s="99"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89" t="s">
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89" t="s">
+      <c r="M3" s="103"/>
+      <c r="N3" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89" t="s">
+      <c r="O3" s="103"/>
+      <c r="P3" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="87" t="s">
+      <c r="Q3" s="103"/>
+      <c r="R3" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="87" t="s">
+      <c r="S3" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="87" t="s">
+      <c r="T3" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="87" t="s">
+      <c r="U3" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="85"/>
-      <c r="W3" s="85"/>
-      <c r="X3" s="93"/>
-      <c r="Y3" s="93"/>
-      <c r="Z3" s="93"/>
-      <c r="AA3" s="93"/>
+      <c r="V3" s="90"/>
+      <c r="W3" s="90"/>
+      <c r="X3" s="87"/>
+      <c r="Y3" s="87"/>
+      <c r="Z3" s="87"/>
+      <c r="AA3" s="87"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="83"/>
+      <c r="A4" s="100"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -11300,7 +11700,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="86"/>
+      <c r="H4" s="91"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -11328,16 +11728,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="86"/>
-      <c r="X4" s="94"/>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="94"/>
-      <c r="AA4" s="93"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="102"/>
+      <c r="V4" s="91"/>
+      <c r="W4" s="91"/>
+      <c r="X4" s="88"/>
+      <c r="Y4" s="88"/>
+      <c r="Z4" s="88"/>
+      <c r="AA4" s="87"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -11838,11 +12238,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -11858,13 +12253,18 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE45FD6-E248-1447-95F1-A5D07360E1EE}">
   <dimension ref="A1:H19"/>
   <sheetViews>
@@ -12335,7 +12735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E1E67AD-5D17-8649-BBCA-56D0D08542BD}">
   <dimension ref="A1:O38"/>
   <sheetViews>
@@ -12725,227 +13125,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2E945CF-9189-764F-9A6E-0EEEF9828B80}">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="16" customHeight="1">
-      <c r="A1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="7"/>
-      <c r="H1" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1">
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2">
-        <f>I2/3</f>
-        <v>240</v>
-      </c>
-      <c r="E2">
-        <f>I2/3</f>
-        <v>240</v>
-      </c>
-      <c r="H2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3">
-        <f>I2/3</f>
-        <v>240</v>
-      </c>
-      <c r="E3">
-        <f>I2/3*2</f>
-        <v>480</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4">
-        <f>I2/3</f>
-        <v>240</v>
-      </c>
-      <c r="E4">
-        <f>I2/3*3</f>
-        <v>720</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5">
-        <f>I2/3*2</f>
-        <v>480</v>
-      </c>
-      <c r="E5">
-        <f>I2/3</f>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6">
-        <f>I2/3*2</f>
-        <v>480</v>
-      </c>
-      <c r="E6">
-        <f>I2/3*2</f>
-        <v>480</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>9</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7">
-        <f>I2/3*2</f>
-        <v>480</v>
-      </c>
-      <c r="E7">
-        <f>I2/3*3</f>
-        <v>720</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8">
-        <f>I2/3*3</f>
-        <v>720</v>
-      </c>
-      <c r="E8">
-        <f>I2/3</f>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>6</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9">
-        <f>I2/3*3</f>
-        <v>720</v>
-      </c>
-      <c r="E9">
-        <f>I2/3*2</f>
-        <v>480</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10">
-        <f>I2/3*3</f>
-        <v>720</v>
-      </c>
-      <c r="E10">
-        <f>I2/3*3</f>
-        <v>720</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Latest changes before loading all treatments.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F26887-8451-AC4D-8CC8-BD1B811A13AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A567B8E-857A-5F4C-AA31-26B4BAACBC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="4" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
@@ -1123,9 +1123,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1144,23 +1141,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1190,6 +1172,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1203,6 +1194,15 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1521,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A1C2A0-9A4B-1A4B-A6D5-91595022903D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9178,7 +9178,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.37944992435215519</v>
+        <v>0.46959523077672327</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -9198,7 +9198,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.76695502669500826</v>
+        <v>0.52580876556960365</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -9219,7 +9219,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>9.9745012579485204E-2</v>
+        <v>0.80411740627482142</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -9239,7 +9239,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>3.1217811428308484E-2</v>
+        <v>0.50578498358851542</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -9315,7 +9315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{804D0482-239B-8D47-86AB-9AF9ADA263D4}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12:C17"/>
     </sheetView>
   </sheetViews>
@@ -9500,48 +9500,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="80" t="s">
+      <c r="C3" s="79" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="81"/>
-      <c r="E3" s="80" t="s">
+      <c r="D3" s="80"/>
+      <c r="E3" s="79" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="81"/>
-      <c r="G3" s="80" t="s">
+      <c r="F3" s="80"/>
+      <c r="G3" s="79" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="81"/>
-      <c r="I3" s="80" t="s">
+      <c r="H3" s="80"/>
+      <c r="I3" s="79" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="81"/>
+      <c r="J3" s="80"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="82" t="s">
+      <c r="M3" s="81" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="83"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="82" t="s">
+      <c r="N3" s="82"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="81" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="83"/>
-      <c r="R3" s="84"/>
-      <c r="S3" s="82" t="s">
+      <c r="Q3" s="82"/>
+      <c r="R3" s="83"/>
+      <c r="S3" s="81" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="83"/>
-      <c r="U3" s="83"/>
-      <c r="V3" s="85" t="s">
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="84" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="85"/>
-      <c r="X3" s="85"/>
+      <c r="W3" s="84"/>
+      <c r="X3" s="84"/>
       <c r="Y3" t="s">
         <v>215</v>
       </c>
@@ -10620,16 +10620,16 @@
       </c>
     </row>
     <row r="29" spans="1:33">
-      <c r="C29" s="79" t="s">
+      <c r="C29" s="85" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="79"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="79" t="s">
+      <c r="D29" s="85"/>
+      <c r="E29" s="85"/>
+      <c r="F29" s="85" t="s">
         <v>169</v>
       </c>
-      <c r="G29" s="79"/>
-      <c r="H29" s="79"/>
+      <c r="G29" s="85"/>
+      <c r="H29" s="85"/>
       <c r="J29" t="s">
         <v>168</v>
       </c>
@@ -11534,16 +11534,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="P3:R3"/>
     <mergeCell ref="S3:U3"/>
     <mergeCell ref="V3:X3"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B26" r:id="rId1" xr:uid="{D2B54FA7-7284-A444-93E2-10BEB7DF1432}"/>
@@ -11583,105 +11583,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="98" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="92" t="s">
+      <c r="A2" s="92" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="92" t="s">
+      <c r="C2" s="87"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="93"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="89" t="s">
+      <c r="F2" s="87"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="104"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="104"/>
-      <c r="M2" s="104"/>
-      <c r="N2" s="104"/>
-      <c r="O2" s="104"/>
-      <c r="P2" s="104"/>
-      <c r="Q2" s="104"/>
-      <c r="R2" s="104" t="s">
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="101"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="104"/>
-      <c r="T2" s="104"/>
-      <c r="U2" s="104"/>
-      <c r="V2" s="89" t="s">
+      <c r="S2" s="101"/>
+      <c r="T2" s="101"/>
+      <c r="U2" s="101"/>
+      <c r="V2" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="89" t="s">
+      <c r="W2" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="86" t="s">
+      <c r="X2" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="86" t="s">
+      <c r="Y2" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="86" t="s">
+      <c r="Z2" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="86" t="s">
+      <c r="AA2" s="103" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="99"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="105" t="s">
+      <c r="A3" s="93"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="103"/>
-      <c r="K3" s="103"/>
-      <c r="L3" s="103" t="s">
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="103"/>
-      <c r="N3" s="103" t="s">
+      <c r="M3" s="100"/>
+      <c r="N3" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="103"/>
-      <c r="P3" s="103" t="s">
+      <c r="O3" s="100"/>
+      <c r="P3" s="100" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="103"/>
-      <c r="R3" s="101" t="s">
+      <c r="Q3" s="100"/>
+      <c r="R3" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="101" t="s">
+      <c r="S3" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="101" t="s">
+      <c r="T3" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="101" t="s">
+      <c r="U3" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="90"/>
-      <c r="W3" s="90"/>
-      <c r="X3" s="87"/>
-      <c r="Y3" s="87"/>
-      <c r="Z3" s="87"/>
-      <c r="AA3" s="87"/>
+      <c r="V3" s="96"/>
+      <c r="W3" s="96"/>
+      <c r="X3" s="104"/>
+      <c r="Y3" s="104"/>
+      <c r="Z3" s="104"/>
+      <c r="AA3" s="104"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="100"/>
+      <c r="A4" s="94"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -11700,7 +11700,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="91"/>
+      <c r="H4" s="97"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -11728,16 +11728,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="102"/>
-      <c r="S4" s="102"/>
-      <c r="T4" s="102"/>
-      <c r="U4" s="102"/>
-      <c r="V4" s="91"/>
-      <c r="W4" s="91"/>
-      <c r="X4" s="88"/>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="88"/>
-      <c r="AA4" s="87"/>
+      <c r="R4" s="99"/>
+      <c r="S4" s="99"/>
+      <c r="T4" s="99"/>
+      <c r="U4" s="99"/>
+      <c r="V4" s="97"/>
+      <c r="W4" s="97"/>
+      <c r="X4" s="105"/>
+      <c r="Y4" s="105"/>
+      <c r="Z4" s="105"/>
+      <c r="AA4" s="104"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -12238,6 +12238,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -12253,11 +12258,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Refactored to support in subject study.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A567B8E-857A-5F4C-AA31-26B4BAACBC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33122EE-DD79-1647-A171-A61518E06A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="1" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
@@ -1123,6 +1123,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1141,8 +1144,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1172,15 +1190,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1194,15 +1203,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1521,7 +1521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A1C2A0-9A4B-1A4B-A6D5-91595022903D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -3510,7 +3510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6462F7B1-F956-1241-A84D-BB94A5075354}">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
@@ -9178,7 +9178,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.46959523077672327</v>
+        <v>0.33184581816253522</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -9198,7 +9198,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.52580876556960365</v>
+        <v>6.0663915074302133E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -9219,7 +9219,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.80411740627482142</v>
+        <v>0.28793463357627902</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -9239,7 +9239,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.50578498358851542</v>
+        <v>0.58553950496263141</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -9500,48 +9500,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="80" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="80"/>
-      <c r="E3" s="79" t="s">
+      <c r="D3" s="81"/>
+      <c r="E3" s="80" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="80"/>
-      <c r="G3" s="79" t="s">
+      <c r="F3" s="81"/>
+      <c r="G3" s="80" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="80"/>
-      <c r="I3" s="79" t="s">
+      <c r="H3" s="81"/>
+      <c r="I3" s="80" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="80"/>
+      <c r="J3" s="81"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="81" t="s">
+      <c r="M3" s="82" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="82"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="81" t="s">
+      <c r="N3" s="83"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="82" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="82"/>
-      <c r="R3" s="83"/>
-      <c r="S3" s="81" t="s">
+      <c r="Q3" s="83"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="82" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="82"/>
-      <c r="U3" s="82"/>
-      <c r="V3" s="84" t="s">
+      <c r="T3" s="83"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="85" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="84"/>
-      <c r="X3" s="84"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="85"/>
       <c r="Y3" t="s">
         <v>215</v>
       </c>
@@ -10620,16 +10620,16 @@
       </c>
     </row>
     <row r="29" spans="1:33">
-      <c r="C29" s="85" t="s">
+      <c r="C29" s="79" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="85"/>
-      <c r="E29" s="85"/>
-      <c r="F29" s="85" t="s">
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="79" t="s">
         <v>169</v>
       </c>
-      <c r="G29" s="85"/>
-      <c r="H29" s="85"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="79"/>
       <c r="J29" t="s">
         <v>168</v>
       </c>
@@ -11534,16 +11534,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B26" r:id="rId1" xr:uid="{D2B54FA7-7284-A444-93E2-10BEB7DF1432}"/>
@@ -11583,105 +11583,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="86" t="s">
+      <c r="A2" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="86" t="s">
+      <c r="C2" s="93"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="87"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="95" t="s">
+      <c r="F2" s="93"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="101" t="s">
+      <c r="I2" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
-      <c r="M2" s="101"/>
-      <c r="N2" s="101"/>
-      <c r="O2" s="101"/>
-      <c r="P2" s="101"/>
-      <c r="Q2" s="101"/>
-      <c r="R2" s="101" t="s">
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="101"/>
-      <c r="T2" s="101"/>
-      <c r="U2" s="101"/>
-      <c r="V2" s="95" t="s">
+      <c r="S2" s="104"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="95" t="s">
+      <c r="W2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="103" t="s">
+      <c r="X2" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="103" t="s">
+      <c r="Y2" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="103" t="s">
+      <c r="Z2" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="103" t="s">
+      <c r="AA2" s="86" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="93"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="102" t="s">
+      <c r="A3" s="99"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
-      <c r="L3" s="100" t="s">
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="100"/>
-      <c r="N3" s="100" t="s">
+      <c r="M3" s="103"/>
+      <c r="N3" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="100"/>
-      <c r="P3" s="100" t="s">
+      <c r="O3" s="103"/>
+      <c r="P3" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="100"/>
-      <c r="R3" s="98" t="s">
+      <c r="Q3" s="103"/>
+      <c r="R3" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="98" t="s">
+      <c r="S3" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="98" t="s">
+      <c r="T3" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="98" t="s">
+      <c r="U3" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="96"/>
-      <c r="W3" s="96"/>
-      <c r="X3" s="104"/>
-      <c r="Y3" s="104"/>
-      <c r="Z3" s="104"/>
-      <c r="AA3" s="104"/>
+      <c r="V3" s="90"/>
+      <c r="W3" s="90"/>
+      <c r="X3" s="87"/>
+      <c r="Y3" s="87"/>
+      <c r="Z3" s="87"/>
+      <c r="AA3" s="87"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="94"/>
+      <c r="A4" s="100"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -11700,7 +11700,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="97"/>
+      <c r="H4" s="91"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -11728,16 +11728,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="99"/>
-      <c r="S4" s="99"/>
-      <c r="T4" s="99"/>
-      <c r="U4" s="99"/>
-      <c r="V4" s="97"/>
-      <c r="W4" s="97"/>
-      <c r="X4" s="105"/>
-      <c r="Y4" s="105"/>
-      <c r="Z4" s="105"/>
-      <c r="AA4" s="104"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="102"/>
+      <c r="V4" s="91"/>
+      <c r="W4" s="91"/>
+      <c r="X4" s="88"/>
+      <c r="Y4" s="88"/>
+      <c r="Z4" s="88"/>
+      <c r="AA4" s="87"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -12238,11 +12238,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -12258,6 +12253,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Debrief text is specific to treatment.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33122EE-DD79-1647-A171-A61518E06A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DA6479-C8FC-5146-97F0-A51AB0FB5CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="1" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="2" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="227">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -757,6 +757,9 @@
   </si>
   <si>
     <t>or with numbers</t>
+  </si>
+  <si>
+    <t>random</t>
   </si>
 </sst>
 </file>
@@ -1123,9 +1126,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1144,23 +1144,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1190,6 +1175,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1203,6 +1197,15 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3510,7 +3513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6462F7B1-F956-1241-A84D-BB94A5075354}">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
@@ -4845,11 +4848,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:X88"/>
+  <dimension ref="A1:X115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I71" sqref="I71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V125" sqref="V125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -9122,6 +9125,1230 @@
         <v>185</v>
       </c>
     </row>
+    <row r="89" spans="1:24">
+      <c r="A89">
+        <v>23</v>
+      </c>
+      <c r="B89" t="s">
+        <v>226</v>
+      </c>
+      <c r="C89" t="s">
+        <v>120</v>
+      </c>
+      <c r="D89" t="s">
+        <v>118</v>
+      </c>
+      <c r="E89" t="s">
+        <v>118</v>
+      </c>
+      <c r="F89">
+        <v>350</v>
+      </c>
+      <c r="G89">
+        <v>4</v>
+      </c>
+      <c r="H89"/>
+      <c r="I89">
+        <v>430</v>
+      </c>
+      <c r="J89">
+        <v>13</v>
+      </c>
+      <c r="K89"/>
+      <c r="L89">
+        <v>430</v>
+      </c>
+      <c r="X89" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24">
+      <c r="A90">
+        <v>23</v>
+      </c>
+      <c r="B90" t="s">
+        <v>226</v>
+      </c>
+      <c r="C90" t="s">
+        <v>120</v>
+      </c>
+      <c r="D90" t="s">
+        <v>118</v>
+      </c>
+      <c r="E90" t="s">
+        <v>118</v>
+      </c>
+      <c r="F90">
+        <v>490</v>
+      </c>
+      <c r="G90">
+        <v>2</v>
+      </c>
+      <c r="H90"/>
+      <c r="I90">
+        <v>700</v>
+      </c>
+      <c r="J90">
+        <v>18</v>
+      </c>
+      <c r="K90"/>
+      <c r="L90">
+        <v>700</v>
+      </c>
+      <c r="X90" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:24">
+      <c r="A91">
+        <v>23</v>
+      </c>
+      <c r="B91" t="s">
+        <v>226</v>
+      </c>
+      <c r="C91" t="s">
+        <v>120</v>
+      </c>
+      <c r="D91" t="s">
+        <v>118</v>
+      </c>
+      <c r="E91" t="s">
+        <v>118</v>
+      </c>
+      <c r="F91">
+        <v>720</v>
+      </c>
+      <c r="G91">
+        <v>6</v>
+      </c>
+      <c r="H91"/>
+      <c r="I91">
+        <v>1390</v>
+      </c>
+      <c r="J91">
+        <v>24</v>
+      </c>
+      <c r="K91"/>
+      <c r="L91">
+        <v>1390</v>
+      </c>
+      <c r="X91" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="92" spans="1:24">
+      <c r="A92">
+        <v>23</v>
+      </c>
+      <c r="B92" t="s">
+        <v>226</v>
+      </c>
+      <c r="C92" t="s">
+        <v>120</v>
+      </c>
+      <c r="D92" t="s">
+        <v>118</v>
+      </c>
+      <c r="E92" t="s">
+        <v>118</v>
+      </c>
+      <c r="F92">
+        <v>840</v>
+      </c>
+      <c r="G92">
+        <v>3</v>
+      </c>
+      <c r="H92"/>
+      <c r="I92">
+        <v>1120</v>
+      </c>
+      <c r="J92">
+        <v>16</v>
+      </c>
+      <c r="K92"/>
+      <c r="L92">
+        <v>1120</v>
+      </c>
+      <c r="X92" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24">
+      <c r="A93">
+        <v>23</v>
+      </c>
+      <c r="B93" t="s">
+        <v>226</v>
+      </c>
+      <c r="C93" t="s">
+        <v>120</v>
+      </c>
+      <c r="D93" t="s">
+        <v>118</v>
+      </c>
+      <c r="E93" t="s">
+        <v>118</v>
+      </c>
+      <c r="F93">
+        <v>32</v>
+      </c>
+      <c r="G93">
+        <v>4</v>
+      </c>
+      <c r="H93"/>
+      <c r="I93">
+        <v>39</v>
+      </c>
+      <c r="J93">
+        <v>13</v>
+      </c>
+      <c r="K93"/>
+      <c r="L93">
+        <v>40</v>
+      </c>
+      <c r="X93" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24">
+      <c r="A94">
+        <v>23</v>
+      </c>
+      <c r="B94" t="s">
+        <v>226</v>
+      </c>
+      <c r="C94" t="s">
+        <v>120</v>
+      </c>
+      <c r="D94" t="s">
+        <v>118</v>
+      </c>
+      <c r="E94" t="s">
+        <v>118</v>
+      </c>
+      <c r="F94">
+        <v>45</v>
+      </c>
+      <c r="G94">
+        <v>2</v>
+      </c>
+      <c r="H94"/>
+      <c r="I94">
+        <v>70</v>
+      </c>
+      <c r="J94">
+        <v>18</v>
+      </c>
+      <c r="K94"/>
+      <c r="L94">
+        <v>70</v>
+      </c>
+      <c r="X94" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24">
+      <c r="A95">
+        <v>23</v>
+      </c>
+      <c r="B95" t="s">
+        <v>226</v>
+      </c>
+      <c r="C95" t="s">
+        <v>120</v>
+      </c>
+      <c r="D95" t="s">
+        <v>118</v>
+      </c>
+      <c r="E95" t="s">
+        <v>118</v>
+      </c>
+      <c r="F95">
+        <v>66</v>
+      </c>
+      <c r="G95">
+        <v>6</v>
+      </c>
+      <c r="H95"/>
+      <c r="I95">
+        <v>110</v>
+      </c>
+      <c r="J95">
+        <v>24</v>
+      </c>
+      <c r="K95"/>
+      <c r="L95">
+        <v>110</v>
+      </c>
+      <c r="X95" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="96" spans="1:24">
+      <c r="A96">
+        <v>23</v>
+      </c>
+      <c r="B96" t="s">
+        <v>226</v>
+      </c>
+      <c r="C96" t="s">
+        <v>120</v>
+      </c>
+      <c r="D96" t="s">
+        <v>118</v>
+      </c>
+      <c r="E96" t="s">
+        <v>118</v>
+      </c>
+      <c r="F96">
+        <v>77</v>
+      </c>
+      <c r="G96">
+        <v>3</v>
+      </c>
+      <c r="H96"/>
+      <c r="I96">
+        <v>118</v>
+      </c>
+      <c r="J96">
+        <v>16</v>
+      </c>
+      <c r="K96"/>
+      <c r="L96">
+        <v>120</v>
+      </c>
+      <c r="X96" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="97" spans="1:24">
+      <c r="A97">
+        <v>23</v>
+      </c>
+      <c r="B97" t="s">
+        <v>194</v>
+      </c>
+      <c r="C97" t="s">
+        <v>120</v>
+      </c>
+      <c r="D97" t="s">
+        <v>118</v>
+      </c>
+      <c r="E97" t="s">
+        <v>118</v>
+      </c>
+      <c r="F97">
+        <v>300</v>
+      </c>
+      <c r="G97">
+        <v>2</v>
+      </c>
+      <c r="H97"/>
+      <c r="I97">
+        <v>700</v>
+      </c>
+      <c r="J97">
+        <v>7</v>
+      </c>
+      <c r="K97"/>
+      <c r="L97">
+        <v>1000</v>
+      </c>
+      <c r="W97" t="s">
+        <v>203</v>
+      </c>
+      <c r="X97" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="98" spans="1:24">
+      <c r="A98">
+        <v>24</v>
+      </c>
+      <c r="B98" t="s">
+        <v>226</v>
+      </c>
+      <c r="C98" t="s">
+        <v>104</v>
+      </c>
+      <c r="D98" t="s">
+        <v>118</v>
+      </c>
+      <c r="E98" t="s">
+        <v>118</v>
+      </c>
+      <c r="F98">
+        <v>350</v>
+      </c>
+      <c r="G98">
+        <v>4</v>
+      </c>
+      <c r="H98"/>
+      <c r="I98">
+        <v>430</v>
+      </c>
+      <c r="J98">
+        <v>13</v>
+      </c>
+      <c r="K98"/>
+      <c r="L98">
+        <v>430</v>
+      </c>
+      <c r="M98">
+        <v>14</v>
+      </c>
+      <c r="N98">
+        <v>600</v>
+      </c>
+      <c r="O98">
+        <v>300</v>
+      </c>
+      <c r="V98" t="s">
+        <v>187</v>
+      </c>
+      <c r="X98" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="99" spans="1:24">
+      <c r="A99">
+        <v>24</v>
+      </c>
+      <c r="B99" t="s">
+        <v>226</v>
+      </c>
+      <c r="C99" t="s">
+        <v>104</v>
+      </c>
+      <c r="D99" t="s">
+        <v>118</v>
+      </c>
+      <c r="E99" t="s">
+        <v>118</v>
+      </c>
+      <c r="F99">
+        <v>490</v>
+      </c>
+      <c r="G99">
+        <v>2</v>
+      </c>
+      <c r="H99"/>
+      <c r="I99">
+        <v>700</v>
+      </c>
+      <c r="J99">
+        <v>18</v>
+      </c>
+      <c r="K99"/>
+      <c r="L99">
+        <v>700</v>
+      </c>
+      <c r="M99">
+        <v>19</v>
+      </c>
+      <c r="N99">
+        <v>600</v>
+      </c>
+      <c r="O99">
+        <v>300</v>
+      </c>
+      <c r="V99" t="s">
+        <v>187</v>
+      </c>
+      <c r="X99" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="100" spans="1:24">
+      <c r="A100">
+        <v>24</v>
+      </c>
+      <c r="B100" t="s">
+        <v>226</v>
+      </c>
+      <c r="C100" t="s">
+        <v>104</v>
+      </c>
+      <c r="D100" t="s">
+        <v>118</v>
+      </c>
+      <c r="E100" t="s">
+        <v>118</v>
+      </c>
+      <c r="F100">
+        <v>720</v>
+      </c>
+      <c r="G100">
+        <v>6</v>
+      </c>
+      <c r="H100"/>
+      <c r="I100">
+        <v>1390</v>
+      </c>
+      <c r="J100">
+        <v>24</v>
+      </c>
+      <c r="K100"/>
+      <c r="L100">
+        <v>1390</v>
+      </c>
+      <c r="M100">
+        <v>25</v>
+      </c>
+      <c r="N100">
+        <v>600</v>
+      </c>
+      <c r="O100">
+        <v>300</v>
+      </c>
+      <c r="V100" t="s">
+        <v>187</v>
+      </c>
+      <c r="X100" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="101" spans="1:24">
+      <c r="A101">
+        <v>24</v>
+      </c>
+      <c r="B101" t="s">
+        <v>226</v>
+      </c>
+      <c r="C101" t="s">
+        <v>104</v>
+      </c>
+      <c r="D101" t="s">
+        <v>118</v>
+      </c>
+      <c r="E101" t="s">
+        <v>118</v>
+      </c>
+      <c r="F101">
+        <v>840</v>
+      </c>
+      <c r="G101">
+        <v>3</v>
+      </c>
+      <c r="H101"/>
+      <c r="I101">
+        <v>1120</v>
+      </c>
+      <c r="J101">
+        <v>16</v>
+      </c>
+      <c r="K101"/>
+      <c r="L101">
+        <v>1120</v>
+      </c>
+      <c r="M101">
+        <v>17</v>
+      </c>
+      <c r="N101">
+        <v>600</v>
+      </c>
+      <c r="O101">
+        <v>300</v>
+      </c>
+      <c r="V101" t="s">
+        <v>187</v>
+      </c>
+      <c r="X101" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="102" spans="1:24">
+      <c r="A102">
+        <v>24</v>
+      </c>
+      <c r="B102" t="s">
+        <v>226</v>
+      </c>
+      <c r="C102" t="s">
+        <v>104</v>
+      </c>
+      <c r="D102" t="s">
+        <v>118</v>
+      </c>
+      <c r="E102" t="s">
+        <v>118</v>
+      </c>
+      <c r="F102">
+        <v>32</v>
+      </c>
+      <c r="G102">
+        <v>4</v>
+      </c>
+      <c r="H102"/>
+      <c r="I102">
+        <v>39</v>
+      </c>
+      <c r="J102">
+        <v>13</v>
+      </c>
+      <c r="K102"/>
+      <c r="L102">
+        <v>40</v>
+      </c>
+      <c r="M102">
+        <v>14</v>
+      </c>
+      <c r="N102">
+        <v>600</v>
+      </c>
+      <c r="O102">
+        <v>300</v>
+      </c>
+      <c r="V102" t="s">
+        <v>187</v>
+      </c>
+      <c r="X102" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="103" spans="1:24">
+      <c r="A103">
+        <v>24</v>
+      </c>
+      <c r="B103" t="s">
+        <v>226</v>
+      </c>
+      <c r="C103" t="s">
+        <v>104</v>
+      </c>
+      <c r="D103" t="s">
+        <v>118</v>
+      </c>
+      <c r="E103" t="s">
+        <v>118</v>
+      </c>
+      <c r="F103">
+        <v>45</v>
+      </c>
+      <c r="G103">
+        <v>2</v>
+      </c>
+      <c r="H103"/>
+      <c r="I103">
+        <v>70</v>
+      </c>
+      <c r="J103">
+        <v>18</v>
+      </c>
+      <c r="K103"/>
+      <c r="L103">
+        <v>70</v>
+      </c>
+      <c r="M103">
+        <v>19</v>
+      </c>
+      <c r="N103">
+        <v>600</v>
+      </c>
+      <c r="O103">
+        <v>300</v>
+      </c>
+      <c r="V103" t="s">
+        <v>187</v>
+      </c>
+      <c r="X103" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="104" spans="1:24">
+      <c r="A104">
+        <v>24</v>
+      </c>
+      <c r="B104" t="s">
+        <v>226</v>
+      </c>
+      <c r="C104" t="s">
+        <v>104</v>
+      </c>
+      <c r="D104" t="s">
+        <v>118</v>
+      </c>
+      <c r="E104" t="s">
+        <v>118</v>
+      </c>
+      <c r="F104">
+        <v>66</v>
+      </c>
+      <c r="G104">
+        <v>6</v>
+      </c>
+      <c r="H104"/>
+      <c r="I104">
+        <v>110</v>
+      </c>
+      <c r="J104">
+        <v>24</v>
+      </c>
+      <c r="K104"/>
+      <c r="L104">
+        <v>110</v>
+      </c>
+      <c r="M104">
+        <v>25</v>
+      </c>
+      <c r="N104">
+        <v>600</v>
+      </c>
+      <c r="O104">
+        <v>300</v>
+      </c>
+      <c r="V104" t="s">
+        <v>187</v>
+      </c>
+      <c r="X104" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="105" spans="1:24">
+      <c r="A105">
+        <v>24</v>
+      </c>
+      <c r="B105" t="s">
+        <v>226</v>
+      </c>
+      <c r="C105" t="s">
+        <v>104</v>
+      </c>
+      <c r="D105" t="s">
+        <v>118</v>
+      </c>
+      <c r="E105" t="s">
+        <v>118</v>
+      </c>
+      <c r="F105">
+        <v>77</v>
+      </c>
+      <c r="G105">
+        <v>3</v>
+      </c>
+      <c r="H105"/>
+      <c r="I105">
+        <v>118</v>
+      </c>
+      <c r="J105">
+        <v>16</v>
+      </c>
+      <c r="K105"/>
+      <c r="L105">
+        <v>120</v>
+      </c>
+      <c r="M105">
+        <v>17</v>
+      </c>
+      <c r="N105">
+        <v>600</v>
+      </c>
+      <c r="O105">
+        <v>300</v>
+      </c>
+      <c r="V105" t="s">
+        <v>187</v>
+      </c>
+      <c r="X105" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="106" spans="1:24">
+      <c r="A106">
+        <v>24</v>
+      </c>
+      <c r="B106" t="s">
+        <v>194</v>
+      </c>
+      <c r="C106" t="s">
+        <v>104</v>
+      </c>
+      <c r="D106" t="s">
+        <v>118</v>
+      </c>
+      <c r="E106" t="s">
+        <v>118</v>
+      </c>
+      <c r="F106">
+        <v>300</v>
+      </c>
+      <c r="G106">
+        <v>2</v>
+      </c>
+      <c r="H106"/>
+      <c r="I106">
+        <v>700</v>
+      </c>
+      <c r="J106">
+        <v>7</v>
+      </c>
+      <c r="K106"/>
+      <c r="L106">
+        <v>1000</v>
+      </c>
+      <c r="M106">
+        <v>8</v>
+      </c>
+      <c r="N106">
+        <v>600</v>
+      </c>
+      <c r="O106">
+        <v>300</v>
+      </c>
+      <c r="V106" t="s">
+        <v>187</v>
+      </c>
+      <c r="W106" t="s">
+        <v>201</v>
+      </c>
+      <c r="X106" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="107" spans="1:24">
+      <c r="A107">
+        <v>25</v>
+      </c>
+      <c r="B107" t="s">
+        <v>226</v>
+      </c>
+      <c r="C107" t="s">
+        <v>104</v>
+      </c>
+      <c r="D107" t="s">
+        <v>118</v>
+      </c>
+      <c r="E107" t="s">
+        <v>118</v>
+      </c>
+      <c r="F107">
+        <v>350</v>
+      </c>
+      <c r="G107">
+        <v>4</v>
+      </c>
+      <c r="H107"/>
+      <c r="I107">
+        <v>430</v>
+      </c>
+      <c r="J107">
+        <v>13</v>
+      </c>
+      <c r="K107"/>
+      <c r="L107">
+        <v>430</v>
+      </c>
+      <c r="M107">
+        <v>27</v>
+      </c>
+      <c r="N107">
+        <v>1200</v>
+      </c>
+      <c r="O107">
+        <v>300</v>
+      </c>
+      <c r="V107" t="s">
+        <v>187</v>
+      </c>
+      <c r="X107" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="108" spans="1:24">
+      <c r="A108">
+        <v>25</v>
+      </c>
+      <c r="B108" t="s">
+        <v>226</v>
+      </c>
+      <c r="C108" t="s">
+        <v>104</v>
+      </c>
+      <c r="D108" t="s">
+        <v>118</v>
+      </c>
+      <c r="E108" t="s">
+        <v>118</v>
+      </c>
+      <c r="F108">
+        <v>490</v>
+      </c>
+      <c r="G108">
+        <v>2</v>
+      </c>
+      <c r="H108"/>
+      <c r="I108">
+        <v>700</v>
+      </c>
+      <c r="J108">
+        <v>18</v>
+      </c>
+      <c r="K108"/>
+      <c r="L108">
+        <v>700</v>
+      </c>
+      <c r="M108">
+        <v>37</v>
+      </c>
+      <c r="N108">
+        <v>1200</v>
+      </c>
+      <c r="O108">
+        <v>300</v>
+      </c>
+      <c r="V108" t="s">
+        <v>187</v>
+      </c>
+      <c r="X108" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="109" spans="1:24">
+      <c r="A109">
+        <v>25</v>
+      </c>
+      <c r="B109" t="s">
+        <v>226</v>
+      </c>
+      <c r="C109" t="s">
+        <v>104</v>
+      </c>
+      <c r="D109" t="s">
+        <v>118</v>
+      </c>
+      <c r="E109" t="s">
+        <v>118</v>
+      </c>
+      <c r="F109">
+        <v>720</v>
+      </c>
+      <c r="G109">
+        <v>6</v>
+      </c>
+      <c r="H109"/>
+      <c r="I109">
+        <v>1390</v>
+      </c>
+      <c r="J109">
+        <v>24</v>
+      </c>
+      <c r="K109"/>
+      <c r="L109">
+        <v>1390</v>
+      </c>
+      <c r="M109">
+        <v>49</v>
+      </c>
+      <c r="N109">
+        <v>1200</v>
+      </c>
+      <c r="O109">
+        <v>300</v>
+      </c>
+      <c r="V109" t="s">
+        <v>187</v>
+      </c>
+      <c r="X109" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="110" spans="1:24">
+      <c r="A110">
+        <v>25</v>
+      </c>
+      <c r="B110" t="s">
+        <v>226</v>
+      </c>
+      <c r="C110" t="s">
+        <v>104</v>
+      </c>
+      <c r="D110" t="s">
+        <v>118</v>
+      </c>
+      <c r="E110" t="s">
+        <v>118</v>
+      </c>
+      <c r="F110">
+        <v>840</v>
+      </c>
+      <c r="G110">
+        <v>3</v>
+      </c>
+      <c r="H110"/>
+      <c r="I110">
+        <v>1120</v>
+      </c>
+      <c r="J110">
+        <v>16</v>
+      </c>
+      <c r="K110"/>
+      <c r="L110">
+        <v>1120</v>
+      </c>
+      <c r="M110">
+        <v>33</v>
+      </c>
+      <c r="N110">
+        <v>1200</v>
+      </c>
+      <c r="O110">
+        <v>300</v>
+      </c>
+      <c r="V110" t="s">
+        <v>187</v>
+      </c>
+      <c r="X110" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="111" spans="1:24">
+      <c r="A111">
+        <v>25</v>
+      </c>
+      <c r="B111" t="s">
+        <v>226</v>
+      </c>
+      <c r="C111" t="s">
+        <v>104</v>
+      </c>
+      <c r="D111" t="s">
+        <v>118</v>
+      </c>
+      <c r="E111" t="s">
+        <v>118</v>
+      </c>
+      <c r="F111">
+        <v>32</v>
+      </c>
+      <c r="G111">
+        <v>4</v>
+      </c>
+      <c r="H111"/>
+      <c r="I111">
+        <v>39</v>
+      </c>
+      <c r="J111">
+        <v>13</v>
+      </c>
+      <c r="K111"/>
+      <c r="L111">
+        <v>40</v>
+      </c>
+      <c r="M111">
+        <v>27</v>
+      </c>
+      <c r="N111">
+        <v>1200</v>
+      </c>
+      <c r="O111">
+        <v>300</v>
+      </c>
+      <c r="V111" t="s">
+        <v>187</v>
+      </c>
+      <c r="X111" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="112" spans="1:24">
+      <c r="A112">
+        <v>25</v>
+      </c>
+      <c r="B112" t="s">
+        <v>226</v>
+      </c>
+      <c r="C112" t="s">
+        <v>104</v>
+      </c>
+      <c r="D112" t="s">
+        <v>118</v>
+      </c>
+      <c r="E112" t="s">
+        <v>118</v>
+      </c>
+      <c r="F112">
+        <v>45</v>
+      </c>
+      <c r="G112">
+        <v>2</v>
+      </c>
+      <c r="H112"/>
+      <c r="I112">
+        <v>70</v>
+      </c>
+      <c r="J112">
+        <v>18</v>
+      </c>
+      <c r="K112"/>
+      <c r="L112">
+        <v>70</v>
+      </c>
+      <c r="M112">
+        <v>37</v>
+      </c>
+      <c r="N112">
+        <v>1200</v>
+      </c>
+      <c r="O112">
+        <v>300</v>
+      </c>
+      <c r="V112" t="s">
+        <v>187</v>
+      </c>
+      <c r="X112" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="113" spans="1:24">
+      <c r="A113">
+        <v>25</v>
+      </c>
+      <c r="B113" t="s">
+        <v>226</v>
+      </c>
+      <c r="C113" t="s">
+        <v>104</v>
+      </c>
+      <c r="D113" t="s">
+        <v>118</v>
+      </c>
+      <c r="E113" t="s">
+        <v>118</v>
+      </c>
+      <c r="F113">
+        <v>66</v>
+      </c>
+      <c r="G113">
+        <v>6</v>
+      </c>
+      <c r="H113"/>
+      <c r="I113">
+        <v>110</v>
+      </c>
+      <c r="J113">
+        <v>24</v>
+      </c>
+      <c r="K113"/>
+      <c r="L113">
+        <v>110</v>
+      </c>
+      <c r="M113">
+        <v>49</v>
+      </c>
+      <c r="N113">
+        <v>1200</v>
+      </c>
+      <c r="O113">
+        <v>300</v>
+      </c>
+      <c r="V113" t="s">
+        <v>187</v>
+      </c>
+      <c r="X113" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="114" spans="1:24">
+      <c r="A114">
+        <v>25</v>
+      </c>
+      <c r="B114" t="s">
+        <v>226</v>
+      </c>
+      <c r="C114" t="s">
+        <v>104</v>
+      </c>
+      <c r="D114" t="s">
+        <v>118</v>
+      </c>
+      <c r="E114" t="s">
+        <v>118</v>
+      </c>
+      <c r="F114">
+        <v>77</v>
+      </c>
+      <c r="G114">
+        <v>3</v>
+      </c>
+      <c r="H114"/>
+      <c r="I114">
+        <v>118</v>
+      </c>
+      <c r="J114">
+        <v>16</v>
+      </c>
+      <c r="K114"/>
+      <c r="L114">
+        <v>120</v>
+      </c>
+      <c r="M114">
+        <v>33</v>
+      </c>
+      <c r="N114">
+        <v>1200</v>
+      </c>
+      <c r="O114">
+        <v>300</v>
+      </c>
+      <c r="V114" t="s">
+        <v>187</v>
+      </c>
+      <c r="X114" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="115" spans="1:24">
+      <c r="A115">
+        <v>25</v>
+      </c>
+      <c r="B115" t="s">
+        <v>194</v>
+      </c>
+      <c r="C115" t="s">
+        <v>104</v>
+      </c>
+      <c r="D115" t="s">
+        <v>118</v>
+      </c>
+      <c r="E115" t="s">
+        <v>118</v>
+      </c>
+      <c r="F115">
+        <v>300</v>
+      </c>
+      <c r="G115">
+        <v>2</v>
+      </c>
+      <c r="H115"/>
+      <c r="I115">
+        <v>700</v>
+      </c>
+      <c r="J115">
+        <v>7</v>
+      </c>
+      <c r="K115"/>
+      <c r="L115">
+        <v>1000</v>
+      </c>
+      <c r="M115">
+        <v>15</v>
+      </c>
+      <c r="N115">
+        <v>1200</v>
+      </c>
+      <c r="O115">
+        <v>300</v>
+      </c>
+      <c r="V115" t="s">
+        <v>187</v>
+      </c>
+      <c r="W115" t="s">
+        <v>202</v>
+      </c>
+      <c r="X115" t="s">
+        <v>185</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:X88" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9178,7 +10405,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.33184581816253522</v>
+        <v>0.33450492928833142</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -9198,7 +10425,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>6.0663915074302133E-2</v>
+        <v>0.32841052280124816</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -9219,7 +10446,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.28793463357627902</v>
+        <v>0.72552774198150016</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -9239,7 +10466,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.58553950496263141</v>
+        <v>0.39607956337884942</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -9500,48 +10727,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="80" t="s">
+      <c r="C3" s="79" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="81"/>
-      <c r="E3" s="80" t="s">
+      <c r="D3" s="80"/>
+      <c r="E3" s="79" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="81"/>
-      <c r="G3" s="80" t="s">
+      <c r="F3" s="80"/>
+      <c r="G3" s="79" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="81"/>
-      <c r="I3" s="80" t="s">
+      <c r="H3" s="80"/>
+      <c r="I3" s="79" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="81"/>
+      <c r="J3" s="80"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="82" t="s">
+      <c r="M3" s="81" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="83"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="82" t="s">
+      <c r="N3" s="82"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="81" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="83"/>
-      <c r="R3" s="84"/>
-      <c r="S3" s="82" t="s">
+      <c r="Q3" s="82"/>
+      <c r="R3" s="83"/>
+      <c r="S3" s="81" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="83"/>
-      <c r="U3" s="83"/>
-      <c r="V3" s="85" t="s">
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="84" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="85"/>
-      <c r="X3" s="85"/>
+      <c r="W3" s="84"/>
+      <c r="X3" s="84"/>
       <c r="Y3" t="s">
         <v>215</v>
       </c>
@@ -10620,16 +11847,16 @@
       </c>
     </row>
     <row r="29" spans="1:33">
-      <c r="C29" s="79" t="s">
+      <c r="C29" s="85" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="79"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="79" t="s">
+      <c r="D29" s="85"/>
+      <c r="E29" s="85"/>
+      <c r="F29" s="85" t="s">
         <v>169</v>
       </c>
-      <c r="G29" s="79"/>
-      <c r="H29" s="79"/>
+      <c r="G29" s="85"/>
+      <c r="H29" s="85"/>
       <c r="J29" t="s">
         <v>168</v>
       </c>
@@ -11534,16 +12761,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="P3:R3"/>
     <mergeCell ref="S3:U3"/>
     <mergeCell ref="V3:X3"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B26" r:id="rId1" xr:uid="{D2B54FA7-7284-A444-93E2-10BEB7DF1432}"/>
@@ -11583,105 +12810,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="98" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="92" t="s">
+      <c r="A2" s="92" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="92" t="s">
+      <c r="C2" s="87"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="93"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="89" t="s">
+      <c r="F2" s="87"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="104"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="104"/>
-      <c r="M2" s="104"/>
-      <c r="N2" s="104"/>
-      <c r="O2" s="104"/>
-      <c r="P2" s="104"/>
-      <c r="Q2" s="104"/>
-      <c r="R2" s="104" t="s">
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="101"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="104"/>
-      <c r="T2" s="104"/>
-      <c r="U2" s="104"/>
-      <c r="V2" s="89" t="s">
+      <c r="S2" s="101"/>
+      <c r="T2" s="101"/>
+      <c r="U2" s="101"/>
+      <c r="V2" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="89" t="s">
+      <c r="W2" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="86" t="s">
+      <c r="X2" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="86" t="s">
+      <c r="Y2" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="86" t="s">
+      <c r="Z2" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="86" t="s">
+      <c r="AA2" s="103" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="99"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="105" t="s">
+      <c r="A3" s="93"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="103"/>
-      <c r="K3" s="103"/>
-      <c r="L3" s="103" t="s">
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="103"/>
-      <c r="N3" s="103" t="s">
+      <c r="M3" s="100"/>
+      <c r="N3" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="103"/>
-      <c r="P3" s="103" t="s">
+      <c r="O3" s="100"/>
+      <c r="P3" s="100" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="103"/>
-      <c r="R3" s="101" t="s">
+      <c r="Q3" s="100"/>
+      <c r="R3" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="101" t="s">
+      <c r="S3" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="101" t="s">
+      <c r="T3" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="101" t="s">
+      <c r="U3" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="90"/>
-      <c r="W3" s="90"/>
-      <c r="X3" s="87"/>
-      <c r="Y3" s="87"/>
-      <c r="Z3" s="87"/>
-      <c r="AA3" s="87"/>
+      <c r="V3" s="96"/>
+      <c r="W3" s="96"/>
+      <c r="X3" s="104"/>
+      <c r="Y3" s="104"/>
+      <c r="Z3" s="104"/>
+      <c r="AA3" s="104"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="100"/>
+      <c r="A4" s="94"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -11700,7 +12927,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="91"/>
+      <c r="H4" s="97"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -11728,16 +12955,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="102"/>
-      <c r="S4" s="102"/>
-      <c r="T4" s="102"/>
-      <c r="U4" s="102"/>
-      <c r="V4" s="91"/>
-      <c r="W4" s="91"/>
-      <c r="X4" s="88"/>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="88"/>
-      <c r="AA4" s="87"/>
+      <c r="R4" s="99"/>
+      <c r="S4" s="99"/>
+      <c r="T4" s="99"/>
+      <c r="U4" s="99"/>
+      <c r="V4" s="97"/>
+      <c r="W4" s="97"/>
+      <c r="X4" s="105"/>
+      <c r="Y4" s="105"/>
+      <c r="Z4" s="105"/>
+      <c r="AA4" s="104"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -12238,6 +13465,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -12253,11 +13485,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Incorporated Yahel's treatments in dev list.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DA6479-C8FC-5146-97F0-A51AB0FB5CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6534540-EB3B-3042-A47B-E993FFC9A6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="2" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
-    <sheet name="MCL questions prod" sheetId="10" r:id="rId2"/>
+    <sheet name="MCL questions prod exp 1" sheetId="10" r:id="rId2"/>
     <sheet name="Web Parameters Dev" sheetId="8" r:id="rId3"/>
     <sheet name="Web Parameters Random" sheetId="11" r:id="rId4"/>
     <sheet name="Latin Square Treatment Order" sheetId="13" r:id="rId5"/>
@@ -27,7 +27,7 @@
     <sheet name="Web Parameters v1" sheetId="1" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MCL questions prod'!$A$1:$X$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MCL questions prod exp 1'!$A$1:$X$28</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Web Parameters Dev'!$A$1:$X$88</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -4851,7 +4851,7 @@
   <dimension ref="A1:X115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="V125" sqref="V125"/>
     </sheetView>
   </sheetViews>
@@ -10405,7 +10405,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.33450492928833142</v>
+        <v>0.16552693345305181</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -10425,7 +10425,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.32841052280124816</v>
+        <v>0.16324288851674096</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -10446,7 +10446,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.72552774198150016</v>
+        <v>0.60161766272830919</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -10466,7 +10466,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.39607956337884942</v>
+        <v>0.43438902522090428</v>
       </c>
     </row>
     <row r="6" spans="1:7">

</xml_diff>

<commit_message>
Jest working for CLI and started to add firebase.
Got jest working in the CLI project.
Added firebase functions.
Got writing batch to firestore working.
Fixed FileIOAdapter.tedst.js due to expect string comparison.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6534540-EB3B-3042-A47B-E993FFC9A6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089749E4-C85D-194C-AF89-F9A466062B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="2" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -1126,6 +1126,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1144,8 +1147,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1175,15 +1193,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1197,15 +1206,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4851,8 +4851,8 @@
   <dimension ref="A1:X115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V125" sqref="V125"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -10405,7 +10405,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.16552693345305181</v>
+        <v>0.70926613894984814</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -10425,7 +10425,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.16324288851674096</v>
+        <v>0.23197501336242499</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -10446,7 +10446,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.60161766272830919</v>
+        <v>0.10989702360321685</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -10466,7 +10466,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.43438902522090428</v>
+        <v>9.295568271133936E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -10727,48 +10727,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="80" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="80"/>
-      <c r="E3" s="79" t="s">
+      <c r="D3" s="81"/>
+      <c r="E3" s="80" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="80"/>
-      <c r="G3" s="79" t="s">
+      <c r="F3" s="81"/>
+      <c r="G3" s="80" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="80"/>
-      <c r="I3" s="79" t="s">
+      <c r="H3" s="81"/>
+      <c r="I3" s="80" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="80"/>
+      <c r="J3" s="81"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="81" t="s">
+      <c r="M3" s="82" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="82"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="81" t="s">
+      <c r="N3" s="83"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="82" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="82"/>
-      <c r="R3" s="83"/>
-      <c r="S3" s="81" t="s">
+      <c r="Q3" s="83"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="82" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="82"/>
-      <c r="U3" s="82"/>
-      <c r="V3" s="84" t="s">
+      <c r="T3" s="83"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="85" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="84"/>
-      <c r="X3" s="84"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="85"/>
       <c r="Y3" t="s">
         <v>215</v>
       </c>
@@ -11847,16 +11847,16 @@
       </c>
     </row>
     <row r="29" spans="1:33">
-      <c r="C29" s="85" t="s">
+      <c r="C29" s="79" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="85"/>
-      <c r="E29" s="85"/>
-      <c r="F29" s="85" t="s">
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="79" t="s">
         <v>169</v>
       </c>
-      <c r="G29" s="85"/>
-      <c r="H29" s="85"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="79"/>
       <c r="J29" t="s">
         <v>168</v>
       </c>
@@ -12761,16 +12761,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B26" r:id="rId1" xr:uid="{D2B54FA7-7284-A444-93E2-10BEB7DF1432}"/>
@@ -12810,105 +12810,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="86" t="s">
+      <c r="A2" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="86" t="s">
+      <c r="C2" s="93"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="87"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="95" t="s">
+      <c r="F2" s="93"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="101" t="s">
+      <c r="I2" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
-      <c r="M2" s="101"/>
-      <c r="N2" s="101"/>
-      <c r="O2" s="101"/>
-      <c r="P2" s="101"/>
-      <c r="Q2" s="101"/>
-      <c r="R2" s="101" t="s">
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="101"/>
-      <c r="T2" s="101"/>
-      <c r="U2" s="101"/>
-      <c r="V2" s="95" t="s">
+      <c r="S2" s="104"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="95" t="s">
+      <c r="W2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="103" t="s">
+      <c r="X2" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="103" t="s">
+      <c r="Y2" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="103" t="s">
+      <c r="Z2" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="103" t="s">
+      <c r="AA2" s="86" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="93"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="102" t="s">
+      <c r="A3" s="99"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
-      <c r="L3" s="100" t="s">
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="100"/>
-      <c r="N3" s="100" t="s">
+      <c r="M3" s="103"/>
+      <c r="N3" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="100"/>
-      <c r="P3" s="100" t="s">
+      <c r="O3" s="103"/>
+      <c r="P3" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="100"/>
-      <c r="R3" s="98" t="s">
+      <c r="Q3" s="103"/>
+      <c r="R3" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="98" t="s">
+      <c r="S3" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="98" t="s">
+      <c r="T3" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="98" t="s">
+      <c r="U3" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="96"/>
-      <c r="W3" s="96"/>
-      <c r="X3" s="104"/>
-      <c r="Y3" s="104"/>
-      <c r="Z3" s="104"/>
-      <c r="AA3" s="104"/>
+      <c r="V3" s="90"/>
+      <c r="W3" s="90"/>
+      <c r="X3" s="87"/>
+      <c r="Y3" s="87"/>
+      <c r="Z3" s="87"/>
+      <c r="AA3" s="87"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="94"/>
+      <c r="A4" s="100"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -12927,7 +12927,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="97"/>
+      <c r="H4" s="91"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -12955,16 +12955,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="99"/>
-      <c r="S4" s="99"/>
-      <c r="T4" s="99"/>
-      <c r="U4" s="99"/>
-      <c r="V4" s="97"/>
-      <c r="W4" s="97"/>
-      <c r="X4" s="105"/>
-      <c r="Y4" s="105"/>
-      <c r="Z4" s="105"/>
-      <c r="AA4" s="104"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="102"/>
+      <c r="V4" s="91"/>
+      <c r="W4" s="91"/>
+      <c r="X4" s="88"/>
+      <c r="Y4" s="88"/>
+      <c r="Z4" s="88"/>
+      <c r="AA4" s="87"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -13465,11 +13465,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -13485,6 +13480,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Renamed seven_square field to latin_square
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B033407-6D32-E546-80F5-C66C4D22AF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E021942-DF55-5B48-BF0D-1DA16E4F3099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="4" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="1" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="Fire participants" sheetId="21" r:id="rId3"/>
     <sheet name="Fire survey answers" sheetId="24" r:id="rId4"/>
     <sheet name="Fire question answers" sheetId="22" r:id="rId5"/>
-    <sheet name="Fire ques prod" sheetId="16" r:id="rId6"/>
-    <sheet name="Fire treat ques prod" sheetId="19" r:id="rId7"/>
-    <sheet name="Fire treat prod" sheetId="17" r:id="rId8"/>
+    <sheet name="fire_ques_prod" sheetId="16" r:id="rId6"/>
+    <sheet name="fire_treat_ques_prod" sheetId="19" r:id="rId7"/>
+    <sheet name="fire_treat_prod" sheetId="17" r:id="rId8"/>
     <sheet name="MCL questions prod exp 1" sheetId="10" r:id="rId9"/>
     <sheet name="Firestore MEL Import Dev" sheetId="14" r:id="rId10"/>
     <sheet name="Web Parameters Dev" sheetId="8" r:id="rId11"/>
@@ -908,9 +908,6 @@
     <t>Within subject based on power analysis to reach statistical significance.</t>
   </si>
   <si>
-    <t>seven_squares</t>
-  </si>
-  <si>
     <t>[[1, 2, 3], [1, 3, 2],[3, 1, 2],[3, 2, 1],[2, 3, 1],[2, 1, 3]]</t>
   </si>
   <si>
@@ -1239,6 +1236,9 @@
   </si>
   <si>
     <t>choice_time_sec</t>
+  </si>
+  <si>
+    <t>latin_square</t>
   </si>
 </sst>
 </file>
@@ -1502,7 +1502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1608,6 +1608,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1626,8 +1629,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1657,15 +1675,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1680,16 +1689,6 @@
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -14487,7 +14486,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.91772226650365651</v>
+        <v>0.57074944608081002</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -14507,7 +14506,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.6743826534083539</v>
+        <v>0.7709950283025121</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -14528,7 +14527,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.14291722095502124</v>
+        <v>0.80005591890160044</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -14548,7 +14547,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.1946400025961692</v>
+        <v>0.48253859109007002</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -14809,48 +14808,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="82" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="82"/>
-      <c r="E3" s="81" t="s">
+      <c r="D3" s="83"/>
+      <c r="E3" s="82" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="82"/>
-      <c r="G3" s="81" t="s">
+      <c r="F3" s="83"/>
+      <c r="G3" s="82" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="82"/>
-      <c r="I3" s="81" t="s">
+      <c r="H3" s="83"/>
+      <c r="I3" s="82" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="82"/>
+      <c r="J3" s="83"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="83" t="s">
+      <c r="M3" s="84" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="84"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="83" t="s">
+      <c r="N3" s="85"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="84" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="83" t="s">
+      <c r="Q3" s="85"/>
+      <c r="R3" s="86"/>
+      <c r="S3" s="84" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="84"/>
-      <c r="U3" s="84"/>
-      <c r="V3" s="86" t="s">
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
+      <c r="V3" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="86"/>
-      <c r="X3" s="86"/>
+      <c r="W3" s="87"/>
+      <c r="X3" s="87"/>
       <c r="Y3" t="s">
         <v>215</v>
       </c>
@@ -15929,16 +15928,16 @@
       </c>
     </row>
     <row r="29" spans="1:33">
-      <c r="C29" s="87" t="s">
+      <c r="C29" s="81" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="87"/>
-      <c r="E29" s="87"/>
-      <c r="F29" s="87" t="s">
+      <c r="D29" s="81"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="81" t="s">
         <v>169</v>
       </c>
-      <c r="G29" s="87"/>
-      <c r="H29" s="87"/>
+      <c r="G29" s="81"/>
+      <c r="H29" s="81"/>
       <c r="J29" t="s">
         <v>168</v>
       </c>
@@ -16843,16 +16842,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B26" r:id="rId1" xr:uid="{D2B54FA7-7284-A444-93E2-10BEB7DF1432}"/>
@@ -16892,105 +16891,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="88" t="s">
+      <c r="C2" s="95"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="89"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="97" t="s">
+      <c r="F2" s="95"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="103" t="s">
+      <c r="I2" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103" t="s">
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="106"/>
+      <c r="R2" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="97" t="s">
+      <c r="S2" s="106"/>
+      <c r="T2" s="106"/>
+      <c r="U2" s="106"/>
+      <c r="V2" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="97" t="s">
+      <c r="W2" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="105" t="s">
+      <c r="X2" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="105" t="s">
+      <c r="Y2" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="105" t="s">
+      <c r="Z2" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="105" t="s">
+      <c r="AA2" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="95"/>
-      <c r="B3" s="91"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="104" t="s">
+      <c r="A3" s="101"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="102"/>
-      <c r="K3" s="102"/>
-      <c r="L3" s="102" t="s">
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="102"/>
-      <c r="N3" s="102" t="s">
+      <c r="M3" s="105"/>
+      <c r="N3" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="102"/>
-      <c r="P3" s="102" t="s">
+      <c r="O3" s="105"/>
+      <c r="P3" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="102"/>
-      <c r="R3" s="100" t="s">
+      <c r="Q3" s="105"/>
+      <c r="R3" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="100" t="s">
+      <c r="S3" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="100" t="s">
+      <c r="T3" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="100" t="s">
+      <c r="U3" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="98"/>
-      <c r="W3" s="98"/>
-      <c r="X3" s="106"/>
-      <c r="Y3" s="106"/>
-      <c r="Z3" s="106"/>
-      <c r="AA3" s="106"/>
+      <c r="V3" s="92"/>
+      <c r="W3" s="92"/>
+      <c r="X3" s="89"/>
+      <c r="Y3" s="89"/>
+      <c r="Z3" s="89"/>
+      <c r="AA3" s="89"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="96"/>
+      <c r="A4" s="102"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -17009,7 +17008,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="99"/>
+      <c r="H4" s="93"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -17037,16 +17036,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="101"/>
-      <c r="S4" s="101"/>
-      <c r="T4" s="101"/>
-      <c r="U4" s="101"/>
-      <c r="V4" s="99"/>
-      <c r="W4" s="99"/>
-      <c r="X4" s="107"/>
-      <c r="Y4" s="107"/>
-      <c r="Z4" s="107"/>
-      <c r="AA4" s="106"/>
+      <c r="R4" s="104"/>
+      <c r="S4" s="104"/>
+      <c r="T4" s="104"/>
+      <c r="U4" s="104"/>
+      <c r="V4" s="93"/>
+      <c r="W4" s="93"/>
+      <c r="X4" s="90"/>
+      <c r="Y4" s="90"/>
+      <c r="Z4" s="90"/>
+      <c r="AA4" s="89"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -17547,11 +17546,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -17567,6 +17561,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -18728,8 +18727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAA32EA-3DA8-BD44-8758-9048DFA42915}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18749,16 +18748,16 @@
         <v>267</v>
       </c>
       <c r="C1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D1" t="s">
         <v>276</v>
-      </c>
-      <c r="D1" t="s">
-        <v>277</v>
       </c>
       <c r="E1" t="s">
         <v>255</v>
       </c>
       <c r="F1" t="s">
-        <v>273</v>
+        <v>383</v>
       </c>
       <c r="G1" s="36" t="s">
         <v>258</v>
@@ -18796,7 +18795,7 @@
         <v>253</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G2" s="36">
         <v>44922</v>
@@ -18828,7 +18827,7 @@
         <v>253</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G3" s="36">
         <v>44940</v>
@@ -18860,7 +18859,7 @@
         <v>253</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G4" s="36">
         <v>44942</v>
@@ -18892,7 +18891,7 @@
         <v>253</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G5" s="36">
         <v>44994</v>
@@ -18927,7 +18926,7 @@
         <v>253</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I6">
         <v>150</v>
@@ -18956,7 +18955,7 @@
         <v>270</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I7">
         <v>450</v>
@@ -20658,7 +20657,7 @@
   <dimension ref="A1:BD2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20669,169 +20668,169 @@
   <sheetData>
     <row r="1" spans="1:56" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>279</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>280</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>116</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AF1" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AG1" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AH1" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AI1" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AJ1" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="AK1" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="AL1" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="AJ1" s="8" t="s">
-        <v>346</v>
-      </c>
-      <c r="AK1" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AM1" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AN1" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AO1" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AP1" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="AP1" s="8" t="s">
+      <c r="AQ1" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="AQ1" s="8" t="s">
+      <c r="AR1" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="AR1" s="8" t="s">
+      <c r="AS1" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="AS1" s="8" t="s">
+      <c r="AT1" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="AT1" s="8" t="s">
+      <c r="AU1" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="AU1" s="8" t="s">
+      <c r="AV1" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="AV1" s="8" t="s">
+      <c r="AW1" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="AW1" s="8" t="s">
+      <c r="AX1" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="AX1" s="8" t="s">
+      <c r="AY1" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="AY1" s="8" t="s">
+      <c r="AZ1" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="AZ1" s="8" t="s">
+      <c r="BA1" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="BA1" s="8" t="s">
+      <c r="BB1" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="BB1" s="8" t="s">
-        <v>328</v>
-      </c>
       <c r="BD1" s="8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:56">
@@ -20848,73 +20847,73 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
+        <v>348</v>
+      </c>
+      <c r="F2" t="s">
         <v>349</v>
-      </c>
-      <c r="F2" t="s">
-        <v>350</v>
       </c>
       <c r="G2">
         <v>30.965</v>
       </c>
       <c r="H2" t="s">
+        <v>350</v>
+      </c>
+      <c r="I2" t="s">
         <v>351</v>
-      </c>
-      <c r="I2" t="s">
-        <v>352</v>
       </c>
       <c r="J2">
         <v>49.71</v>
       </c>
       <c r="K2" t="s">
+        <v>352</v>
+      </c>
+      <c r="L2" t="s">
         <v>353</v>
-      </c>
-      <c r="L2" t="s">
-        <v>354</v>
       </c>
       <c r="M2">
         <v>51.975999999999999</v>
       </c>
       <c r="N2" t="s">
+        <v>354</v>
+      </c>
+      <c r="O2" t="s">
         <v>355</v>
-      </c>
-      <c r="O2" t="s">
-        <v>356</v>
       </c>
       <c r="P2">
         <v>17.925000000000001</v>
       </c>
       <c r="Q2" t="s">
+        <v>356</v>
+      </c>
+      <c r="R2" t="s">
         <v>357</v>
-      </c>
-      <c r="R2" t="s">
-        <v>358</v>
       </c>
       <c r="S2">
         <v>34.722999999999999</v>
       </c>
       <c r="T2" t="s">
+        <v>358</v>
+      </c>
+      <c r="U2" t="s">
         <v>359</v>
-      </c>
-      <c r="U2" t="s">
-        <v>360</v>
       </c>
       <c r="V2">
         <v>32.575000000000003</v>
       </c>
       <c r="W2" t="s">
+        <v>360</v>
+      </c>
+      <c r="X2" t="s">
         <v>361</v>
-      </c>
-      <c r="X2" t="s">
-        <v>362</v>
       </c>
       <c r="Y2">
         <v>25.481999999999999</v>
       </c>
       <c r="Z2" t="s">
+        <v>362</v>
+      </c>
+      <c r="AA2" t="s">
         <v>363</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>364</v>
       </c>
       <c r="AB2">
         <v>16.695</v>
@@ -20923,7 +20922,7 @@
         <v>1</v>
       </c>
       <c r="AD2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AE2">
         <v>5</v>
@@ -20932,19 +20931,19 @@
         <v>63</v>
       </c>
       <c r="AG2" t="s">
+        <v>365</v>
+      </c>
+      <c r="AI2" t="s">
         <v>366</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>367</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AL2" t="s">
         <v>368</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>369</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>370</v>
       </c>
       <c r="AP2">
         <v>24</v>
@@ -20959,7 +20958,7 @@
         <v>0</v>
       </c>
       <c r="AT2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AU2">
         <v>24</v>
@@ -21007,64 +21006,64 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>280</v>
-      </c>
       <c r="D1" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="K1" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>343</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -21078,55 +21077,55 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E2" t="s">
+        <v>372</v>
+      </c>
+      <c r="F2" t="s">
+        <v>372</v>
+      </c>
+      <c r="G2" t="s">
+        <v>372</v>
+      </c>
+      <c r="H2" t="s">
+        <v>372</v>
+      </c>
+      <c r="I2" t="s">
+        <v>372</v>
+      </c>
+      <c r="J2" t="s">
         <v>373</v>
       </c>
-      <c r="E2" t="s">
-        <v>373</v>
-      </c>
-      <c r="F2" t="s">
-        <v>373</v>
-      </c>
-      <c r="G2" t="s">
-        <v>373</v>
-      </c>
-      <c r="H2" t="s">
-        <v>373</v>
-      </c>
-      <c r="I2" t="s">
-        <v>373</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>372</v>
+      </c>
+      <c r="L2" t="s">
         <v>374</v>
       </c>
-      <c r="K2" t="s">
-        <v>373</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>375</v>
-      </c>
-      <c r="M2" t="s">
-        <v>376</v>
       </c>
       <c r="N2" t="b">
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="Q2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="R2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="S2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="T2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -21138,7 +21137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15AF778C-CAE3-C443-97C4-16CFC28CEAF9}">
   <dimension ref="A1:AD39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -21169,28 +21168,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
-      <c r="A1" s="108" t="s">
+      <c r="A1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" t="s">
         <v>278</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="C1" t="s">
         <v>279</v>
       </c>
-      <c r="C1" s="108" t="s">
-        <v>280</v>
-      </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1" t="s">
         <v>380</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="F1" t="s">
         <v>381</v>
       </c>
-      <c r="F1" s="108" t="s">
+      <c r="G1" t="s">
         <v>382</v>
       </c>
-      <c r="G1" s="108" t="s">
-        <v>383</v>
-      </c>
-      <c r="H1" s="108" t="s">
+      <c r="H1" t="s">
         <v>85</v>
       </c>
       <c r="I1" s="43" t="s">
@@ -21217,46 +21216,46 @@
       <c r="P1" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="Q1" s="108" t="s">
+      <c r="Q1" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="108" t="s">
+      <c r="R1" t="s">
         <v>122</v>
       </c>
-      <c r="S1" s="108" t="s">
+      <c r="S1" t="s">
         <v>123</v>
       </c>
-      <c r="T1" s="108" t="s">
+      <c r="T1" t="s">
         <v>95</v>
       </c>
-      <c r="U1" s="108" t="s">
+      <c r="U1" t="s">
         <v>96</v>
       </c>
-      <c r="V1" s="108" t="s">
+      <c r="V1" t="s">
         <v>97</v>
       </c>
-      <c r="W1" s="108" t="s">
+      <c r="W1" t="s">
         <v>98</v>
       </c>
-      <c r="X1" s="108" t="s">
+      <c r="X1" t="s">
         <v>99</v>
       </c>
-      <c r="Y1" s="108" t="s">
+      <c r="Y1" t="s">
         <v>100</v>
       </c>
-      <c r="Z1" s="108" t="s">
+      <c r="Z1" t="s">
         <v>101</v>
       </c>
-      <c r="AA1" s="108" t="s">
+      <c r="AA1" t="s">
         <v>102</v>
       </c>
-      <c r="AB1" s="108" t="s">
+      <c r="AB1" t="s">
         <v>191</v>
       </c>
-      <c r="AC1" s="108" t="s">
+      <c r="AC1" t="s">
         <v>245</v>
       </c>
-      <c r="AD1" s="108" t="s">
+      <c r="AD1" t="s">
         <v>199</v>
       </c>
     </row>
@@ -21274,10 +21273,10 @@
         <v>119</v>
       </c>
       <c r="E2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F2" t="s">
         <v>378</v>
-      </c>
-      <c r="F2" t="s">
-        <v>379</v>
       </c>
       <c r="G2">
         <v>4.4870000000000001</v>

</xml_diff>

<commit_message>
Importing sub collection works.
Also refactored common classes to @the-discounters/util and @the-discounters/types.
Still need to modify link CLI command to support sub collections.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027176E8-D6C3-E246-9368-4245FDFDB120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA24516-B31A-DD43-B3F1-2FFD2DEF4705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="3" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="1" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2489" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2496" uniqueCount="662">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -2057,6 +2057,21 @@
   </si>
   <si>
     <t>treatment_question_id</t>
+  </si>
+  <si>
+    <t>63853f2e1e9627b509ddeda0</t>
+  </si>
+  <si>
+    <t>63bf6a1798241e6c697023f2</t>
+  </si>
+  <si>
+    <t>640659902a48bd7fca2cd58d</t>
+  </si>
+  <si>
+    <t>649f3cffea5a1b2817d17d7e</t>
+  </si>
+  <si>
+    <t>[1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48]</t>
   </si>
 </sst>
 </file>
@@ -2069,7 +2084,7 @@
     <numFmt numFmtId="166" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2133,6 +2148,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2320,7 +2340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2426,6 +2446,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2526,9 +2547,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2566,7 +2587,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2672,7 +2693,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2814,7 +2835,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10165,7 +10186,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.60912194960520172</v>
+        <v>0.83955492169188684</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -10185,7 +10206,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.75063470062599591</v>
+        <v>0.13053123893464047</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -10206,7 +10227,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.6772723676177691</v>
+        <v>0.47676078037495762</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -10226,7 +10247,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.15081016955357662</v>
+        <v>0.97190898206677367</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -10487,48 +10508,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="82" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="82"/>
-      <c r="E3" s="81" t="s">
+      <c r="D3" s="83"/>
+      <c r="E3" s="82" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="82"/>
-      <c r="G3" s="81" t="s">
+      <c r="F3" s="83"/>
+      <c r="G3" s="82" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="82"/>
-      <c r="I3" s="81" t="s">
+      <c r="H3" s="83"/>
+      <c r="I3" s="82" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="82"/>
+      <c r="J3" s="83"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="83" t="s">
+      <c r="M3" s="84" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="84"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="83" t="s">
+      <c r="N3" s="85"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="84" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="83" t="s">
+      <c r="Q3" s="85"/>
+      <c r="R3" s="86"/>
+      <c r="S3" s="84" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="84"/>
-      <c r="U3" s="84"/>
-      <c r="V3" s="86" t="s">
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
+      <c r="V3" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="86"/>
-      <c r="X3" s="86"/>
+      <c r="W3" s="87"/>
+      <c r="X3" s="87"/>
       <c r="Y3" t="s">
         <v>215</v>
       </c>
@@ -11607,16 +11628,16 @@
       </c>
     </row>
     <row r="29" spans="1:33">
-      <c r="C29" s="87" t="s">
+      <c r="C29" s="88" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="87"/>
-      <c r="E29" s="87"/>
-      <c r="F29" s="87" t="s">
+      <c r="D29" s="88"/>
+      <c r="E29" s="88"/>
+      <c r="F29" s="88" t="s">
         <v>169</v>
       </c>
-      <c r="G29" s="87"/>
-      <c r="H29" s="87"/>
+      <c r="G29" s="88"/>
+      <c r="H29" s="88"/>
       <c r="J29" t="s">
         <v>168</v>
       </c>
@@ -12570,105 +12591,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="88" t="s">
+      <c r="C2" s="90"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="89"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="97" t="s">
+      <c r="F2" s="90"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="103" t="s">
+      <c r="I2" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103" t="s">
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="97" t="s">
+      <c r="S2" s="104"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="97" t="s">
+      <c r="W2" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="105" t="s">
+      <c r="X2" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="105" t="s">
+      <c r="Y2" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="105" t="s">
+      <c r="Z2" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="105" t="s">
+      <c r="AA2" s="106" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="95"/>
-      <c r="B3" s="91"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="104" t="s">
+      <c r="A3" s="96"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="102"/>
-      <c r="K3" s="102"/>
-      <c r="L3" s="102" t="s">
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="102"/>
-      <c r="N3" s="102" t="s">
+      <c r="M3" s="103"/>
+      <c r="N3" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="102"/>
-      <c r="P3" s="102" t="s">
+      <c r="O3" s="103"/>
+      <c r="P3" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="102"/>
-      <c r="R3" s="100" t="s">
+      <c r="Q3" s="103"/>
+      <c r="R3" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="100" t="s">
+      <c r="S3" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="100" t="s">
+      <c r="T3" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="100" t="s">
+      <c r="U3" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="98"/>
-      <c r="W3" s="98"/>
-      <c r="X3" s="106"/>
-      <c r="Y3" s="106"/>
-      <c r="Z3" s="106"/>
-      <c r="AA3" s="106"/>
+      <c r="V3" s="99"/>
+      <c r="W3" s="99"/>
+      <c r="X3" s="107"/>
+      <c r="Y3" s="107"/>
+      <c r="Z3" s="107"/>
+      <c r="AA3" s="107"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="96"/>
+      <c r="A4" s="97"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -12687,7 +12708,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="99"/>
+      <c r="H4" s="100"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -12715,16 +12736,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="101"/>
-      <c r="S4" s="101"/>
-      <c r="T4" s="101"/>
-      <c r="U4" s="101"/>
-      <c r="V4" s="99"/>
-      <c r="W4" s="99"/>
-      <c r="X4" s="107"/>
-      <c r="Y4" s="107"/>
-      <c r="Z4" s="107"/>
-      <c r="AA4" s="106"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="102"/>
+      <c r="V4" s="100"/>
+      <c r="W4" s="100"/>
+      <c r="X4" s="108"/>
+      <c r="Y4" s="108"/>
+      <c r="Z4" s="108"/>
+      <c r="AA4" s="107"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -16080,254 +16101,278 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAA32EA-3DA8-BD44-8758-9048DFA42915}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="6" width="21.5" customWidth="1"/>
-    <col min="7" max="8" width="21.5" style="36" customWidth="1"/>
-    <col min="9" max="10" width="21.5" customWidth="1"/>
-    <col min="11" max="11" width="28.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="4" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="7" width="21.5" customWidth="1"/>
+    <col min="8" max="9" width="21.5" style="36" customWidth="1"/>
+    <col min="10" max="11" width="21.5" customWidth="1"/>
+    <col min="12" max="12" width="28.83203125" customWidth="1"/>
+    <col min="13" max="13" width="63.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>254</v>
       </c>
       <c r="B1" t="s">
+        <v>656</v>
+      </c>
+      <c r="C1" t="s">
         <v>267</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>275</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>276</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>255</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>368</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="H1" s="36" t="s">
         <v>258</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="I1" s="36" t="s">
         <v>259</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>257</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>261</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>271</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="17">
+    <row r="2" spans="1:13" ht="17">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>268</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>253</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="G2" s="36">
+      <c r="H2" s="36">
         <v>44922</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>262</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="81" t="s">
+        <v>657</v>
+      </c>
+      <c r="M2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="17">
+    <row r="3" spans="1:13" ht="17">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>268</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>253</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="G3" s="36">
+      <c r="H3" s="36">
         <v>44940</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>3</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>262</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="81" t="s">
+        <v>658</v>
+      </c>
+      <c r="M3" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="17">
+    <row r="4" spans="1:13" ht="17">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>268</v>
-      </c>
-      <c r="C4">
-        <v>26</v>
       </c>
       <c r="D4">
         <v>26</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
         <v>253</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="G4" s="36">
+      <c r="H4" s="36">
         <v>44942</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>26</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>262</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="81" t="s">
+        <v>658</v>
+      </c>
+      <c r="M4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="17">
+    <row r="5" spans="1:13" ht="17">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>268</v>
-      </c>
-      <c r="C5">
-        <v>100</v>
       </c>
       <c r="D5">
         <v>100</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5" t="s">
         <v>253</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="G5" s="36">
+      <c r="H5" s="36">
         <v>44994</v>
       </c>
-      <c r="H5" s="36">
+      <c r="I5" s="36">
         <v>44995</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>100</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>262</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="81" t="s">
+        <v>659</v>
+      </c>
+      <c r="M5" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="17">
+    <row r="6" spans="1:13" ht="17">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>661</v>
+      </c>
+      <c r="C6" t="s">
         <v>269</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
         <v>253</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>150</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>262</v>
       </c>
       <c r="L6" t="s">
+        <v>660</v>
+      </c>
+      <c r="M6" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="51">
+    <row r="7" spans="1:13" ht="51">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>269</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
         <v>270</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>450</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>262</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="E14" s="68"/>
+    <row r="14" spans="1:13">
       <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -16674,7 +16719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5679E-80EB-0346-A65A-B2618C23925D}">
   <dimension ref="A1:KS2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -19263,7 +19308,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="A2" sqref="A2:A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Modified import for ids to be unique and got writing survey questions and participant working.
Refactored functions code into helper file and wrote unit tests for participant signup method.
Refactored shared unit test code into a mono repo so that it could be included as a dev dependency.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41671AF-AB60-EA44-AE7F-66ECF8E5A159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CDB16E-B9DA-5843-8A2A-17FED928EA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
-    <sheet name="fire_exp_prod" sheetId="20" r:id="rId2"/>
-    <sheet name="Fire participants" sheetId="21" r:id="rId3"/>
-    <sheet name="fire_survey_answers" sheetId="24" r:id="rId4"/>
+    <sheet name="Fire participants" sheetId="21" r:id="rId2"/>
+    <sheet name="fire_survey_answers" sheetId="24" r:id="rId3"/>
+    <sheet name="fire_exp_prod" sheetId="20" r:id="rId4"/>
     <sheet name="fire_ques_prod" sheetId="16" r:id="rId5"/>
     <sheet name="fire_treat_ques_prod" sheetId="19" r:id="rId6"/>
     <sheet name="fire_treat_prod" sheetId="17" r:id="rId7"/>
@@ -34,7 +34,7 @@
     <sheet name="Web Parameters v1" sheetId="1" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">fire_treat_ques_prod!$A$1:$E$207</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">fire_treat_ques_prod!$A$1:$E$234</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'MCL questions prod exp 1'!$A$1:$X$28</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Web Parameters Dev'!$B$1:$Y$88</definedName>
   </definedNames>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2722" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2757" uniqueCount="675">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -845,15 +845,9 @@
     <t>Not implemented.</t>
   </si>
   <si>
-    <t>exp_id</t>
-  </si>
-  <si>
     <t>betweenSubject</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -2100,6 +2094,24 @@
   </si>
   <si>
     <t>instruction_question</t>
+  </si>
+  <si>
+    <t>treatment_comment</t>
+  </si>
+  <si>
+    <t>question_comment</t>
+  </si>
+  <si>
+    <t>experiment_id</t>
+  </si>
+  <si>
+    <t>next</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Between subject test experiment.</t>
   </si>
 </sst>
 </file>
@@ -2475,6 +2487,9 @@
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2493,8 +2508,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2524,15 +2554,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2546,15 +2567,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10214,7 +10226,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.42949099779355437</v>
+        <v>0.31057826210619821</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -10234,7 +10246,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.94362798086247235</v>
+        <v>0.63314311976286941</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -10255,7 +10267,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.48742528213932368</v>
+        <v>0.63710912997502733</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -10275,7 +10287,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.36605314130497835</v>
+        <v>0.53792716883490477</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -10536,48 +10548,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="83" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="82" t="s">
+      <c r="D3" s="84"/>
+      <c r="E3" s="83" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="83"/>
-      <c r="G3" s="82" t="s">
+      <c r="F3" s="84"/>
+      <c r="G3" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="83"/>
-      <c r="I3" s="82" t="s">
+      <c r="H3" s="84"/>
+      <c r="I3" s="83" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="83"/>
+      <c r="J3" s="84"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="84" t="s">
+      <c r="M3" s="85" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="85"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="84" t="s">
+      <c r="N3" s="86"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="85" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="86"/>
-      <c r="S3" s="84" t="s">
+      <c r="Q3" s="86"/>
+      <c r="R3" s="87"/>
+      <c r="S3" s="85" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="85"/>
-      <c r="U3" s="85"/>
-      <c r="V3" s="87" t="s">
+      <c r="T3" s="86"/>
+      <c r="U3" s="86"/>
+      <c r="V3" s="88" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="87"/>
-      <c r="X3" s="87"/>
+      <c r="W3" s="88"/>
+      <c r="X3" s="88"/>
       <c r="Y3" t="s">
         <v>215</v>
       </c>
@@ -11656,16 +11668,16 @@
       </c>
     </row>
     <row r="29" spans="1:33">
-      <c r="C29" s="88" t="s">
+      <c r="C29" s="82" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="88"/>
-      <c r="E29" s="88"/>
-      <c r="F29" s="88" t="s">
+      <c r="D29" s="82"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="82" t="s">
         <v>169</v>
       </c>
-      <c r="G29" s="88"/>
-      <c r="H29" s="88"/>
+      <c r="G29" s="82"/>
+      <c r="H29" s="82"/>
       <c r="J29" t="s">
         <v>168</v>
       </c>
@@ -12570,16 +12582,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B26" r:id="rId1" xr:uid="{D2B54FA7-7284-A444-93E2-10BEB7DF1432}"/>
@@ -12619,105 +12631,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="95" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="89" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="89" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="90"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="98" t="s">
+      <c r="A2" s="101" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="95" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="96"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="95" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="96"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="104"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="104"/>
-      <c r="M2" s="104"/>
-      <c r="N2" s="104"/>
-      <c r="O2" s="104"/>
-      <c r="P2" s="104"/>
-      <c r="Q2" s="104"/>
-      <c r="R2" s="104" t="s">
+      <c r="J2" s="107"/>
+      <c r="K2" s="107"/>
+      <c r="L2" s="107"/>
+      <c r="M2" s="107"/>
+      <c r="N2" s="107"/>
+      <c r="O2" s="107"/>
+      <c r="P2" s="107"/>
+      <c r="Q2" s="107"/>
+      <c r="R2" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="104"/>
-      <c r="T2" s="104"/>
-      <c r="U2" s="104"/>
-      <c r="V2" s="98" t="s">
+      <c r="S2" s="107"/>
+      <c r="T2" s="107"/>
+      <c r="U2" s="107"/>
+      <c r="V2" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="98" t="s">
+      <c r="W2" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="106" t="s">
+      <c r="X2" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="106" t="s">
+      <c r="Y2" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="106" t="s">
+      <c r="Z2" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="106" t="s">
+      <c r="AA2" s="89" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="96"/>
-      <c r="B3" s="92"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="105" t="s">
+      <c r="A3" s="102"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="103"/>
-      <c r="K3" s="103"/>
-      <c r="L3" s="103" t="s">
+      <c r="J3" s="106"/>
+      <c r="K3" s="106"/>
+      <c r="L3" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="103"/>
-      <c r="N3" s="103" t="s">
+      <c r="M3" s="106"/>
+      <c r="N3" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="103"/>
-      <c r="P3" s="103" t="s">
+      <c r="O3" s="106"/>
+      <c r="P3" s="106" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="103"/>
-      <c r="R3" s="101" t="s">
+      <c r="Q3" s="106"/>
+      <c r="R3" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="101" t="s">
+      <c r="S3" s="104" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="101" t="s">
+      <c r="T3" s="104" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="101" t="s">
+      <c r="U3" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="99"/>
-      <c r="W3" s="99"/>
-      <c r="X3" s="107"/>
-      <c r="Y3" s="107"/>
-      <c r="Z3" s="107"/>
-      <c r="AA3" s="107"/>
+      <c r="V3" s="93"/>
+      <c r="W3" s="93"/>
+      <c r="X3" s="90"/>
+      <c r="Y3" s="90"/>
+      <c r="Z3" s="90"/>
+      <c r="AA3" s="90"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="97"/>
+      <c r="A4" s="103"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -12736,7 +12748,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="100"/>
+      <c r="H4" s="94"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -12764,16 +12776,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="102"/>
-      <c r="S4" s="102"/>
-      <c r="T4" s="102"/>
-      <c r="U4" s="102"/>
-      <c r="V4" s="100"/>
-      <c r="W4" s="100"/>
-      <c r="X4" s="108"/>
-      <c r="Y4" s="108"/>
-      <c r="Z4" s="108"/>
-      <c r="AA4" s="107"/>
+      <c r="R4" s="105"/>
+      <c r="S4" s="105"/>
+      <c r="T4" s="105"/>
+      <c r="U4" s="105"/>
+      <c r="V4" s="94"/>
+      <c r="W4" s="94"/>
+      <c r="X4" s="91"/>
+      <c r="Y4" s="91"/>
+      <c r="Z4" s="91"/>
+      <c r="AA4" s="90"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -13274,11 +13286,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -13294,6 +13301,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -16128,342 +16140,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAA32EA-3DA8-BD44-8758-9048DFA42915}">
-  <dimension ref="A1:M15"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="2" max="2" width="113" customWidth="1"/>
-    <col min="4" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="7" width="21.5" customWidth="1"/>
-    <col min="8" max="9" width="21.5" style="36" customWidth="1"/>
-    <col min="10" max="11" width="21.5" customWidth="1"/>
-    <col min="12" max="12" width="28.83203125" customWidth="1"/>
-    <col min="13" max="13" width="63.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" t="s">
-        <v>254</v>
-      </c>
-      <c r="B1" t="s">
-        <v>655</v>
-      </c>
-      <c r="C1" t="s">
-        <v>267</v>
-      </c>
-      <c r="D1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E1" t="s">
-        <v>275</v>
-      </c>
-      <c r="F1" t="s">
-        <v>255</v>
-      </c>
-      <c r="G1" t="s">
-        <v>367</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>258</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>259</v>
-      </c>
-      <c r="J1" t="s">
-        <v>257</v>
-      </c>
-      <c r="K1" t="s">
-        <v>261</v>
-      </c>
-      <c r="L1" t="s">
-        <v>271</v>
-      </c>
-      <c r="M1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="17">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>660</v>
-      </c>
-      <c r="C2" t="s">
-        <v>269</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>253</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>661</v>
-      </c>
-      <c r="H2" s="36">
-        <v>1</v>
-      </c>
-      <c r="I2" s="36">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>662</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="17">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>664</v>
-      </c>
-      <c r="C3" t="s">
-        <v>268</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>253</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>661</v>
-      </c>
-      <c r="H3" s="36">
-        <v>44922</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>262</v>
-      </c>
-      <c r="L3" s="81" t="s">
-        <v>656</v>
-      </c>
-      <c r="M3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="17">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>665</v>
-      </c>
-      <c r="C4" t="s">
-        <v>268</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>253</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>661</v>
-      </c>
-      <c r="H4" s="36">
-        <v>44940</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-      <c r="K4" t="s">
-        <v>262</v>
-      </c>
-      <c r="L4" s="81" t="s">
-        <v>657</v>
-      </c>
-      <c r="M4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="17">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>666</v>
-      </c>
-      <c r="C5" t="s">
-        <v>268</v>
-      </c>
-      <c r="D5">
-        <v>26</v>
-      </c>
-      <c r="E5">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>253</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>661</v>
-      </c>
-      <c r="H5" s="36">
-        <v>44942</v>
-      </c>
-      <c r="J5">
-        <v>26</v>
-      </c>
-      <c r="K5" t="s">
-        <v>262</v>
-      </c>
-      <c r="L5" s="81" t="s">
-        <v>657</v>
-      </c>
-      <c r="M5" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="17">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>667</v>
-      </c>
-      <c r="C6" t="s">
-        <v>268</v>
-      </c>
-      <c r="D6">
-        <v>100</v>
-      </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
-      <c r="F6" t="s">
-        <v>253</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>661</v>
-      </c>
-      <c r="H6" s="36">
-        <v>44994</v>
-      </c>
-      <c r="I6" s="36">
-        <v>44995</v>
-      </c>
-      <c r="J6">
-        <v>100</v>
-      </c>
-      <c r="K6" t="s">
-        <v>262</v>
-      </c>
-      <c r="L6" s="81" t="s">
-        <v>658</v>
-      </c>
-      <c r="M6" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="17">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>668</v>
-      </c>
-      <c r="C7" t="s">
-        <v>268</v>
-      </c>
-      <c r="D7">
-        <v>449</v>
-      </c>
-      <c r="E7">
-        <v>449</v>
-      </c>
-      <c r="F7" t="s">
-        <v>253</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>661</v>
-      </c>
-      <c r="H7" s="36">
-        <v>45119</v>
-      </c>
-      <c r="I7" s="36">
-        <v>45119</v>
-      </c>
-      <c r="J7">
-        <v>150</v>
-      </c>
-      <c r="K7" t="s">
-        <v>262</v>
-      </c>
-      <c r="L7" t="s">
-        <v>659</v>
-      </c>
-      <c r="M7" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="51">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>669</v>
-      </c>
-      <c r="C8" t="s">
-        <v>269</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>270</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="J8">
-        <v>150</v>
-      </c>
-      <c r="K8" t="s">
-        <v>262</v>
-      </c>
-      <c r="M8" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="F15" s="68"/>
-      <c r="G15" s="68"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91309BC-EDBB-B243-A200-766606222923}">
   <dimension ref="A1:BD2"/>
   <sheetViews>
@@ -16479,169 +16155,169 @@
   <sheetData>
     <row r="1" spans="1:56" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>276</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>278</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>116</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AF1" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AG1" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AH1" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AI1" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AJ1" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="AK1" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="AL1" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AM1" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="AJ1" s="8" t="s">
-        <v>338</v>
-      </c>
-      <c r="AK1" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AN1" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AO1" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AP1" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AQ1" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="AP1" s="8" t="s">
+      <c r="AR1" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="AQ1" s="8" t="s">
+      <c r="AS1" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="AR1" s="8" t="s">
+      <c r="AT1" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="AS1" s="8" t="s">
+      <c r="AU1" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="AT1" s="8" t="s">
+      <c r="AV1" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="AU1" s="8" t="s">
+      <c r="AW1" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="AV1" s="8" t="s">
+      <c r="AX1" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="AW1" s="8" t="s">
+      <c r="AY1" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="AX1" s="8" t="s">
+      <c r="AZ1" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="AY1" s="8" t="s">
+      <c r="BA1" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="AZ1" s="8" t="s">
+      <c r="BB1" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="BA1" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="BB1" s="8" t="s">
-        <v>326</v>
-      </c>
       <c r="BD1" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:56">
@@ -16658,73 +16334,73 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G2">
         <v>30.965</v>
       </c>
       <c r="H2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="I2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="J2">
         <v>49.71</v>
       </c>
       <c r="K2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="L2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="M2">
         <v>51.975999999999999</v>
       </c>
       <c r="N2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="O2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="P2">
         <v>17.925000000000001</v>
       </c>
       <c r="Q2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="R2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="S2">
         <v>34.722999999999999</v>
       </c>
       <c r="T2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="U2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="V2">
         <v>32.575000000000003</v>
       </c>
       <c r="W2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="X2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="Y2">
         <v>25.481999999999999</v>
       </c>
       <c r="Z2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="AA2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AB2">
         <v>16.695</v>
@@ -16733,7 +16409,7 @@
         <v>1</v>
       </c>
       <c r="AD2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="AE2">
         <v>5</v>
@@ -16742,19 +16418,19 @@
         <v>63</v>
       </c>
       <c r="AG2" t="s">
+        <v>356</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>357</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>358</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AL2" t="s">
         <v>359</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AM2" t="s">
         <v>360</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>361</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>362</v>
       </c>
       <c r="AP2">
         <v>24</v>
@@ -16769,7 +16445,7 @@
         <v>0</v>
       </c>
       <c r="AT2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="AU2">
         <v>24</v>
@@ -16802,7 +16478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5679E-80EB-0346-A65A-B2618C23925D}">
   <dimension ref="A1:KS2"/>
   <sheetViews>
@@ -16818,919 +16494,919 @@
   <sheetData>
     <row r="1" spans="1:305">
       <c r="A1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1" t="s">
         <v>276</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>653</v>
+      </c>
+      <c r="E1" t="s">
         <v>277</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>278</v>
       </c>
-      <c r="D1" t="s">
-        <v>655</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>279</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>280</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>281</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>282</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>283</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>284</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>285</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>286</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>287</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>288</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
+        <v>366</v>
+      </c>
+      <c r="R1" t="s">
+        <v>367</v>
+      </c>
+      <c r="S1" t="s">
+        <v>368</v>
+      </c>
+      <c r="T1" t="s">
         <v>289</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
         <v>290</v>
       </c>
-      <c r="Q1" t="s">
-        <v>368</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
+        <v>291</v>
+      </c>
+      <c r="W1" t="s">
+        <v>292</v>
+      </c>
+      <c r="X1" t="s">
+        <v>293</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>294</v>
+      </c>
+      <c r="Z1" t="s">
         <v>369</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AA1" t="s">
         <v>370</v>
       </c>
-      <c r="T1" t="s">
-        <v>291</v>
-      </c>
-      <c r="U1" t="s">
-        <v>292</v>
-      </c>
-      <c r="V1" t="s">
-        <v>293</v>
-      </c>
-      <c r="W1" t="s">
-        <v>294</v>
-      </c>
-      <c r="X1" t="s">
-        <v>295</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>296</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>371</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>372</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>373</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>374</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
+        <v>298</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>299</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>300</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>301</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>302</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>304</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>305</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>306</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>307</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>336</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>337</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>308</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>309</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>310</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>311</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>312</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>313</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>314</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>315</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>316</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>318</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>319</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>320</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>321</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>322</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>323</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>324</v>
+      </c>
+      <c r="BI1" t="s">
         <v>375</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="BJ1" t="s">
         <v>376</v>
       </c>
-      <c r="AF1" t="s">
-        <v>300</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>301</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>302</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>303</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>304</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>305</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>306</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>307</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>308</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>309</v>
-      </c>
-      <c r="AP1" t="s">
+      <c r="BK1" t="s">
+        <v>377</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>378</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>379</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>380</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>381</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>382</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>383</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>384</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>385</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>386</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>387</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>388</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>389</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>390</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>391</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>392</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>393</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>394</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>395</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>396</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>397</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>398</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>399</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>400</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>401</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>402</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>403</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>404</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>405</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>406</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>407</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>408</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>409</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>410</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>411</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>412</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>413</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>414</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>415</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>416</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>417</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>418</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>419</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>420</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>421</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>422</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>423</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>424</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>425</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>426</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>427</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>428</v>
+      </c>
+      <c r="DK1" t="s">
+        <v>429</v>
+      </c>
+      <c r="DL1" t="s">
+        <v>430</v>
+      </c>
+      <c r="DM1" t="s">
+        <v>431</v>
+      </c>
+      <c r="DN1" t="s">
+        <v>432</v>
+      </c>
+      <c r="DO1" t="s">
+        <v>433</v>
+      </c>
+      <c r="DP1" t="s">
+        <v>434</v>
+      </c>
+      <c r="DQ1" t="s">
+        <v>435</v>
+      </c>
+      <c r="DR1" t="s">
+        <v>436</v>
+      </c>
+      <c r="DS1" t="s">
+        <v>437</v>
+      </c>
+      <c r="DT1" t="s">
+        <v>438</v>
+      </c>
+      <c r="DU1" t="s">
+        <v>439</v>
+      </c>
+      <c r="DV1" t="s">
+        <v>440</v>
+      </c>
+      <c r="DW1" t="s">
+        <v>441</v>
+      </c>
+      <c r="DX1" t="s">
+        <v>442</v>
+      </c>
+      <c r="DY1" t="s">
+        <v>443</v>
+      </c>
+      <c r="DZ1" t="s">
+        <v>444</v>
+      </c>
+      <c r="EA1" t="s">
+        <v>445</v>
+      </c>
+      <c r="EB1" t="s">
+        <v>446</v>
+      </c>
+      <c r="EC1" t="s">
+        <v>447</v>
+      </c>
+      <c r="ED1" t="s">
+        <v>448</v>
+      </c>
+      <c r="EE1" t="s">
+        <v>449</v>
+      </c>
+      <c r="EF1" t="s">
+        <v>450</v>
+      </c>
+      <c r="EG1" t="s">
+        <v>451</v>
+      </c>
+      <c r="EH1" t="s">
+        <v>452</v>
+      </c>
+      <c r="EI1" t="s">
+        <v>453</v>
+      </c>
+      <c r="EJ1" t="s">
+        <v>454</v>
+      </c>
+      <c r="EK1" t="s">
+        <v>455</v>
+      </c>
+      <c r="EL1" t="s">
+        <v>456</v>
+      </c>
+      <c r="EM1" t="s">
+        <v>457</v>
+      </c>
+      <c r="EN1" t="s">
+        <v>458</v>
+      </c>
+      <c r="EO1" t="s">
+        <v>459</v>
+      </c>
+      <c r="EP1" t="s">
+        <v>460</v>
+      </c>
+      <c r="EQ1" t="s">
+        <v>461</v>
+      </c>
+      <c r="ER1" t="s">
+        <v>462</v>
+      </c>
+      <c r="ES1" t="s">
+        <v>463</v>
+      </c>
+      <c r="ET1" t="s">
+        <v>464</v>
+      </c>
+      <c r="EU1" t="s">
+        <v>465</v>
+      </c>
+      <c r="EV1" t="s">
+        <v>466</v>
+      </c>
+      <c r="EW1" t="s">
+        <v>467</v>
+      </c>
+      <c r="EX1" t="s">
+        <v>468</v>
+      </c>
+      <c r="EY1" t="s">
+        <v>469</v>
+      </c>
+      <c r="EZ1" t="s">
+        <v>470</v>
+      </c>
+      <c r="FA1" t="s">
+        <v>471</v>
+      </c>
+      <c r="FB1" t="s">
+        <v>472</v>
+      </c>
+      <c r="FC1" t="s">
+        <v>473</v>
+      </c>
+      <c r="FD1" t="s">
+        <v>474</v>
+      </c>
+      <c r="FE1" t="s">
+        <v>475</v>
+      </c>
+      <c r="FF1" t="s">
+        <v>476</v>
+      </c>
+      <c r="FG1" t="s">
+        <v>477</v>
+      </c>
+      <c r="FH1" t="s">
+        <v>478</v>
+      </c>
+      <c r="FI1" t="s">
+        <v>479</v>
+      </c>
+      <c r="FJ1" t="s">
+        <v>480</v>
+      </c>
+      <c r="FK1" t="s">
+        <v>481</v>
+      </c>
+      <c r="FL1" t="s">
+        <v>482</v>
+      </c>
+      <c r="FM1" t="s">
+        <v>483</v>
+      </c>
+      <c r="FN1" t="s">
+        <v>484</v>
+      </c>
+      <c r="FO1" t="s">
+        <v>485</v>
+      </c>
+      <c r="FP1" t="s">
+        <v>486</v>
+      </c>
+      <c r="FQ1" t="s">
+        <v>487</v>
+      </c>
+      <c r="FR1" t="s">
+        <v>488</v>
+      </c>
+      <c r="FS1" t="s">
+        <v>489</v>
+      </c>
+      <c r="FT1" t="s">
+        <v>490</v>
+      </c>
+      <c r="FU1" t="s">
+        <v>491</v>
+      </c>
+      <c r="FV1" t="s">
+        <v>492</v>
+      </c>
+      <c r="FW1" t="s">
+        <v>493</v>
+      </c>
+      <c r="FX1" t="s">
+        <v>494</v>
+      </c>
+      <c r="FY1" t="s">
+        <v>495</v>
+      </c>
+      <c r="FZ1" t="s">
+        <v>496</v>
+      </c>
+      <c r="GA1" t="s">
+        <v>497</v>
+      </c>
+      <c r="GB1" t="s">
+        <v>498</v>
+      </c>
+      <c r="GC1" t="s">
+        <v>499</v>
+      </c>
+      <c r="GD1" t="s">
+        <v>500</v>
+      </c>
+      <c r="GE1" t="s">
+        <v>501</v>
+      </c>
+      <c r="GF1" t="s">
+        <v>502</v>
+      </c>
+      <c r="GG1" t="s">
+        <v>503</v>
+      </c>
+      <c r="GH1" t="s">
+        <v>504</v>
+      </c>
+      <c r="GI1" t="s">
+        <v>505</v>
+      </c>
+      <c r="GJ1" t="s">
+        <v>506</v>
+      </c>
+      <c r="GK1" t="s">
+        <v>507</v>
+      </c>
+      <c r="GL1" t="s">
+        <v>508</v>
+      </c>
+      <c r="GM1" t="s">
+        <v>509</v>
+      </c>
+      <c r="GN1" t="s">
+        <v>510</v>
+      </c>
+      <c r="GO1" t="s">
+        <v>511</v>
+      </c>
+      <c r="GP1" t="s">
+        <v>512</v>
+      </c>
+      <c r="GQ1" t="s">
+        <v>513</v>
+      </c>
+      <c r="GR1" t="s">
+        <v>514</v>
+      </c>
+      <c r="GS1" t="s">
+        <v>515</v>
+      </c>
+      <c r="GT1" t="s">
+        <v>516</v>
+      </c>
+      <c r="GU1" t="s">
+        <v>517</v>
+      </c>
+      <c r="GV1" t="s">
+        <v>518</v>
+      </c>
+      <c r="GW1" t="s">
+        <v>519</v>
+      </c>
+      <c r="GX1" t="s">
+        <v>520</v>
+      </c>
+      <c r="GY1" t="s">
+        <v>521</v>
+      </c>
+      <c r="GZ1" t="s">
+        <v>522</v>
+      </c>
+      <c r="HA1" t="s">
+        <v>523</v>
+      </c>
+      <c r="HB1" t="s">
+        <v>524</v>
+      </c>
+      <c r="HC1" t="s">
+        <v>525</v>
+      </c>
+      <c r="HD1" t="s">
+        <v>526</v>
+      </c>
+      <c r="HE1" t="s">
+        <v>527</v>
+      </c>
+      <c r="HF1" t="s">
+        <v>528</v>
+      </c>
+      <c r="HG1" t="s">
+        <v>529</v>
+      </c>
+      <c r="HH1" t="s">
+        <v>530</v>
+      </c>
+      <c r="HI1" t="s">
+        <v>531</v>
+      </c>
+      <c r="HJ1" t="s">
+        <v>532</v>
+      </c>
+      <c r="HK1" t="s">
+        <v>533</v>
+      </c>
+      <c r="HL1" t="s">
+        <v>534</v>
+      </c>
+      <c r="HM1" t="s">
+        <v>535</v>
+      </c>
+      <c r="HN1" t="s">
+        <v>536</v>
+      </c>
+      <c r="HO1" t="s">
+        <v>537</v>
+      </c>
+      <c r="HP1" t="s">
+        <v>538</v>
+      </c>
+      <c r="HQ1" t="s">
+        <v>539</v>
+      </c>
+      <c r="HR1" t="s">
+        <v>540</v>
+      </c>
+      <c r="HS1" t="s">
+        <v>541</v>
+      </c>
+      <c r="HT1" t="s">
+        <v>542</v>
+      </c>
+      <c r="HU1" t="s">
+        <v>543</v>
+      </c>
+      <c r="HV1" t="s">
+        <v>544</v>
+      </c>
+      <c r="HW1" t="s">
+        <v>545</v>
+      </c>
+      <c r="HX1" t="s">
+        <v>546</v>
+      </c>
+      <c r="HY1" t="s">
+        <v>547</v>
+      </c>
+      <c r="HZ1" t="s">
+        <v>548</v>
+      </c>
+      <c r="IA1" t="s">
+        <v>549</v>
+      </c>
+      <c r="IB1" t="s">
+        <v>550</v>
+      </c>
+      <c r="IC1" t="s">
+        <v>551</v>
+      </c>
+      <c r="ID1" t="s">
+        <v>552</v>
+      </c>
+      <c r="IE1" t="s">
+        <v>553</v>
+      </c>
+      <c r="IF1" t="s">
+        <v>554</v>
+      </c>
+      <c r="IG1" t="s">
+        <v>555</v>
+      </c>
+      <c r="IH1" t="s">
+        <v>556</v>
+      </c>
+      <c r="II1" t="s">
+        <v>557</v>
+      </c>
+      <c r="IJ1" t="s">
+        <v>558</v>
+      </c>
+      <c r="IK1" t="s">
+        <v>559</v>
+      </c>
+      <c r="IL1" t="s">
+        <v>560</v>
+      </c>
+      <c r="IM1" t="s">
+        <v>561</v>
+      </c>
+      <c r="IN1" t="s">
+        <v>562</v>
+      </c>
+      <c r="IO1" t="s">
+        <v>563</v>
+      </c>
+      <c r="IP1" t="s">
+        <v>564</v>
+      </c>
+      <c r="IQ1" t="s">
+        <v>565</v>
+      </c>
+      <c r="IR1" t="s">
+        <v>566</v>
+      </c>
+      <c r="IS1" t="s">
+        <v>567</v>
+      </c>
+      <c r="IT1" t="s">
+        <v>568</v>
+      </c>
+      <c r="IU1" t="s">
+        <v>569</v>
+      </c>
+      <c r="IV1" t="s">
+        <v>570</v>
+      </c>
+      <c r="IW1" t="s">
+        <v>571</v>
+      </c>
+      <c r="IX1" t="s">
+        <v>572</v>
+      </c>
+      <c r="IY1" t="s">
+        <v>573</v>
+      </c>
+      <c r="IZ1" t="s">
+        <v>574</v>
+      </c>
+      <c r="JA1" t="s">
+        <v>575</v>
+      </c>
+      <c r="JB1" t="s">
+        <v>576</v>
+      </c>
+      <c r="JC1" t="s">
+        <v>577</v>
+      </c>
+      <c r="JD1" t="s">
+        <v>578</v>
+      </c>
+      <c r="JE1" t="s">
+        <v>579</v>
+      </c>
+      <c r="JF1" t="s">
+        <v>580</v>
+      </c>
+      <c r="JG1" t="s">
+        <v>581</v>
+      </c>
+      <c r="JH1" t="s">
+        <v>582</v>
+      </c>
+      <c r="JI1" t="s">
+        <v>583</v>
+      </c>
+      <c r="JJ1" t="s">
+        <v>584</v>
+      </c>
+      <c r="JK1" t="s">
+        <v>585</v>
+      </c>
+      <c r="JL1" t="s">
+        <v>586</v>
+      </c>
+      <c r="JM1" t="s">
+        <v>587</v>
+      </c>
+      <c r="JN1" t="s">
+        <v>588</v>
+      </c>
+      <c r="JO1" t="s">
+        <v>589</v>
+      </c>
+      <c r="JP1" t="s">
+        <v>590</v>
+      </c>
+      <c r="JQ1" t="s">
+        <v>591</v>
+      </c>
+      <c r="JR1" t="s">
+        <v>592</v>
+      </c>
+      <c r="JS1" t="s">
+        <v>593</v>
+      </c>
+      <c r="JT1" t="s">
+        <v>594</v>
+      </c>
+      <c r="JU1" t="s">
+        <v>595</v>
+      </c>
+      <c r="JV1" t="s">
+        <v>596</v>
+      </c>
+      <c r="JW1" t="s">
+        <v>597</v>
+      </c>
+      <c r="JX1" t="s">
+        <v>598</v>
+      </c>
+      <c r="JY1" t="s">
+        <v>599</v>
+      </c>
+      <c r="JZ1" t="s">
+        <v>325</v>
+      </c>
+      <c r="KA1" t="s">
+        <v>326</v>
+      </c>
+      <c r="KB1" t="s">
+        <v>327</v>
+      </c>
+      <c r="KC1" t="s">
+        <v>328</v>
+      </c>
+      <c r="KD1" t="s">
+        <v>329</v>
+      </c>
+      <c r="KE1" t="s">
+        <v>330</v>
+      </c>
+      <c r="KF1" t="s">
+        <v>331</v>
+      </c>
+      <c r="KG1" t="s">
         <v>338</v>
       </c>
-      <c r="AQ1" t="s">
-        <v>339</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>310</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>311</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>312</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>313</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>314</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>315</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>316</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>317</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>318</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>319</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>320</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>321</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>322</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>323</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>324</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>325</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>326</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>377</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>378</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>379</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>380</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>381</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>382</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>383</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>384</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>385</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>386</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>387</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>388</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>389</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>390</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>391</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>392</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>393</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>394</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>395</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>396</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>397</v>
-      </c>
-      <c r="CD1" t="s">
-        <v>398</v>
-      </c>
-      <c r="CE1" t="s">
-        <v>399</v>
-      </c>
-      <c r="CF1" t="s">
-        <v>400</v>
-      </c>
-      <c r="CG1" t="s">
-        <v>401</v>
-      </c>
-      <c r="CH1" t="s">
-        <v>402</v>
-      </c>
-      <c r="CI1" t="s">
-        <v>403</v>
-      </c>
-      <c r="CJ1" t="s">
-        <v>404</v>
-      </c>
-      <c r="CK1" t="s">
-        <v>405</v>
-      </c>
-      <c r="CL1" t="s">
-        <v>406</v>
-      </c>
-      <c r="CM1" t="s">
-        <v>407</v>
-      </c>
-      <c r="CN1" t="s">
-        <v>408</v>
-      </c>
-      <c r="CO1" t="s">
-        <v>409</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>410</v>
-      </c>
-      <c r="CQ1" t="s">
-        <v>411</v>
-      </c>
-      <c r="CR1" t="s">
-        <v>412</v>
-      </c>
-      <c r="CS1" t="s">
-        <v>413</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>414</v>
-      </c>
-      <c r="CU1" t="s">
-        <v>415</v>
-      </c>
-      <c r="CV1" t="s">
-        <v>416</v>
-      </c>
-      <c r="CW1" t="s">
-        <v>417</v>
-      </c>
-      <c r="CX1" t="s">
-        <v>418</v>
-      </c>
-      <c r="CY1" t="s">
-        <v>419</v>
-      </c>
-      <c r="CZ1" t="s">
-        <v>420</v>
-      </c>
-      <c r="DA1" t="s">
-        <v>421</v>
-      </c>
-      <c r="DB1" t="s">
-        <v>422</v>
-      </c>
-      <c r="DC1" t="s">
-        <v>423</v>
-      </c>
-      <c r="DD1" t="s">
-        <v>424</v>
-      </c>
-      <c r="DE1" t="s">
-        <v>425</v>
-      </c>
-      <c r="DF1" t="s">
-        <v>426</v>
-      </c>
-      <c r="DG1" t="s">
-        <v>427</v>
-      </c>
-      <c r="DH1" t="s">
-        <v>428</v>
-      </c>
-      <c r="DI1" t="s">
-        <v>429</v>
-      </c>
-      <c r="DJ1" t="s">
-        <v>430</v>
-      </c>
-      <c r="DK1" t="s">
-        <v>431</v>
-      </c>
-      <c r="DL1" t="s">
-        <v>432</v>
-      </c>
-      <c r="DM1" t="s">
-        <v>433</v>
-      </c>
-      <c r="DN1" t="s">
-        <v>434</v>
-      </c>
-      <c r="DO1" t="s">
-        <v>435</v>
-      </c>
-      <c r="DP1" t="s">
-        <v>436</v>
-      </c>
-      <c r="DQ1" t="s">
-        <v>437</v>
-      </c>
-      <c r="DR1" t="s">
-        <v>438</v>
-      </c>
-      <c r="DS1" t="s">
-        <v>439</v>
-      </c>
-      <c r="DT1" t="s">
-        <v>440</v>
-      </c>
-      <c r="DU1" t="s">
-        <v>441</v>
-      </c>
-      <c r="DV1" t="s">
-        <v>442</v>
-      </c>
-      <c r="DW1" t="s">
-        <v>443</v>
-      </c>
-      <c r="DX1" t="s">
-        <v>444</v>
-      </c>
-      <c r="DY1" t="s">
-        <v>445</v>
-      </c>
-      <c r="DZ1" t="s">
-        <v>446</v>
-      </c>
-      <c r="EA1" t="s">
-        <v>447</v>
-      </c>
-      <c r="EB1" t="s">
-        <v>448</v>
-      </c>
-      <c r="EC1" t="s">
-        <v>449</v>
-      </c>
-      <c r="ED1" t="s">
-        <v>450</v>
-      </c>
-      <c r="EE1" t="s">
-        <v>451</v>
-      </c>
-      <c r="EF1" t="s">
-        <v>452</v>
-      </c>
-      <c r="EG1" t="s">
-        <v>453</v>
-      </c>
-      <c r="EH1" t="s">
-        <v>454</v>
-      </c>
-      <c r="EI1" t="s">
-        <v>455</v>
-      </c>
-      <c r="EJ1" t="s">
-        <v>456</v>
-      </c>
-      <c r="EK1" t="s">
-        <v>457</v>
-      </c>
-      <c r="EL1" t="s">
-        <v>458</v>
-      </c>
-      <c r="EM1" t="s">
-        <v>459</v>
-      </c>
-      <c r="EN1" t="s">
-        <v>460</v>
-      </c>
-      <c r="EO1" t="s">
-        <v>461</v>
-      </c>
-      <c r="EP1" t="s">
-        <v>462</v>
-      </c>
-      <c r="EQ1" t="s">
-        <v>463</v>
-      </c>
-      <c r="ER1" t="s">
-        <v>464</v>
-      </c>
-      <c r="ES1" t="s">
-        <v>465</v>
-      </c>
-      <c r="ET1" t="s">
-        <v>466</v>
-      </c>
-      <c r="EU1" t="s">
-        <v>467</v>
-      </c>
-      <c r="EV1" t="s">
-        <v>468</v>
-      </c>
-      <c r="EW1" t="s">
-        <v>469</v>
-      </c>
-      <c r="EX1" t="s">
-        <v>470</v>
-      </c>
-      <c r="EY1" t="s">
-        <v>471</v>
-      </c>
-      <c r="EZ1" t="s">
-        <v>472</v>
-      </c>
-      <c r="FA1" t="s">
-        <v>473</v>
-      </c>
-      <c r="FB1" t="s">
-        <v>474</v>
-      </c>
-      <c r="FC1" t="s">
-        <v>475</v>
-      </c>
-      <c r="FD1" t="s">
-        <v>476</v>
-      </c>
-      <c r="FE1" t="s">
-        <v>477</v>
-      </c>
-      <c r="FF1" t="s">
-        <v>478</v>
-      </c>
-      <c r="FG1" t="s">
-        <v>479</v>
-      </c>
-      <c r="FH1" t="s">
-        <v>480</v>
-      </c>
-      <c r="FI1" t="s">
-        <v>481</v>
-      </c>
-      <c r="FJ1" t="s">
-        <v>482</v>
-      </c>
-      <c r="FK1" t="s">
-        <v>483</v>
-      </c>
-      <c r="FL1" t="s">
-        <v>484</v>
-      </c>
-      <c r="FM1" t="s">
-        <v>485</v>
-      </c>
-      <c r="FN1" t="s">
-        <v>486</v>
-      </c>
-      <c r="FO1" t="s">
-        <v>487</v>
-      </c>
-      <c r="FP1" t="s">
-        <v>488</v>
-      </c>
-      <c r="FQ1" t="s">
-        <v>489</v>
-      </c>
-      <c r="FR1" t="s">
-        <v>490</v>
-      </c>
-      <c r="FS1" t="s">
-        <v>491</v>
-      </c>
-      <c r="FT1" t="s">
-        <v>492</v>
-      </c>
-      <c r="FU1" t="s">
-        <v>493</v>
-      </c>
-      <c r="FV1" t="s">
-        <v>494</v>
-      </c>
-      <c r="FW1" t="s">
-        <v>495</v>
-      </c>
-      <c r="FX1" t="s">
-        <v>496</v>
-      </c>
-      <c r="FY1" t="s">
-        <v>497</v>
-      </c>
-      <c r="FZ1" t="s">
-        <v>498</v>
-      </c>
-      <c r="GA1" t="s">
-        <v>499</v>
-      </c>
-      <c r="GB1" t="s">
-        <v>500</v>
-      </c>
-      <c r="GC1" t="s">
-        <v>501</v>
-      </c>
-      <c r="GD1" t="s">
-        <v>502</v>
-      </c>
-      <c r="GE1" t="s">
-        <v>503</v>
-      </c>
-      <c r="GF1" t="s">
-        <v>504</v>
-      </c>
-      <c r="GG1" t="s">
-        <v>505</v>
-      </c>
-      <c r="GH1" t="s">
-        <v>506</v>
-      </c>
-      <c r="GI1" t="s">
-        <v>507</v>
-      </c>
-      <c r="GJ1" t="s">
-        <v>508</v>
-      </c>
-      <c r="GK1" t="s">
-        <v>509</v>
-      </c>
-      <c r="GL1" t="s">
-        <v>510</v>
-      </c>
-      <c r="GM1" t="s">
-        <v>511</v>
-      </c>
-      <c r="GN1" t="s">
-        <v>512</v>
-      </c>
-      <c r="GO1" t="s">
-        <v>513</v>
-      </c>
-      <c r="GP1" t="s">
-        <v>514</v>
-      </c>
-      <c r="GQ1" t="s">
-        <v>515</v>
-      </c>
-      <c r="GR1" t="s">
-        <v>516</v>
-      </c>
-      <c r="GS1" t="s">
-        <v>517</v>
-      </c>
-      <c r="GT1" t="s">
-        <v>518</v>
-      </c>
-      <c r="GU1" t="s">
-        <v>519</v>
-      </c>
-      <c r="GV1" t="s">
-        <v>520</v>
-      </c>
-      <c r="GW1" t="s">
-        <v>521</v>
-      </c>
-      <c r="GX1" t="s">
-        <v>522</v>
-      </c>
-      <c r="GY1" t="s">
-        <v>523</v>
-      </c>
-      <c r="GZ1" t="s">
-        <v>524</v>
-      </c>
-      <c r="HA1" t="s">
-        <v>525</v>
-      </c>
-      <c r="HB1" t="s">
-        <v>526</v>
-      </c>
-      <c r="HC1" t="s">
-        <v>527</v>
-      </c>
-      <c r="HD1" t="s">
-        <v>528</v>
-      </c>
-      <c r="HE1" t="s">
-        <v>529</v>
-      </c>
-      <c r="HF1" t="s">
-        <v>530</v>
-      </c>
-      <c r="HG1" t="s">
-        <v>531</v>
-      </c>
-      <c r="HH1" t="s">
-        <v>532</v>
-      </c>
-      <c r="HI1" t="s">
-        <v>533</v>
-      </c>
-      <c r="HJ1" t="s">
-        <v>534</v>
-      </c>
-      <c r="HK1" t="s">
-        <v>535</v>
-      </c>
-      <c r="HL1" t="s">
-        <v>536</v>
-      </c>
-      <c r="HM1" t="s">
-        <v>537</v>
-      </c>
-      <c r="HN1" t="s">
-        <v>538</v>
-      </c>
-      <c r="HO1" t="s">
-        <v>539</v>
-      </c>
-      <c r="HP1" t="s">
-        <v>540</v>
-      </c>
-      <c r="HQ1" t="s">
-        <v>541</v>
-      </c>
-      <c r="HR1" t="s">
-        <v>542</v>
-      </c>
-      <c r="HS1" t="s">
-        <v>543</v>
-      </c>
-      <c r="HT1" t="s">
-        <v>544</v>
-      </c>
-      <c r="HU1" t="s">
-        <v>545</v>
-      </c>
-      <c r="HV1" t="s">
-        <v>546</v>
-      </c>
-      <c r="HW1" t="s">
-        <v>547</v>
-      </c>
-      <c r="HX1" t="s">
-        <v>548</v>
-      </c>
-      <c r="HY1" t="s">
-        <v>549</v>
-      </c>
-      <c r="HZ1" t="s">
-        <v>550</v>
-      </c>
-      <c r="IA1" t="s">
-        <v>551</v>
-      </c>
-      <c r="IB1" t="s">
-        <v>552</v>
-      </c>
-      <c r="IC1" t="s">
-        <v>553</v>
-      </c>
-      <c r="ID1" t="s">
-        <v>554</v>
-      </c>
-      <c r="IE1" t="s">
-        <v>555</v>
-      </c>
-      <c r="IF1" t="s">
-        <v>556</v>
-      </c>
-      <c r="IG1" t="s">
-        <v>557</v>
-      </c>
-      <c r="IH1" t="s">
-        <v>558</v>
-      </c>
-      <c r="II1" t="s">
-        <v>559</v>
-      </c>
-      <c r="IJ1" t="s">
-        <v>560</v>
-      </c>
-      <c r="IK1" t="s">
-        <v>561</v>
-      </c>
-      <c r="IL1" t="s">
-        <v>562</v>
-      </c>
-      <c r="IM1" t="s">
-        <v>563</v>
-      </c>
-      <c r="IN1" t="s">
-        <v>564</v>
-      </c>
-      <c r="IO1" t="s">
-        <v>565</v>
-      </c>
-      <c r="IP1" t="s">
-        <v>566</v>
-      </c>
-      <c r="IQ1" t="s">
-        <v>567</v>
-      </c>
-      <c r="IR1" t="s">
-        <v>568</v>
-      </c>
-      <c r="IS1" t="s">
-        <v>569</v>
-      </c>
-      <c r="IT1" t="s">
-        <v>570</v>
-      </c>
-      <c r="IU1" t="s">
-        <v>571</v>
-      </c>
-      <c r="IV1" t="s">
-        <v>572</v>
-      </c>
-      <c r="IW1" t="s">
-        <v>573</v>
-      </c>
-      <c r="IX1" t="s">
-        <v>574</v>
-      </c>
-      <c r="IY1" t="s">
-        <v>575</v>
-      </c>
-      <c r="IZ1" t="s">
-        <v>576</v>
-      </c>
-      <c r="JA1" t="s">
-        <v>577</v>
-      </c>
-      <c r="JB1" t="s">
-        <v>578</v>
-      </c>
-      <c r="JC1" t="s">
-        <v>579</v>
-      </c>
-      <c r="JD1" t="s">
-        <v>580</v>
-      </c>
-      <c r="JE1" t="s">
-        <v>581</v>
-      </c>
-      <c r="JF1" t="s">
-        <v>582</v>
-      </c>
-      <c r="JG1" t="s">
-        <v>583</v>
-      </c>
-      <c r="JH1" t="s">
-        <v>584</v>
-      </c>
-      <c r="JI1" t="s">
-        <v>585</v>
-      </c>
-      <c r="JJ1" t="s">
-        <v>586</v>
-      </c>
-      <c r="JK1" t="s">
-        <v>587</v>
-      </c>
-      <c r="JL1" t="s">
-        <v>588</v>
-      </c>
-      <c r="JM1" t="s">
-        <v>589</v>
-      </c>
-      <c r="JN1" t="s">
-        <v>590</v>
-      </c>
-      <c r="JO1" t="s">
-        <v>591</v>
-      </c>
-      <c r="JP1" t="s">
-        <v>592</v>
-      </c>
-      <c r="JQ1" t="s">
-        <v>593</v>
-      </c>
-      <c r="JR1" t="s">
-        <v>594</v>
-      </c>
-      <c r="JS1" t="s">
-        <v>595</v>
-      </c>
-      <c r="JT1" t="s">
-        <v>596</v>
-      </c>
-      <c r="JU1" t="s">
-        <v>597</v>
-      </c>
-      <c r="JV1" t="s">
-        <v>598</v>
-      </c>
-      <c r="JW1" t="s">
-        <v>599</v>
-      </c>
-      <c r="JX1" t="s">
+      <c r="KH1" t="s">
+        <v>332</v>
+      </c>
+      <c r="KI1" t="s">
+        <v>333</v>
+      </c>
+      <c r="KJ1" t="s">
+        <v>334</v>
+      </c>
+      <c r="KK1" t="s">
         <v>600</v>
       </c>
-      <c r="JY1" t="s">
+      <c r="KL1" t="s">
         <v>601</v>
       </c>
-      <c r="JZ1" t="s">
-        <v>327</v>
-      </c>
-      <c r="KA1" t="s">
-        <v>328</v>
-      </c>
-      <c r="KB1" t="s">
-        <v>329</v>
-      </c>
-      <c r="KC1" t="s">
-        <v>330</v>
-      </c>
-      <c r="KD1" t="s">
-        <v>331</v>
-      </c>
-      <c r="KE1" t="s">
-        <v>332</v>
-      </c>
-      <c r="KF1" t="s">
-        <v>333</v>
-      </c>
-      <c r="KG1" t="s">
-        <v>340</v>
-      </c>
-      <c r="KH1" t="s">
-        <v>334</v>
-      </c>
-      <c r="KI1" t="s">
+      <c r="KM1" t="s">
+        <v>602</v>
+      </c>
+      <c r="KN1" t="s">
+        <v>603</v>
+      </c>
+      <c r="KO1" t="s">
+        <v>604</v>
+      </c>
+      <c r="KP1" t="s">
+        <v>605</v>
+      </c>
+      <c r="KQ1" t="s">
+        <v>606</v>
+      </c>
+      <c r="KR1" t="s">
+        <v>607</v>
+      </c>
+      <c r="KS1" t="s">
         <v>335</v>
-      </c>
-      <c r="KJ1" t="s">
-        <v>336</v>
-      </c>
-      <c r="KK1" t="s">
-        <v>602</v>
-      </c>
-      <c r="KL1" t="s">
-        <v>603</v>
-      </c>
-      <c r="KM1" t="s">
-        <v>604</v>
-      </c>
-      <c r="KN1" t="s">
-        <v>605</v>
-      </c>
-      <c r="KO1" t="s">
-        <v>606</v>
-      </c>
-      <c r="KP1" t="s">
-        <v>607</v>
-      </c>
-      <c r="KQ1" t="s">
-        <v>608</v>
-      </c>
-      <c r="KR1" t="s">
-        <v>609</v>
-      </c>
-      <c r="KS1" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:305">
@@ -17747,82 +17423,82 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="F2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="G2">
         <v>15.468</v>
       </c>
       <c r="H2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="I2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="J2">
         <v>35.537999999999997</v>
       </c>
       <c r="K2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="L2" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="M2">
         <v>34.387999999999998</v>
       </c>
       <c r="N2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="O2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="P2">
         <v>5.71</v>
       </c>
       <c r="T2" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="U2" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="V2">
         <v>34.954000000000001</v>
       </c>
       <c r="W2" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="X2" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="Y2">
         <v>25.76</v>
       </c>
       <c r="Z2" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="AA2" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="AB2">
         <v>14.507999999999999</v>
       </c>
       <c r="AC2" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="AD2" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="AE2">
         <v>11.9</v>
       </c>
       <c r="AF2" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="AG2" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="AH2">
         <v>21.475999999999999</v>
@@ -17831,7 +17507,7 @@
         <v>1</v>
       </c>
       <c r="AJ2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="AK2">
         <v>1</v>
@@ -17840,19 +17516,19 @@
         <v>22</v>
       </c>
       <c r="AM2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="AO2" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="AP2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="AR2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="AS2" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="AV2">
         <v>24</v>
@@ -17867,7 +17543,7 @@
         <v>0</v>
       </c>
       <c r="AZ2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="BA2">
         <v>24</v>
@@ -17936,10 +17612,10 @@
         <v>119</v>
       </c>
       <c r="CF2" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="CG2" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="CH2">
         <v>3.24399999999999</v>
@@ -17990,10 +17666,10 @@
         <v>119</v>
       </c>
       <c r="DH2" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="DI2" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="DJ2">
         <v>2.7959999999999998</v>
@@ -18041,10 +17717,10 @@
         <v>124</v>
       </c>
       <c r="EJ2" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="EK2" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="EL2">
         <v>1.611</v>
@@ -18092,10 +17768,10 @@
         <v>119</v>
       </c>
       <c r="FL2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="FM2" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="FN2">
         <v>1.5659999999999901</v>
@@ -18143,10 +17819,10 @@
         <v>119</v>
       </c>
       <c r="GN2" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="GO2" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="GP2">
         <v>1.6559999999999999</v>
@@ -18194,10 +17870,10 @@
         <v>119</v>
       </c>
       <c r="HP2" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="HQ2" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="HR2">
         <v>1.0720000000000001</v>
@@ -18245,10 +17921,10 @@
         <v>119</v>
       </c>
       <c r="IR2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="IS2" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="IT2">
         <v>2.4220000000000002</v>
@@ -18296,71 +17972,449 @@
         <v>119</v>
       </c>
       <c r="JT2" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="JU2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="JV2">
         <v>2.6619999999999999</v>
       </c>
       <c r="JZ2" t="s">
+        <v>644</v>
+      </c>
+      <c r="KA2" t="s">
+        <v>645</v>
+      </c>
+      <c r="KB2" t="s">
+        <v>362</v>
+      </c>
+      <c r="KC2" t="s">
+        <v>362</v>
+      </c>
+      <c r="KD2" t="s">
+        <v>362</v>
+      </c>
+      <c r="KE2" t="s">
+        <v>363</v>
+      </c>
+      <c r="KF2" t="s">
+        <v>363</v>
+      </c>
+      <c r="KG2" t="s">
+        <v>363</v>
+      </c>
+      <c r="KH2" t="s">
         <v>646</v>
       </c>
-      <c r="KA2" t="s">
+      <c r="KI2" t="s">
         <v>647</v>
       </c>
-      <c r="KB2" t="s">
+      <c r="KJ2" t="s">
+        <v>648</v>
+      </c>
+      <c r="KK2" t="s">
+        <v>649</v>
+      </c>
+      <c r="KL2" t="s">
+        <v>650</v>
+      </c>
+      <c r="KM2" t="s">
         <v>364</v>
       </c>
-      <c r="KC2" t="s">
+      <c r="KN2" t="s">
+        <v>650</v>
+      </c>
+      <c r="KO2" t="s">
+        <v>649</v>
+      </c>
+      <c r="KP2" t="s">
+        <v>650</v>
+      </c>
+      <c r="KQ2" t="s">
         <v>364</v>
       </c>
-      <c r="KD2" t="s">
-        <v>364</v>
-      </c>
-      <c r="KE2" t="s">
+      <c r="KR2" t="s">
+        <v>651</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAA32EA-3DA8-BD44-8758-9048DFA42915}">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="113" customWidth="1"/>
+    <col min="4" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="7" width="21.5" customWidth="1"/>
+    <col min="8" max="9" width="21.5" style="36" customWidth="1"/>
+    <col min="10" max="11" width="21.5" customWidth="1"/>
+    <col min="12" max="12" width="28.83203125" customWidth="1"/>
+    <col min="13" max="13" width="63.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>671</v>
+      </c>
+      <c r="B1" t="s">
+        <v>653</v>
+      </c>
+      <c r="C1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G1" t="s">
         <v>365</v>
       </c>
-      <c r="KF2" t="s">
-        <v>365</v>
-      </c>
-      <c r="KG2" t="s">
-        <v>365</v>
-      </c>
-      <c r="KH2" t="s">
-        <v>648</v>
-      </c>
-      <c r="KI2" t="s">
-        <v>649</v>
-      </c>
-      <c r="KJ2" t="s">
-        <v>650</v>
-      </c>
-      <c r="KK2" t="s">
-        <v>651</v>
-      </c>
-      <c r="KL2" t="s">
-        <v>652</v>
-      </c>
-      <c r="KM2" t="s">
-        <v>366</v>
-      </c>
-      <c r="KN2" t="s">
-        <v>652</v>
-      </c>
-      <c r="KO2" t="s">
-        <v>651</v>
-      </c>
-      <c r="KP2" t="s">
-        <v>652</v>
-      </c>
-      <c r="KQ2" t="s">
-        <v>366</v>
-      </c>
-      <c r="KR2" t="s">
-        <v>653</v>
-      </c>
+      <c r="H1" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="J1" t="s">
+        <v>255</v>
+      </c>
+      <c r="K1" t="s">
+        <v>259</v>
+      </c>
+      <c r="L1" t="s">
+        <v>269</v>
+      </c>
+      <c r="M1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>658</v>
+      </c>
+      <c r="C2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="H2" s="36">
+        <v>1</v>
+      </c>
+      <c r="I2" s="36">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>660</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>662</v>
+      </c>
+      <c r="C3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="H3" s="36">
+        <v>44922</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>260</v>
+      </c>
+      <c r="L3" s="81" t="s">
+        <v>654</v>
+      </c>
+      <c r="M3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>663</v>
+      </c>
+      <c r="C4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>252</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="H4" s="36">
+        <v>44940</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>260</v>
+      </c>
+      <c r="L4" s="81" t="s">
+        <v>655</v>
+      </c>
+      <c r="M4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="17">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>664</v>
+      </c>
+      <c r="C5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D5">
+        <v>26</v>
+      </c>
+      <c r="E5">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="H5" s="36">
+        <v>44942</v>
+      </c>
+      <c r="J5">
+        <v>26</v>
+      </c>
+      <c r="K5" t="s">
+        <v>260</v>
+      </c>
+      <c r="L5" s="81" t="s">
+        <v>655</v>
+      </c>
+      <c r="M5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>665</v>
+      </c>
+      <c r="C6" t="s">
+        <v>266</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6" t="s">
+        <v>252</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="H6" s="36">
+        <v>44994</v>
+      </c>
+      <c r="I6" s="36">
+        <v>44995</v>
+      </c>
+      <c r="J6">
+        <v>100</v>
+      </c>
+      <c r="K6" t="s">
+        <v>260</v>
+      </c>
+      <c r="L6" s="81" t="s">
+        <v>656</v>
+      </c>
+      <c r="M6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>666</v>
+      </c>
+      <c r="C7" t="s">
+        <v>266</v>
+      </c>
+      <c r="D7">
+        <v>449</v>
+      </c>
+      <c r="E7">
+        <v>449</v>
+      </c>
+      <c r="F7" t="s">
+        <v>252</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="H7" s="36">
+        <v>45119</v>
+      </c>
+      <c r="I7" s="36">
+        <v>45119</v>
+      </c>
+      <c r="J7">
+        <v>150</v>
+      </c>
+      <c r="K7" t="s">
+        <v>260</v>
+      </c>
+      <c r="L7" t="s">
+        <v>657</v>
+      </c>
+      <c r="M7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="17">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>666</v>
+      </c>
+      <c r="C8" t="s">
+        <v>267</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>252</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="J8">
+        <v>150</v>
+      </c>
+      <c r="K8" t="s">
+        <v>260</v>
+      </c>
+      <c r="L8" s="81" t="s">
+        <v>673</v>
+      </c>
+      <c r="M8" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="51">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>667</v>
+      </c>
+      <c r="C9" t="s">
+        <v>267</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>268</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="J9">
+        <v>150</v>
+      </c>
+      <c r="K9" t="s">
+        <v>260</v>
+      </c>
+      <c r="L9" s="81" t="s">
+        <v>672</v>
+      </c>
+      <c r="M9" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18373,7 +18427,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -18388,7 +18442,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B1" s="43" t="s">
         <v>87</v>
@@ -18415,7 +18469,7 @@
         <v>94</v>
       </c>
       <c r="J1" t="s">
-        <v>103</v>
+        <v>670</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -19387,29 +19441,34 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF0298B-43F7-F849-959B-1EFC1ADC8C4E}">
-  <dimension ref="A1:F215"/>
+  <dimension ref="A1:F242"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="B218" sqref="B218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>254</v>
+        <v>653</v>
       </c>
       <c r="B1" t="s">
-        <v>252</v>
+        <v>671</v>
       </c>
       <c r="C1" t="s">
         <v>244</v>
@@ -19421,7 +19480,7 @@
         <v>239</v>
       </c>
       <c r="F1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -23704,9 +23763,550 @@
         <v>188</v>
       </c>
     </row>
+    <row r="216" spans="1:6">
+      <c r="A216">
+        <v>215</v>
+      </c>
+      <c r="B216">
+        <v>7</v>
+      </c>
+      <c r="C216">
+        <v>1</v>
+      </c>
+      <c r="D216">
+        <v>1</v>
+      </c>
+      <c r="E216">
+        <v>1</v>
+      </c>
+      <c r="F216" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6">
+      <c r="A217">
+        <v>216</v>
+      </c>
+      <c r="B217">
+        <v>7</v>
+      </c>
+      <c r="C217">
+        <v>2</v>
+      </c>
+      <c r="D217">
+        <v>1</v>
+      </c>
+      <c r="E217">
+        <v>2</v>
+      </c>
+      <c r="F217" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6">
+      <c r="A218">
+        <v>217</v>
+      </c>
+      <c r="B218">
+        <v>7</v>
+      </c>
+      <c r="C218">
+        <v>3</v>
+      </c>
+      <c r="D218">
+        <v>1</v>
+      </c>
+      <c r="E218">
+        <v>3</v>
+      </c>
+      <c r="F218" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6">
+      <c r="A219">
+        <v>218</v>
+      </c>
+      <c r="B219">
+        <v>7</v>
+      </c>
+      <c r="C219">
+        <v>4</v>
+      </c>
+      <c r="D219">
+        <v>1</v>
+      </c>
+      <c r="E219">
+        <v>4</v>
+      </c>
+      <c r="F219" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6">
+      <c r="A220">
+        <v>219</v>
+      </c>
+      <c r="B220">
+        <v>7</v>
+      </c>
+      <c r="C220">
+        <v>5</v>
+      </c>
+      <c r="D220">
+        <v>1</v>
+      </c>
+      <c r="E220">
+        <v>5</v>
+      </c>
+      <c r="F220" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6">
+      <c r="A221">
+        <v>220</v>
+      </c>
+      <c r="B221">
+        <v>7</v>
+      </c>
+      <c r="C221">
+        <v>6</v>
+      </c>
+      <c r="D221">
+        <v>1</v>
+      </c>
+      <c r="E221">
+        <v>6</v>
+      </c>
+      <c r="F221" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6">
+      <c r="A222">
+        <v>221</v>
+      </c>
+      <c r="B222">
+        <v>7</v>
+      </c>
+      <c r="C222">
+        <v>7</v>
+      </c>
+      <c r="D222">
+        <v>1</v>
+      </c>
+      <c r="E222">
+        <v>7</v>
+      </c>
+      <c r="F222" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6">
+      <c r="A223">
+        <v>222</v>
+      </c>
+      <c r="B223">
+        <v>7</v>
+      </c>
+      <c r="C223">
+        <v>8</v>
+      </c>
+      <c r="D223">
+        <v>1</v>
+      </c>
+      <c r="E223">
+        <v>8</v>
+      </c>
+      <c r="F223" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6">
+      <c r="A224">
+        <v>223</v>
+      </c>
+      <c r="B224">
+        <v>7</v>
+      </c>
+      <c r="C224">
+        <v>1</v>
+      </c>
+      <c r="D224">
+        <v>1</v>
+      </c>
+      <c r="E224">
+        <v>9</v>
+      </c>
+      <c r="F224" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6">
+      <c r="A225">
+        <v>224</v>
+      </c>
+      <c r="B225">
+        <v>7</v>
+      </c>
+      <c r="C225">
+        <v>1</v>
+      </c>
+      <c r="D225">
+        <v>2</v>
+      </c>
+      <c r="E225">
+        <v>1</v>
+      </c>
+      <c r="F225" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6">
+      <c r="A226">
+        <v>225</v>
+      </c>
+      <c r="B226">
+        <v>7</v>
+      </c>
+      <c r="C226">
+        <v>2</v>
+      </c>
+      <c r="D226">
+        <v>2</v>
+      </c>
+      <c r="E226">
+        <v>2</v>
+      </c>
+      <c r="F226" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6">
+      <c r="A227">
+        <v>226</v>
+      </c>
+      <c r="B227">
+        <v>7</v>
+      </c>
+      <c r="C227">
+        <v>3</v>
+      </c>
+      <c r="D227">
+        <v>2</v>
+      </c>
+      <c r="E227">
+        <v>3</v>
+      </c>
+      <c r="F227" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6">
+      <c r="A228">
+        <v>227</v>
+      </c>
+      <c r="B228">
+        <v>7</v>
+      </c>
+      <c r="C228">
+        <v>4</v>
+      </c>
+      <c r="D228">
+        <v>2</v>
+      </c>
+      <c r="E228">
+        <v>4</v>
+      </c>
+      <c r="F228" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6">
+      <c r="A229">
+        <v>228</v>
+      </c>
+      <c r="B229">
+        <v>7</v>
+      </c>
+      <c r="C229">
+        <v>5</v>
+      </c>
+      <c r="D229">
+        <v>2</v>
+      </c>
+      <c r="E229">
+        <v>5</v>
+      </c>
+      <c r="F229" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6">
+      <c r="A230">
+        <v>229</v>
+      </c>
+      <c r="B230">
+        <v>7</v>
+      </c>
+      <c r="C230">
+        <v>6</v>
+      </c>
+      <c r="D230">
+        <v>2</v>
+      </c>
+      <c r="E230">
+        <v>6</v>
+      </c>
+      <c r="F230" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6">
+      <c r="A231">
+        <v>230</v>
+      </c>
+      <c r="B231">
+        <v>7</v>
+      </c>
+      <c r="C231">
+        <v>7</v>
+      </c>
+      <c r="D231">
+        <v>2</v>
+      </c>
+      <c r="E231">
+        <v>7</v>
+      </c>
+      <c r="F231" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6">
+      <c r="A232">
+        <v>231</v>
+      </c>
+      <c r="B232">
+        <v>7</v>
+      </c>
+      <c r="C232">
+        <v>8</v>
+      </c>
+      <c r="D232">
+        <v>2</v>
+      </c>
+      <c r="E232">
+        <v>8</v>
+      </c>
+      <c r="F232" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6">
+      <c r="A233">
+        <v>232</v>
+      </c>
+      <c r="B233">
+        <v>7</v>
+      </c>
+      <c r="C233">
+        <v>1</v>
+      </c>
+      <c r="D233">
+        <v>2</v>
+      </c>
+      <c r="E233">
+        <v>9</v>
+      </c>
+      <c r="F233" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6">
+      <c r="A234">
+        <v>233</v>
+      </c>
+      <c r="B234">
+        <v>7</v>
+      </c>
+      <c r="C234">
+        <v>1</v>
+      </c>
+      <c r="D234">
+        <v>3</v>
+      </c>
+      <c r="E234">
+        <v>1</v>
+      </c>
+      <c r="F234" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6">
+      <c r="A235">
+        <v>234</v>
+      </c>
+      <c r="B235">
+        <v>7</v>
+      </c>
+      <c r="C235">
+        <v>2</v>
+      </c>
+      <c r="D235">
+        <v>3</v>
+      </c>
+      <c r="E235">
+        <v>2</v>
+      </c>
+      <c r="F235" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6">
+      <c r="A236">
+        <v>235</v>
+      </c>
+      <c r="B236">
+        <v>7</v>
+      </c>
+      <c r="C236">
+        <v>3</v>
+      </c>
+      <c r="D236">
+        <v>3</v>
+      </c>
+      <c r="E236">
+        <v>3</v>
+      </c>
+      <c r="F236" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6">
+      <c r="A237">
+        <v>236</v>
+      </c>
+      <c r="B237">
+        <v>7</v>
+      </c>
+      <c r="C237">
+        <v>4</v>
+      </c>
+      <c r="D237">
+        <v>3</v>
+      </c>
+      <c r="E237">
+        <v>4</v>
+      </c>
+      <c r="F237" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6">
+      <c r="A238">
+        <v>237</v>
+      </c>
+      <c r="B238">
+        <v>7</v>
+      </c>
+      <c r="C238">
+        <v>5</v>
+      </c>
+      <c r="D238">
+        <v>3</v>
+      </c>
+      <c r="E238">
+        <v>5</v>
+      </c>
+      <c r="F238" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6">
+      <c r="A239">
+        <v>238</v>
+      </c>
+      <c r="B239">
+        <v>7</v>
+      </c>
+      <c r="C239">
+        <v>6</v>
+      </c>
+      <c r="D239">
+        <v>3</v>
+      </c>
+      <c r="E239">
+        <v>6</v>
+      </c>
+      <c r="F239" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6">
+      <c r="A240">
+        <v>239</v>
+      </c>
+      <c r="B240">
+        <v>7</v>
+      </c>
+      <c r="C240">
+        <v>7</v>
+      </c>
+      <c r="D240">
+        <v>3</v>
+      </c>
+      <c r="E240">
+        <v>7</v>
+      </c>
+      <c r="F240" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6">
+      <c r="A241">
+        <v>240</v>
+      </c>
+      <c r="B241">
+        <v>7</v>
+      </c>
+      <c r="C241">
+        <v>8</v>
+      </c>
+      <c r="D241">
+        <v>3</v>
+      </c>
+      <c r="E241">
+        <v>8</v>
+      </c>
+      <c r="F241" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6">
+      <c r="A242">
+        <v>241</v>
+      </c>
+      <c r="B242">
+        <v>7</v>
+      </c>
+      <c r="C242">
+        <v>1</v>
+      </c>
+      <c r="D242">
+        <v>3</v>
+      </c>
+      <c r="E242">
+        <v>9</v>
+      </c>
+      <c r="F242" t="s">
+        <v>188</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E207" xr:uid="{8EF0298B-43F7-F849-959B-1EFC1ADC8C4E}"/>
+  <autoFilter ref="A1:E234" xr:uid="{8EF0298B-43F7-F849-959B-1EFC1ADC8C4E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -23715,11 +24315,12 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="2" max="2" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="14.5" customWidth="1"/>
     <col min="5" max="5" width="19.5" customWidth="1"/>
@@ -23737,7 +24338,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>254</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
         <v>86</v>
@@ -23782,7 +24383,7 @@
         <v>199</v>
       </c>
       <c r="P1" t="s">
-        <v>103</v>
+        <v>669</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -23961,6 +24562,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Application is now retrieving data from google function!
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CDB16E-B9DA-5843-8A2A-17FED928EA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756E484D-07F4-0946-9129-67A8A648A42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="3" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <sheet name="Web Parameters v1" sheetId="1" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">fire_treat_ques_prod!$A$1:$E$234</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">fire_treat_ques_prod!$A$1:$E$242</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'MCL questions prod exp 1'!$A$1:$X$28</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Web Parameters Dev'!$B$1:$Y$88</definedName>
   </definedNames>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2757" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2757" uniqueCount="676">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -2105,13 +2105,16 @@
     <t>experiment_id</t>
   </si>
   <si>
-    <t>next</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>Between subject test experiment.</t>
+  </si>
+  <si>
+    <t>testbetween</t>
+  </si>
+  <si>
+    <t>testwithin</t>
+  </si>
+  <si>
+    <t>active</t>
   </si>
 </sst>
 </file>
@@ -10226,7 +10229,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.31057826210619821</v>
+        <v>0.22625759311606564</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -10246,7 +10249,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.63314311976286941</v>
+        <v>0.47349689138424134</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -10267,7 +10270,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.63710912997502733</v>
+        <v>0.53241170936980375</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -10287,7 +10290,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.53792716883490477</v>
+        <v>0.22196105846930037</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -18048,8 +18051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAA32EA-3DA8-BD44-8758-9048DFA42915}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18350,7 +18353,7 @@
         <v>666</v>
       </c>
       <c r="C8" t="s">
-        <v>267</v>
+        <v>675</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -18374,7 +18377,7 @@
         <v>673</v>
       </c>
       <c r="M8" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="51">
@@ -18385,7 +18388,7 @@
         <v>667</v>
       </c>
       <c r="C9" t="s">
-        <v>267</v>
+        <v>675</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -18406,7 +18409,7 @@
         <v>260</v>
       </c>
       <c r="L9" s="81" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="M9" t="s">
         <v>270</v>
@@ -18427,7 +18430,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -18490,8 +18493,12 @@
         <v>13</v>
       </c>
       <c r="G2" s="79"/>
-      <c r="H2"/>
-      <c r="I2"/>
+      <c r="H2">
+        <v>430</v>
+      </c>
+      <c r="I2">
+        <v>14</v>
+      </c>
       <c r="J2" t="s">
         <v>240</v>
       </c>
@@ -18514,8 +18521,12 @@
         <v>18</v>
       </c>
       <c r="G3" s="79"/>
-      <c r="H3"/>
-      <c r="I3"/>
+      <c r="H3">
+        <v>700</v>
+      </c>
+      <c r="I3">
+        <v>19</v>
+      </c>
       <c r="J3" t="s">
         <v>240</v>
       </c>
@@ -18539,8 +18550,12 @@
         <v>24</v>
       </c>
       <c r="G4" s="79"/>
-      <c r="H4"/>
-      <c r="I4"/>
+      <c r="H4">
+        <v>1390</v>
+      </c>
+      <c r="I4">
+        <v>25</v>
+      </c>
       <c r="J4" t="s">
         <v>240</v>
       </c>
@@ -18563,8 +18578,12 @@
         <v>16</v>
       </c>
       <c r="G5" s="79"/>
-      <c r="H5"/>
-      <c r="I5"/>
+      <c r="H5">
+        <v>1120</v>
+      </c>
+      <c r="I5">
+        <v>17</v>
+      </c>
       <c r="J5" t="s">
         <v>240</v>
       </c>
@@ -18587,8 +18606,12 @@
         <v>13</v>
       </c>
       <c r="G6" s="79"/>
-      <c r="H6"/>
-      <c r="I6"/>
+      <c r="H6">
+        <v>40</v>
+      </c>
+      <c r="I6">
+        <v>14</v>
+      </c>
       <c r="J6" t="s">
         <v>241</v>
       </c>
@@ -18611,8 +18634,12 @@
         <v>18</v>
       </c>
       <c r="G7" s="79"/>
-      <c r="H7"/>
-      <c r="I7"/>
+      <c r="H7">
+        <v>70</v>
+      </c>
+      <c r="I7">
+        <v>19</v>
+      </c>
       <c r="J7" t="s">
         <v>241</v>
       </c>
@@ -18635,8 +18662,12 @@
         <v>24</v>
       </c>
       <c r="G8" s="79"/>
-      <c r="H8"/>
-      <c r="I8"/>
+      <c r="H8">
+        <v>110</v>
+      </c>
+      <c r="I8">
+        <v>25</v>
+      </c>
       <c r="J8" t="s">
         <v>241</v>
       </c>
@@ -18659,8 +18690,12 @@
         <v>16</v>
       </c>
       <c r="G9" s="79"/>
-      <c r="H9"/>
-      <c r="I9"/>
+      <c r="H9">
+        <v>120</v>
+      </c>
+      <c r="I9">
+        <v>17</v>
+      </c>
       <c r="J9" t="s">
         <v>241</v>
       </c>
@@ -18683,8 +18718,12 @@
         <v>7</v>
       </c>
       <c r="G10" s="79"/>
-      <c r="H10"/>
-      <c r="I10"/>
+      <c r="H10">
+        <v>1000</v>
+      </c>
+      <c r="I10">
+        <v>8</v>
+      </c>
       <c r="J10" t="s">
         <v>243</v>
       </c>
@@ -19235,7 +19274,9 @@
       <c r="G30" s="80">
         <v>44944</v>
       </c>
-      <c r="H30" s="1"/>
+      <c r="H30">
+        <v>700</v>
+      </c>
       <c r="I30" s="1"/>
       <c r="J30" t="s">
         <v>240</v>
@@ -19257,7 +19298,9 @@
       <c r="G31" s="80">
         <v>44950</v>
       </c>
-      <c r="H31" s="1"/>
+      <c r="H31">
+        <v>1390</v>
+      </c>
       <c r="I31" s="1"/>
       <c r="J31" t="s">
         <v>240</v>
@@ -19279,7 +19322,9 @@
       <c r="G32" s="80">
         <v>44942</v>
       </c>
-      <c r="H32" s="1"/>
+      <c r="H32">
+        <v>1120</v>
+      </c>
       <c r="I32" s="1"/>
       <c r="J32" t="s">
         <v>240</v>
@@ -19301,7 +19346,9 @@
       <c r="G33" s="80">
         <v>44939</v>
       </c>
-      <c r="H33" s="1"/>
+      <c r="H33">
+        <v>40</v>
+      </c>
       <c r="I33" s="1"/>
       <c r="J33" t="s">
         <v>241</v>
@@ -19323,7 +19370,9 @@
       <c r="G34" s="80">
         <v>44944</v>
       </c>
-      <c r="H34" s="1"/>
+      <c r="H34">
+        <v>70</v>
+      </c>
       <c r="I34" s="1"/>
       <c r="J34" t="s">
         <v>241</v>
@@ -19345,7 +19394,9 @@
       <c r="G35" s="80">
         <v>44950</v>
       </c>
-      <c r="H35" s="1"/>
+      <c r="H35">
+        <v>110</v>
+      </c>
       <c r="I35" s="1"/>
       <c r="J35" t="s">
         <v>241</v>
@@ -19367,7 +19418,9 @@
       <c r="G36" s="80">
         <v>44942</v>
       </c>
-      <c r="H36" s="1"/>
+      <c r="H36">
+        <v>120</v>
+      </c>
       <c r="I36" s="1"/>
       <c r="J36" t="s">
         <v>241</v>
@@ -19389,7 +19442,9 @@
       <c r="G37" s="80">
         <v>44933</v>
       </c>
-      <c r="H37" s="1"/>
+      <c r="H37">
+        <v>1000</v>
+      </c>
       <c r="I37" s="1"/>
       <c r="J37" t="s">
         <v>243</v>
@@ -19411,7 +19466,9 @@
       <c r="G38" s="80">
         <v>45201</v>
       </c>
-      <c r="H38" s="1"/>
+      <c r="H38">
+        <v>1000</v>
+      </c>
       <c r="I38" s="1"/>
       <c r="J38" t="s">
         <v>243</v>
@@ -19433,7 +19490,9 @@
       <c r="G39" s="80">
         <v>44933</v>
       </c>
-      <c r="H39" s="1"/>
+      <c r="H39">
+        <v>1000</v>
+      </c>
       <c r="I39" s="1"/>
       <c r="J39" t="s">
         <v>243</v>
@@ -19449,8 +19508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF0298B-43F7-F849-959B-1EFC1ADC8C4E}">
   <dimension ref="A1:F242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="B218" sqref="B218"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -24304,7 +24363,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E234" xr:uid="{8EF0298B-43F7-F849-959B-1EFC1ADC8C4E}"/>
+  <autoFilter ref="A1:E242" xr:uid="{8EF0298B-43F7-F849-959B-1EFC1ADC8C4E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -24572,7 +24631,7 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Added sequence in state updates.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756E484D-07F4-0946-9129-67A8A648A42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B41F878-C693-A549-9589-52C4E30DB8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="3" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="4" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <sheet name="Web Parameters v1" sheetId="1" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">fire_treat_ques_prod!$A$1:$E$242</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">fire_treat_ques_prod!$A$1:$F$242</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'MCL questions prod exp 1'!$A$1:$X$28</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Web Parameters Dev'!$B$1:$Y$88</definedName>
   </definedNames>
@@ -2490,9 +2490,6 @@
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2511,23 +2508,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2557,6 +2539,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2570,6 +2561,15 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10229,7 +10229,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.22625759311606564</v>
+        <v>0.81425101386490806</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -10249,7 +10249,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.47349689138424134</v>
+        <v>0.82034145767661026</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -10270,7 +10270,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.53241170936980375</v>
+        <v>1.3616296915581416E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -10290,7 +10290,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.22196105846930037</v>
+        <v>0.67421594975002086</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -10551,48 +10551,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="82" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="83" t="s">
+      <c r="D3" s="83"/>
+      <c r="E3" s="82" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="84"/>
-      <c r="G3" s="83" t="s">
+      <c r="F3" s="83"/>
+      <c r="G3" s="82" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="84"/>
-      <c r="I3" s="83" t="s">
+      <c r="H3" s="83"/>
+      <c r="I3" s="82" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="84"/>
+      <c r="J3" s="83"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="85" t="s">
+      <c r="M3" s="84" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="86"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="85" t="s">
+      <c r="N3" s="85"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="84" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="86"/>
-      <c r="R3" s="87"/>
-      <c r="S3" s="85" t="s">
+      <c r="Q3" s="85"/>
+      <c r="R3" s="86"/>
+      <c r="S3" s="84" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="86"/>
-      <c r="U3" s="86"/>
-      <c r="V3" s="88" t="s">
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
+      <c r="V3" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="88"/>
-      <c r="X3" s="88"/>
+      <c r="W3" s="87"/>
+      <c r="X3" s="87"/>
       <c r="Y3" t="s">
         <v>215</v>
       </c>
@@ -11671,16 +11671,16 @@
       </c>
     </row>
     <row r="29" spans="1:33">
-      <c r="C29" s="82" t="s">
+      <c r="C29" s="88" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="82"/>
-      <c r="E29" s="82"/>
-      <c r="F29" s="82" t="s">
+      <c r="D29" s="88"/>
+      <c r="E29" s="88"/>
+      <c r="F29" s="88" t="s">
         <v>169</v>
       </c>
-      <c r="G29" s="82"/>
-      <c r="H29" s="82"/>
+      <c r="G29" s="88"/>
+      <c r="H29" s="88"/>
       <c r="J29" t="s">
         <v>168</v>
       </c>
@@ -12585,16 +12585,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="P3:R3"/>
     <mergeCell ref="S3:U3"/>
     <mergeCell ref="V3:X3"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B26" r:id="rId1" xr:uid="{D2B54FA7-7284-A444-93E2-10BEB7DF1432}"/>
@@ -12634,105 +12634,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="101" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="95" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="95" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="96"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="92" t="s">
+      <c r="A2" s="95" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="89" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="90"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="89" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="90"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="107" t="s">
+      <c r="I2" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="107"/>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="107" t="s">
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="107"/>
-      <c r="T2" s="107"/>
-      <c r="U2" s="107"/>
-      <c r="V2" s="92" t="s">
+      <c r="S2" s="104"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="92" t="s">
+      <c r="W2" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="89" t="s">
+      <c r="X2" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="89" t="s">
+      <c r="Y2" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="89" t="s">
+      <c r="Z2" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="89" t="s">
+      <c r="AA2" s="106" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="102"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="108" t="s">
+      <c r="A3" s="96"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="106"/>
-      <c r="K3" s="106"/>
-      <c r="L3" s="106" t="s">
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="106"/>
-      <c r="N3" s="106" t="s">
+      <c r="M3" s="103"/>
+      <c r="N3" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="106"/>
-      <c r="P3" s="106" t="s">
+      <c r="O3" s="103"/>
+      <c r="P3" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="106"/>
-      <c r="R3" s="104" t="s">
+      <c r="Q3" s="103"/>
+      <c r="R3" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="104" t="s">
+      <c r="S3" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="104" t="s">
+      <c r="T3" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="104" t="s">
+      <c r="U3" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="93"/>
-      <c r="W3" s="93"/>
-      <c r="X3" s="90"/>
-      <c r="Y3" s="90"/>
-      <c r="Z3" s="90"/>
-      <c r="AA3" s="90"/>
+      <c r="V3" s="99"/>
+      <c r="W3" s="99"/>
+      <c r="X3" s="107"/>
+      <c r="Y3" s="107"/>
+      <c r="Z3" s="107"/>
+      <c r="AA3" s="107"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="103"/>
+      <c r="A4" s="97"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -12751,7 +12751,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="94"/>
+      <c r="H4" s="100"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -12779,16 +12779,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="105"/>
-      <c r="S4" s="105"/>
-      <c r="T4" s="105"/>
-      <c r="U4" s="105"/>
-      <c r="V4" s="94"/>
-      <c r="W4" s="94"/>
-      <c r="X4" s="91"/>
-      <c r="Y4" s="91"/>
-      <c r="Z4" s="91"/>
-      <c r="AA4" s="90"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="102"/>
+      <c r="V4" s="100"/>
+      <c r="W4" s="100"/>
+      <c r="X4" s="108"/>
+      <c r="Y4" s="108"/>
+      <c r="Z4" s="108"/>
+      <c r="AA4" s="107"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -13289,6 +13289,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -13304,11 +13309,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -18051,7 +18051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAA32EA-3DA8-BD44-8758-9048DFA42915}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -18429,8 +18429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE6320D-B1FD-E344-B304-B9DCE6A3C0D3}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -18441,6 +18441,7 @@
     <col min="5" max="5" width="19.1640625" customWidth="1"/>
     <col min="7" max="7" width="11" style="80"/>
     <col min="8" max="9" width="13.6640625" style="36" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -19509,7 +19510,7 @@
   <dimension ref="A1:F242"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -23656,7 +23657,7 @@
         <v>3</v>
       </c>
       <c r="E207">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F207" t="s">
         <v>187</v>
@@ -23676,7 +23677,7 @@
         <v>3</v>
       </c>
       <c r="E208">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F208" t="s">
         <v>187</v>
@@ -23696,7 +23697,7 @@
         <v>3</v>
       </c>
       <c r="E209">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F209" t="s">
         <v>187</v>
@@ -23716,7 +23717,7 @@
         <v>3</v>
       </c>
       <c r="E210">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F210" t="s">
         <v>187</v>
@@ -23736,7 +23737,7 @@
         <v>3</v>
       </c>
       <c r="E211">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="F211" t="s">
         <v>187</v>
@@ -23756,7 +23757,7 @@
         <v>3</v>
       </c>
       <c r="E212">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="F212" t="s">
         <v>187</v>
@@ -23776,7 +23777,7 @@
         <v>3</v>
       </c>
       <c r="E213">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F213" t="s">
         <v>187</v>
@@ -23796,7 +23797,7 @@
         <v>3</v>
       </c>
       <c r="E214">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F214" t="s">
         <v>187</v>
@@ -23816,7 +23817,7 @@
         <v>3</v>
       </c>
       <c r="E215">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F215" t="s">
         <v>188</v>
@@ -24363,7 +24364,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E242" xr:uid="{8EF0298B-43F7-F849-959B-1EFC1ADC8C4E}"/>
+  <autoFilter ref="A1:F242" xr:uid="{8EF0298B-43F7-F849-959B-1EFC1ADC8C4E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -24374,7 +24375,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P1"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Moved experiment parameters out of property file.
Moved experiment parameters out of property file and into experiment definition in firestore.
Fixed bug with CSV file not exporting all values.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B41F878-C693-A549-9589-52C4E30DB8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD82E339-1443-254C-94DE-C368F6B56FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="4" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21060" activeTab="3" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2757" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2893" uniqueCount="707">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -2115,19 +2115,113 @@
   </si>
   <si>
     <t>active</t>
+  </si>
+  <si>
+    <t>full_screen</t>
+  </si>
+  <si>
+    <t>enabled</t>
+  </si>
+  <si>
+    <t>payment_amount</t>
+  </si>
+  <si>
+    <t>time_to_complete_min</t>
+  </si>
+  <si>
+    <t>5 to 10</t>
+  </si>
+  <si>
+    <t>research_title</t>
+  </si>
+  <si>
+    <t>Choices About Money</t>
+  </si>
+  <si>
+    <t>researcher_names</t>
+  </si>
+  <si>
+    <t>Peter Cordone, Yahel Nachum, Ravit Heskiau, Lane Harrison, Daniel Reichman</t>
+  </si>
+  <si>
+    <t>contact_name</t>
+  </si>
+  <si>
+    <t>Peter Cordone</t>
+  </si>
+  <si>
+    <t>contact_email</t>
+  </si>
+  <si>
+    <t>pncordone@wpi.edu</t>
+  </si>
+  <si>
+    <t>contact_phone</t>
+  </si>
+  <si>
+    <t>(617)678-5190</t>
+  </si>
+  <si>
+    <t>sponsor_name</t>
+  </si>
+  <si>
+    <t>Prof. Daniel Reichman</t>
+  </si>
+  <si>
+    <t>sponsor_email</t>
+  </si>
+  <si>
+    <t>dreichman@wpi.edu</t>
+  </si>
+  <si>
+    <t>IRB_name</t>
+  </si>
+  <si>
+    <t>IRB Manager Ruth McKeogh</t>
+  </si>
+  <si>
+    <t>IRB_email</t>
+  </si>
+  <si>
+    <t>irb@wpi.edu</t>
+  </si>
+  <si>
+    <t>IRB_phone</t>
+  </si>
+  <si>
+    <t>(508)831-6699</t>
+  </si>
+  <si>
+    <t>Human Protection Administrator Gabriel Johnson</t>
+  </si>
+  <si>
+    <t>HPA_name</t>
+  </si>
+  <si>
+    <t>HPA_email</t>
+  </si>
+  <si>
+    <t>gjohnson@wpi.edu</t>
+  </si>
+  <si>
+    <t>HPA_phone</t>
+  </si>
+  <si>
+    <t>(508)831-4989</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2196,6 +2290,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2383,7 +2483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2490,6 +2590,8 @@
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -10229,7 +10331,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.81425101386490806</v>
+        <v>6.2865291111590782E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -10249,7 +10351,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.82034145767661026</v>
+        <v>0.97933949551891075</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -10270,7 +10372,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>1.3616296915581416E-2</v>
+        <v>0.52846736147141371</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -10290,7 +10392,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.67421594975002086</v>
+        <v>0.20646759939969328</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -10551,48 +10653,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="84" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="82" t="s">
+      <c r="D3" s="85"/>
+      <c r="E3" s="84" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="83"/>
-      <c r="G3" s="82" t="s">
+      <c r="F3" s="85"/>
+      <c r="G3" s="84" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="83"/>
-      <c r="I3" s="82" t="s">
+      <c r="H3" s="85"/>
+      <c r="I3" s="84" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="83"/>
+      <c r="J3" s="85"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="84" t="s">
+      <c r="M3" s="86" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="85"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="84" t="s">
+      <c r="N3" s="87"/>
+      <c r="O3" s="88"/>
+      <c r="P3" s="86" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="86"/>
-      <c r="S3" s="84" t="s">
+      <c r="Q3" s="87"/>
+      <c r="R3" s="88"/>
+      <c r="S3" s="86" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="85"/>
-      <c r="U3" s="85"/>
-      <c r="V3" s="87" t="s">
+      <c r="T3" s="87"/>
+      <c r="U3" s="87"/>
+      <c r="V3" s="89" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="87"/>
-      <c r="X3" s="87"/>
+      <c r="W3" s="89"/>
+      <c r="X3" s="89"/>
       <c r="Y3" t="s">
         <v>215</v>
       </c>
@@ -11671,16 +11773,16 @@
       </c>
     </row>
     <row r="29" spans="1:33">
-      <c r="C29" s="88" t="s">
+      <c r="C29" s="90" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="88"/>
-      <c r="E29" s="88"/>
-      <c r="F29" s="88" t="s">
+      <c r="D29" s="90"/>
+      <c r="E29" s="90"/>
+      <c r="F29" s="90" t="s">
         <v>169</v>
       </c>
-      <c r="G29" s="88"/>
-      <c r="H29" s="88"/>
+      <c r="G29" s="90"/>
+      <c r="H29" s="90"/>
       <c r="J29" t="s">
         <v>168</v>
       </c>
@@ -12634,105 +12736,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="95" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="89" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="89" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="90"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="98" t="s">
+      <c r="A2" s="97" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="92"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="91" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="92"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="104"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="104"/>
-      <c r="M2" s="104"/>
-      <c r="N2" s="104"/>
-      <c r="O2" s="104"/>
-      <c r="P2" s="104"/>
-      <c r="Q2" s="104"/>
-      <c r="R2" s="104" t="s">
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="106"/>
+      <c r="R2" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="104"/>
-      <c r="T2" s="104"/>
-      <c r="U2" s="104"/>
-      <c r="V2" s="98" t="s">
+      <c r="S2" s="106"/>
+      <c r="T2" s="106"/>
+      <c r="U2" s="106"/>
+      <c r="V2" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="98" t="s">
+      <c r="W2" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="106" t="s">
+      <c r="X2" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="106" t="s">
+      <c r="Y2" s="108" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="106" t="s">
+      <c r="Z2" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="106" t="s">
+      <c r="AA2" s="108" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="96"/>
-      <c r="B3" s="92"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="105" t="s">
+      <c r="A3" s="98"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="103"/>
-      <c r="K3" s="103"/>
-      <c r="L3" s="103" t="s">
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="103"/>
-      <c r="N3" s="103" t="s">
+      <c r="M3" s="105"/>
+      <c r="N3" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="103"/>
-      <c r="P3" s="103" t="s">
+      <c r="O3" s="105"/>
+      <c r="P3" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="103"/>
-      <c r="R3" s="101" t="s">
+      <c r="Q3" s="105"/>
+      <c r="R3" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="101" t="s">
+      <c r="S3" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="101" t="s">
+      <c r="T3" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="101" t="s">
+      <c r="U3" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="99"/>
-      <c r="W3" s="99"/>
-      <c r="X3" s="107"/>
-      <c r="Y3" s="107"/>
-      <c r="Z3" s="107"/>
-      <c r="AA3" s="107"/>
+      <c r="V3" s="101"/>
+      <c r="W3" s="101"/>
+      <c r="X3" s="109"/>
+      <c r="Y3" s="109"/>
+      <c r="Z3" s="109"/>
+      <c r="AA3" s="109"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="97"/>
+      <c r="A4" s="99"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -12751,7 +12853,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="100"/>
+      <c r="H4" s="102"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -12779,16 +12881,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="102"/>
-      <c r="S4" s="102"/>
-      <c r="T4" s="102"/>
-      <c r="U4" s="102"/>
-      <c r="V4" s="100"/>
-      <c r="W4" s="100"/>
-      <c r="X4" s="108"/>
-      <c r="Y4" s="108"/>
-      <c r="Z4" s="108"/>
-      <c r="AA4" s="107"/>
+      <c r="R4" s="104"/>
+      <c r="S4" s="104"/>
+      <c r="T4" s="104"/>
+      <c r="U4" s="104"/>
+      <c r="V4" s="102"/>
+      <c r="W4" s="102"/>
+      <c r="X4" s="110"/>
+      <c r="Y4" s="110"/>
+      <c r="Z4" s="110"/>
+      <c r="AA4" s="109"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -18049,10 +18151,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAA32EA-3DA8-BD44-8758-9048DFA42915}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="128" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18062,12 +18164,12 @@
     <col min="4" max="5" width="22.6640625" customWidth="1"/>
     <col min="6" max="7" width="21.5" customWidth="1"/>
     <col min="8" max="9" width="21.5" style="36" customWidth="1"/>
-    <col min="10" max="11" width="21.5" customWidth="1"/>
-    <col min="12" max="12" width="28.83203125" customWidth="1"/>
-    <col min="13" max="13" width="63.5" customWidth="1"/>
+    <col min="10" max="27" width="21.5" customWidth="1"/>
+    <col min="28" max="28" width="28.83203125" customWidth="1"/>
+    <col min="29" max="29" width="63.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>671</v>
       </c>
@@ -18102,13 +18204,61 @@
         <v>259</v>
       </c>
       <c r="L1" t="s">
+        <v>676</v>
+      </c>
+      <c r="M1" t="s">
+        <v>678</v>
+      </c>
+      <c r="N1" t="s">
+        <v>679</v>
+      </c>
+      <c r="O1" t="s">
+        <v>681</v>
+      </c>
+      <c r="P1" t="s">
+        <v>683</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>685</v>
+      </c>
+      <c r="R1" t="s">
+        <v>687</v>
+      </c>
+      <c r="S1" t="s">
+        <v>689</v>
+      </c>
+      <c r="T1" t="s">
+        <v>691</v>
+      </c>
+      <c r="U1" t="s">
+        <v>693</v>
+      </c>
+      <c r="V1" t="s">
+        <v>695</v>
+      </c>
+      <c r="W1" t="s">
+        <v>697</v>
+      </c>
+      <c r="X1" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>702</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>703</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>705</v>
+      </c>
+      <c r="AB1" t="s">
         <v>269</v>
       </c>
-      <c r="M1" t="s">
+      <c r="AC1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17">
+    <row r="2" spans="1:29" ht="17">
       <c r="A2">
         <v>0</v>
       </c>
@@ -18142,14 +18292,62 @@
       <c r="K2" t="s">
         <v>660</v>
       </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="L2" t="s">
+        <v>677</v>
+      </c>
+      <c r="M2" s="82">
+        <v>1.5</v>
+      </c>
+      <c r="N2" s="82" t="s">
+        <v>680</v>
+      </c>
+      <c r="O2" s="82" t="s">
+        <v>682</v>
+      </c>
+      <c r="P2" s="82" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q2" s="82" t="s">
+        <v>686</v>
+      </c>
+      <c r="R2" t="s">
+        <v>688</v>
+      </c>
+      <c r="S2" s="83" t="s">
+        <v>690</v>
+      </c>
+      <c r="T2" s="83" t="s">
+        <v>692</v>
+      </c>
+      <c r="U2" s="83" t="s">
+        <v>694</v>
+      </c>
+      <c r="V2" s="83" t="s">
+        <v>696</v>
+      </c>
+      <c r="W2" s="83" t="s">
+        <v>698</v>
+      </c>
+      <c r="X2" s="83" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y2" s="83" t="s">
+        <v>701</v>
+      </c>
+      <c r="Z2" s="83" t="s">
+        <v>704</v>
+      </c>
+      <c r="AA2" s="83" t="s">
+        <v>706</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="17">
+    <row r="3" spans="1:29" ht="17">
       <c r="A3">
         <v>1</v>
       </c>
@@ -18180,14 +18378,62 @@
       <c r="K3" t="s">
         <v>260</v>
       </c>
-      <c r="L3" s="81" t="s">
+      <c r="L3" t="s">
+        <v>677</v>
+      </c>
+      <c r="M3" s="82">
+        <v>1.5</v>
+      </c>
+      <c r="N3" s="82" t="s">
+        <v>680</v>
+      </c>
+      <c r="O3" s="82" t="s">
+        <v>682</v>
+      </c>
+      <c r="P3" s="82" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q3" s="82" t="s">
+        <v>686</v>
+      </c>
+      <c r="R3" t="s">
+        <v>688</v>
+      </c>
+      <c r="S3" s="83" t="s">
+        <v>690</v>
+      </c>
+      <c r="T3" s="83" t="s">
+        <v>692</v>
+      </c>
+      <c r="U3" s="83" t="s">
+        <v>694</v>
+      </c>
+      <c r="V3" s="83" t="s">
+        <v>696</v>
+      </c>
+      <c r="W3" s="83" t="s">
+        <v>698</v>
+      </c>
+      <c r="X3" s="83" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y3" s="83" t="s">
+        <v>701</v>
+      </c>
+      <c r="Z3" s="83" t="s">
+        <v>704</v>
+      </c>
+      <c r="AA3" s="83" t="s">
+        <v>706</v>
+      </c>
+      <c r="AB3" s="81" t="s">
         <v>654</v>
       </c>
-      <c r="M3" t="s">
+      <c r="AC3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17">
+    <row r="4" spans="1:29" ht="17">
       <c r="A4">
         <v>2</v>
       </c>
@@ -18218,14 +18464,62 @@
       <c r="K4" t="s">
         <v>260</v>
       </c>
-      <c r="L4" s="81" t="s">
+      <c r="L4" t="s">
+        <v>677</v>
+      </c>
+      <c r="M4" s="82">
+        <v>1.5</v>
+      </c>
+      <c r="N4" s="82" t="s">
+        <v>680</v>
+      </c>
+      <c r="O4" s="82" t="s">
+        <v>682</v>
+      </c>
+      <c r="P4" s="82" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q4" s="82" t="s">
+        <v>686</v>
+      </c>
+      <c r="R4" t="s">
+        <v>688</v>
+      </c>
+      <c r="S4" s="83" t="s">
+        <v>690</v>
+      </c>
+      <c r="T4" s="83" t="s">
+        <v>692</v>
+      </c>
+      <c r="U4" s="83" t="s">
+        <v>694</v>
+      </c>
+      <c r="V4" s="83" t="s">
+        <v>696</v>
+      </c>
+      <c r="W4" s="83" t="s">
+        <v>698</v>
+      </c>
+      <c r="X4" s="83" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y4" s="83" t="s">
+        <v>701</v>
+      </c>
+      <c r="Z4" s="83" t="s">
+        <v>704</v>
+      </c>
+      <c r="AA4" s="83" t="s">
+        <v>706</v>
+      </c>
+      <c r="AB4" s="81" t="s">
         <v>655</v>
       </c>
-      <c r="M4" t="s">
+      <c r="AC4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17">
+    <row r="5" spans="1:29" ht="17">
       <c r="A5">
         <v>3</v>
       </c>
@@ -18256,14 +18550,62 @@
       <c r="K5" t="s">
         <v>260</v>
       </c>
-      <c r="L5" s="81" t="s">
+      <c r="L5" t="s">
+        <v>677</v>
+      </c>
+      <c r="M5" s="82">
+        <v>1.5</v>
+      </c>
+      <c r="N5" s="82" t="s">
+        <v>680</v>
+      </c>
+      <c r="O5" s="82" t="s">
+        <v>682</v>
+      </c>
+      <c r="P5" s="82" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q5" s="82" t="s">
+        <v>686</v>
+      </c>
+      <c r="R5" t="s">
+        <v>688</v>
+      </c>
+      <c r="S5" s="83" t="s">
+        <v>690</v>
+      </c>
+      <c r="T5" s="83" t="s">
+        <v>692</v>
+      </c>
+      <c r="U5" s="83" t="s">
+        <v>694</v>
+      </c>
+      <c r="V5" s="83" t="s">
+        <v>696</v>
+      </c>
+      <c r="W5" s="83" t="s">
+        <v>698</v>
+      </c>
+      <c r="X5" s="83" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y5" s="83" t="s">
+        <v>701</v>
+      </c>
+      <c r="Z5" s="83" t="s">
+        <v>704</v>
+      </c>
+      <c r="AA5" s="83" t="s">
+        <v>706</v>
+      </c>
+      <c r="AB5" s="81" t="s">
         <v>655</v>
       </c>
-      <c r="M5" t="s">
+      <c r="AC5" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="17">
+    <row r="6" spans="1:29" ht="17">
       <c r="A6">
         <v>4</v>
       </c>
@@ -18297,14 +18639,62 @@
       <c r="K6" t="s">
         <v>260</v>
       </c>
-      <c r="L6" s="81" t="s">
+      <c r="L6" t="s">
+        <v>677</v>
+      </c>
+      <c r="M6" s="82">
+        <v>1.5</v>
+      </c>
+      <c r="N6" s="82" t="s">
+        <v>680</v>
+      </c>
+      <c r="O6" s="82" t="s">
+        <v>682</v>
+      </c>
+      <c r="P6" s="82" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q6" s="82" t="s">
+        <v>686</v>
+      </c>
+      <c r="R6" t="s">
+        <v>688</v>
+      </c>
+      <c r="S6" s="83" t="s">
+        <v>690</v>
+      </c>
+      <c r="T6" s="83" t="s">
+        <v>692</v>
+      </c>
+      <c r="U6" s="83" t="s">
+        <v>694</v>
+      </c>
+      <c r="V6" s="83" t="s">
+        <v>696</v>
+      </c>
+      <c r="W6" s="83" t="s">
+        <v>698</v>
+      </c>
+      <c r="X6" s="83" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y6" s="83" t="s">
+        <v>701</v>
+      </c>
+      <c r="Z6" s="83" t="s">
+        <v>704</v>
+      </c>
+      <c r="AA6" s="83" t="s">
+        <v>706</v>
+      </c>
+      <c r="AB6" s="81" t="s">
         <v>656</v>
       </c>
-      <c r="M6" t="s">
+      <c r="AC6" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17">
+    <row r="7" spans="1:29" ht="17">
       <c r="A7">
         <v>5</v>
       </c>
@@ -18339,13 +18729,61 @@
         <v>260</v>
       </c>
       <c r="L7" t="s">
+        <v>677</v>
+      </c>
+      <c r="M7" s="82">
+        <v>1.5</v>
+      </c>
+      <c r="N7" s="82" t="s">
+        <v>680</v>
+      </c>
+      <c r="O7" s="82" t="s">
+        <v>682</v>
+      </c>
+      <c r="P7" s="82" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q7" s="82" t="s">
+        <v>686</v>
+      </c>
+      <c r="R7" t="s">
+        <v>688</v>
+      </c>
+      <c r="S7" s="83" t="s">
+        <v>690</v>
+      </c>
+      <c r="T7" s="83" t="s">
+        <v>692</v>
+      </c>
+      <c r="U7" s="83" t="s">
+        <v>694</v>
+      </c>
+      <c r="V7" s="83" t="s">
+        <v>696</v>
+      </c>
+      <c r="W7" s="83" t="s">
+        <v>698</v>
+      </c>
+      <c r="X7" s="83" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y7" s="83" t="s">
+        <v>701</v>
+      </c>
+      <c r="Z7" s="83" t="s">
+        <v>704</v>
+      </c>
+      <c r="AA7" s="83" t="s">
+        <v>706</v>
+      </c>
+      <c r="AB7" t="s">
         <v>657</v>
       </c>
-      <c r="M7" t="s">
+      <c r="AC7" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="17">
+    <row r="8" spans="1:29" ht="17">
       <c r="A8">
         <v>6</v>
       </c>
@@ -18373,14 +18811,62 @@
       <c r="K8" t="s">
         <v>260</v>
       </c>
-      <c r="L8" s="81" t="s">
+      <c r="L8" t="s">
+        <v>677</v>
+      </c>
+      <c r="M8" s="82">
+        <v>1.5</v>
+      </c>
+      <c r="N8" s="82" t="s">
+        <v>680</v>
+      </c>
+      <c r="O8" s="82" t="s">
+        <v>682</v>
+      </c>
+      <c r="P8" s="82" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q8" s="82" t="s">
+        <v>686</v>
+      </c>
+      <c r="R8" t="s">
+        <v>688</v>
+      </c>
+      <c r="S8" s="83" t="s">
+        <v>690</v>
+      </c>
+      <c r="T8" s="83" t="s">
+        <v>692</v>
+      </c>
+      <c r="U8" s="83" t="s">
+        <v>694</v>
+      </c>
+      <c r="V8" s="83" t="s">
+        <v>696</v>
+      </c>
+      <c r="W8" s="83" t="s">
+        <v>698</v>
+      </c>
+      <c r="X8" s="83" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y8" s="83" t="s">
+        <v>701</v>
+      </c>
+      <c r="Z8" s="83" t="s">
+        <v>704</v>
+      </c>
+      <c r="AA8" s="83" t="s">
+        <v>706</v>
+      </c>
+      <c r="AB8" s="81" t="s">
         <v>673</v>
       </c>
-      <c r="M8" t="s">
+      <c r="AC8" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="51">
+    <row r="9" spans="1:29" ht="51">
       <c r="A9">
         <v>7</v>
       </c>
@@ -18408,18 +18894,74 @@
       <c r="K9" t="s">
         <v>260</v>
       </c>
-      <c r="L9" s="81" t="s">
+      <c r="L9" t="s">
+        <v>677</v>
+      </c>
+      <c r="M9" s="82">
+        <v>1.5</v>
+      </c>
+      <c r="N9" s="82" t="s">
+        <v>680</v>
+      </c>
+      <c r="O9" s="82" t="s">
+        <v>682</v>
+      </c>
+      <c r="P9" s="82" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q9" s="82" t="s">
+        <v>686</v>
+      </c>
+      <c r="R9" t="s">
+        <v>688</v>
+      </c>
+      <c r="S9" s="83" t="s">
+        <v>690</v>
+      </c>
+      <c r="T9" s="83" t="s">
+        <v>692</v>
+      </c>
+      <c r="U9" s="83" t="s">
+        <v>694</v>
+      </c>
+      <c r="V9" s="83" t="s">
+        <v>696</v>
+      </c>
+      <c r="W9" s="83" t="s">
+        <v>698</v>
+      </c>
+      <c r="X9" s="83" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y9" s="83" t="s">
+        <v>701</v>
+      </c>
+      <c r="Z9" s="83" t="s">
+        <v>704</v>
+      </c>
+      <c r="AA9" s="83" t="s">
+        <v>706</v>
+      </c>
+      <c r="AB9" s="81" t="s">
         <v>674</v>
       </c>
-      <c r="M9" t="s">
+      <c r="AC9" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:29">
       <c r="F16" s="68"/>
       <c r="G16" s="68"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{5F1D8459-3B99-CA40-B42B-866472E16B6A}"/>
+    <hyperlink ref="U3:U9" r:id="rId2" display="dreichman@wpi.edu" xr:uid="{F8A3D820-0B66-AD44-B58B-6E847DFE1CF9}"/>
+    <hyperlink ref="W2" r:id="rId3" xr:uid="{260637A7-4B8B-7B4B-96FB-7DE015CC464D}"/>
+    <hyperlink ref="W3:W9" r:id="rId4" display="irb@wpi.edu" xr:uid="{085D0EDD-1C67-B844-AFC2-55C863DB96BD}"/>
+    <hyperlink ref="Z2" r:id="rId5" xr:uid="{52FEA23D-DDD3-9644-9790-75496081EB78}"/>
+    <hyperlink ref="Z3:Z9" r:id="rId6" display="gjohnson@wpi.edu" xr:uid="{3592C6B3-7E3C-1F43-9B66-AF5AD20C7256}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -18429,7 +18971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE6320D-B1FD-E344-B304-B9DCE6A3C0D3}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed rendering issues, deleted unused files, fixed monitor.
Replaced enter and arrow images with svg images.
Deleted unused files from docs folder.
Deleted treatments.js file since experiment definitions were shifted to firestore.
Deleted console.log messages.
Added field to experiment definitions to specify if order of treatments is randomized.  Changed algorithm in the function to randomize question order so that for within subject study, questions for each treatment will be in the same order.
Got CLI monitor working with refactored data stored in firestore using firestore realtime update API.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD82E339-1443-254C-94DE-C368F6B56FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4539C194-1D03-294C-A399-BE998AE1C040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21060" activeTab="3" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2893" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2902" uniqueCount="709">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -2208,6 +2208,12 @@
   </si>
   <si>
     <t>(508)831-4989</t>
+  </si>
+  <si>
+    <t>question_order</t>
+  </si>
+  <si>
+    <t>fixed</t>
   </si>
 </sst>
 </file>
@@ -2592,6 +2598,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2610,8 +2619,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2641,15 +2665,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2663,15 +2678,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10331,7 +10337,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>6.2865291111590782E-2</v>
+        <v>0.8897192469267754</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -10351,7 +10357,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.97933949551891075</v>
+        <v>0.39718412257460378</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -10372,7 +10378,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.52846736147141371</v>
+        <v>0.17651004073418186</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -10392,7 +10398,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.20646759939969328</v>
+        <v>0.18852592870791474</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -10653,48 +10659,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="85" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="85"/>
-      <c r="E3" s="84" t="s">
+      <c r="D3" s="86"/>
+      <c r="E3" s="85" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="85"/>
-      <c r="G3" s="84" t="s">
+      <c r="F3" s="86"/>
+      <c r="G3" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="85"/>
-      <c r="I3" s="84" t="s">
+      <c r="H3" s="86"/>
+      <c r="I3" s="85" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="85"/>
+      <c r="J3" s="86"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="86" t="s">
+      <c r="M3" s="87" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="87"/>
-      <c r="O3" s="88"/>
-      <c r="P3" s="86" t="s">
+      <c r="N3" s="88"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="87" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="87"/>
-      <c r="R3" s="88"/>
-      <c r="S3" s="86" t="s">
+      <c r="Q3" s="88"/>
+      <c r="R3" s="89"/>
+      <c r="S3" s="87" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="87"/>
-      <c r="U3" s="87"/>
-      <c r="V3" s="89" t="s">
+      <c r="T3" s="88"/>
+      <c r="U3" s="88"/>
+      <c r="V3" s="90" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="89"/>
-      <c r="X3" s="89"/>
+      <c r="W3" s="90"/>
+      <c r="X3" s="90"/>
       <c r="Y3" t="s">
         <v>215</v>
       </c>
@@ -11773,16 +11779,16 @@
       </c>
     </row>
     <row r="29" spans="1:33">
-      <c r="C29" s="90" t="s">
+      <c r="C29" s="84" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="90"/>
-      <c r="E29" s="90"/>
-      <c r="F29" s="90" t="s">
+      <c r="D29" s="84"/>
+      <c r="E29" s="84"/>
+      <c r="F29" s="84" t="s">
         <v>169</v>
       </c>
-      <c r="G29" s="90"/>
-      <c r="H29" s="90"/>
+      <c r="G29" s="84"/>
+      <c r="H29" s="84"/>
       <c r="J29" t="s">
         <v>168</v>
       </c>
@@ -12687,16 +12693,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B26" r:id="rId1" xr:uid="{D2B54FA7-7284-A444-93E2-10BEB7DF1432}"/>
@@ -12736,105 +12742,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="97" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="91" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="91" t="s">
+      <c r="A2" s="103" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="97" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="98"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="92"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="100" t="s">
+      <c r="F2" s="98"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="106" t="s">
+      <c r="I2" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="106"/>
-      <c r="K2" s="106"/>
-      <c r="L2" s="106"/>
-      <c r="M2" s="106"/>
-      <c r="N2" s="106"/>
-      <c r="O2" s="106"/>
-      <c r="P2" s="106"/>
-      <c r="Q2" s="106"/>
-      <c r="R2" s="106" t="s">
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="109"/>
+      <c r="O2" s="109"/>
+      <c r="P2" s="109"/>
+      <c r="Q2" s="109"/>
+      <c r="R2" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="106"/>
-      <c r="T2" s="106"/>
-      <c r="U2" s="106"/>
-      <c r="V2" s="100" t="s">
+      <c r="S2" s="109"/>
+      <c r="T2" s="109"/>
+      <c r="U2" s="109"/>
+      <c r="V2" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="100" t="s">
+      <c r="W2" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="108" t="s">
+      <c r="X2" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="108" t="s">
+      <c r="Y2" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="108" t="s">
+      <c r="Z2" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="108" t="s">
+      <c r="AA2" s="91" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="98"/>
-      <c r="B3" s="94"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="107" t="s">
+      <c r="A3" s="104"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105" t="s">
+      <c r="J3" s="108"/>
+      <c r="K3" s="108"/>
+      <c r="L3" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="105"/>
-      <c r="N3" s="105" t="s">
+      <c r="M3" s="108"/>
+      <c r="N3" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="105"/>
-      <c r="P3" s="105" t="s">
+      <c r="O3" s="108"/>
+      <c r="P3" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="105"/>
-      <c r="R3" s="103" t="s">
+      <c r="Q3" s="108"/>
+      <c r="R3" s="106" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="103" t="s">
+      <c r="S3" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="103" t="s">
+      <c r="T3" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="103" t="s">
+      <c r="U3" s="106" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="101"/>
-      <c r="W3" s="101"/>
-      <c r="X3" s="109"/>
-      <c r="Y3" s="109"/>
-      <c r="Z3" s="109"/>
-      <c r="AA3" s="109"/>
+      <c r="V3" s="95"/>
+      <c r="W3" s="95"/>
+      <c r="X3" s="92"/>
+      <c r="Y3" s="92"/>
+      <c r="Z3" s="92"/>
+      <c r="AA3" s="92"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="99"/>
+      <c r="A4" s="105"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -12853,7 +12859,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="102"/>
+      <c r="H4" s="96"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -12881,16 +12887,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="104"/>
-      <c r="S4" s="104"/>
-      <c r="T4" s="104"/>
-      <c r="U4" s="104"/>
-      <c r="V4" s="102"/>
-      <c r="W4" s="102"/>
-      <c r="X4" s="110"/>
-      <c r="Y4" s="110"/>
-      <c r="Z4" s="110"/>
-      <c r="AA4" s="109"/>
+      <c r="R4" s="107"/>
+      <c r="S4" s="107"/>
+      <c r="T4" s="107"/>
+      <c r="U4" s="107"/>
+      <c r="V4" s="96"/>
+      <c r="W4" s="96"/>
+      <c r="X4" s="93"/>
+      <c r="Y4" s="93"/>
+      <c r="Z4" s="93"/>
+      <c r="AA4" s="92"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -13391,11 +13397,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -13411,6 +13412,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -18151,10 +18157,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAA32EA-3DA8-BD44-8758-9048DFA42915}">
-  <dimension ref="A1:AC16"/>
+  <dimension ref="A1:AD16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="128" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+    <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18162,14 +18168,14 @@
     <col min="1" max="1" width="14.1640625" customWidth="1"/>
     <col min="2" max="2" width="113" customWidth="1"/>
     <col min="4" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="7" width="21.5" customWidth="1"/>
-    <col min="8" max="9" width="21.5" style="36" customWidth="1"/>
-    <col min="10" max="27" width="21.5" customWidth="1"/>
-    <col min="28" max="28" width="28.83203125" customWidth="1"/>
-    <col min="29" max="29" width="63.5" customWidth="1"/>
+    <col min="6" max="8" width="21.5" customWidth="1"/>
+    <col min="9" max="10" width="21.5" style="36" customWidth="1"/>
+    <col min="11" max="28" width="21.5" customWidth="1"/>
+    <col min="29" max="29" width="28.83203125" customWidth="1"/>
+    <col min="30" max="30" width="63.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>671</v>
       </c>
@@ -18191,74 +18197,77 @@
       <c r="G1" t="s">
         <v>365</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" t="s">
+        <v>707</v>
+      </c>
+      <c r="I1" s="36" t="s">
         <v>256</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="J1" s="36" t="s">
         <v>257</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>255</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>259</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>676</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>678</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>679</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>681</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>683</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>685</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>687</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>689</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>691</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>693</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>695</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>697</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>699</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>702</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>703</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>705</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>269</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="17">
+    <row r="2" spans="1:30" ht="17">
       <c r="A2">
         <v>0</v>
       </c>
@@ -18280,74 +18289,77 @@
       <c r="G2" s="7" t="s">
         <v>659</v>
       </c>
-      <c r="H2" s="36">
-        <v>1</v>
+      <c r="H2" s="7" t="s">
+        <v>708</v>
       </c>
       <c r="I2" s="36">
         <v>1</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="J2" s="36">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
         <v>660</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>677</v>
       </c>
-      <c r="M2" s="82">
+      <c r="N2" s="82">
         <v>1.5</v>
       </c>
-      <c r="N2" s="82" t="s">
+      <c r="O2" s="82" t="s">
         <v>680</v>
       </c>
-      <c r="O2" s="82" t="s">
+      <c r="P2" s="82" t="s">
         <v>682</v>
       </c>
-      <c r="P2" s="82" t="s">
+      <c r="Q2" s="82" t="s">
         <v>684</v>
       </c>
-      <c r="Q2" s="82" t="s">
+      <c r="R2" s="82" t="s">
         <v>686</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>688</v>
       </c>
-      <c r="S2" s="83" t="s">
+      <c r="T2" s="83" t="s">
         <v>690</v>
       </c>
-      <c r="T2" s="83" t="s">
+      <c r="U2" s="83" t="s">
         <v>692</v>
       </c>
-      <c r="U2" s="83" t="s">
+      <c r="V2" s="83" t="s">
         <v>694</v>
       </c>
-      <c r="V2" s="83" t="s">
+      <c r="W2" s="83" t="s">
         <v>696</v>
       </c>
-      <c r="W2" s="83" t="s">
+      <c r="X2" s="83" t="s">
         <v>698</v>
       </c>
-      <c r="X2" s="83" t="s">
+      <c r="Y2" s="83" t="s">
         <v>700</v>
       </c>
-      <c r="Y2" s="83" t="s">
+      <c r="Z2" s="83" t="s">
         <v>701</v>
       </c>
-      <c r="Z2" s="83" t="s">
+      <c r="AA2" s="83" t="s">
         <v>704</v>
       </c>
-      <c r="AA2" s="83" t="s">
+      <c r="AB2" s="83" t="s">
         <v>706</v>
       </c>
-      <c r="AB2">
-        <v>1</v>
-      </c>
-      <c r="AC2" t="s">
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="17">
+    <row r="3" spans="1:30" ht="17">
       <c r="A3">
         <v>1</v>
       </c>
@@ -18369,71 +18381,74 @@
       <c r="G3" s="7" t="s">
         <v>659</v>
       </c>
-      <c r="H3" s="36">
+      <c r="H3" s="7" t="s">
+        <v>708</v>
+      </c>
+      <c r="I3" s="36">
         <v>44922</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
         <v>260</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>677</v>
       </c>
-      <c r="M3" s="82">
+      <c r="N3" s="82">
         <v>1.5</v>
       </c>
-      <c r="N3" s="82" t="s">
+      <c r="O3" s="82" t="s">
         <v>680</v>
       </c>
-      <c r="O3" s="82" t="s">
+      <c r="P3" s="82" t="s">
         <v>682</v>
       </c>
-      <c r="P3" s="82" t="s">
+      <c r="Q3" s="82" t="s">
         <v>684</v>
       </c>
-      <c r="Q3" s="82" t="s">
+      <c r="R3" s="82" t="s">
         <v>686</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>688</v>
       </c>
-      <c r="S3" s="83" t="s">
+      <c r="T3" s="83" t="s">
         <v>690</v>
       </c>
-      <c r="T3" s="83" t="s">
+      <c r="U3" s="83" t="s">
         <v>692</v>
       </c>
-      <c r="U3" s="83" t="s">
+      <c r="V3" s="83" t="s">
         <v>694</v>
       </c>
-      <c r="V3" s="83" t="s">
+      <c r="W3" s="83" t="s">
         <v>696</v>
       </c>
-      <c r="W3" s="83" t="s">
+      <c r="X3" s="83" t="s">
         <v>698</v>
       </c>
-      <c r="X3" s="83" t="s">
+      <c r="Y3" s="83" t="s">
         <v>700</v>
       </c>
-      <c r="Y3" s="83" t="s">
+      <c r="Z3" s="83" t="s">
         <v>701</v>
       </c>
-      <c r="Z3" s="83" t="s">
+      <c r="AA3" s="83" t="s">
         <v>704</v>
       </c>
-      <c r="AA3" s="83" t="s">
+      <c r="AB3" s="83" t="s">
         <v>706</v>
       </c>
-      <c r="AB3" s="81" t="s">
+      <c r="AC3" s="81" t="s">
         <v>654</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="17">
+    <row r="4" spans="1:30" ht="17">
       <c r="A4">
         <v>2</v>
       </c>
@@ -18455,71 +18470,74 @@
       <c r="G4" s="7" t="s">
         <v>659</v>
       </c>
-      <c r="H4" s="36">
+      <c r="H4" s="7" t="s">
+        <v>708</v>
+      </c>
+      <c r="I4" s="36">
         <v>44940</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>3</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>260</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>677</v>
       </c>
-      <c r="M4" s="82">
+      <c r="N4" s="82">
         <v>1.5</v>
       </c>
-      <c r="N4" s="82" t="s">
+      <c r="O4" s="82" t="s">
         <v>680</v>
       </c>
-      <c r="O4" s="82" t="s">
+      <c r="P4" s="82" t="s">
         <v>682</v>
       </c>
-      <c r="P4" s="82" t="s">
+      <c r="Q4" s="82" t="s">
         <v>684</v>
       </c>
-      <c r="Q4" s="82" t="s">
+      <c r="R4" s="82" t="s">
         <v>686</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>688</v>
       </c>
-      <c r="S4" s="83" t="s">
+      <c r="T4" s="83" t="s">
         <v>690</v>
       </c>
-      <c r="T4" s="83" t="s">
+      <c r="U4" s="83" t="s">
         <v>692</v>
       </c>
-      <c r="U4" s="83" t="s">
+      <c r="V4" s="83" t="s">
         <v>694</v>
       </c>
-      <c r="V4" s="83" t="s">
+      <c r="W4" s="83" t="s">
         <v>696</v>
       </c>
-      <c r="W4" s="83" t="s">
+      <c r="X4" s="83" t="s">
         <v>698</v>
       </c>
-      <c r="X4" s="83" t="s">
+      <c r="Y4" s="83" t="s">
         <v>700</v>
       </c>
-      <c r="Y4" s="83" t="s">
+      <c r="Z4" s="83" t="s">
         <v>701</v>
       </c>
-      <c r="Z4" s="83" t="s">
+      <c r="AA4" s="83" t="s">
         <v>704</v>
       </c>
-      <c r="AA4" s="83" t="s">
+      <c r="AB4" s="83" t="s">
         <v>706</v>
       </c>
-      <c r="AB4" s="81" t="s">
+      <c r="AC4" s="81" t="s">
         <v>655</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="17">
+    <row r="5" spans="1:30" ht="17">
       <c r="A5">
         <v>3</v>
       </c>
@@ -18541,71 +18559,74 @@
       <c r="G5" s="7" t="s">
         <v>659</v>
       </c>
-      <c r="H5" s="36">
+      <c r="H5" s="7" t="s">
+        <v>708</v>
+      </c>
+      <c r="I5" s="36">
         <v>44942</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>26</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>260</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>677</v>
       </c>
-      <c r="M5" s="82">
+      <c r="N5" s="82">
         <v>1.5</v>
       </c>
-      <c r="N5" s="82" t="s">
+      <c r="O5" s="82" t="s">
         <v>680</v>
       </c>
-      <c r="O5" s="82" t="s">
+      <c r="P5" s="82" t="s">
         <v>682</v>
       </c>
-      <c r="P5" s="82" t="s">
+      <c r="Q5" s="82" t="s">
         <v>684</v>
       </c>
-      <c r="Q5" s="82" t="s">
+      <c r="R5" s="82" t="s">
         <v>686</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>688</v>
       </c>
-      <c r="S5" s="83" t="s">
+      <c r="T5" s="83" t="s">
         <v>690</v>
       </c>
-      <c r="T5" s="83" t="s">
+      <c r="U5" s="83" t="s">
         <v>692</v>
       </c>
-      <c r="U5" s="83" t="s">
+      <c r="V5" s="83" t="s">
         <v>694</v>
       </c>
-      <c r="V5" s="83" t="s">
+      <c r="W5" s="83" t="s">
         <v>696</v>
       </c>
-      <c r="W5" s="83" t="s">
+      <c r="X5" s="83" t="s">
         <v>698</v>
       </c>
-      <c r="X5" s="83" t="s">
+      <c r="Y5" s="83" t="s">
         <v>700</v>
       </c>
-      <c r="Y5" s="83" t="s">
+      <c r="Z5" s="83" t="s">
         <v>701</v>
       </c>
-      <c r="Z5" s="83" t="s">
+      <c r="AA5" s="83" t="s">
         <v>704</v>
       </c>
-      <c r="AA5" s="83" t="s">
+      <c r="AB5" s="83" t="s">
         <v>706</v>
       </c>
-      <c r="AB5" s="81" t="s">
+      <c r="AC5" s="81" t="s">
         <v>655</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="17">
+    <row r="6" spans="1:30" ht="17">
       <c r="A6">
         <v>4</v>
       </c>
@@ -18627,74 +18648,77 @@
       <c r="G6" s="7" t="s">
         <v>659</v>
       </c>
-      <c r="H6" s="36">
+      <c r="H6" s="7" t="s">
+        <v>708</v>
+      </c>
+      <c r="I6" s="36">
         <v>44994</v>
       </c>
-      <c r="I6" s="36">
+      <c r="J6" s="36">
         <v>44995</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>100</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>260</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>677</v>
       </c>
-      <c r="M6" s="82">
+      <c r="N6" s="82">
         <v>1.5</v>
       </c>
-      <c r="N6" s="82" t="s">
+      <c r="O6" s="82" t="s">
         <v>680</v>
       </c>
-      <c r="O6" s="82" t="s">
+      <c r="P6" s="82" t="s">
         <v>682</v>
       </c>
-      <c r="P6" s="82" t="s">
+      <c r="Q6" s="82" t="s">
         <v>684</v>
       </c>
-      <c r="Q6" s="82" t="s">
+      <c r="R6" s="82" t="s">
         <v>686</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>688</v>
       </c>
-      <c r="S6" s="83" t="s">
+      <c r="T6" s="83" t="s">
         <v>690</v>
       </c>
-      <c r="T6" s="83" t="s">
+      <c r="U6" s="83" t="s">
         <v>692</v>
       </c>
-      <c r="U6" s="83" t="s">
+      <c r="V6" s="83" t="s">
         <v>694</v>
       </c>
-      <c r="V6" s="83" t="s">
+      <c r="W6" s="83" t="s">
         <v>696</v>
       </c>
-      <c r="W6" s="83" t="s">
+      <c r="X6" s="83" t="s">
         <v>698</v>
       </c>
-      <c r="X6" s="83" t="s">
+      <c r="Y6" s="83" t="s">
         <v>700</v>
       </c>
-      <c r="Y6" s="83" t="s">
+      <c r="Z6" s="83" t="s">
         <v>701</v>
       </c>
-      <c r="Z6" s="83" t="s">
+      <c r="AA6" s="83" t="s">
         <v>704</v>
       </c>
-      <c r="AA6" s="83" t="s">
+      <c r="AB6" s="83" t="s">
         <v>706</v>
       </c>
-      <c r="AB6" s="81" t="s">
+      <c r="AC6" s="81" t="s">
         <v>656</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="17">
+    <row r="7" spans="1:30" ht="17">
       <c r="A7">
         <v>5</v>
       </c>
@@ -18716,74 +18740,77 @@
       <c r="G7" s="7" t="s">
         <v>659</v>
       </c>
-      <c r="H7" s="36">
-        <v>45119</v>
+      <c r="H7" s="7" t="s">
+        <v>708</v>
       </c>
       <c r="I7" s="36">
         <v>45119</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="36">
+        <v>45119</v>
+      </c>
+      <c r="K7">
         <v>150</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>260</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>677</v>
       </c>
-      <c r="M7" s="82">
+      <c r="N7" s="82">
         <v>1.5</v>
       </c>
-      <c r="N7" s="82" t="s">
+      <c r="O7" s="82" t="s">
         <v>680</v>
       </c>
-      <c r="O7" s="82" t="s">
+      <c r="P7" s="82" t="s">
         <v>682</v>
       </c>
-      <c r="P7" s="82" t="s">
+      <c r="Q7" s="82" t="s">
         <v>684</v>
       </c>
-      <c r="Q7" s="82" t="s">
+      <c r="R7" s="82" t="s">
         <v>686</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>688</v>
       </c>
-      <c r="S7" s="83" t="s">
+      <c r="T7" s="83" t="s">
         <v>690</v>
       </c>
-      <c r="T7" s="83" t="s">
+      <c r="U7" s="83" t="s">
         <v>692</v>
       </c>
-      <c r="U7" s="83" t="s">
+      <c r="V7" s="83" t="s">
         <v>694</v>
       </c>
-      <c r="V7" s="83" t="s">
+      <c r="W7" s="83" t="s">
         <v>696</v>
       </c>
-      <c r="W7" s="83" t="s">
+      <c r="X7" s="83" t="s">
         <v>698</v>
       </c>
-      <c r="X7" s="83" t="s">
+      <c r="Y7" s="83" t="s">
         <v>700</v>
       </c>
-      <c r="Y7" s="83" t="s">
+      <c r="Z7" s="83" t="s">
         <v>701</v>
       </c>
-      <c r="Z7" s="83" t="s">
+      <c r="AA7" s="83" t="s">
         <v>704</v>
       </c>
-      <c r="AA7" s="83" t="s">
+      <c r="AB7" s="83" t="s">
         <v>706</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>657</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="17">
+    <row r="8" spans="1:30" ht="17">
       <c r="A8">
         <v>6</v>
       </c>
@@ -18805,68 +18832,71 @@
       <c r="G8" s="7" t="s">
         <v>659</v>
       </c>
-      <c r="J8">
+      <c r="H8" s="7" t="s">
+        <v>708</v>
+      </c>
+      <c r="K8">
         <v>150</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>260</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>677</v>
       </c>
-      <c r="M8" s="82">
+      <c r="N8" s="82">
         <v>1.5</v>
       </c>
-      <c r="N8" s="82" t="s">
+      <c r="O8" s="82" t="s">
         <v>680</v>
       </c>
-      <c r="O8" s="82" t="s">
+      <c r="P8" s="82" t="s">
         <v>682</v>
       </c>
-      <c r="P8" s="82" t="s">
+      <c r="Q8" s="82" t="s">
         <v>684</v>
       </c>
-      <c r="Q8" s="82" t="s">
+      <c r="R8" s="82" t="s">
         <v>686</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>688</v>
       </c>
-      <c r="S8" s="83" t="s">
+      <c r="T8" s="83" t="s">
         <v>690</v>
       </c>
-      <c r="T8" s="83" t="s">
+      <c r="U8" s="83" t="s">
         <v>692</v>
       </c>
-      <c r="U8" s="83" t="s">
+      <c r="V8" s="83" t="s">
         <v>694</v>
       </c>
-      <c r="V8" s="83" t="s">
+      <c r="W8" s="83" t="s">
         <v>696</v>
       </c>
-      <c r="W8" s="83" t="s">
+      <c r="X8" s="83" t="s">
         <v>698</v>
       </c>
-      <c r="X8" s="83" t="s">
+      <c r="Y8" s="83" t="s">
         <v>700</v>
       </c>
-      <c r="Y8" s="83" t="s">
+      <c r="Z8" s="83" t="s">
         <v>701</v>
       </c>
-      <c r="Z8" s="83" t="s">
+      <c r="AA8" s="83" t="s">
         <v>704</v>
       </c>
-      <c r="AA8" s="83" t="s">
+      <c r="AB8" s="83" t="s">
         <v>706</v>
       </c>
-      <c r="AB8" s="81" t="s">
+      <c r="AC8" s="81" t="s">
         <v>673</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="51">
+    <row r="9" spans="1:30" ht="51">
       <c r="A9">
         <v>7</v>
       </c>
@@ -18888,79 +18918,83 @@
       <c r="G9" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="J9">
+      <c r="H9" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="K9">
         <v>150</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>260</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>677</v>
       </c>
-      <c r="M9" s="82">
+      <c r="N9" s="82">
         <v>1.5</v>
       </c>
-      <c r="N9" s="82" t="s">
+      <c r="O9" s="82" t="s">
         <v>680</v>
       </c>
-      <c r="O9" s="82" t="s">
+      <c r="P9" s="82" t="s">
         <v>682</v>
       </c>
-      <c r="P9" s="82" t="s">
+      <c r="Q9" s="82" t="s">
         <v>684</v>
       </c>
-      <c r="Q9" s="82" t="s">
+      <c r="R9" s="82" t="s">
         <v>686</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>688</v>
       </c>
-      <c r="S9" s="83" t="s">
+      <c r="T9" s="83" t="s">
         <v>690</v>
       </c>
-      <c r="T9" s="83" t="s">
+      <c r="U9" s="83" t="s">
         <v>692</v>
       </c>
-      <c r="U9" s="83" t="s">
+      <c r="V9" s="83" t="s">
         <v>694</v>
       </c>
-      <c r="V9" s="83" t="s">
+      <c r="W9" s="83" t="s">
         <v>696</v>
       </c>
-      <c r="W9" s="83" t="s">
+      <c r="X9" s="83" t="s">
         <v>698</v>
       </c>
-      <c r="X9" s="83" t="s">
+      <c r="Y9" s="83" t="s">
         <v>700</v>
       </c>
-      <c r="Y9" s="83" t="s">
+      <c r="Z9" s="83" t="s">
         <v>701</v>
       </c>
-      <c r="Z9" s="83" t="s">
+      <c r="AA9" s="83" t="s">
         <v>704</v>
       </c>
-      <c r="AA9" s="83" t="s">
+      <c r="AB9" s="83" t="s">
         <v>706</v>
       </c>
-      <c r="AB9" s="81" t="s">
+      <c r="AC9" s="81" t="s">
         <v>674</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AD9" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:30">
       <c r="F16" s="68"/>
       <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1" xr:uid="{5F1D8459-3B99-CA40-B42B-866472E16B6A}"/>
-    <hyperlink ref="U3:U9" r:id="rId2" display="dreichman@wpi.edu" xr:uid="{F8A3D820-0B66-AD44-B58B-6E847DFE1CF9}"/>
-    <hyperlink ref="W2" r:id="rId3" xr:uid="{260637A7-4B8B-7B4B-96FB-7DE015CC464D}"/>
-    <hyperlink ref="W3:W9" r:id="rId4" display="irb@wpi.edu" xr:uid="{085D0EDD-1C67-B844-AFC2-55C863DB96BD}"/>
-    <hyperlink ref="Z2" r:id="rId5" xr:uid="{52FEA23D-DDD3-9644-9790-75496081EB78}"/>
-    <hyperlink ref="Z3:Z9" r:id="rId6" display="gjohnson@wpi.edu" xr:uid="{3592C6B3-7E3C-1F43-9B66-AF5AD20C7256}"/>
+    <hyperlink ref="V2" r:id="rId1" xr:uid="{5F1D8459-3B99-CA40-B42B-866472E16B6A}"/>
+    <hyperlink ref="V3:V9" r:id="rId2" display="dreichman@wpi.edu" xr:uid="{F8A3D820-0B66-AD44-B58B-6E847DFE1CF9}"/>
+    <hyperlink ref="X2" r:id="rId3" xr:uid="{260637A7-4B8B-7B4B-96FB-7DE015CC464D}"/>
+    <hyperlink ref="X3:X9" r:id="rId4" display="irb@wpi.edu" xr:uid="{085D0EDD-1C67-B844-AFC2-55C863DB96BD}"/>
+    <hyperlink ref="AA2" r:id="rId5" xr:uid="{52FEA23D-DDD3-9644-9790-75496081EB78}"/>
+    <hyperlink ref="AA3:AA9" r:id="rId6" display="gjohnson@wpi.edu" xr:uid="{3592C6B3-7E3C-1F43-9B66-AF5AD20C7256}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -20051,8 +20085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF0298B-43F7-F849-959B-1EFC1ADC8C4E}">
   <dimension ref="A1:F242"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A203" workbookViewId="0">
+      <selection activeCell="E240" sqref="E240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -24372,9 +24406,6 @@
       <c r="B216">
         <v>7</v>
       </c>
-      <c r="C216">
-        <v>1</v>
-      </c>
       <c r="D216">
         <v>1</v>
       </c>
@@ -24392,9 +24423,6 @@
       <c r="B217">
         <v>7</v>
       </c>
-      <c r="C217">
-        <v>2</v>
-      </c>
       <c r="D217">
         <v>1</v>
       </c>
@@ -24412,9 +24440,6 @@
       <c r="B218">
         <v>7</v>
       </c>
-      <c r="C218">
-        <v>3</v>
-      </c>
       <c r="D218">
         <v>1</v>
       </c>
@@ -24432,9 +24457,6 @@
       <c r="B219">
         <v>7</v>
       </c>
-      <c r="C219">
-        <v>4</v>
-      </c>
       <c r="D219">
         <v>1</v>
       </c>
@@ -24452,9 +24474,6 @@
       <c r="B220">
         <v>7</v>
       </c>
-      <c r="C220">
-        <v>5</v>
-      </c>
       <c r="D220">
         <v>1</v>
       </c>
@@ -24472,9 +24491,6 @@
       <c r="B221">
         <v>7</v>
       </c>
-      <c r="C221">
-        <v>6</v>
-      </c>
       <c r="D221">
         <v>1</v>
       </c>
@@ -24492,9 +24508,6 @@
       <c r="B222">
         <v>7</v>
       </c>
-      <c r="C222">
-        <v>7</v>
-      </c>
       <c r="D222">
         <v>1</v>
       </c>
@@ -24512,9 +24525,6 @@
       <c r="B223">
         <v>7</v>
       </c>
-      <c r="C223">
-        <v>8</v>
-      </c>
       <c r="D223">
         <v>1</v>
       </c>
@@ -24532,9 +24542,6 @@
       <c r="B224">
         <v>7</v>
       </c>
-      <c r="C224">
-        <v>1</v>
-      </c>
       <c r="D224">
         <v>1</v>
       </c>
@@ -24552,9 +24559,6 @@
       <c r="B225">
         <v>7</v>
       </c>
-      <c r="C225">
-        <v>1</v>
-      </c>
       <c r="D225">
         <v>2</v>
       </c>
@@ -24572,9 +24576,6 @@
       <c r="B226">
         <v>7</v>
       </c>
-      <c r="C226">
-        <v>2</v>
-      </c>
       <c r="D226">
         <v>2</v>
       </c>
@@ -24592,9 +24593,6 @@
       <c r="B227">
         <v>7</v>
       </c>
-      <c r="C227">
-        <v>3</v>
-      </c>
       <c r="D227">
         <v>2</v>
       </c>
@@ -24612,9 +24610,6 @@
       <c r="B228">
         <v>7</v>
       </c>
-      <c r="C228">
-        <v>4</v>
-      </c>
       <c r="D228">
         <v>2</v>
       </c>
@@ -24632,9 +24627,6 @@
       <c r="B229">
         <v>7</v>
       </c>
-      <c r="C229">
-        <v>5</v>
-      </c>
       <c r="D229">
         <v>2</v>
       </c>
@@ -24652,9 +24644,6 @@
       <c r="B230">
         <v>7</v>
       </c>
-      <c r="C230">
-        <v>6</v>
-      </c>
       <c r="D230">
         <v>2</v>
       </c>
@@ -24672,9 +24661,6 @@
       <c r="B231">
         <v>7</v>
       </c>
-      <c r="C231">
-        <v>7</v>
-      </c>
       <c r="D231">
         <v>2</v>
       </c>
@@ -24692,9 +24678,6 @@
       <c r="B232">
         <v>7</v>
       </c>
-      <c r="C232">
-        <v>8</v>
-      </c>
       <c r="D232">
         <v>2</v>
       </c>
@@ -24712,9 +24695,6 @@
       <c r="B233">
         <v>7</v>
       </c>
-      <c r="C233">
-        <v>1</v>
-      </c>
       <c r="D233">
         <v>2</v>
       </c>
@@ -24732,9 +24712,6 @@
       <c r="B234">
         <v>7</v>
       </c>
-      <c r="C234">
-        <v>1</v>
-      </c>
       <c r="D234">
         <v>3</v>
       </c>
@@ -24752,9 +24729,6 @@
       <c r="B235">
         <v>7</v>
       </c>
-      <c r="C235">
-        <v>2</v>
-      </c>
       <c r="D235">
         <v>3</v>
       </c>
@@ -24772,9 +24746,6 @@
       <c r="B236">
         <v>7</v>
       </c>
-      <c r="C236">
-        <v>3</v>
-      </c>
       <c r="D236">
         <v>3</v>
       </c>
@@ -24792,9 +24763,6 @@
       <c r="B237">
         <v>7</v>
       </c>
-      <c r="C237">
-        <v>4</v>
-      </c>
       <c r="D237">
         <v>3</v>
       </c>
@@ -24812,9 +24780,6 @@
       <c r="B238">
         <v>7</v>
       </c>
-      <c r="C238">
-        <v>5</v>
-      </c>
       <c r="D238">
         <v>3</v>
       </c>
@@ -24832,9 +24797,6 @@
       <c r="B239">
         <v>7</v>
       </c>
-      <c r="C239">
-        <v>6</v>
-      </c>
       <c r="D239">
         <v>3</v>
       </c>
@@ -24852,9 +24814,6 @@
       <c r="B240">
         <v>7</v>
       </c>
-      <c r="C240">
-        <v>7</v>
-      </c>
       <c r="D240">
         <v>3</v>
       </c>
@@ -24872,9 +24831,6 @@
       <c r="B241">
         <v>7</v>
       </c>
-      <c r="C241">
-        <v>8</v>
-      </c>
       <c r="D241">
         <v>3</v>
       </c>
@@ -24891,9 +24847,6 @@
       </c>
       <c r="B242">
         <v>7</v>
-      </c>
-      <c r="C242">
-        <v>1</v>
       </c>
       <c r="D242">
         <v>3</v>

</xml_diff>

<commit_message>
Fixed MEL choice instruction text and within subject definition.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4539C194-1D03-294C-A399-BE998AE1C040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72523503-2D0F-2B4A-B247-0C5DB0A84765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21060" activeTab="3" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
@@ -2598,9 +2598,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2619,23 +2616,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2665,6 +2647,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2678,6 +2669,15 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10337,7 +10337,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.8897192469267754</v>
+        <v>2.62211179141425E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -10357,7 +10357,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.39718412257460378</v>
+        <v>0.78697852766720422</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -10378,7 +10378,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.17651004073418186</v>
+        <v>0.54638140961877824</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -10398,7 +10398,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.18852592870791474</v>
+        <v>0.80569251228750027</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -10659,48 +10659,48 @@
         <v>145</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="84" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="86"/>
-      <c r="E3" s="85" t="s">
+      <c r="D3" s="85"/>
+      <c r="E3" s="84" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="86"/>
-      <c r="G3" s="85" t="s">
+      <c r="F3" s="85"/>
+      <c r="G3" s="84" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="86"/>
-      <c r="I3" s="85" t="s">
+      <c r="H3" s="85"/>
+      <c r="I3" s="84" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="86"/>
+      <c r="J3" s="85"/>
       <c r="K3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="87" t="s">
+      <c r="M3" s="86" t="s">
         <v>160</v>
       </c>
-      <c r="N3" s="88"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="87" t="s">
+      <c r="N3" s="87"/>
+      <c r="O3" s="88"/>
+      <c r="P3" s="86" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="88"/>
-      <c r="R3" s="89"/>
-      <c r="S3" s="87" t="s">
+      <c r="Q3" s="87"/>
+      <c r="R3" s="88"/>
+      <c r="S3" s="86" t="s">
         <v>162</v>
       </c>
-      <c r="T3" s="88"/>
-      <c r="U3" s="88"/>
-      <c r="V3" s="90" t="s">
+      <c r="T3" s="87"/>
+      <c r="U3" s="87"/>
+      <c r="V3" s="89" t="s">
         <v>163</v>
       </c>
-      <c r="W3" s="90"/>
-      <c r="X3" s="90"/>
+      <c r="W3" s="89"/>
+      <c r="X3" s="89"/>
       <c r="Y3" t="s">
         <v>215</v>
       </c>
@@ -11779,16 +11779,16 @@
       </c>
     </row>
     <row r="29" spans="1:33">
-      <c r="C29" s="84" t="s">
+      <c r="C29" s="90" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="84"/>
-      <c r="E29" s="84"/>
-      <c r="F29" s="84" t="s">
+      <c r="D29" s="90"/>
+      <c r="E29" s="90"/>
+      <c r="F29" s="90" t="s">
         <v>169</v>
       </c>
-      <c r="G29" s="84"/>
-      <c r="H29" s="84"/>
+      <c r="G29" s="90"/>
+      <c r="H29" s="90"/>
       <c r="J29" t="s">
         <v>168</v>
       </c>
@@ -12693,16 +12693,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="P3:R3"/>
     <mergeCell ref="S3:U3"/>
     <mergeCell ref="V3:X3"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B26" r:id="rId1" xr:uid="{D2B54FA7-7284-A444-93E2-10BEB7DF1432}"/>
@@ -12742,105 +12742,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="103" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="97" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="97" t="s">
+      <c r="A2" s="97" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="92"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="98"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="94" t="s">
+      <c r="F2" s="92"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="109" t="s">
+      <c r="I2" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="109"/>
-      <c r="K2" s="109"/>
-      <c r="L2" s="109"/>
-      <c r="M2" s="109"/>
-      <c r="N2" s="109"/>
-      <c r="O2" s="109"/>
-      <c r="P2" s="109"/>
-      <c r="Q2" s="109"/>
-      <c r="R2" s="109" t="s">
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="106"/>
+      <c r="R2" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="109"/>
-      <c r="T2" s="109"/>
-      <c r="U2" s="109"/>
-      <c r="V2" s="94" t="s">
+      <c r="S2" s="106"/>
+      <c r="T2" s="106"/>
+      <c r="U2" s="106"/>
+      <c r="V2" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="94" t="s">
+      <c r="W2" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="91" t="s">
+      <c r="X2" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="91" t="s">
+      <c r="Y2" s="108" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="91" t="s">
+      <c r="Z2" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="91" t="s">
+      <c r="AA2" s="108" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="104"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="110" t="s">
+      <c r="A3" s="98"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="108"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="108" t="s">
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108" t="s">
+      <c r="M3" s="105"/>
+      <c r="N3" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108" t="s">
+      <c r="O3" s="105"/>
+      <c r="P3" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="106" t="s">
+      <c r="Q3" s="105"/>
+      <c r="R3" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="106" t="s">
+      <c r="S3" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="106" t="s">
+      <c r="T3" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="106" t="s">
+      <c r="U3" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="95"/>
-      <c r="W3" s="95"/>
-      <c r="X3" s="92"/>
-      <c r="Y3" s="92"/>
-      <c r="Z3" s="92"/>
-      <c r="AA3" s="92"/>
+      <c r="V3" s="101"/>
+      <c r="W3" s="101"/>
+      <c r="X3" s="109"/>
+      <c r="Y3" s="109"/>
+      <c r="Z3" s="109"/>
+      <c r="AA3" s="109"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="105"/>
+      <c r="A4" s="99"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -12859,7 +12859,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="96"/>
+      <c r="H4" s="102"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -12887,16 +12887,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="107"/>
-      <c r="S4" s="107"/>
-      <c r="T4" s="107"/>
-      <c r="U4" s="107"/>
-      <c r="V4" s="96"/>
-      <c r="W4" s="96"/>
-      <c r="X4" s="93"/>
-      <c r="Y4" s="93"/>
-      <c r="Z4" s="93"/>
-      <c r="AA4" s="92"/>
+      <c r="R4" s="104"/>
+      <c r="S4" s="104"/>
+      <c r="T4" s="104"/>
+      <c r="U4" s="104"/>
+      <c r="V4" s="102"/>
+      <c r="W4" s="102"/>
+      <c r="X4" s="110"/>
+      <c r="Y4" s="110"/>
+      <c r="Z4" s="110"/>
+      <c r="AA4" s="109"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -13397,6 +13397,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -13412,11 +13417,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -16594,7 +16594,7 @@
   <dimension ref="A1:KS2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18159,8 +18159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAA32EA-3DA8-BD44-8758-9048DFA42915}">
   <dimension ref="A1:AD16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView zoomScale="128" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19006,7 +19006,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -20083,10 +20083,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF0298B-43F7-F849-959B-1EFC1ADC8C4E}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F242"/>
   <sheetViews>
-    <sheetView topLeftCell="A203" workbookViewId="0">
-      <selection activeCell="E240" sqref="E240"/>
+    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
+      <selection activeCell="F244" sqref="F244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20119,7 +20120,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" hidden="1">
       <c r="A2">
         <v>1</v>
       </c>
@@ -20139,7 +20140,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" hidden="1">
       <c r="A3">
         <v>2</v>
       </c>
@@ -20159,7 +20160,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" hidden="1">
       <c r="A4">
         <v>3</v>
       </c>
@@ -20179,7 +20180,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" hidden="1">
       <c r="A5">
         <v>4</v>
       </c>
@@ -20199,7 +20200,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" hidden="1">
       <c r="A6">
         <v>5</v>
       </c>
@@ -20219,7 +20220,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" hidden="1">
       <c r="A7">
         <v>6</v>
       </c>
@@ -20239,7 +20240,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" hidden="1">
       <c r="A8">
         <v>7</v>
       </c>
@@ -20259,7 +20260,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" hidden="1">
       <c r="A9">
         <v>8</v>
       </c>
@@ -20279,7 +20280,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" hidden="1">
       <c r="A10">
         <v>9</v>
       </c>
@@ -20299,7 +20300,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" hidden="1">
       <c r="A11">
         <v>10</v>
       </c>
@@ -20319,7 +20320,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" hidden="1">
       <c r="A12">
         <v>11</v>
       </c>
@@ -20339,7 +20340,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" hidden="1">
       <c r="A13">
         <v>12</v>
       </c>
@@ -20359,7 +20360,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" hidden="1">
       <c r="A14">
         <v>13</v>
       </c>
@@ -20379,7 +20380,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" hidden="1">
       <c r="A15">
         <v>14</v>
       </c>
@@ -20399,7 +20400,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" hidden="1">
       <c r="A16">
         <v>15</v>
       </c>
@@ -20419,7 +20420,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" hidden="1">
       <c r="A17">
         <v>16</v>
       </c>
@@ -20439,7 +20440,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" hidden="1">
       <c r="A18">
         <v>17</v>
       </c>
@@ -20459,7 +20460,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" hidden="1">
       <c r="A19">
         <v>18</v>
       </c>
@@ -20479,7 +20480,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" hidden="1">
       <c r="A20">
         <v>19</v>
       </c>
@@ -20499,7 +20500,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" hidden="1">
       <c r="A21">
         <v>20</v>
       </c>
@@ -20519,7 +20520,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" hidden="1">
       <c r="A22">
         <v>21</v>
       </c>
@@ -20539,7 +20540,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" hidden="1">
       <c r="A23">
         <v>22</v>
       </c>
@@ -20559,7 +20560,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" hidden="1">
       <c r="A24">
         <v>23</v>
       </c>
@@ -20579,7 +20580,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" hidden="1">
       <c r="A25">
         <v>24</v>
       </c>
@@ -20599,7 +20600,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" hidden="1">
       <c r="A26">
         <v>25</v>
       </c>
@@ -20619,7 +20620,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" hidden="1">
       <c r="A27">
         <v>26</v>
       </c>
@@ -20639,7 +20640,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" hidden="1">
       <c r="A28">
         <v>27</v>
       </c>
@@ -20659,7 +20660,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" hidden="1">
       <c r="A29">
         <v>28</v>
       </c>
@@ -20679,7 +20680,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" hidden="1">
       <c r="A30">
         <v>29</v>
       </c>
@@ -20699,7 +20700,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" hidden="1">
       <c r="A31">
         <v>30</v>
       </c>
@@ -20719,7 +20720,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" hidden="1">
       <c r="A32">
         <v>31</v>
       </c>
@@ -20739,7 +20740,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" hidden="1">
       <c r="A33">
         <v>32</v>
       </c>
@@ -20759,7 +20760,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" hidden="1">
       <c r="A34">
         <v>33</v>
       </c>
@@ -20779,7 +20780,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" hidden="1">
       <c r="A35">
         <v>34</v>
       </c>
@@ -20799,7 +20800,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" hidden="1">
       <c r="A36">
         <v>35</v>
       </c>
@@ -20819,7 +20820,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" hidden="1">
       <c r="A37">
         <v>36</v>
       </c>
@@ -20839,7 +20840,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" hidden="1">
       <c r="A38">
         <v>37</v>
       </c>
@@ -20859,7 +20860,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" hidden="1">
       <c r="A39">
         <v>38</v>
       </c>
@@ -20879,7 +20880,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" hidden="1">
       <c r="A40">
         <v>39</v>
       </c>
@@ -20899,7 +20900,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" hidden="1">
       <c r="A41">
         <v>40</v>
       </c>
@@ -20919,7 +20920,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" hidden="1">
       <c r="A42">
         <v>41</v>
       </c>
@@ -20939,7 +20940,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" hidden="1">
       <c r="A43">
         <v>42</v>
       </c>
@@ -20959,7 +20960,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" hidden="1">
       <c r="A44">
         <v>43</v>
       </c>
@@ -20979,7 +20980,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" hidden="1">
       <c r="A45">
         <v>44</v>
       </c>
@@ -20999,7 +21000,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" hidden="1">
       <c r="A46">
         <v>45</v>
       </c>
@@ -21019,7 +21020,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" hidden="1">
       <c r="A47">
         <v>46</v>
       </c>
@@ -21039,7 +21040,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" hidden="1">
       <c r="A48">
         <v>47</v>
       </c>
@@ -21059,7 +21060,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" hidden="1">
       <c r="A49">
         <v>48</v>
       </c>
@@ -21079,7 +21080,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" hidden="1">
       <c r="A50">
         <v>49</v>
       </c>
@@ -21099,7 +21100,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" hidden="1">
       <c r="A51">
         <v>50</v>
       </c>
@@ -21119,7 +21120,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" hidden="1">
       <c r="A52">
         <v>51</v>
       </c>
@@ -21139,7 +21140,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" hidden="1">
       <c r="A53">
         <v>52</v>
       </c>
@@ -21159,7 +21160,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" hidden="1">
       <c r="A54">
         <v>53</v>
       </c>
@@ -21179,7 +21180,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" hidden="1">
       <c r="A55">
         <v>54</v>
       </c>
@@ -21199,7 +21200,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" hidden="1">
       <c r="A56">
         <v>55</v>
       </c>
@@ -21219,7 +21220,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" hidden="1">
       <c r="A57">
         <v>56</v>
       </c>
@@ -21239,7 +21240,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" hidden="1">
       <c r="A58">
         <v>57</v>
       </c>
@@ -21259,7 +21260,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" hidden="1">
       <c r="A59">
         <v>58</v>
       </c>
@@ -21279,7 +21280,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" hidden="1">
       <c r="A60">
         <v>59</v>
       </c>
@@ -21299,7 +21300,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" hidden="1">
       <c r="A61">
         <v>60</v>
       </c>
@@ -21319,7 +21320,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" hidden="1">
       <c r="A62">
         <v>61</v>
       </c>
@@ -21339,7 +21340,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" hidden="1">
       <c r="A63">
         <v>62</v>
       </c>
@@ -21359,7 +21360,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" hidden="1">
       <c r="A64">
         <v>63</v>
       </c>
@@ -21379,7 +21380,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" hidden="1">
       <c r="A65">
         <v>64</v>
       </c>
@@ -21399,7 +21400,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" hidden="1">
       <c r="A66">
         <v>65</v>
       </c>
@@ -21419,7 +21420,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" hidden="1">
       <c r="A67">
         <v>66</v>
       </c>
@@ -21439,7 +21440,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" hidden="1">
       <c r="A68">
         <v>67</v>
       </c>
@@ -21459,7 +21460,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" hidden="1">
       <c r="A69">
         <v>68</v>
       </c>
@@ -21479,7 +21480,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" hidden="1">
       <c r="A70">
         <v>69</v>
       </c>
@@ -21499,7 +21500,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" hidden="1">
       <c r="A71">
         <v>70</v>
       </c>
@@ -21519,7 +21520,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" hidden="1">
       <c r="A72">
         <v>71</v>
       </c>
@@ -21539,7 +21540,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" hidden="1">
       <c r="A73">
         <v>72</v>
       </c>
@@ -21559,7 +21560,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" hidden="1">
       <c r="A74">
         <v>73</v>
       </c>
@@ -21579,7 +21580,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" hidden="1">
       <c r="A75">
         <v>74</v>
       </c>
@@ -21599,7 +21600,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" hidden="1">
       <c r="A76">
         <v>75</v>
       </c>
@@ -21619,7 +21620,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" hidden="1">
       <c r="A77">
         <v>76</v>
       </c>
@@ -21639,7 +21640,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" hidden="1">
       <c r="A78">
         <v>77</v>
       </c>
@@ -21659,7 +21660,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" hidden="1">
       <c r="A79">
         <v>78</v>
       </c>
@@ -21679,7 +21680,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" hidden="1">
       <c r="A80">
         <v>79</v>
       </c>
@@ -21699,7 +21700,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" hidden="1">
       <c r="A81">
         <v>80</v>
       </c>
@@ -21719,7 +21720,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" hidden="1">
       <c r="A82">
         <v>81</v>
       </c>
@@ -21739,7 +21740,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" hidden="1">
       <c r="A83">
         <v>82</v>
       </c>
@@ -21759,7 +21760,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" hidden="1">
       <c r="A84">
         <v>83</v>
       </c>
@@ -21779,7 +21780,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" hidden="1">
       <c r="A85">
         <v>84</v>
       </c>
@@ -21799,7 +21800,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" hidden="1">
       <c r="A86">
         <v>85</v>
       </c>
@@ -21819,7 +21820,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" hidden="1">
       <c r="A87">
         <v>86</v>
       </c>
@@ -21839,7 +21840,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" hidden="1">
       <c r="A88">
         <v>87</v>
       </c>
@@ -21859,7 +21860,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" hidden="1">
       <c r="A89">
         <v>88</v>
       </c>
@@ -21879,7 +21880,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" hidden="1">
       <c r="A90">
         <v>89</v>
       </c>
@@ -21899,7 +21900,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" hidden="1">
       <c r="A91">
         <v>90</v>
       </c>
@@ -21919,7 +21920,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" hidden="1">
       <c r="A92">
         <v>91</v>
       </c>
@@ -21939,7 +21940,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" hidden="1">
       <c r="A93">
         <v>92</v>
       </c>
@@ -21959,7 +21960,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" hidden="1">
       <c r="A94">
         <v>93</v>
       </c>
@@ -21979,7 +21980,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" hidden="1">
       <c r="A95">
         <v>94</v>
       </c>
@@ -21999,7 +22000,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" hidden="1">
       <c r="A96">
         <v>95</v>
       </c>
@@ -22019,7 +22020,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" hidden="1">
       <c r="A97">
         <v>96</v>
       </c>
@@ -22039,7 +22040,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" hidden="1">
       <c r="A98">
         <v>97</v>
       </c>
@@ -22059,7 +22060,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" hidden="1">
       <c r="A99">
         <v>98</v>
       </c>
@@ -22079,7 +22080,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" hidden="1">
       <c r="A100">
         <v>99</v>
       </c>
@@ -22099,7 +22100,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" hidden="1">
       <c r="A101">
         <v>100</v>
       </c>
@@ -22119,7 +22120,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" hidden="1">
       <c r="A102">
         <v>101</v>
       </c>
@@ -22139,7 +22140,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" hidden="1">
       <c r="A103">
         <v>102</v>
       </c>
@@ -22159,7 +22160,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" hidden="1">
       <c r="A104">
         <v>103</v>
       </c>
@@ -22179,7 +22180,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" hidden="1">
       <c r="A105">
         <v>104</v>
       </c>
@@ -22199,7 +22200,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" hidden="1">
       <c r="A106">
         <v>105</v>
       </c>
@@ -22219,7 +22220,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" hidden="1">
       <c r="A107">
         <v>106</v>
       </c>
@@ -22239,7 +22240,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" hidden="1">
       <c r="A108">
         <v>107</v>
       </c>
@@ -22259,7 +22260,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" hidden="1">
       <c r="A109">
         <v>108</v>
       </c>
@@ -22279,7 +22280,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" hidden="1">
       <c r="A110">
         <v>109</v>
       </c>
@@ -22299,7 +22300,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" hidden="1">
       <c r="A111">
         <v>110</v>
       </c>
@@ -22319,7 +22320,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" hidden="1">
       <c r="A112">
         <v>111</v>
       </c>
@@ -22339,7 +22340,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" hidden="1">
       <c r="A113">
         <v>112</v>
       </c>
@@ -22359,7 +22360,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" hidden="1">
       <c r="A114">
         <v>113</v>
       </c>
@@ -22379,7 +22380,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" hidden="1">
       <c r="A115">
         <v>114</v>
       </c>
@@ -22399,7 +22400,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" hidden="1">
       <c r="A116">
         <v>115</v>
       </c>
@@ -22419,7 +22420,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" hidden="1">
       <c r="A117">
         <v>116</v>
       </c>
@@ -22439,7 +22440,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" hidden="1">
       <c r="A118">
         <v>117</v>
       </c>
@@ -22459,7 +22460,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" hidden="1">
       <c r="A119">
         <v>118</v>
       </c>
@@ -22479,7 +22480,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" hidden="1">
       <c r="A120">
         <v>119</v>
       </c>
@@ -22499,7 +22500,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" hidden="1">
       <c r="A121">
         <v>120</v>
       </c>
@@ -22519,7 +22520,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" hidden="1">
       <c r="A122">
         <v>121</v>
       </c>
@@ -22539,7 +22540,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" hidden="1">
       <c r="A123">
         <v>122</v>
       </c>
@@ -22559,7 +22560,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" hidden="1">
       <c r="A124">
         <v>123</v>
       </c>
@@ -22579,7 +22580,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" hidden="1">
       <c r="A125">
         <v>124</v>
       </c>
@@ -22599,7 +22600,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" hidden="1">
       <c r="A126">
         <v>125</v>
       </c>
@@ -22619,7 +22620,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" hidden="1">
       <c r="A127">
         <v>126</v>
       </c>
@@ -22639,7 +22640,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" hidden="1">
       <c r="A128">
         <v>127</v>
       </c>
@@ -22659,7 +22660,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" hidden="1">
       <c r="A129">
         <v>128</v>
       </c>
@@ -22679,7 +22680,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" hidden="1">
       <c r="A130">
         <v>129</v>
       </c>
@@ -22699,7 +22700,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" hidden="1">
       <c r="A131">
         <v>130</v>
       </c>
@@ -22719,7 +22720,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" hidden="1">
       <c r="A132">
         <v>131</v>
       </c>
@@ -22739,7 +22740,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" hidden="1">
       <c r="A133">
         <v>132</v>
       </c>
@@ -22759,7 +22760,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" hidden="1">
       <c r="A134">
         <v>133</v>
       </c>
@@ -22779,7 +22780,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" hidden="1">
       <c r="A135">
         <v>134</v>
       </c>
@@ -22799,7 +22800,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" hidden="1">
       <c r="A136">
         <v>135</v>
       </c>
@@ -22819,7 +22820,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" hidden="1">
       <c r="A137">
         <v>136</v>
       </c>
@@ -22839,7 +22840,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" hidden="1">
       <c r="A138">
         <v>137</v>
       </c>
@@ -22859,7 +22860,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" hidden="1">
       <c r="A139">
         <v>138</v>
       </c>
@@ -22879,7 +22880,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" hidden="1">
       <c r="A140">
         <v>139</v>
       </c>
@@ -22899,7 +22900,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" hidden="1">
       <c r="A141">
         <v>140</v>
       </c>
@@ -22919,7 +22920,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" hidden="1">
       <c r="A142">
         <v>141</v>
       </c>
@@ -22939,7 +22940,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" hidden="1">
       <c r="A143">
         <v>142</v>
       </c>
@@ -22959,7 +22960,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" hidden="1">
       <c r="A144">
         <v>143</v>
       </c>
@@ -22979,7 +22980,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" hidden="1">
       <c r="A145">
         <v>144</v>
       </c>
@@ -22999,7 +23000,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" hidden="1">
       <c r="A146">
         <v>145</v>
       </c>
@@ -23019,7 +23020,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" hidden="1">
       <c r="A147">
         <v>146</v>
       </c>
@@ -23039,7 +23040,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" hidden="1">
       <c r="A148">
         <v>147</v>
       </c>
@@ -23059,7 +23060,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" hidden="1">
       <c r="A149">
         <v>148</v>
       </c>
@@ -23079,7 +23080,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:6" hidden="1">
       <c r="A150">
         <v>149</v>
       </c>
@@ -23099,7 +23100,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" hidden="1">
       <c r="A151">
         <v>150</v>
       </c>
@@ -23119,7 +23120,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:6" hidden="1">
       <c r="A152">
         <v>151</v>
       </c>
@@ -23139,7 +23140,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:6" hidden="1">
       <c r="A153">
         <v>152</v>
       </c>
@@ -23159,7 +23160,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:6" hidden="1">
       <c r="A154">
         <v>153</v>
       </c>
@@ -23179,7 +23180,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:6" hidden="1">
       <c r="A155">
         <v>154</v>
       </c>
@@ -23199,7 +23200,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:6" hidden="1">
       <c r="A156">
         <v>155</v>
       </c>
@@ -23219,7 +23220,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
+    <row r="157" spans="1:6" hidden="1">
       <c r="A157">
         <v>156</v>
       </c>
@@ -23239,7 +23240,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:6" hidden="1">
       <c r="A158">
         <v>157</v>
       </c>
@@ -23259,7 +23260,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:6" hidden="1">
       <c r="A159">
         <v>158</v>
       </c>
@@ -23279,7 +23280,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" spans="1:6" hidden="1">
       <c r="A160">
         <v>159</v>
       </c>
@@ -23299,7 +23300,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" hidden="1">
       <c r="A161">
         <v>160</v>
       </c>
@@ -23319,7 +23320,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" hidden="1">
       <c r="A162">
         <v>161</v>
       </c>
@@ -23339,7 +23340,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" hidden="1">
       <c r="A163">
         <v>162</v>
       </c>
@@ -23359,7 +23360,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="164" spans="1:6">
+    <row r="164" spans="1:6" hidden="1">
       <c r="A164">
         <v>163</v>
       </c>
@@ -23379,7 +23380,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" hidden="1">
       <c r="A165">
         <v>164</v>
       </c>
@@ -23399,7 +23400,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:6" hidden="1">
       <c r="A166">
         <v>165</v>
       </c>
@@ -23419,7 +23420,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" hidden="1">
       <c r="A167">
         <v>166</v>
       </c>
@@ -23439,7 +23440,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="168" spans="1:6">
+    <row r="168" spans="1:6" hidden="1">
       <c r="A168">
         <v>167</v>
       </c>
@@ -23459,7 +23460,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="169" spans="1:6">
+    <row r="169" spans="1:6" hidden="1">
       <c r="A169">
         <v>168</v>
       </c>
@@ -23479,7 +23480,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="170" spans="1:6">
+    <row r="170" spans="1:6" hidden="1">
       <c r="A170">
         <v>169</v>
       </c>
@@ -23499,7 +23500,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" spans="1:6" hidden="1">
       <c r="A171">
         <v>170</v>
       </c>
@@ -23519,7 +23520,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="172" spans="1:6">
+    <row r="172" spans="1:6" hidden="1">
       <c r="A172">
         <v>171</v>
       </c>
@@ -23539,7 +23540,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="173" spans="1:6">
+    <row r="173" spans="1:6" hidden="1">
       <c r="A173">
         <v>172</v>
       </c>
@@ -23559,7 +23560,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="174" spans="1:6">
+    <row r="174" spans="1:6" hidden="1">
       <c r="A174">
         <v>173</v>
       </c>
@@ -23579,7 +23580,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="175" spans="1:6">
+    <row r="175" spans="1:6" hidden="1">
       <c r="A175">
         <v>174</v>
       </c>
@@ -23599,7 +23600,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="176" spans="1:6">
+    <row r="176" spans="1:6" hidden="1">
       <c r="A176">
         <v>175</v>
       </c>
@@ -23619,7 +23620,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:6" hidden="1">
       <c r="A177">
         <v>176</v>
       </c>
@@ -23639,7 +23640,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="178" spans="1:6">
+    <row r="178" spans="1:6" hidden="1">
       <c r="A178">
         <v>177</v>
       </c>
@@ -23659,7 +23660,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" spans="1:6" hidden="1">
       <c r="A179">
         <v>178</v>
       </c>
@@ -23679,7 +23680,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" spans="1:6" hidden="1">
       <c r="A180">
         <v>179</v>
       </c>
@@ -23699,7 +23700,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:6" hidden="1">
       <c r="A181">
         <v>180</v>
       </c>
@@ -23719,7 +23720,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="182" spans="1:6">
+    <row r="182" spans="1:6" hidden="1">
       <c r="A182">
         <v>181</v>
       </c>
@@ -23739,7 +23740,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:6" hidden="1">
       <c r="A183">
         <v>182</v>
       </c>
@@ -23759,7 +23760,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="184" spans="1:6">
+    <row r="184" spans="1:6" hidden="1">
       <c r="A184">
         <v>183</v>
       </c>
@@ -23779,7 +23780,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:6" hidden="1">
       <c r="A185">
         <v>184</v>
       </c>
@@ -23799,7 +23800,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:6" hidden="1">
       <c r="A186">
         <v>185</v>
       </c>
@@ -23819,7 +23820,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:6" hidden="1">
       <c r="A187">
         <v>186</v>
       </c>
@@ -23839,7 +23840,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:6" hidden="1">
       <c r="A188">
         <v>187</v>
       </c>
@@ -23859,7 +23860,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:6" hidden="1">
       <c r="A189">
         <v>188</v>
       </c>
@@ -23879,7 +23880,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
+    <row r="190" spans="1:6" hidden="1">
       <c r="A190">
         <v>189</v>
       </c>
@@ -23899,7 +23900,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:6" hidden="1">
       <c r="A191">
         <v>190</v>
       </c>
@@ -23919,7 +23920,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="192" spans="1:6">
+    <row r="192" spans="1:6" hidden="1">
       <c r="A192">
         <v>191</v>
       </c>
@@ -23939,7 +23940,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="193" spans="1:6">
+    <row r="193" spans="1:6" hidden="1">
       <c r="A193">
         <v>192</v>
       </c>
@@ -23959,7 +23960,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="194" spans="1:6">
+    <row r="194" spans="1:6" hidden="1">
       <c r="A194">
         <v>193</v>
       </c>
@@ -23979,7 +23980,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="195" spans="1:6">
+    <row r="195" spans="1:6" hidden="1">
       <c r="A195">
         <v>194</v>
       </c>
@@ -23999,7 +24000,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="196" spans="1:6">
+    <row r="196" spans="1:6" hidden="1">
       <c r="A196">
         <v>195</v>
       </c>
@@ -24019,7 +24020,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:6" hidden="1">
       <c r="A197">
         <v>196</v>
       </c>
@@ -24039,7 +24040,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="198" spans="1:6">
+    <row r="198" spans="1:6" hidden="1">
       <c r="A198">
         <v>197</v>
       </c>
@@ -24059,7 +24060,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="199" spans="1:6">
+    <row r="199" spans="1:6" hidden="1">
       <c r="A199">
         <v>198</v>
       </c>
@@ -24079,7 +24080,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="200" spans="1:6">
+    <row r="200" spans="1:6" hidden="1">
       <c r="A200">
         <v>199</v>
       </c>
@@ -24099,7 +24100,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="201" spans="1:6">
+    <row r="201" spans="1:6" hidden="1">
       <c r="A201">
         <v>200</v>
       </c>
@@ -24119,7 +24120,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="202" spans="1:6">
+    <row r="202" spans="1:6" hidden="1">
       <c r="A202">
         <v>201</v>
       </c>
@@ -24139,7 +24140,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="203" spans="1:6">
+    <row r="203" spans="1:6" hidden="1">
       <c r="A203">
         <v>202</v>
       </c>
@@ -24159,7 +24160,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="204" spans="1:6">
+    <row r="204" spans="1:6" hidden="1">
       <c r="A204">
         <v>203</v>
       </c>
@@ -24179,7 +24180,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="205" spans="1:6">
+    <row r="205" spans="1:6" hidden="1">
       <c r="A205">
         <v>204</v>
       </c>
@@ -24199,7 +24200,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="206" spans="1:6">
+    <row r="206" spans="1:6" hidden="1">
       <c r="A206">
         <v>205</v>
       </c>
@@ -24219,7 +24220,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="207" spans="1:6">
+    <row r="207" spans="1:6" hidden="1">
       <c r="A207">
         <v>206</v>
       </c>
@@ -24239,7 +24240,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="208" spans="1:6">
+    <row r="208" spans="1:6" hidden="1">
       <c r="A208">
         <v>207</v>
       </c>
@@ -24259,7 +24260,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="209" spans="1:6">
+    <row r="209" spans="1:6" hidden="1">
       <c r="A209">
         <v>208</v>
       </c>
@@ -24279,7 +24280,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="210" spans="1:6">
+    <row r="210" spans="1:6" hidden="1">
       <c r="A210">
         <v>209</v>
       </c>
@@ -24299,7 +24300,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="211" spans="1:6">
+    <row r="211" spans="1:6" hidden="1">
       <c r="A211">
         <v>210</v>
       </c>
@@ -24319,7 +24320,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="212" spans="1:6">
+    <row r="212" spans="1:6" hidden="1">
       <c r="A212">
         <v>211</v>
       </c>
@@ -24339,7 +24340,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="213" spans="1:6">
+    <row r="213" spans="1:6" hidden="1">
       <c r="A213">
         <v>212</v>
       </c>
@@ -24359,7 +24360,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="214" spans="1:6">
+    <row r="214" spans="1:6" hidden="1">
       <c r="A214">
         <v>213</v>
       </c>
@@ -24379,7 +24380,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="215" spans="1:6">
+    <row r="215" spans="1:6" hidden="1">
       <c r="A215">
         <v>214</v>
       </c>
@@ -24716,7 +24717,7 @@
         <v>3</v>
       </c>
       <c r="E234">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F234" t="s">
         <v>187</v>
@@ -24733,7 +24734,7 @@
         <v>3</v>
       </c>
       <c r="E235">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F235" t="s">
         <v>187</v>
@@ -24750,7 +24751,7 @@
         <v>3</v>
       </c>
       <c r="E236">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F236" t="s">
         <v>187</v>
@@ -24767,7 +24768,7 @@
         <v>3</v>
       </c>
       <c r="E237">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F237" t="s">
         <v>187</v>
@@ -24784,7 +24785,7 @@
         <v>3</v>
       </c>
       <c r="E238">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="F238" t="s">
         <v>187</v>
@@ -24801,7 +24802,7 @@
         <v>3</v>
       </c>
       <c r="E239">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="F239" t="s">
         <v>187</v>
@@ -24818,7 +24819,7 @@
         <v>3</v>
       </c>
       <c r="E240">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F240" t="s">
         <v>187</v>
@@ -24835,7 +24836,7 @@
         <v>3</v>
       </c>
       <c r="E241">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F241" t="s">
         <v>187</v>
@@ -24852,14 +24853,20 @@
         <v>3</v>
       </c>
       <c r="E242">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F242" t="s">
         <v>188</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F242" xr:uid="{8EF0298B-43F7-F849-959B-1EFC1ADC8C4E}"/>
+  <autoFilter ref="A1:F242" xr:uid="{8EF0298B-43F7-F849-959B-1EFC1ADC8C4E}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="7"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Moved instruction text to bottom of choice.
Cleaned up grid true errors in the logs.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53824E0-9063-C542-8809-9F2693765E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B040A985-D5A7-CA49-8243-8A3EBC89762B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -41,6 +41,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Web Parameters Dev'!$B$1:$Y$88</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2686,6 +2687,24 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2714,15 +2733,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2736,15 +2746,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -15543,7 +15544,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>6.7182120023452363E-3</v>
+        <v>0.31357924229650602</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -15563,7 +15564,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.20513875168458628</v>
+        <v>0.76566313152276777</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -15584,7 +15585,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.10145717611392568</v>
+        <v>0.85892014412077189</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -15604,7 +15605,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.73850843011304423</v>
+        <v>0.21670298209662719</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -18154,16 +18155,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B26" r:id="rId1" xr:uid="{D2B54FA7-7284-A444-93E2-10BEB7DF1432}"/>
@@ -18203,105 +18204,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="100" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="94" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="94" t="s">
+      <c r="A2" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="100" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="101"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="95"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="103" t="s">
+      <c r="F2" s="101"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="109" t="s">
+      <c r="I2" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="109"/>
-      <c r="K2" s="109"/>
-      <c r="L2" s="109"/>
-      <c r="M2" s="109"/>
-      <c r="N2" s="109"/>
-      <c r="O2" s="109"/>
-      <c r="P2" s="109"/>
-      <c r="Q2" s="109"/>
-      <c r="R2" s="109" t="s">
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="112"/>
+      <c r="M2" s="112"/>
+      <c r="N2" s="112"/>
+      <c r="O2" s="112"/>
+      <c r="P2" s="112"/>
+      <c r="Q2" s="112"/>
+      <c r="R2" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="109"/>
-      <c r="T2" s="109"/>
-      <c r="U2" s="109"/>
-      <c r="V2" s="103" t="s">
+      <c r="S2" s="112"/>
+      <c r="T2" s="112"/>
+      <c r="U2" s="112"/>
+      <c r="V2" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="103" t="s">
+      <c r="W2" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="111" t="s">
+      <c r="X2" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="111" t="s">
+      <c r="Y2" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="111" t="s">
+      <c r="Z2" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="111" t="s">
+      <c r="AA2" s="94" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="101"/>
-      <c r="B3" s="97"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="110" t="s">
+      <c r="A3" s="107"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="108"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="108" t="s">
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108" t="s">
+      <c r="M3" s="111"/>
+      <c r="N3" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108" t="s">
+      <c r="O3" s="111"/>
+      <c r="P3" s="111" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="106" t="s">
+      <c r="Q3" s="111"/>
+      <c r="R3" s="109" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="106" t="s">
+      <c r="S3" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="106" t="s">
+      <c r="T3" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="106" t="s">
+      <c r="U3" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="104"/>
-      <c r="W3" s="104"/>
-      <c r="X3" s="112"/>
-      <c r="Y3" s="112"/>
-      <c r="Z3" s="112"/>
-      <c r="AA3" s="112"/>
+      <c r="V3" s="98"/>
+      <c r="W3" s="98"/>
+      <c r="X3" s="95"/>
+      <c r="Y3" s="95"/>
+      <c r="Z3" s="95"/>
+      <c r="AA3" s="95"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="102"/>
+      <c r="A4" s="108"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -18320,7 +18321,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="105"/>
+      <c r="H4" s="99"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -18348,16 +18349,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="107"/>
-      <c r="S4" s="107"/>
-      <c r="T4" s="107"/>
-      <c r="U4" s="107"/>
-      <c r="V4" s="105"/>
-      <c r="W4" s="105"/>
-      <c r="X4" s="113"/>
-      <c r="Y4" s="113"/>
-      <c r="Z4" s="113"/>
-      <c r="AA4" s="112"/>
+      <c r="R4" s="110"/>
+      <c r="S4" s="110"/>
+      <c r="T4" s="110"/>
+      <c r="U4" s="110"/>
+      <c r="V4" s="99"/>
+      <c r="W4" s="99"/>
+      <c r="X4" s="96"/>
+      <c r="Y4" s="96"/>
+      <c r="Z4" s="96"/>
+      <c r="AA4" s="95"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -18858,11 +18859,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -18878,6 +18874,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Dynamic text doesn't jump around.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B040A985-D5A7-CA49-8243-8A3EBC89762B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A94602-9D25-5B4A-8DC8-BA2A5CC8AB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -23622,7 +23622,7 @@
   <dimension ref="A1:AD16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Cypress tests working for word treatment.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10602"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A94602-9D25-5B4A-8DC8-BA2A5CC8AB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5442FE-3FB0-184F-9CB8-FC289B7D63BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="17120" yWindow="4100" windowWidth="34560" windowHeight="21100" activeTab="3" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
@@ -41,7 +41,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Web Parameters Dev'!$B$1:$Y$88</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2550,7 +2549,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2747,6 +2746,13 @@
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -15544,7 +15550,7 @@
       <c r="F2" s="66"/>
       <c r="G2">
         <f ca="1">RAND()</f>
-        <v>0.31357924229650602</v>
+        <v>0.92259223604596774</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -15564,7 +15570,7 @@
       <c r="F3" s="66"/>
       <c r="G3">
         <f ca="1">RAND()</f>
-        <v>0.76566313152276777</v>
+        <v>0.11887214186883766</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -15585,7 +15591,7 @@
       <c r="F4" s="66"/>
       <c r="G4">
         <f ca="1">RAND()</f>
-        <v>0.85892014412077189</v>
+        <v>5.2246186673260087E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -15605,7 +15611,7 @@
       <c r="F5" s="66"/>
       <c r="G5">
         <f ca="1">RAND()</f>
-        <v>0.21670298209662719</v>
+        <v>0.23670399157412247</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -23621,8 +23627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAA32EA-3DA8-BD44-8758-9048DFA42915}">
   <dimension ref="A1:AD16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="128" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AC7" sqref="AC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -23821,454 +23827,457 @@
         <v>661</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="17">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:30" s="5" customFormat="1" ht="17">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>662</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="114" t="s">
         <v>659</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="114" t="s">
         <v>708</v>
       </c>
-      <c r="I3" s="36">
+      <c r="I3" s="115">
         <v>44922</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="J3" s="115"/>
+      <c r="K3" s="5">
+        <v>1</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="5" t="s">
         <v>677</v>
       </c>
-      <c r="N3" s="82">
+      <c r="N3" s="116">
         <v>1.5</v>
       </c>
-      <c r="O3" s="82" t="s">
+      <c r="O3" s="116" t="s">
         <v>680</v>
       </c>
-      <c r="P3" s="82" t="s">
+      <c r="P3" s="116" t="s">
         <v>682</v>
       </c>
-      <c r="Q3" s="82" t="s">
+      <c r="Q3" s="116" t="s">
         <v>684</v>
       </c>
-      <c r="R3" s="82" t="s">
+      <c r="R3" s="116" t="s">
         <v>686</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="5" t="s">
         <v>688</v>
       </c>
-      <c r="T3" s="83" t="s">
+      <c r="T3" s="117" t="s">
         <v>690</v>
       </c>
-      <c r="U3" s="83" t="s">
+      <c r="U3" s="117" t="s">
         <v>692</v>
       </c>
-      <c r="V3" s="83" t="s">
+      <c r="V3" s="117" t="s">
         <v>694</v>
       </c>
-      <c r="W3" s="83" t="s">
+      <c r="W3" s="117" t="s">
         <v>696</v>
       </c>
-      <c r="X3" s="83" t="s">
+      <c r="X3" s="117" t="s">
         <v>698</v>
       </c>
-      <c r="Y3" s="83" t="s">
+      <c r="Y3" s="117" t="s">
         <v>700</v>
       </c>
-      <c r="Z3" s="83" t="s">
+      <c r="Z3" s="117" t="s">
         <v>701</v>
       </c>
-      <c r="AA3" s="83" t="s">
+      <c r="AA3" s="117" t="s">
         <v>704</v>
       </c>
-      <c r="AB3" s="83" t="s">
+      <c r="AB3" s="117" t="s">
         <v>706</v>
       </c>
-      <c r="AC3" s="81" t="s">
+      <c r="AC3" s="118" t="s">
         <v>654</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AD3" s="5" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="17">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:30" s="5" customFormat="1" ht="17">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>663</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="114" t="s">
         <v>659</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="114" t="s">
         <v>708</v>
       </c>
-      <c r="I4" s="36">
+      <c r="I4" s="115">
         <v>44940</v>
       </c>
-      <c r="K4">
+      <c r="J4" s="115"/>
+      <c r="K4" s="5">
         <v>3</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="5" t="s">
         <v>677</v>
       </c>
-      <c r="N4" s="82">
+      <c r="N4" s="116">
         <v>1.5</v>
       </c>
-      <c r="O4" s="82" t="s">
+      <c r="O4" s="116" t="s">
         <v>680</v>
       </c>
-      <c r="P4" s="82" t="s">
+      <c r="P4" s="116" t="s">
         <v>682</v>
       </c>
-      <c r="Q4" s="82" t="s">
+      <c r="Q4" s="116" t="s">
         <v>684</v>
       </c>
-      <c r="R4" s="82" t="s">
+      <c r="R4" s="116" t="s">
         <v>686</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" s="5" t="s">
         <v>688</v>
       </c>
-      <c r="T4" s="83" t="s">
+      <c r="T4" s="117" t="s">
         <v>690</v>
       </c>
-      <c r="U4" s="83" t="s">
+      <c r="U4" s="117" t="s">
         <v>692</v>
       </c>
-      <c r="V4" s="83" t="s">
+      <c r="V4" s="117" t="s">
         <v>694</v>
       </c>
-      <c r="W4" s="83" t="s">
+      <c r="W4" s="117" t="s">
         <v>696</v>
       </c>
-      <c r="X4" s="83" t="s">
+      <c r="X4" s="117" t="s">
         <v>698</v>
       </c>
-      <c r="Y4" s="83" t="s">
+      <c r="Y4" s="117" t="s">
         <v>700</v>
       </c>
-      <c r="Z4" s="83" t="s">
+      <c r="Z4" s="117" t="s">
         <v>701</v>
       </c>
-      <c r="AA4" s="83" t="s">
+      <c r="AA4" s="117" t="s">
         <v>704</v>
       </c>
-      <c r="AB4" s="83" t="s">
+      <c r="AB4" s="117" t="s">
         <v>706</v>
       </c>
-      <c r="AC4" s="81" t="s">
+      <c r="AC4" s="118" t="s">
         <v>655</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AD4" s="5" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="17">
-      <c r="A5">
+    <row r="5" spans="1:30" s="5" customFormat="1" ht="17">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>664</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>26</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="114" t="s">
         <v>659</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="114" t="s">
         <v>708</v>
       </c>
-      <c r="I5" s="36">
+      <c r="I5" s="115">
         <v>44942</v>
       </c>
-      <c r="K5">
+      <c r="J5" s="115"/>
+      <c r="K5" s="5">
         <v>26</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="5" t="s">
         <v>677</v>
       </c>
-      <c r="N5" s="82">
+      <c r="N5" s="116">
         <v>1.5</v>
       </c>
-      <c r="O5" s="82" t="s">
+      <c r="O5" s="116" t="s">
         <v>680</v>
       </c>
-      <c r="P5" s="82" t="s">
+      <c r="P5" s="116" t="s">
         <v>682</v>
       </c>
-      <c r="Q5" s="82" t="s">
+      <c r="Q5" s="116" t="s">
         <v>684</v>
       </c>
-      <c r="R5" s="82" t="s">
+      <c r="R5" s="116" t="s">
         <v>686</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5" s="5" t="s">
         <v>688</v>
       </c>
-      <c r="T5" s="83" t="s">
+      <c r="T5" s="117" t="s">
         <v>690</v>
       </c>
-      <c r="U5" s="83" t="s">
+      <c r="U5" s="117" t="s">
         <v>692</v>
       </c>
-      <c r="V5" s="83" t="s">
+      <c r="V5" s="117" t="s">
         <v>694</v>
       </c>
-      <c r="W5" s="83" t="s">
+      <c r="W5" s="117" t="s">
         <v>696</v>
       </c>
-      <c r="X5" s="83" t="s">
+      <c r="X5" s="117" t="s">
         <v>698</v>
       </c>
-      <c r="Y5" s="83" t="s">
+      <c r="Y5" s="117" t="s">
         <v>700</v>
       </c>
-      <c r="Z5" s="83" t="s">
+      <c r="Z5" s="117" t="s">
         <v>701</v>
       </c>
-      <c r="AA5" s="83" t="s">
+      <c r="AA5" s="117" t="s">
         <v>704</v>
       </c>
-      <c r="AB5" s="83" t="s">
+      <c r="AB5" s="117" t="s">
         <v>706</v>
       </c>
-      <c r="AC5" s="81" t="s">
+      <c r="AC5" s="118" t="s">
         <v>655</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AD5" s="5" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="17">
-      <c r="A6">
+    <row r="6" spans="1:30" s="5" customFormat="1" ht="17">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>665</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>100</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="5">
         <v>100</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="114" t="s">
         <v>659</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="114" t="s">
         <v>708</v>
       </c>
-      <c r="I6" s="36">
+      <c r="I6" s="115">
         <v>44994</v>
       </c>
-      <c r="J6" s="36">
+      <c r="J6" s="115">
         <v>44995</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="5">
         <v>100</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="5" t="s">
         <v>677</v>
       </c>
-      <c r="N6" s="82">
+      <c r="N6" s="116">
         <v>1.5</v>
       </c>
-      <c r="O6" s="82" t="s">
+      <c r="O6" s="116" t="s">
         <v>680</v>
       </c>
-      <c r="P6" s="82" t="s">
+      <c r="P6" s="116" t="s">
         <v>682</v>
       </c>
-      <c r="Q6" s="82" t="s">
+      <c r="Q6" s="116" t="s">
         <v>684</v>
       </c>
-      <c r="R6" s="82" t="s">
+      <c r="R6" s="116" t="s">
         <v>686</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S6" s="5" t="s">
         <v>688</v>
       </c>
-      <c r="T6" s="83" t="s">
+      <c r="T6" s="117" t="s">
         <v>690</v>
       </c>
-      <c r="U6" s="83" t="s">
+      <c r="U6" s="117" t="s">
         <v>692</v>
       </c>
-      <c r="V6" s="83" t="s">
+      <c r="V6" s="117" t="s">
         <v>694</v>
       </c>
-      <c r="W6" s="83" t="s">
+      <c r="W6" s="117" t="s">
         <v>696</v>
       </c>
-      <c r="X6" s="83" t="s">
+      <c r="X6" s="117" t="s">
         <v>698</v>
       </c>
-      <c r="Y6" s="83" t="s">
+      <c r="Y6" s="117" t="s">
         <v>700</v>
       </c>
-      <c r="Z6" s="83" t="s">
+      <c r="Z6" s="117" t="s">
         <v>701</v>
       </c>
-      <c r="AA6" s="83" t="s">
+      <c r="AA6" s="117" t="s">
         <v>704</v>
       </c>
-      <c r="AB6" s="83" t="s">
+      <c r="AB6" s="117" t="s">
         <v>706</v>
       </c>
-      <c r="AC6" s="81" t="s">
+      <c r="AC6" s="118" t="s">
         <v>656</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AD6" s="5" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="17">
-      <c r="A7">
+    <row r="7" spans="1:30" s="5" customFormat="1" ht="17">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>666</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>449</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="5">
         <v>449</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="114" t="s">
         <v>659</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="114" t="s">
         <v>708</v>
       </c>
-      <c r="I7" s="36">
+      <c r="I7" s="115">
         <v>45119</v>
       </c>
-      <c r="J7" s="36">
+      <c r="J7" s="115">
         <v>45119</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="5">
         <v>150</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="5" t="s">
         <v>677</v>
       </c>
-      <c r="N7" s="82">
+      <c r="N7" s="116">
         <v>1.5</v>
       </c>
-      <c r="O7" s="82" t="s">
+      <c r="O7" s="116" t="s">
         <v>680</v>
       </c>
-      <c r="P7" s="82" t="s">
+      <c r="P7" s="116" t="s">
         <v>682</v>
       </c>
-      <c r="Q7" s="82" t="s">
+      <c r="Q7" s="116" t="s">
         <v>684</v>
       </c>
-      <c r="R7" s="82" t="s">
+      <c r="R7" s="116" t="s">
         <v>686</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S7" s="5" t="s">
         <v>688</v>
       </c>
-      <c r="T7" s="83" t="s">
+      <c r="T7" s="117" t="s">
         <v>690</v>
       </c>
-      <c r="U7" s="83" t="s">
+      <c r="U7" s="117" t="s">
         <v>692</v>
       </c>
-      <c r="V7" s="83" t="s">
+      <c r="V7" s="117" t="s">
         <v>694</v>
       </c>
-      <c r="W7" s="83" t="s">
+      <c r="W7" s="117" t="s">
         <v>696</v>
       </c>
-      <c r="X7" s="83" t="s">
+      <c r="X7" s="117" t="s">
         <v>698</v>
       </c>
-      <c r="Y7" s="83" t="s">
+      <c r="Y7" s="117" t="s">
         <v>700</v>
       </c>
-      <c r="Z7" s="83" t="s">
+      <c r="Z7" s="117" t="s">
         <v>701</v>
       </c>
-      <c r="AA7" s="83" t="s">
+      <c r="AA7" s="117" t="s">
         <v>704</v>
       </c>
-      <c r="AB7" s="83" t="s">
+      <c r="AB7" s="117" t="s">
         <v>706</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AC7" s="5" t="s">
         <v>657</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AD7" s="5" t="s">
         <v>263</v>
       </c>
     </row>
@@ -24384,7 +24393,7 @@
         <v>226</v>
       </c>
       <c r="K9">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="L9" t="s">
         <v>260</v>

</xml_diff>